<commit_message>
Added new illustrations for vscom
</commit_message>
<xml_diff>
--- a/src/assets/data.xlsx
+++ b/src/assets/data.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="283">
   <si>
     <t>SeattleSkyline</t>
   </si>
@@ -824,6 +824,60 @@
   </si>
   <si>
     <t>A person looking through a telescope. Used for no results match/found pattern.</t>
+  </si>
+  <si>
+    <t>hero-extend-vside</t>
+  </si>
+  <si>
+    <t>swimlane-create-your-own-extension</t>
+  </si>
+  <si>
+    <t>swimlane-marketplace</t>
+  </si>
+  <si>
+    <t>swimlane-partner-program</t>
+  </si>
+  <si>
+    <t>swimlane-what-are-extensions</t>
+  </si>
+  <si>
+    <t>vscom</t>
+  </si>
+  <si>
+    <t>hero</t>
+  </si>
+  <si>
+    <t>swimlane</t>
+  </si>
+  <si>
+    <t>monitor computer code ide extension build extend vside robot arm tools construction</t>
+  </si>
+  <si>
+    <t>Robot arms building extensions into Visual Studio IDE.</t>
+  </si>
+  <si>
+    <t>tools toolbox hammer wrench pen work cloud clipboard</t>
+  </si>
+  <si>
+    <t>A toolbox with some tools and a cloud.</t>
+  </si>
+  <si>
+    <t>marketplace store shop market storefront</t>
+  </si>
+  <si>
+    <t>Used to represent Visual Studio Marketplace.</t>
+  </si>
+  <si>
+    <t>Four people riding on a bike. Used for Visual Studio Partner Program.</t>
+  </si>
+  <si>
+    <t>team collaboration people bike bicycle engineer businessmen doctor man woman developer hardhat lab coat</t>
+  </si>
+  <si>
+    <t>extension plugin plug puzzle extend addon people woman man ladder gear chart clipboard task</t>
+  </si>
+  <si>
+    <t>People putting plugins together. Used to represent Visual Studio extensions.</t>
   </si>
 </sst>
 </file>
@@ -1663,15 +1717,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>171450</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1428750</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>1257300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1700,8 +1754,258 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="590550" y="19183350"/>
-          <a:ext cx="1428750" cy="1428750"/>
+          <a:off x="762000" y="19183350"/>
+          <a:ext cx="1257300" cy="1257300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>86541</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>59336</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0DF9087C-ABD6-4BCA-B3F0-C7DD22EFD7C3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="677091" y="20497799"/>
+          <a:ext cx="2323284" cy="1278537"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>1136710</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0388BEDA-4736-45E2-BA24-8CDB23B80951}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="590550" y="21717000"/>
+          <a:ext cx="2409825" cy="1136710"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2322195</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>1095375</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{977FFDF0-9A86-41E7-ABEF-A29090E5B301}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="590550" y="22983825"/>
+          <a:ext cx="2322195" cy="1095375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>32385</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>1143000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E8398A7-AB95-43B4-B7DB-70D3F3088FCF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="590550" y="24250650"/>
+          <a:ext cx="2423160" cy="1143000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>72772</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>1162051</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C947040E-E0E8-41A7-A058-75992C4D36F1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="590551" y="25517476"/>
+          <a:ext cx="2463546" cy="1162050"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4533,13 +4837,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I2" sqref="I2:I17"/>
+      <selection pane="bottomRight" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4609,7 +4913,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="2" t="str">
-        <f t="shared" ref="I2:I17" si="0">SUBSTITUTE(_xlfn.CONCAT("{'id':",A2,",'title':'",C2,"','group':'",D2,"','area':'",E2,"','keywords':['",SUBSTITUTE(F2," ","','"),"'],'description':'",G2,"','publish':",H2,"}"),"'","""")</f>
+        <f t="shared" ref="I2:I22" si="0">SUBSTITUTE(_xlfn.CONCAT("{'id':",A2,",'title':'",C2,"','group':'",D2,"','area':'",E2,"','keywords':['",SUBSTITUTE(F2," ","','"),"'],'description':'",G2,"','publish':",H2,"}"),"'","""")</f>
         <v>{"id":1,"title":"general-something-wrong-on-server","group":"general","area":"common","keywords":["server","computer","tower","error","disconnect","problem"],"description":"One of three servers is down. Indicates that there is something wrong on the server side.","publish":1}</v>
       </c>
     </row>
@@ -5016,6 +5320,141 @@
       <c r="I17" s="2" t="str">
         <f t="shared" si="0"/>
         <v>{"id":16,"title":"general-no-results-found","group":"general","area":"common","keywords":["person","telescope","explore","find","search"],"description":"A person looking through a telescope. Used for no results match/found pattern.","publish":1}</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>17</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="D18" t="s">
+        <v>270</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="H18" s="2">
+        <v>1</v>
+      </c>
+      <c r="I18" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":17,"title":"hero-extend-vside","group":"vscom","area":"hero","keywords":["monitor","computer","code","ide","extension","build","extend","vside","robot","arm","tools","construction"],"description":"Robot arms building extensions into Visual Studio IDE.","publish":1}</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>18</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D19" t="s">
+        <v>270</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="H19" s="2">
+        <v>1</v>
+      </c>
+      <c r="I19" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":18,"title":"swimlane-create-your-own-extension","group":"vscom","area":"swimlane","keywords":["tools","toolbox","hammer","wrench","pen","work","cloud","clipboard"],"description":"A toolbox with some tools and a cloud.","publish":1}</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>19</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="D20" t="s">
+        <v>270</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="H20" s="2">
+        <v>1</v>
+      </c>
+      <c r="I20" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":19,"title":"swimlane-marketplace","group":"vscom","area":"swimlane","keywords":["marketplace","store","shop","market","storefront"],"description":"Used to represent Visual Studio Marketplace.","publish":1}</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>20</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="D21" t="s">
+        <v>270</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="H21" s="2">
+        <v>1</v>
+      </c>
+      <c r="I21" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":20,"title":"swimlane-partner-program","group":"vscom","area":"swimlane","keywords":["team","collaboration","people","bike","bicycle","engineer","businessmen","doctor","man","woman","developer","hardhat","lab","coat"],"description":"Four people riding on a bike. Used for Visual Studio Partner Program.","publish":1}</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>21</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="D22" t="s">
+        <v>270</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="H22" s="2">
+        <v>1</v>
+      </c>
+      <c r="I22" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":21,"title":"swimlane-what-are-extensions","group":"vscom","area":"swimlane","keywords":["extension","plugin","plug","puzzle","extend","addon","people","woman","man","ladder","gear","chart","clipboard","task"],"description":"People putting plugins together. Used to represent Visual Studio extensions.","publish":1}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new illustrations for VSTS
</commit_message>
<xml_diff>
--- a/src/assets/data.xlsx
+++ b/src/assets/data.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="290">
   <si>
     <t>SeattleSkyline</t>
   </si>
@@ -878,6 +878,27 @@
   </si>
   <si>
     <t>People putting plugins together. Used to represent Visual Studio extensions.</t>
+  </si>
+  <si>
+    <t>zerodata-add-product</t>
+  </si>
+  <si>
+    <t>zerodata-configure-component-governance</t>
+  </si>
+  <si>
+    <t>compliance</t>
+  </si>
+  <si>
+    <t>product box woman package label</t>
+  </si>
+  <si>
+    <t>A woman putting shipping label on a product box. Used to represent add a product.</t>
+  </si>
+  <si>
+    <t>A product box going through x-ray scan. Used to represent configure component governance.</t>
+  </si>
+  <si>
+    <t>product box scan xray package compliance screen component governance</t>
   </si>
 </sst>
 </file>
@@ -1917,15 +1938,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>139032</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>65580</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>32385</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>1143000</xdr:rowOff>
+      <xdr:rowOff>1142999</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1954,8 +1975,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="590550" y="24250650"/>
-          <a:ext cx="2423160" cy="1143000"/>
+          <a:off x="1024857" y="24316230"/>
+          <a:ext cx="2284128" cy="1077419"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1967,13 +1988,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
+      <xdr:colOff>141349</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>72772</xdr:colOff>
+      <xdr:colOff>72771</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>1162051</xdr:rowOff>
     </xdr:to>
@@ -2004,8 +2025,108 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="590551" y="25517476"/>
-          <a:ext cx="2463546" cy="1162050"/>
+          <a:off x="1027174" y="25584150"/>
+          <a:ext cx="2322197" cy="1095376"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>115570</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2200275</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>2564</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6140668B-9905-493F-BF3C-C9F98F48D2A4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1001395" y="26850975"/>
+          <a:ext cx="2084705" cy="1202714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2247900</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>1204232</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{919D8921-241D-4C71-BE4C-E10AFE713B94}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="590550" y="28051125"/>
+          <a:ext cx="2247900" cy="1204232"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4837,18 +4958,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H16" sqref="H16"/>
+      <selection pane="bottomRight" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="7" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" style="7" customWidth="1"/>
     <col min="2" max="2" width="35.85546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="38.140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
@@ -4913,7 +5034,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="2" t="str">
-        <f t="shared" ref="I2:I22" si="0">SUBSTITUTE(_xlfn.CONCAT("{'id':",A2,",'title':'",C2,"','group':'",D2,"','area':'",E2,"','keywords':['",SUBSTITUTE(F2," ","','"),"'],'description':'",G2,"','publish':",H2,"}"),"'","""")</f>
+        <f t="shared" ref="I2:I24" si="0">SUBSTITUTE(_xlfn.CONCAT("{'id':",A2,",'title':'",C2,"','group':'",D2,"','area':'",E2,"','keywords':['",SUBSTITUTE(F2," ","','"),"'],'description':'",G2,"','publish':",H2,"}"),"'","""")</f>
         <v>{"id":1,"title":"general-something-wrong-on-server","group":"general","area":"common","keywords":["server","computer","tower","error","disconnect","problem"],"description":"One of three servers is down. Indicates that there is something wrong on the server side.","publish":1}</v>
       </c>
     </row>
@@ -5455,6 +5576,60 @@
       <c r="I22" s="2" t="str">
         <f t="shared" si="0"/>
         <v>{"id":21,"title":"swimlane-what-are-extensions","group":"vscom","area":"swimlane","keywords":["extension","plugin","plug","puzzle","extend","addon","people","woman","man","ladder","gear","chart","clipboard","task"],"description":"People putting plugins together. Used to represent Visual Studio extensions.","publish":1}</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>22</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="D23" t="s">
+        <v>246</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="H23" s="2">
+        <v>1</v>
+      </c>
+      <c r="I23" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":22,"title":"zerodata-add-product","group":"zerodata","area":"compliance","keywords":["product","box","woman","package","label"],"description":"A woman putting shipping label on a product box. Used to represent add a product.","publish":1}</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>23</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="D24" t="s">
+        <v>246</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="H24" s="2">
+        <v>1</v>
+      </c>
+      <c r="I24" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":23,"title":"zerodata-configure-component-governance","group":"zerodata","area":"compliance","keywords":["product","box","scan","xray","package","compliance","screen","component","governance"],"description":"A product box going through x-ray scan. Used to represent configure component governance.","publish":1}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added some finalized illustrations for VSTS
</commit_message>
<xml_diff>
--- a/src/assets/data.xlsx
+++ b/src/assets/data.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="327">
   <si>
     <t>SeattleSkyline</t>
   </si>
@@ -899,6 +899,117 @@
   </si>
   <si>
     <t>product box scan xray package compliance screen component governance</t>
+  </si>
+  <si>
+    <t>zerodata-release-management</t>
+  </si>
+  <si>
+    <t>zerodata-this-repository-has-no-tags-yet</t>
+  </si>
+  <si>
+    <t>zerodata-add-deployment-group</t>
+  </si>
+  <si>
+    <t>zerodata-automate-build-definitions</t>
+  </si>
+  <si>
+    <t>zerodata-choose-a-template</t>
+  </si>
+  <si>
+    <t>zerodata-cloud-based-load-testing</t>
+  </si>
+  <si>
+    <t>zerodata-favorites</t>
+  </si>
+  <si>
+    <t>zerodata-get-everyone-on-same-page</t>
+  </si>
+  <si>
+    <t>zerodata-no-plan</t>
+  </si>
+  <si>
+    <t>zerodata-no-variable-groups</t>
+  </si>
+  <si>
+    <t>zerodata-pull-request</t>
+  </si>
+  <si>
+    <t>build</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>wiki</t>
+  </si>
+  <si>
+    <t>rocket release launch cloud</t>
+  </si>
+  <si>
+    <t>A rocket on a launch pad. Used for release management.</t>
+  </si>
+  <si>
+    <t>folder tag repository</t>
+  </si>
+  <si>
+    <t>A dotted line tag on a folder. Used to represent there is no tag on this repository.</t>
+  </si>
+  <si>
+    <t>server pin computer deployment group target</t>
+  </si>
+  <si>
+    <t>A map pin on a server. Used to represent targeted deployment group.</t>
+  </si>
+  <si>
+    <t>build robot arm box construction</t>
+  </si>
+  <si>
+    <t>A robot arm lifting building blocks. Used to represent build.</t>
+  </si>
+  <si>
+    <t>template shape cookie cutter star arrow diamond hexagon</t>
+  </si>
+  <si>
+    <t>A template with several shapes. Used in Build area for selecting templates.</t>
+  </si>
+  <si>
+    <t>cloud gauge stress test performance load test</t>
+  </si>
+  <si>
+    <t>A gauge on a cloud. Used for cloud based load testing.</t>
+  </si>
+  <si>
+    <t>favorite star box folder question chat work bullet list</t>
+  </si>
+  <si>
+    <t>Favorite star on frequently used work objects.</t>
+  </si>
+  <si>
+    <t>wiki page book people team knowledge share man woman</t>
+  </si>
+  <si>
+    <t>People sharing knowledge via wiki.</t>
+  </si>
+  <si>
+    <t>plan draft collaborate hands paper triangle tool ruler magnifier pen</t>
+  </si>
+  <si>
+    <t>Four hands holding tools and working on a drafting paper. Used when there is no plan for the current project.</t>
+  </si>
+  <si>
+    <t>variable group (x) box stack</t>
+  </si>
+  <si>
+    <t>Stacked blocks with variables. Used when there is no variable group.</t>
+  </si>
+  <si>
+    <t>code pull request people team</t>
+  </si>
+  <si>
+    <t>A person making pull request and asking for code review.</t>
   </si>
 </sst>
 </file>
@@ -2127,6 +2238,556 @@
         <a:xfrm>
           <a:off x="590550" y="28051125"/>
           <a:ext cx="2247900" cy="1204232"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1647825</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>1240300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A6C5CC5-D18C-4A32-B188-C04D09F027D8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1257300" y="29346526"/>
+          <a:ext cx="1276350" cy="1211724"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1590675</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>1147709</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BE21A94-C8F0-4FC7-9A99-EA4FE98B5D8E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1295400" y="30737175"/>
+          <a:ext cx="1181100" cy="995309"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>161926</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1558291</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>1209676</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BED2315-FAB2-4E58-8C19-D7ABFBF1F29C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1438275" y="32013526"/>
+          <a:ext cx="1005841" cy="1047750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1541653</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>1209676</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B1568B5-3143-4D3C-9A15-E7B5C85F32E7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1333500" y="33204151"/>
+          <a:ext cx="1093978" cy="1123950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1590675</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>1174227</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{483B9019-325C-40E4-84FC-D4F839232139}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1400175" y="34537650"/>
+          <a:ext cx="1076325" cy="1021827"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1937703</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>1133475</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04189C31-0992-4D4D-AF15-D73F86BDC125}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1123950" y="35823525"/>
+          <a:ext cx="1699578" cy="962025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1647825</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>1215070</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Picture 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AC4D5B5-3C0E-48BE-B47D-85924BBC7D25}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1304925" y="37023676"/>
+          <a:ext cx="1228725" cy="1110294"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1543050</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>1226127</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Picture 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D291E593-DB3E-46B3-ACA2-6A99462BB570}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1314450" y="38242875"/>
+          <a:ext cx="1114425" cy="1168977"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>466726</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1695450</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>1265490</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Picture 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F80B4C27-5043-4AD1-9925-E1C2119D073B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1352551" y="39481125"/>
+          <a:ext cx="1228724" cy="1236915"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>209551</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1809751</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>1237269</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Picture 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0754D54-C853-4AA9-9545-A3575506D428}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1095376" y="40719376"/>
+          <a:ext cx="1600200" cy="1237268"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1699768</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>1228725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="34" name="Picture 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D644A222-C555-4725-8C34-55E3A07A1E5F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1371600" y="42062400"/>
+          <a:ext cx="1213993" cy="1152525"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4958,13 +5619,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G23" sqref="G23"/>
+      <selection pane="bottomRight" activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5034,7 +5695,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="2" t="str">
-        <f t="shared" ref="I2:I24" si="0">SUBSTITUTE(_xlfn.CONCAT("{'id':",A2,",'title':'",C2,"','group':'",D2,"','area':'",E2,"','keywords':['",SUBSTITUTE(F2," ","','"),"'],'description':'",G2,"','publish':",H2,"}"),"'","""")</f>
+        <f t="shared" ref="I2:I35" si="0">SUBSTITUTE(_xlfn.CONCAT("{'id':",A2,",'title':'",C2,"','group':'",D2,"','area':'",E2,"','keywords':['",SUBSTITUTE(F2," ","','"),"'],'description':'",G2,"','publish':",H2,"}"),"'","""")</f>
         <v>{"id":1,"title":"general-something-wrong-on-server","group":"general","area":"common","keywords":["server","computer","tower","error","disconnect","problem"],"description":"One of three servers is down. Indicates that there is something wrong on the server side.","publish":1}</v>
       </c>
     </row>
@@ -5630,6 +6291,303 @@
       <c r="I24" s="2" t="str">
         <f t="shared" si="0"/>
         <v>{"id":23,"title":"zerodata-configure-component-governance","group":"zerodata","area":"compliance","keywords":["product","box","scan","xray","package","compliance","screen","component","governance"],"description":"A product box going through x-ray scan. Used to represent configure component governance.","publish":1}</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>290</v>
+      </c>
+      <c r="D25" t="s">
+        <v>246</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="H25" s="2">
+        <v>1</v>
+      </c>
+      <c r="I25" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":24,"title":"zerodata-release-management","group":"zerodata","area":"build","keywords":["rocket","release","launch","cloud"],"description":"A rocket on a launch pad. Used for release management.","publish":1}</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>291</v>
+      </c>
+      <c r="D26" t="s">
+        <v>246</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="H26" s="2">
+        <v>1</v>
+      </c>
+      <c r="I26" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":25,"title":"zerodata-this-repository-has-no-tags-yet","group":"zerodata","area":"code","keywords":["folder","tag","repository"],"description":"A dotted line tag on a folder. Used to represent there is no tag on this repository.","publish":1}</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>26</v>
+      </c>
+      <c r="C27" t="s">
+        <v>292</v>
+      </c>
+      <c r="D27" t="s">
+        <v>246</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="H27" s="2">
+        <v>1</v>
+      </c>
+      <c r="I27" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":26,"title":"zerodata-add-deployment-group","group":"zerodata","area":"build","keywords":["server","pin","computer","deployment","group","target"],"description":"A map pin on a server. Used to represent targeted deployment group.","publish":1}</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>27</v>
+      </c>
+      <c r="C28" t="s">
+        <v>293</v>
+      </c>
+      <c r="D28" t="s">
+        <v>246</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="H28" s="2">
+        <v>1</v>
+      </c>
+      <c r="I28" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":27,"title":"zerodata-automate-build-definitions","group":"zerodata","area":"build","keywords":["build","robot","arm","box","construction"],"description":"A robot arm lifting building blocks. Used to represent build.","publish":1}</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>28</v>
+      </c>
+      <c r="C29" t="s">
+        <v>294</v>
+      </c>
+      <c r="D29" t="s">
+        <v>246</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="H29" s="2">
+        <v>1</v>
+      </c>
+      <c r="I29" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":28,"title":"zerodata-choose-a-template","group":"zerodata","area":"build","keywords":["template","shape","cookie","cutter","star","arrow","diamond","hexagon"],"description":"A template with several shapes. Used in Build area for selecting templates.","publish":1}</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>29</v>
+      </c>
+      <c r="C30" t="s">
+        <v>295</v>
+      </c>
+      <c r="D30" t="s">
+        <v>246</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="H30" s="2">
+        <v>1</v>
+      </c>
+      <c r="I30" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":29,"title":"zerodata-cloud-based-load-testing","group":"zerodata","area":"test","keywords":["cloud","gauge","stress","test","performance","load","test"],"description":"A gauge on a cloud. Used for cloud based load testing.","publish":1}</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>30</v>
+      </c>
+      <c r="C31" t="s">
+        <v>296</v>
+      </c>
+      <c r="D31" t="s">
+        <v>246</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="H31" s="2">
+        <v>1</v>
+      </c>
+      <c r="I31" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":30,"title":"zerodata-favorites","group":"zerodata","area":"common","keywords":["favorite","star","box","folder","question","chat","work","bullet","list"],"description":"Favorite star on frequently used work objects.","publish":1}</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>31</v>
+      </c>
+      <c r="C32" t="s">
+        <v>297</v>
+      </c>
+      <c r="D32" t="s">
+        <v>246</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="H32" s="2">
+        <v>1</v>
+      </c>
+      <c r="I32" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":31,"title":"zerodata-get-everyone-on-same-page","group":"zerodata","area":"wiki","keywords":["wiki","page","book","people","team","knowledge","share","man","woman"],"description":"People sharing knowledge via wiki.","publish":1}</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>32</v>
+      </c>
+      <c r="C33" t="s">
+        <v>298</v>
+      </c>
+      <c r="D33" t="s">
+        <v>246</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="H33" s="2">
+        <v>1</v>
+      </c>
+      <c r="I33" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":32,"title":"zerodata-no-plan","group":"zerodata","area":"work","keywords":["plan","draft","collaborate","hands","paper","triangle","tool","ruler","magnifier","pen"],"description":"Four hands holding tools and working on a drafting paper. Used when there is no plan for the current project.","publish":1}</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>33</v>
+      </c>
+      <c r="C34" t="s">
+        <v>299</v>
+      </c>
+      <c r="D34" t="s">
+        <v>246</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="H34" s="2">
+        <v>1</v>
+      </c>
+      <c r="I34" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":33,"title":"zerodata-no-variable-groups","group":"zerodata","area":"build","keywords":["variable","group","(x)","box","stack"],"description":"Stacked blocks with variables. Used when there is no variable group.","publish":1}</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>34</v>
+      </c>
+      <c r="C35" t="s">
+        <v>300</v>
+      </c>
+      <c r="D35" t="s">
+        <v>246</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="H35" s="2">
+        <v>1</v>
+      </c>
+      <c r="I35" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":34,"title":"zerodata-pull-request","group":"zerodata","area":"code","keywords":["code","pull","request","people","team"],"description":"A person making pull request and asking for code review.","publish":1}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new illustration. Re-exported svg
</commit_message>
<xml_diff>
--- a/src/assets/data.xlsx
+++ b/src/assets/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwang\Dropbox\Code\vsimages\src\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cherr\Dropbox\Code\vsimages\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="378">
   <si>
     <t>SeattleSkyline</t>
   </si>
@@ -1154,6 +1154,15 @@
   </si>
   <si>
     <t>For assessments page zero data state.</t>
+  </si>
+  <si>
+    <t>zerodata-initializing-test-results</t>
+  </si>
+  <si>
+    <t>test initialize result beaker lab flask clock wait loading</t>
+  </si>
+  <si>
+    <t>Waiting screen image when test result is being loaded.</t>
   </si>
 </sst>
 </file>
@@ -3332,6 +3341,456 @@
         <a:xfrm>
           <a:off x="1009650" y="52158900"/>
           <a:ext cx="2000250" cy="1153990"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>600076</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1476376</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>1205593</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A117520-7BFF-4555-956F-F4F12EE9321C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1485901" y="53435250"/>
+          <a:ext cx="876300" cy="1157968"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>1257300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1494138</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>1181100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Picture 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4B8DD36-B7BB-4AB3-9BD8-E6299C82D81B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1285875" y="54644925"/>
+          <a:ext cx="1094088" cy="1190625"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>1257300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1495295</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>1209675</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="36" name="Picture 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E339EF8-50CB-49A6-BAEA-E50F688C18E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId45">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1228725" y="55911750"/>
+          <a:ext cx="1152395" cy="1219200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1485900</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>1204352</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="39" name="Picture 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACAB151F-DB08-413F-B4DF-DACC0B25471E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId46">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1352550" y="57283350"/>
+          <a:ext cx="1019175" cy="1109102"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1504950</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>1206874</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="41" name="Picture 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16B379D4-ADFE-41DC-9377-7A837B684A3B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId47">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1343025" y="58521600"/>
+          <a:ext cx="1047750" cy="1140199"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1419225</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>1188541</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="43" name="Picture 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FBC7F62-F415-4995-A726-CE2B5127E4FE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId48">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1343025" y="59797950"/>
+          <a:ext cx="962025" cy="1112341"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1593249</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>1209675</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="45" name="Picture 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90DB288E-3D7C-4826-A596-40C62026F44D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId49">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1428750" y="61055250"/>
+          <a:ext cx="1050324" cy="1143000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1924050</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>1163444</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="47" name="Picture 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54C2B3DA-6DE7-45D5-928F-1325341C524E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId50">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1104900" y="62379225"/>
+          <a:ext cx="1704975" cy="1039619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1764031</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>1171575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="49" name="Picture 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38F93CA9-3421-4B58-BAB0-ECCF30E6E5E9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId51">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1238250" y="63579375"/>
+          <a:ext cx="1411606" cy="1114425"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6163,13 +6622,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C50" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B47" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I51" sqref="I51"/>
+      <selection pane="bottomRight" activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6239,7 +6698,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="2" t="str">
-        <f t="shared" ref="I2:I51" si="0">SUBSTITUTE(_xlfn.CONCAT("{'id':",A2,",'title':'",C2,"','group':'",D2,"','area':'",E2,"','keywords':['",SUBSTITUTE(F2," ","','"),"'],'description':'",G2,"','publish':",H2,"}"),"'","""")</f>
+        <f t="shared" ref="I2:I52" si="0">SUBSTITUTE(_xlfn.CONCAT("{'id':",A2,",'title':'",C2,"','group':'",D2,"','area':'",E2,"','keywords':['",SUBSTITUTE(F2," ","','"),"'],'description':'",G2,"','publish':",H2,"}"),"'","""")</f>
         <v>{"id":1,"title":"general-something-wrong-on-server","group":"general","area":"common","keywords":["server","computer","tower","error","disconnect","problem"],"description":"One of three servers is down. Indicates that there is something wrong on the server side.","publish":1}</v>
       </c>
     </row>
@@ -7564,6 +8023,33 @@
       <c r="I51" s="2" t="str">
         <f t="shared" si="0"/>
         <v>{"id":50,"title":"zerodata-no-assessments","group":"zerodata","area":"compliance","keywords":["assessments","compliance","analysis","laptop","magnifier","clipboard","chart"],"description":"For assessments page zero data state.","publish":1}</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="5">
+        <v>51</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="D52" t="s">
+        <v>246</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="H52" s="2">
+        <v>1</v>
+      </c>
+      <c r="I52" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":51,"title":"zerodata-initializing-test-results","group":"zerodata","area":"test","keywords":["test","initialize","result","beaker","lab","flask","clock","wait","loading"],"description":"Waiting screen image when test result is being loaded.","publish":1}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new illustrations for .NET site
</commit_message>
<xml_diff>
--- a/src/assets/data.xlsx
+++ b/src/assets/data.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="460">
   <si>
     <t>SeattleSkyline</t>
   </si>
@@ -1190,6 +1190,225 @@
   </si>
   <si>
     <t>Used for Enable seamless debugging with symbols swimlane.</t>
+  </si>
+  <si>
+    <t>dotnet</t>
+  </si>
+  <si>
+    <t>swimlane-xamarin-cross-platform</t>
+  </si>
+  <si>
+    <t>swimlane-azure-machine-learning</t>
+  </si>
+  <si>
+    <t>swimlane-cognitive-services</t>
+  </si>
+  <si>
+    <t>swimlane-congratulations-finished-setup</t>
+  </si>
+  <si>
+    <t>swimlane-cross-platform</t>
+  </si>
+  <si>
+    <t>swimlane-cryengine-game-development</t>
+  </si>
+  <si>
+    <t>swimlane-developer-meetup</t>
+  </si>
+  <si>
+    <t>swimlane-dotnet-core</t>
+  </si>
+  <si>
+    <t>swimlane-dotnet-enterprise</t>
+  </si>
+  <si>
+    <t>swimlane-download-target</t>
+  </si>
+  <si>
+    <t>swimlane-enterprise-customer-stories</t>
+  </si>
+  <si>
+    <t>swimlane-feedback-survey</t>
+  </si>
+  <si>
+    <t>swimlane-fsharp-data-science</t>
+  </si>
+  <si>
+    <t>swimlane-machine-learning-library</t>
+  </si>
+  <si>
+    <t>swimlane-one-consistent-api</t>
+  </si>
+  <si>
+    <t>swimlane-package-library</t>
+  </si>
+  <si>
+    <t>swimlane-programming-languages</t>
+  </si>
+  <si>
+    <t>swimlane-thank-you-for-downloading</t>
+  </si>
+  <si>
+    <t>swimlane-unity-game-development</t>
+  </si>
+  <si>
+    <t>swimlane-universal-windows-platform</t>
+  </si>
+  <si>
+    <t>swimlane-uwp-iot-core</t>
+  </si>
+  <si>
+    <t>swimlane-winform</t>
+  </si>
+  <si>
+    <t>swimlane-wpf</t>
+  </si>
+  <si>
+    <t>swimlane-xamarin</t>
+  </si>
+  <si>
+    <t>xamarin cross platform computer laptop tablet phone</t>
+  </si>
+  <si>
+    <t>azure machine learning process cloud lightbulb clock analytics magnifier charts</t>
+  </si>
+  <si>
+    <t>Azure Machine Learning.</t>
+  </si>
+  <si>
+    <t>cognitive services vision sound voice speech microphone input speaker bubble eye magnifier</t>
+  </si>
+  <si>
+    <t>Xamarin.Mac allows user to create native iOS, Android and Mac apps.</t>
+  </si>
+  <si>
+    <t>Cognitive services such as voice recognition, vision detection, language processing, etc.</t>
+  </si>
+  <si>
+    <t>finish complete race car monitor flag people</t>
+  </si>
+  <si>
+    <t>Used on a screen when user successfully finishes setup.</t>
+  </si>
+  <si>
+    <t>cross platform windows mac linux computer laptop mobile phone</t>
+  </si>
+  <si>
+    <t>Used to represent multiple Oss and devices.</t>
+  </si>
+  <si>
+    <t>cryengine video game development computer monitor keyboard mouse 3d</t>
+  </si>
+  <si>
+    <t>An example 3d game screen created with CRYENGINE.</t>
+  </si>
+  <si>
+    <t>meetup people chat discussion idea light bulb</t>
+  </si>
+  <si>
+    <t>Three people talking about ideas.</t>
+  </si>
+  <si>
+    <t>developer people computer laptop work office team startup</t>
+  </si>
+  <si>
+    <t>A small team of developers working together.</t>
+  </si>
+  <si>
+    <t>developer people enterprise building company laptop computer work office</t>
+  </si>
+  <si>
+    <t>A developer working in an enterprise scale environment.</t>
+  </si>
+  <si>
+    <t>people download welcome computer table chair</t>
+  </si>
+  <si>
+    <t>A generic download landing screen.</t>
+  </si>
+  <si>
+    <t>building company team people enterprise</t>
+  </si>
+  <si>
+    <t>Enterprise user stories.</t>
+  </si>
+  <si>
+    <t>feedback people survey listen paper cup</t>
+  </si>
+  <si>
+    <t>A person listening user feedback with paper cup telephone.</t>
+  </si>
+  <si>
+    <t>data science lab test tube beaker chart analytics laptop scientist</t>
+  </si>
+  <si>
+    <t>A data scientist working in the lab.</t>
+  </si>
+  <si>
+    <t>machine learning library ai test beaker book</t>
+  </si>
+  <si>
+    <t>Used for machine learning AI library.</t>
+  </si>
+  <si>
+    <t>one api consistent people tool library book light bulb idea ui code</t>
+  </si>
+  <si>
+    <t>A person surrounded by multiple developer tools.</t>
+  </si>
+  <si>
+    <t>package box circuit</t>
+  </si>
+  <si>
+    <t>A few packages soldered on a circuit.</t>
+  </si>
+  <si>
+    <t>developer programming language keyboard c# VB F#</t>
+  </si>
+  <si>
+    <t>Developers of different programming languages.</t>
+  </si>
+  <si>
+    <t>download cloud document file</t>
+  </si>
+  <si>
+    <t>A generic download screen after download started/finished.</t>
+  </si>
+  <si>
+    <t>2d 3d video game castle unity</t>
+  </si>
+  <si>
+    <t>An example 3d game screen created with Unity.</t>
+  </si>
+  <si>
+    <t>uwp universal windows platform octopus hololens iot surface phone tablet band game controller drone</t>
+  </si>
+  <si>
+    <t>A octopus holding and wearing many devices built with UWP.</t>
+  </si>
+  <si>
+    <t>iot core drone security camera microwave thermometer smart home</t>
+  </si>
+  <si>
+    <t>Common smart devices built with UWP IoT Core.</t>
+  </si>
+  <si>
+    <t>winform drag drop designer pencil ruler dialog ui</t>
+  </si>
+  <si>
+    <t>Drag and drop designer for building Winform applications.</t>
+  </si>
+  <si>
+    <t>wpf windows presentation foundation ui design code screen monitor computer</t>
+  </si>
+  <si>
+    <t>A code and designer view used to represent WPF.</t>
+  </si>
+  <si>
+    <t>xamarin mobile cross platform development phone laptop code</t>
+  </si>
+  <si>
+    <t>Build cross-platform apps with Xamarin and one code base.</t>
   </si>
 </sst>
 </file>
@@ -3968,6 +4187,1209 @@
         <a:xfrm>
           <a:off x="1008530" y="67403383"/>
           <a:ext cx="2061882" cy="1131709"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>67236</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>67235</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2297206</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>1119108</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="40" name="Picture 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A18FA27B-C2B4-44A2-8167-1B27B130E6E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId55" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="952501" y="68624823"/>
+          <a:ext cx="2229970" cy="1051873"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>134472</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>112059</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2330823</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>1148074</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="44" name="Picture 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB592048-7059-4707-8A13-4025B2950407}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId56" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1019737" y="69935912"/>
+          <a:ext cx="2196351" cy="1036015"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2308411</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>1088873</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="48" name="Picture 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E511A456-4316-4D9A-B3F9-42FBA9481D71}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId57" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="885266" y="71090118"/>
+          <a:ext cx="2308410" cy="1088873"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2319617</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>1094159</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="51" name="Picture 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C234904A-9CA6-4E3B-B12A-4479578C79A6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId58" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="885265" y="72356382"/>
+          <a:ext cx="2319617" cy="1094159"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>56030</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>100854</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2218764</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>1121011</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="53" name="Picture 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4178E6A1-C30A-4DBA-BF7C-10914E2E6C58}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId59" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="941295" y="73723501"/>
+          <a:ext cx="2162734" cy="1020157"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2351891</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>1109383</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="55" name="Picture 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB6A5F7C-C514-419F-844F-F559F725DF78}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId60" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="885266" y="74888913"/>
+          <a:ext cx="2351890" cy="1109382"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>56030</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>56030</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2330822</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>1129045</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="57" name="Picture 56">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C1054FD-101F-4256-ABC1-5CA4EA904D8D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId61" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="941295" y="76211206"/>
+          <a:ext cx="2274792" cy="1073015"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>1125875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="59" name="Picture 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD72DF58-EE3C-4104-A553-9FEF880FE05E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId62" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="885265" y="77421442"/>
+          <a:ext cx="2386853" cy="1125874"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2364441</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>1115303</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="62" name="Picture 61">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54550CFC-9BEE-4323-B362-AC5AA61817F8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId63" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="885265" y="78687707"/>
+          <a:ext cx="2364441" cy="1115302"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2280622</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>1075765</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="66" name="Picture 65">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{433815F6-980A-4D29-A882-0467383D20A1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId64" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="885267" y="79953972"/>
+          <a:ext cx="2280620" cy="1075764"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>60064</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>1154206</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="70" name="Picture 69">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F0FD153-1044-4CE4-BAB9-ACBAC1D25EC1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId65" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="885265" y="81220235"/>
+          <a:ext cx="2446917" cy="1154206"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2256863</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>1064559</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="74" name="Picture 73">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2449BA56-B4ED-4861-9F11-F5A7D46027A1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId66" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="885265" y="82486501"/>
+          <a:ext cx="2256863" cy="1064558"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>78441</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>56030</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>138505</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>1210236</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="82" name="Picture 81">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A29A3BCC-0CE0-449E-A186-06AC991CD008}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId67" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="963706" y="83808795"/>
+          <a:ext cx="2446917" cy="1154206"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2304379</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>1086971</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="85" name="Picture 84">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A78B5D9-BBA4-4D24-B0FF-F17F5F4E38C5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId68" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="885266" y="86285294"/>
+          <a:ext cx="2304378" cy="1086971"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>123266</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>124812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>22412</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>1203114</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="87" name="Picture 86">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{038CBE17-C68E-4180-88BF-1F5534EDE1F8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId69" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1008531" y="87676371"/>
+          <a:ext cx="2285999" cy="1078302"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>134470</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>179295</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2285999</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>1194167</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="89" name="Picture 88">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE748D69-54A6-4AEE-967E-8C3D09CC0572}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId70" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1019735" y="88997119"/>
+          <a:ext cx="2151529" cy="1014872"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2351893</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>1109383</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="91" name="Picture 90">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{191D61C1-8B0B-410E-9914-F4486D6257A2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId71" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="885266" y="90084088"/>
+          <a:ext cx="2351892" cy="1109383"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>123266</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>78441</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2308861</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>1109382</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="93" name="Picture 92">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CE7A95D-F23F-4844-B91E-32FDB7B2E566}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId72" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1008531" y="91428794"/>
+          <a:ext cx="2185595" cy="1030941"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>123266</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>78443</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>159573</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>1221443</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="97" name="Picture 96">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA5F742F-045D-48E1-864B-B14FAEF17F59}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId73" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1008531" y="91428796"/>
+          <a:ext cx="2423160" cy="1143000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2280621</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>1075765</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="101" name="Graphic 100">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9024B81F-D52D-4B84-A94A-9FDABC5F37AB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId74" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId75"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="885265" y="95149147"/>
+          <a:ext cx="2280621" cy="1075765"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>1125875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="103" name="Picture 102">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A45B75A2-A05A-4D24-99DF-FB144F6B35C2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId76" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="885265" y="96415413"/>
+          <a:ext cx="2386853" cy="1125874"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2342029</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>1104731</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="105" name="Picture 104">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5C81AE0-544C-476C-8C2A-E934ADA6732B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId77" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="885265" y="97681676"/>
+          <a:ext cx="2342029" cy="1104731"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>155091</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>1199031</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="107" name="Picture 106">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C13FF32-FED4-41DA-B3F9-69C12FE48E8A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId78" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="885266" y="98947942"/>
+          <a:ext cx="2541943" cy="1199030"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>1125875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="109" name="Picture 108">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30D56146-AB94-4529-93C4-0F4DCFD3795E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId79" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="885265" y="100214207"/>
+          <a:ext cx="2386853" cy="1125874"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6799,13 +8221,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:I79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B78" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomRight" activeCell="F80" sqref="F80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6875,7 +8297,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="2" t="str">
-        <f t="shared" ref="I2:I55" si="0">SUBSTITUTE(_xlfn.CONCAT("{'id':",A2,",'title':'",C2,"','group':'",D2,"','area':'",E2,"','keywords':['",SUBSTITUTE(F2," ","','"),"'],'description':'",G2,"','publish':",H2,"}"),"'","""")</f>
+        <f t="shared" ref="I2:I79" si="0">SUBSTITUTE(_xlfn.CONCAT("{'id':",A2,",'title':'",C2,"','group':'",D2,"','area':'",E2,"','keywords':['",SUBSTITUTE(F2," ","','"),"'],'description':'",G2,"','publish':",H2,"}"),"'","""")</f>
         <v>{"id":1,"title":"general-something-wrong-on-server","group":"general","area":"common","keywords":["server","computer","tower","error","disconnect","problem"],"description":"One of three servers is down. Indicates that there is something wrong on the server side.","publish":1}</v>
       </c>
     </row>
@@ -8308,6 +9730,654 @@
       <c r="I55" s="2" t="str">
         <f t="shared" si="0"/>
         <v>{"id":54,"title":"swimlane-seamless-debugging-with-symbols","group":"vscom","area":"swimlane","keywords":["symbol","code","tag","label","identifier","file"],"description":"Used for Enable seamless debugging with symbols swimlane.","publish":1}</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="5">
+        <v>55</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="D56" t="s">
+        <v>387</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="H56" s="2">
+        <v>1</v>
+      </c>
+      <c r="I56" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":55,"title":"swimlane-xamarin-cross-platform","group":"dotnet","area":"swimlane","keywords":["xamarin","cross","platform","computer","laptop","tablet","phone"],"description":"Xamarin.Mac allows user to create native iOS, Android and Mac apps.","publish":1}</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="5">
+        <v>56</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="D57" t="s">
+        <v>387</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="H57" s="2">
+        <v>1</v>
+      </c>
+      <c r="I57" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":56,"title":"swimlane-azure-machine-learning","group":"dotnet","area":"swimlane","keywords":["azure","machine","learning","process","cloud","lightbulb","clock","analytics","magnifier","charts"],"description":"Azure Machine Learning.","publish":1}</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="5">
+        <v>57</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="D58" t="s">
+        <v>387</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="H58" s="2">
+        <v>1</v>
+      </c>
+      <c r="I58" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":57,"title":"swimlane-cognitive-services","group":"dotnet","area":"swimlane","keywords":["cognitive","services","vision","sound","voice","speech","microphone","input","speaker","bubble","eye","magnifier"],"description":"Cognitive services such as voice recognition, vision detection, language processing, etc.","publish":1}</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="5">
+        <v>58</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D59" t="s">
+        <v>387</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="H59" s="2">
+        <v>1</v>
+      </c>
+      <c r="I59" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":58,"title":"swimlane-congratulations-finished-setup","group":"dotnet","area":"swimlane","keywords":["finish","complete","race","car","monitor","flag","people"],"description":"Used on a screen when user successfully finishes setup.","publish":1}</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="5">
+        <v>59</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="D60" t="s">
+        <v>387</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="H60" s="2">
+        <v>1</v>
+      </c>
+      <c r="I60" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":59,"title":"swimlane-cross-platform","group":"dotnet","area":"swimlane","keywords":["cross","platform","windows","mac","linux","computer","laptop","mobile","phone"],"description":"Used to represent multiple Oss and devices.","publish":1}</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="5">
+        <v>60</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="D61" t="s">
+        <v>387</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="H61" s="2">
+        <v>1</v>
+      </c>
+      <c r="I61" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":60,"title":"swimlane-cryengine-game-development","group":"dotnet","area":"swimlane","keywords":["cryengine","video","game","development","computer","monitor","keyboard","mouse","3d"],"description":"An example 3d game screen created with CRYENGINE.","publish":1}</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="5">
+        <v>61</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="D62" t="s">
+        <v>387</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="H62" s="2">
+        <v>1</v>
+      </c>
+      <c r="I62" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":61,"title":"swimlane-developer-meetup","group":"dotnet","area":"swimlane","keywords":["meetup","people","chat","discussion","idea","light","bulb"],"description":"Three people talking about ideas.","publish":1}</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="5">
+        <v>62</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="D63" t="s">
+        <v>387</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="H63" s="2">
+        <v>1</v>
+      </c>
+      <c r="I63" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":62,"title":"swimlane-dotnet-core","group":"dotnet","area":"swimlane","keywords":["developer","people","computer","laptop","work","office","team","startup"],"description":"A small team of developers working together.","publish":1}</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="5">
+        <v>63</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="D64" t="s">
+        <v>387</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="H64" s="2">
+        <v>1</v>
+      </c>
+      <c r="I64" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":63,"title":"swimlane-dotnet-enterprise","group":"dotnet","area":"swimlane","keywords":["developer","people","enterprise","building","company","laptop","computer","work","office"],"description":"A developer working in an enterprise scale environment.","publish":1}</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="5">
+        <v>64</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="D65" t="s">
+        <v>387</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="H65" s="2">
+        <v>1</v>
+      </c>
+      <c r="I65" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":64,"title":"swimlane-download-target","group":"dotnet","area":"swimlane","keywords":["people","download","welcome","computer","table","chair"],"description":"A generic download landing screen.","publish":1}</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="5">
+        <v>65</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="D66" t="s">
+        <v>387</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="H66" s="2">
+        <v>1</v>
+      </c>
+      <c r="I66" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":65,"title":"swimlane-enterprise-customer-stories","group":"dotnet","area":"swimlane","keywords":["building","company","team","people","enterprise"],"description":"Enterprise user stories.","publish":1}</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="5">
+        <v>66</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="D67" t="s">
+        <v>387</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="H67" s="2">
+        <v>1</v>
+      </c>
+      <c r="I67" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":66,"title":"swimlane-feedback-survey","group":"dotnet","area":"swimlane","keywords":["feedback","people","survey","listen","paper","cup"],"description":"A person listening user feedback with paper cup telephone.","publish":1}</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="5">
+        <v>67</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="D68" t="s">
+        <v>387</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="H68" s="2">
+        <v>1</v>
+      </c>
+      <c r="I68" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":67,"title":"swimlane-fsharp-data-science","group":"dotnet","area":"swimlane","keywords":["data","science","lab","test","tube","beaker","chart","analytics","laptop","scientist"],"description":"A data scientist working in the lab.","publish":1}</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="5">
+        <v>68</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="D69" t="s">
+        <v>387</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="H69" s="2">
+        <v>1</v>
+      </c>
+      <c r="I69" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":68,"title":"swimlane-machine-learning-library","group":"dotnet","area":"swimlane","keywords":["machine","learning","library","ai","test","beaker","book"],"description":"Used for machine learning AI library.","publish":1}</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="5">
+        <v>69</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="D70" t="s">
+        <v>387</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="H70" s="2">
+        <v>1</v>
+      </c>
+      <c r="I70" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":69,"title":"swimlane-one-consistent-api","group":"dotnet","area":"swimlane","keywords":["one","api","consistent","people","tool","library","book","light","bulb","idea","ui","code"],"description":"A person surrounded by multiple developer tools.","publish":1}</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="5">
+        <v>70</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="D71" t="s">
+        <v>387</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="H71" s="2">
+        <v>1</v>
+      </c>
+      <c r="I71" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":70,"title":"swimlane-package-library","group":"dotnet","area":"swimlane","keywords":["package","box","circuit"],"description":"A few packages soldered on a circuit.","publish":1}</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="5">
+        <v>71</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="D72" t="s">
+        <v>387</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="H72" s="2">
+        <v>1</v>
+      </c>
+      <c r="I72" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":71,"title":"swimlane-programming-languages","group":"dotnet","area":"swimlane","keywords":["developer","programming","language","keyboard","c#","VB","F#"],"description":"Developers of different programming languages.","publish":1}</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="5">
+        <v>72</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="D73" t="s">
+        <v>387</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="H73" s="2">
+        <v>1</v>
+      </c>
+      <c r="I73" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":72,"title":"swimlane-thank-you-for-downloading","group":"dotnet","area":"swimlane","keywords":["download","cloud","document","file"],"description":"A generic download screen after download started/finished.","publish":1}</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="5">
+        <v>73</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="D74" t="s">
+        <v>387</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="H74" s="2">
+        <v>1</v>
+      </c>
+      <c r="I74" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":73,"title":"swimlane-unity-game-development","group":"dotnet","area":"swimlane","keywords":["2d","3d","video","game","castle","unity"],"description":"An example 3d game screen created with Unity.","publish":1}</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="5">
+        <v>74</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="D75" t="s">
+        <v>387</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="H75" s="2">
+        <v>1</v>
+      </c>
+      <c r="I75" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":74,"title":"swimlane-universal-windows-platform","group":"dotnet","area":"swimlane","keywords":["uwp","universal","windows","platform","octopus","hololens","iot","surface","phone","tablet","band","game","controller","drone"],"description":"A octopus holding and wearing many devices built with UWP.","publish":1}</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="5">
+        <v>75</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="D76" t="s">
+        <v>387</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="H76" s="2">
+        <v>1</v>
+      </c>
+      <c r="I76" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":75,"title":"swimlane-uwp-iot-core","group":"dotnet","area":"swimlane","keywords":["iot","core","drone","security","camera","microwave","thermometer","smart","home"],"description":"Common smart devices built with UWP IoT Core.","publish":1}</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="5">
+        <v>76</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="D77" t="s">
+        <v>387</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="H77" s="2">
+        <v>1</v>
+      </c>
+      <c r="I77" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":76,"title":"swimlane-winform","group":"dotnet","area":"swimlane","keywords":["winform","drag","drop","designer","pencil","ruler","dialog","ui"],"description":"Drag and drop designer for building Winform applications.","publish":1}</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="5">
+        <v>77</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="D78" t="s">
+        <v>387</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="G78" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="H78" s="2">
+        <v>1</v>
+      </c>
+      <c r="I78" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":77,"title":"swimlane-wpf","group":"dotnet","area":"swimlane","keywords":["wpf","windows","presentation","foundation","ui","design","code","screen","monitor","computer"],"description":"A code and designer view used to represent WPF.","publish":1}</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="5">
+        <v>78</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="D79" t="s">
+        <v>387</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="H79" s="2">
+        <v>1</v>
+      </c>
+      <c r="I79" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":78,"title":"swimlane-xamarin","group":"dotnet","area":"swimlane","keywords":["xamarin","mobile","cross","platform","development","phone","laptop","code"],"description":"Build cross-platform apps with Xamarin and one code base.","publish":1}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new illustration for .NET site
</commit_message>
<xml_diff>
--- a/src/assets/data.xlsx
+++ b/src/assets/data.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="463">
   <si>
     <t>SeattleSkyline</t>
   </si>
@@ -1409,6 +1409,15 @@
   </si>
   <si>
     <t>Build cross-platform apps with Xamarin and one code base.</t>
+  </si>
+  <si>
+    <t>swimlane-dotnet-perf-diagram</t>
+  </si>
+  <si>
+    <t>.net diagram bar chart</t>
+  </si>
+  <si>
+    <t>A bar chart comparing requests per second of three frameworks.</t>
   </si>
 </sst>
 </file>
@@ -5390,6 +5399,56 @@
         <a:xfrm>
           <a:off x="885265" y="100214207"/>
           <a:ext cx="2386853" cy="1125874"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2375647</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>1120589</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="42" name="Picture 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE9041C7-1169-489C-AFFE-771A18B45F48}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId80" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="885266" y="98947942"/>
+          <a:ext cx="2375646" cy="1120588"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8221,13 +8280,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I79"/>
+  <dimension ref="A1:I80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B78" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F80" sqref="F80"/>
+      <selection pane="bottomRight" activeCell="I80" sqref="I80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8297,7 +8356,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="2" t="str">
-        <f t="shared" ref="I2:I79" si="0">SUBSTITUTE(_xlfn.CONCAT("{'id':",A2,",'title':'",C2,"','group':'",D2,"','area':'",E2,"','keywords':['",SUBSTITUTE(F2," ","','"),"'],'description':'",G2,"','publish':",H2,"}"),"'","""")</f>
+        <f t="shared" ref="I2:I80" si="0">SUBSTITUTE(_xlfn.CONCAT("{'id':",A2,",'title':'",C2,"','group':'",D2,"','area':'",E2,"','keywords':['",SUBSTITUTE(F2," ","','"),"'],'description':'",G2,"','publish':",H2,"}"),"'","""")</f>
         <v>{"id":1,"title":"general-something-wrong-on-server","group":"general","area":"common","keywords":["server","computer","tower","error","disconnect","problem"],"description":"One of three servers is down. Indicates that there is something wrong on the server side.","publish":1}</v>
       </c>
     </row>
@@ -10378,6 +10437,33 @@
       <c r="I79" s="2" t="str">
         <f t="shared" si="0"/>
         <v>{"id":78,"title":"swimlane-xamarin","group":"dotnet","area":"swimlane","keywords":["xamarin","mobile","cross","platform","development","phone","laptop","code"],"description":"Build cross-platform apps with Xamarin and one code base.","publish":1}</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="5">
+        <v>79</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="D80" t="s">
+        <v>387</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="H80" s="2">
+        <v>0</v>
+      </c>
+      <c r="I80" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":79,"title":"swimlane-dotnet-perf-diagram","group":"dotnet","area":"swimlane","keywords":[".net","diagram","bar","chart"],"description":"A bar chart comparing requests per second of three frameworks.","publish":0}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new illustration for snapshot debugger page hero
</commit_message>
<xml_diff>
--- a/src/assets/data.xlsx
+++ b/src/assets/data.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="466">
   <si>
     <t>SeattleSkyline</t>
   </si>
@@ -1418,6 +1418,15 @@
   </si>
   <si>
     <t>A bar chart comparing requests per second of three frameworks.</t>
+  </si>
+  <si>
+    <t>hero-snapshot-debugger</t>
+  </si>
+  <si>
+    <t>snapshot debugger debug bug magnifier code cloud</t>
+  </si>
+  <si>
+    <t>Debugging code on the cloud.</t>
   </si>
 </sst>
 </file>
@@ -5449,6 +5458,56 @@
         <a:xfrm>
           <a:off x="885266" y="98947942"/>
           <a:ext cx="2375646" cy="1120588"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>145677</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>56030</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2222672</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>1199030</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="46" name="Picture 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C716B9CE-04ED-408C-B211-A78407A0ADFE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId81" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1030942" y="100270236"/>
+          <a:ext cx="2076995" cy="1143000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8280,13 +8339,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I80"/>
+  <dimension ref="A1:I81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B78" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I80" sqref="I80"/>
+      <selection pane="bottomRight" activeCell="I81" sqref="I81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8356,7 +8415,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="2" t="str">
-        <f t="shared" ref="I2:I80" si="0">SUBSTITUTE(_xlfn.CONCAT("{'id':",A2,",'title':'",C2,"','group':'",D2,"','area':'",E2,"','keywords':['",SUBSTITUTE(F2," ","','"),"'],'description':'",G2,"','publish':",H2,"}"),"'","""")</f>
+        <f t="shared" ref="I2:I81" si="0">SUBSTITUTE(_xlfn.CONCAT("{'id':",A2,",'title':'",C2,"','group':'",D2,"','area':'",E2,"','keywords':['",SUBSTITUTE(F2," ","','"),"'],'description':'",G2,"','publish':",H2,"}"),"'","""")</f>
         <v>{"id":1,"title":"general-something-wrong-on-server","group":"general","area":"common","keywords":["server","computer","tower","error","disconnect","problem"],"description":"One of three servers is down. Indicates that there is something wrong on the server side.","publish":1}</v>
       </c>
     </row>
@@ -10464,6 +10523,33 @@
       <c r="I80" s="2" t="str">
         <f t="shared" si="0"/>
         <v>{"id":79,"title":"swimlane-dotnet-perf-diagram","group":"dotnet","area":"swimlane","keywords":[".net","diagram","bar","chart"],"description":"A bar chart comparing requests per second of three frameworks.","publish":0}</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="5">
+        <v>80</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="D81" t="s">
+        <v>270</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="G81" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="H81" s="2">
+        <v>1</v>
+      </c>
+      <c r="I81" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":80,"title":"hero-snapshot-debugger","group":"vscom","area":"hero","keywords":["snapshot","debugger","debug","bug","magnifier","code","cloud"],"description":"Debugging code on the cloud.","publish":1}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new illustrations for vscode vnext
</commit_message>
<xml_diff>
--- a/src/assets/data.xlsx
+++ b/src/assets/data.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="478">
   <si>
     <t>SeattleSkyline</t>
   </si>
@@ -1427,6 +1427,42 @@
   </si>
   <si>
     <t>Debugging code on the cloud.</t>
+  </si>
+  <si>
+    <t>swimlane-collaborative-debugging</t>
+  </si>
+  <si>
+    <t>swimlane-collaborative-editing</t>
+  </si>
+  <si>
+    <t>swimlane-shared-full-context</t>
+  </si>
+  <si>
+    <t>swimlane-real-time-sharing</t>
+  </si>
+  <si>
+    <t>collaborate debug teamwork hands plan draw ruler design pen triangle bug magnifier lightbulb</t>
+  </si>
+  <si>
+    <t>collaborate editor code people</t>
+  </si>
+  <si>
+    <t>share context code editor environment computer laptop</t>
+  </si>
+  <si>
+    <t>people work team office real time code developer clock</t>
+  </si>
+  <si>
+    <t>Collaborative code editing.</t>
+  </si>
+  <si>
+    <t>Collaborative debugging.</t>
+  </si>
+  <si>
+    <t>Share code and full context.</t>
+  </si>
+  <si>
+    <t>Real-time sharing with your tools.</t>
   </si>
 </sst>
 </file>
@@ -5508,6 +5544,206 @@
         <a:xfrm>
           <a:off x="1030942" y="100270236"/>
           <a:ext cx="2076995" cy="1143000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>156883</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>22412</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2017059</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>1262529</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="50" name="Picture 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3469536-E92E-41F3-A2A3-6801793C6756}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId82" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1042148" y="101502883"/>
+          <a:ext cx="1860176" cy="1240117"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1905000</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>3736</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="54" name="Picture 53">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4046FC1B-CD06-439E-8BDE-C458A33465F7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId83">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="885265" y="102746736"/>
+          <a:ext cx="1905000" cy="1270000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1764927</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>1176619</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="58" name="Picture 57">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7FD584D-12E2-40BF-8DE7-C0BFED4C5D83}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId84" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="885265" y="104013001"/>
+          <a:ext cx="1764927" cy="1176618"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1949823</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>33619</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="64" name="Picture 63">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E19B3CDB-EDD5-4D8C-8DA9-53BC41BC430B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId85">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="885265" y="105279266"/>
+          <a:ext cx="1949823" cy="1299882"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8339,13 +8575,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I81"/>
+  <dimension ref="A1:I85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B78" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B81" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I81" sqref="I81"/>
+      <selection pane="bottomRight" activeCell="J85" sqref="J85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8415,7 +8651,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="2" t="str">
-        <f t="shared" ref="I2:I81" si="0">SUBSTITUTE(_xlfn.CONCAT("{'id':",A2,",'title':'",C2,"','group':'",D2,"','area':'",E2,"','keywords':['",SUBSTITUTE(F2," ","','"),"'],'description':'",G2,"','publish':",H2,"}"),"'","""")</f>
+        <f t="shared" ref="I2:I82" si="0">SUBSTITUTE(_xlfn.CONCAT("{'id':",A2,",'title':'",C2,"','group':'",D2,"','area':'",E2,"','keywords':['",SUBSTITUTE(F2," ","','"),"'],'description':'",G2,"','publish':",H2,"}"),"'","""")</f>
         <v>{"id":1,"title":"general-something-wrong-on-server","group":"general","area":"common","keywords":["server","computer","tower","error","disconnect","problem"],"description":"One of three servers is down. Indicates that there is something wrong on the server side.","publish":1}</v>
       </c>
     </row>
@@ -10550,6 +10786,114 @@
       <c r="I81" s="2" t="str">
         <f t="shared" si="0"/>
         <v>{"id":80,"title":"hero-snapshot-debugger","group":"vscom","area":"hero","keywords":["snapshot","debugger","debug","bug","magnifier","code","cloud"],"description":"Debugging code on the cloud.","publish":1}</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="5">
+        <v>81</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="D82" t="s">
+        <v>270</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="H82" s="2">
+        <v>1</v>
+      </c>
+      <c r="I82" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{"id":81,"title":"swimlane-collaborative-debugging","group":"vscom","area":"swimlane","keywords":["collaborate","debug","teamwork","hands","plan","draw","ruler","design","pen","triangle","bug","magnifier","lightbulb"],"description":"Collaborative debugging.","publish":1}</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="5">
+        <v>82</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="D83" t="s">
+        <v>270</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="G83" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="H83" s="2">
+        <v>1</v>
+      </c>
+      <c r="I83" s="2" t="str">
+        <f t="shared" ref="I83:I85" si="1">SUBSTITUTE(_xlfn.CONCAT("{'id':",A83,",'title':'",C83,"','group':'",D83,"','area':'",E83,"','keywords':['",SUBSTITUTE(F83," ","','"),"'],'description':'",G83,"','publish':",H83,"}"),"'","""")</f>
+        <v>{"id":82,"title":"swimlane-collaborative-editing","group":"vscom","area":"swimlane","keywords":["collaborate","editor","code","people"],"description":"Collaborative code editing.","publish":1}</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="5">
+        <v>83</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="D84" t="s">
+        <v>270</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="G84" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="H84" s="2">
+        <v>1</v>
+      </c>
+      <c r="I84" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>{"id":83,"title":"swimlane-shared-full-context","group":"vscom","area":"swimlane","keywords":["share","context","code","editor","environment","computer","laptop"],"description":"Share code and full context.","publish":1}</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="5">
+        <v>84</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="D85" t="s">
+        <v>270</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="G85" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="H85" s="2">
+        <v>1</v>
+      </c>
+      <c r="I85" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>{"id":84,"title":"swimlane-real-time-sharing","group":"vscom","area":"swimlane","keywords":["people","work","team","office","real","time","code","developer","clock"],"description":"Real-time sharing with your tools.","publish":1}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new illustrations for vscode blog
</commit_message>
<xml_diff>
--- a/src/assets/data.xlsx
+++ b/src/assets/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwang\Dropbox\Code\vsimages\src\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\Code\vsimages\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="489">
   <si>
     <t>SeattleSkyline</t>
   </si>
@@ -1463,6 +1463,39 @@
   </si>
   <si>
     <t>Real-time sharing with your tools.</t>
+  </si>
+  <si>
+    <t>blog-rocket-launch-timeline</t>
+  </si>
+  <si>
+    <t>blog-vscode-metrics</t>
+  </si>
+  <si>
+    <t>blog-vscode-roadmap</t>
+  </si>
+  <si>
+    <t>vscode</t>
+  </si>
+  <si>
+    <t>blog</t>
+  </si>
+  <si>
+    <t>rocket release launch cloud timeline</t>
+  </si>
+  <si>
+    <t>metrics</t>
+  </si>
+  <si>
+    <t>roadmap car road milestone pin timeline</t>
+  </si>
+  <si>
+    <t>Rocket launch timeline.</t>
+  </si>
+  <si>
+    <t>Download and install metrics of Visual Studio Code.</t>
+  </si>
+  <si>
+    <t>A roadmap showing Visual Studio Code major release milestones</t>
   </si>
 </sst>
 </file>
@@ -5705,31 +5738,31 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>100852</xdr:colOff>
       <xdr:row>84</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1949823</xdr:colOff>
-      <xdr:row>85</xdr:row>
-      <xdr:rowOff>33619</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="64" name="Picture 63">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E19B3CDB-EDD5-4D8C-8DA9-53BC41BC430B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId85">
+      <xdr:rowOff>67235</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1860175</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>1240117</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="52" name="Picture 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD57491D-509A-4EAD-A026-4B4C6E3EB735}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId85" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -5742,8 +5775,158 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="885265" y="105279266"/>
-          <a:ext cx="1949823" cy="1299882"/>
+          <a:off x="986117" y="105346500"/>
+          <a:ext cx="1759323" cy="1172882"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>145676</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>22412</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1927411</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>1210235</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="60" name="Picture 59">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6ABE0A0-EA6E-4982-9638-A8C8337686F0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId86" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1030941" y="106567941"/>
+          <a:ext cx="1781735" cy="1187823"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>112059</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>22412</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1927412</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>1232647</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="72" name="Picture 71">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1813428F-7995-4583-AEE1-C0F87AE12A9D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId87" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="997324" y="107834206"/>
+          <a:ext cx="1815353" cy="1210235"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>112059</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>11206</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1905000</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>1206500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="78" name="Picture 77">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8289DBA9-2C8A-4B1C-9643-FBF54E127260}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId88" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="997324" y="109089265"/>
+          <a:ext cx="1792941" cy="1195294"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8575,13 +8758,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I85"/>
+  <dimension ref="A1:I88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B81" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B84" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J85" sqref="J85"/>
+      <selection pane="bottomRight" activeCell="H87" sqref="H87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -10796,7 +10979,7 @@
         <v>466</v>
       </c>
       <c r="D82" t="s">
-        <v>270</v>
+        <v>481</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>272</v>
@@ -10812,7 +10995,7 @@
       </c>
       <c r="I82" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{"id":81,"title":"swimlane-collaborative-debugging","group":"vscom","area":"swimlane","keywords":["collaborate","debug","teamwork","hands","plan","draw","ruler","design","pen","triangle","bug","magnifier","lightbulb"],"description":"Collaborative debugging.","publish":1}</v>
+        <v>{"id":81,"title":"swimlane-collaborative-debugging","group":"vscode","area":"swimlane","keywords":["collaborate","debug","teamwork","hands","plan","draw","ruler","design","pen","triangle","bug","magnifier","lightbulb"],"description":"Collaborative debugging.","publish":1}</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -10823,7 +11006,7 @@
         <v>467</v>
       </c>
       <c r="D83" t="s">
-        <v>270</v>
+        <v>481</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>272</v>
@@ -10838,8 +11021,8 @@
         <v>1</v>
       </c>
       <c r="I83" s="2" t="str">
-        <f t="shared" ref="I83:I85" si="1">SUBSTITUTE(_xlfn.CONCAT("{'id':",A83,",'title':'",C83,"','group':'",D83,"','area':'",E83,"','keywords':['",SUBSTITUTE(F83," ","','"),"'],'description':'",G83,"','publish':",H83,"}"),"'","""")</f>
-        <v>{"id":82,"title":"swimlane-collaborative-editing","group":"vscom","area":"swimlane","keywords":["collaborate","editor","code","people"],"description":"Collaborative code editing.","publish":1}</v>
+        <f t="shared" ref="I83:I88" si="1">SUBSTITUTE(_xlfn.CONCAT("{'id':",A83,",'title':'",C83,"','group':'",D83,"','area':'",E83,"','keywords':['",SUBSTITUTE(F83," ","','"),"'],'description':'",G83,"','publish':",H83,"}"),"'","""")</f>
+        <v>{"id":82,"title":"swimlane-collaborative-editing","group":"vscode","area":"swimlane","keywords":["collaborate","editor","code","people"],"description":"Collaborative code editing.","publish":1}</v>
       </c>
     </row>
     <row r="84" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -10850,7 +11033,7 @@
         <v>468</v>
       </c>
       <c r="D84" t="s">
-        <v>270</v>
+        <v>481</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>272</v>
@@ -10866,7 +11049,7 @@
       </c>
       <c r="I84" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{"id":83,"title":"swimlane-shared-full-context","group":"vscom","area":"swimlane","keywords":["share","context","code","editor","environment","computer","laptop"],"description":"Share code and full context.","publish":1}</v>
+        <v>{"id":83,"title":"swimlane-shared-full-context","group":"vscode","area":"swimlane","keywords":["share","context","code","editor","environment","computer","laptop"],"description":"Share code and full context.","publish":1}</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -10877,7 +11060,7 @@
         <v>469</v>
       </c>
       <c r="D85" t="s">
-        <v>270</v>
+        <v>481</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>272</v>
@@ -10893,7 +11076,88 @@
       </c>
       <c r="I85" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{"id":84,"title":"swimlane-real-time-sharing","group":"vscom","area":"swimlane","keywords":["people","work","team","office","real","time","code","developer","clock"],"description":"Real-time sharing with your tools.","publish":1}</v>
+        <v>{"id":84,"title":"swimlane-real-time-sharing","group":"vscode","area":"swimlane","keywords":["people","work","team","office","real","time","code","developer","clock"],"description":"Real-time sharing with your tools.","publish":1}</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="5">
+        <v>85</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="D86" t="s">
+        <v>481</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="G86" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="H86" s="2">
+        <v>1</v>
+      </c>
+      <c r="I86" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>{"id":85,"title":"blog-rocket-launch-timeline","group":"vscode","area":"blog","keywords":["rocket","release","launch","cloud","timeline"],"description":"Rocket launch timeline.","publish":1}</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="5">
+        <v>86</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="D87" t="s">
+        <v>270</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="G87" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="H87" s="2">
+        <v>1</v>
+      </c>
+      <c r="I87" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>{"id":86,"title":"blog-vscode-metrics","group":"vscom","area":"blog","keywords":["metrics"],"description":"Download and install metrics of Visual Studio Code.","publish":1}</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="5">
+        <v>87</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="D88" t="s">
+        <v>270</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="G88" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="H88" s="2">
+        <v>1</v>
+      </c>
+      <c r="I88" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>{"id":87,"title":"blog-vscode-roadmap","group":"vscom","area":"blog","keywords":["roadmap","car","road","milestone","pin","timeline"],"description":"A roadmap showing Visual Studio Code major release milestones","publish":1}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new illustration for dotnet
</commit_message>
<xml_diff>
--- a/src/assets/data.xlsx
+++ b/src/assets/data.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="492">
   <si>
     <t>SeattleSkyline</t>
   </si>
@@ -1496,6 +1496,15 @@
   </si>
   <si>
     <t>A roadmap showing Visual Studio Code major release milestones</t>
+  </si>
+  <si>
+    <t>swimlane-monogame-game-development</t>
+  </si>
+  <si>
+    <t>monogame game development screen platform psvita windows mac video game</t>
+  </si>
+  <si>
+    <t>Cross platform game development with MonoGame engine.</t>
   </si>
 </sst>
 </file>
@@ -5927,6 +5936,56 @@
         <a:xfrm>
           <a:off x="997324" y="109089265"/>
           <a:ext cx="1792941" cy="1195294"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>78442</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2375648</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>1083589</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="56" name="Picture 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A6596F2-09EF-4CA5-AABD-DE8D1EA82476}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId89" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="963707" y="110344325"/>
+          <a:ext cx="2297206" cy="1083588"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8758,13 +8817,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I88"/>
+  <dimension ref="A1:I89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B84" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B87" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H87" sqref="H87"/>
+      <selection pane="bottomRight" activeCell="G91" sqref="G91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -11021,7 +11080,7 @@
         <v>1</v>
       </c>
       <c r="I83" s="2" t="str">
-        <f t="shared" ref="I83:I88" si="1">SUBSTITUTE(_xlfn.CONCAT("{'id':",A83,",'title':'",C83,"','group':'",D83,"','area':'",E83,"','keywords':['",SUBSTITUTE(F83," ","','"),"'],'description':'",G83,"','publish':",H83,"}"),"'","""")</f>
+        <f t="shared" ref="I83:I89" si="1">SUBSTITUTE(_xlfn.CONCAT("{'id':",A83,",'title':'",C83,"','group':'",D83,"','area':'",E83,"','keywords':['",SUBSTITUTE(F83," ","','"),"'],'description':'",G83,"','publish':",H83,"}"),"'","""")</f>
         <v>{"id":82,"title":"swimlane-collaborative-editing","group":"vscode","area":"swimlane","keywords":["collaborate","editor","code","people"],"description":"Collaborative code editing.","publish":1}</v>
       </c>
     </row>
@@ -11158,6 +11217,33 @@
       <c r="I88" s="2" t="str">
         <f t="shared" si="1"/>
         <v>{"id":87,"title":"blog-vscode-roadmap","group":"vscom","area":"blog","keywords":["roadmap","car","road","milestone","pin","timeline"],"description":"A roadmap showing Visual Studio Code major release milestones","publish":1}</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="5">
+        <v>88</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="D89" t="s">
+        <v>387</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="G89" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="H89" s="2">
+        <v>1</v>
+      </c>
+      <c r="I89" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>{"id":88,"title":"swimlane-monogame-game-development","group":"dotnet","area":"swimlane","keywords":["monogame","game","development","screen","platform","psvita","windows","mac","video","game"],"description":"Cross platform game development with MonoGame engine.","publish":1}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new illustration for account page project zero data
</commit_message>
<xml_diff>
--- a/src/assets/data.xlsx
+++ b/src/assets/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\Code\vsimages\src\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chryw\Dropbox\Code\vsimages\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="495">
   <si>
     <t>SeattleSkyline</t>
   </si>
@@ -1505,6 +1505,15 @@
   </si>
   <si>
     <t>Cross platform game development with MonoGame engine.</t>
+  </si>
+  <si>
+    <t>zerodata-you-have-no-project</t>
+  </si>
+  <si>
+    <t>project plan work briefcase pencil document triangle ruler</t>
+  </si>
+  <si>
+    <t>Used in account page when you have no projects yet.</t>
   </si>
 </sst>
 </file>
@@ -5986,6 +5995,56 @@
         <a:xfrm>
           <a:off x="963707" y="110344325"/>
           <a:ext cx="2297206" cy="1083588"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>210671</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>89648</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2241176</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>1177418</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="64" name="Picture 63">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{018731C9-A74A-4B4A-9A54-89F4AB9C69E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId90">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1169895" y="111897460"/>
+          <a:ext cx="2030505" cy="1087770"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8817,31 +8876,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I89"/>
+  <dimension ref="A1:I90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B87" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C90" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G91" sqref="G91"/>
+      <selection pane="bottomRight" activeCell="F91" sqref="F91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="100" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="35.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="38.140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="13.26171875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="35.83984375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="38.15625" style="2" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
     <col min="5" max="5" width="18" style="2" customWidth="1"/>
-    <col min="6" max="6" width="33.7109375" style="2" customWidth="1"/>
-    <col min="7" max="8" width="20.7109375" style="2" customWidth="1"/>
-    <col min="9" max="10" width="24.140625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="33.140625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="66.42578125" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="2"/>
+    <col min="6" max="6" width="33.68359375" style="2" customWidth="1"/>
+    <col min="7" max="8" width="20.68359375" style="2" customWidth="1"/>
+    <col min="9" max="10" width="24.15625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="33.15625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="66.41796875" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="9.15625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
         <v>201</v>
       </c>
@@ -8870,7 +8929,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -8897,7 +8956,7 @@
         <v>{"id":1,"title":"general-something-wrong-on-server","group":"general","area":"common","keywords":["server","computer","tower","error","disconnect","problem"],"description":"One of three servers is down. Indicates that there is something wrong on the server side.","publish":1}</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -8924,7 +8983,7 @@
         <v>{"id":2,"title":"widget-you-dont-have-permission","group":"widget","area":"dashboard","keywords":["permission","access","man","lock","error","problem"],"description":"A man holding a lock sign. Indicates that you do not have permission to the content.","publish":1}</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -8951,7 +9010,7 @@
         <v>{"id":3,"title":"zerodata-charting-not-supported","group":"zerodata","area":"work","keywords":["chart","hierachy","error","warning","support","tree","exclamation","diagram"],"description":"Hierachy diagram with a warning sign. Indicates that charting is not supported for hierachical query. Users need to change to flat list query to use charting feature.","publish":1}</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -8978,7 +9037,7 @@
         <v>{"id":4,"title":"zerodata-custom-rules","group":"zerodata","area":"policies","keywords":["custom","build","car","arm","customization","vehicle","parts","hook","transportation"],"description":"Robot arms building a customized car. Used in Rules area to represent custom rules.","publish":1}</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -9005,7 +9064,7 @@
         <v>{"id":5,"title":"zerodata-get-back-to-recent-work","group":"zerodata","area":"account","keywords":["history","back","rewind","clock","recent","previous","arrow","time"],"description":"Backward clock. Represents recent work.","publish":1}</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -9032,7 +9091,7 @@
         <v>{"id":6,"title":"zerodata-invalid-workitem-type","group":"zerodata","area":"work","keywords":["plug","disconnect"],"description":"Plugs of two different standards that are not compatible with each other. Used when users try to create a work item which type does not exist in the current project.","publish":1}</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -9059,7 +9118,7 @@
         <v>{"id":7,"title":"zerodata-keep-an-eye-on-important-work","group":"zerodata","area":"account","keywords":["man","people","mail","message","idea","code","envelope","lightbulb","chat","bubble","brackets"],"description":"A man looking at some workspace tools. Used to represent all relevant works can be found in one place.","publish":1}</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -9086,7 +9145,7 @@
         <v>{"id":8,"title":"zerodata-mention-someone","group":"zerodata","area":"account","keywords":["mention","at","@","message","chat","conversation","discussion","people","avatar","woman","man"],"description":"A conversation between two users with an @ in the chat bubble that mimics the mention feature.","publish":1}</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -9113,7 +9172,7 @@
         <v>{"id":9,"title":"zerodata-no-charts","group":"zerodata","area":"work","keywords":["chart","pie","bar","area"],"description":"Several common chart types. Used in Work hub analytics when there is no data to create chart.","publish":1}</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -9140,7 +9199,7 @@
         <v>{"id":10,"title":"zerodata-unsaved-query","group":"zerodata","area":"work","keywords":["chart","dotted","line","invisible","temporary","save","floppy","disk","pie","bar"],"description":"Dotted line charts with save icon. Indicates that charting is not available until you save query.","publish":1}</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -9167,7 +9226,7 @@
         <v>{"id":11,"title":"zerodata-workitem-not-found","group":"zerodata","area":"work","keywords":["tools","hammer","drill","saw","plier","missing","dotted","line"],"description":"A hammer missing from a set of tools. Indicates that work item is not found or you do not have permission to view it.","publish":1}</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -9194,7 +9253,7 @@
         <v>{"id":12,"title":"zerodata-your-work-in-one-place","group":"zerodata","area":"account","keywords":["woman","avatar","people"],"description":"A woman avatar in circle. Used in Account page when you do not have works assigned to you yet.","publish":1}</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -9221,7 +9280,7 @@
         <v>{"id":13,"title":"zerodata-get-started-with-sprint","group":"zerodata","area":"work","keywords":["sprint","people"],"description":"3 people discussing sprint work. Used in Work Sprint page when there is no sprint in the current project.","publish":1}</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -9248,7 +9307,7 @@
         <v>{"id":14,"title":"zerodata-add-a-feed","group":"zerodata","area":"package","keywords":["cloud","host","package","feed","box","people","ladder"],"description":"A person standing on a ladder and putting a virtual box up on the cloud. Used in the Package page when there is no package feed set up for the current project.","publish":1}</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -9275,7 +9334,7 @@
         <v>{"id":15,"title":"zerodata-connect-to-feed","group":"zerodata","area":"package","keywords":["cloud","host","package","feed","arrow","connect","box","plug"],"description":"A solid box connected to a remote virtual box on the cloud. Used in Package page when there is no packages connected to a feed.","publish":1}</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -9302,7 +9361,7 @@
         <v>{"id":16,"title":"general-no-results-found","group":"general","area":"common","keywords":["person","telescope","explore","find","search"],"description":"A person looking through a telescope. Used for no results match/found pattern.","publish":1}</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -9329,7 +9388,7 @@
         <v>{"id":17,"title":"hero-extend-vside","group":"vscom","area":"hero","keywords":["monitor","computer","code","ide","extension","build","extend","vside","robot","arm","tools","construction"],"description":"Robot arms building extensions into Visual Studio IDE.","publish":1}</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -9356,7 +9415,7 @@
         <v>{"id":18,"title":"swimlane-create-your-own-extension","group":"vscom","area":"swimlane","keywords":["tools","toolbox","hammer","wrench","pen","work","cloud","clipboard"],"description":"A toolbox with some tools and a cloud.","publish":1}</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -9383,7 +9442,7 @@
         <v>{"id":19,"title":"swimlane-marketplace","group":"vscom","area":"swimlane","keywords":["marketplace","store","shop","market","storefront"],"description":"Used to represent Visual Studio Marketplace.","publish":1}</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -9410,7 +9469,7 @@
         <v>{"id":20,"title":"swimlane-partner-program","group":"vscom","area":"swimlane","keywords":["team","collaboration","people","bike","bicycle","engineer","businessmen","doctor","man","woman","developer","hardhat","lab","coat"],"description":"Four people riding on a bike. Used for Visual Studio Partner Program.","publish":1}</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -9437,7 +9496,7 @@
         <v>{"id":21,"title":"swimlane-what-are-extensions","group":"vscom","area":"swimlane","keywords":["extension","plugin","plug","puzzle","extend","addon","people","woman","man","ladder","gear","chart","clipboard","task"],"description":"People putting plugins together. Used to represent Visual Studio extensions.","publish":1}</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -9464,7 +9523,7 @@
         <v>{"id":22,"title":"zerodata-add-product","group":"zerodata","area":"compliance","keywords":["product","box","woman","package","label"],"description":"A woman putting shipping label on a product box. Used to represent add a product.","publish":1}</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -9491,7 +9550,7 @@
         <v>{"id":23,"title":"zerodata-configure-component-governance","group":"zerodata","area":"compliance","keywords":["product","box","scan","xray","package","compliance","screen","component","governance"],"description":"A product box going through x-ray scan. Used to represent configure component governance.","publish":1}</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -9518,7 +9577,7 @@
         <v>{"id":24,"title":"zerodata-release-management","group":"zerodata","area":"build","keywords":["rocket","release","launch","cloud"],"description":"A rocket on a launch pad. Used for release management.","publish":1}</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -9545,7 +9604,7 @@
         <v>{"id":25,"title":"zerodata-this-repository-has-no-tags-yet","group":"zerodata","area":"code","keywords":["folder","tag","repository"],"description":"A dotted line tag on a folder. Used to represent there is no tag on this repository.","publish":1}</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -9572,7 +9631,7 @@
         <v>{"id":26,"title":"zerodata-add-deployment-group","group":"zerodata","area":"build","keywords":["server","pin","computer","deployment","group","target"],"description":"A map pin on a server. Used to represent targeted deployment group.","publish":1}</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -9599,7 +9658,7 @@
         <v>{"id":27,"title":"zerodata-automate-build-definitions","group":"zerodata","area":"build","keywords":["build","robot","arm","box","construction"],"description":"A robot arm lifting building blocks. Used to represent build.","publish":1}</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -9626,7 +9685,7 @@
         <v>{"id":28,"title":"zerodata-choose-a-template","group":"zerodata","area":"build","keywords":["template","shape","cookie","cutter","star","arrow","diamond","hexagon"],"description":"A template with several shapes. Used in Build area for selecting templates.","publish":1}</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -9653,7 +9712,7 @@
         <v>{"id":29,"title":"zerodata-cloud-based-load-testing","group":"zerodata","area":"test","keywords":["cloud","gauge","stress","test","performance","load","test"],"description":"A gauge on a cloud. Used for cloud based load testing.","publish":1}</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -9680,7 +9739,7 @@
         <v>{"id":30,"title":"zerodata-favorites","group":"zerodata","area":"common","keywords":["favorite","star","box","folder","question","chat","work","bullet","list"],"description":"Favorite star on frequently used work objects.","publish":1}</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -9707,7 +9766,7 @@
         <v>{"id":31,"title":"zerodata-get-everyone-on-same-page","group":"zerodata","area":"wiki","keywords":["wiki","page","book","people","team","knowledge","share","man","woman"],"description":"People sharing knowledge via wiki.","publish":1}</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -9734,7 +9793,7 @@
         <v>{"id":32,"title":"zerodata-no-plan","group":"zerodata","area":"work","keywords":["plan","draft","collaborate","hands","paper","triangle","tool","ruler","magnifier","pen"],"description":"Four hands holding tools and working on a drafting paper. Used when there is no plan for the current project.","publish":1}</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -9761,7 +9820,7 @@
         <v>{"id":33,"title":"zerodata-no-variable-groups","group":"zerodata","area":"build","keywords":["variable","group","(x)","box","stack"],"description":"Stacked blocks with variables. Used when there is no variable group.","publish":1}</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -9788,7 +9847,7 @@
         <v>{"id":34,"title":"zerodata-pull-request","group":"zerodata","area":"code","keywords":["code","pull","request","people","team"],"description":"A person making pull request and asking for code review.","publish":1}</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -9815,7 +9874,7 @@
         <v>{"id":35,"title":"hero-swiss-army-knife","group":"vscom","area":"hero","keywords":["swiss","army","knife","tools","extension","productivity","wrench","scissors","screwdriver"],"description":"A Swiss Army knife representing a bundle of developer tools. Used on Visual Studio pricing page for comparing different levels of subscription.","publish":1}</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -9842,7 +9901,7 @@
         <v>{"id":36,"title":"swimlane-all-your-code-hosted-free","group":"vscom","area":"swimlane","keywords":["team","people","work","desk","office","man","woman","developer","cloud","git","version","control","host","laptop","chair"],"description":"Unlimited Git repository support for individuals and up to four team members. Used on Git page.","publish":1}</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -9869,7 +9928,7 @@
         <v>{"id":37,"title":"swimlane-any-client-any-platform","group":"vscom","area":"swimlane","keywords":["laptop","computer","desktop","monitor","windows","mac","osx","linux","ubuntu","cross","platform","device"],"description":"Three computers with typical Windows, Mac OS and Linux screens. Used to indicate Git support on any platform and any client on Git page.","publish":1}</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -9896,7 +9955,7 @@
         <v>{"id":38,"title":"swimlane-but-wait-theres-more","group":"vscom","area":"swimlane","keywords":["tree","node","branch","woman","people","feature","laptop","computer","smartphone","control","panel","tools","document","rocket","chart"],"description":"A woman standing on a tree of features. Used on VS Enterprise page.","publish":1}</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -9923,7 +9982,7 @@
         <v>{"id":39,"title":"swimlane-pricing","group":"vscom","area":"swimlane","keywords":["pricing","calculator","pen","laptop"],"description":"Used on pricing pages.","publish":1}</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -9950,7 +10009,7 @@
         <v>{"id":40,"title":"swimlane-were-in-your-neighborhood","group":"vscom","area":"swimlane","keywords":["globe","world","map","woman"],"description":"A woman standing in front of a world map. Used to represent data center available around the world.","publish":1}</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -9977,7 +10036,7 @@
         <v>{"id":41,"title":"hero-pricing-calculator","group":"vscom","area":"hero","keywords":["pricing","calculator","pen","laptop"],"description":"Used on pricing pages. Bottom shadow removed. Use this version on dark background.","publish":1}</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -10004,7 +10063,7 @@
         <v>{"id":42,"title":"zerodata-you-have-no-organizations-yet","group":"nuget","area":"zerodata","keywords":["empty","organization","team","office","desk","clock","chair"],"description":"An office space with empty chairs. Used for zero data state when users have not created organizations.","publish":1}</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -10031,7 +10090,7 @@
         <v>{"id":43,"title":"general-robot-errorcode-503","group":"general","area":"common","keywords":["error","code","503","robot","server","down","broken","offline"],"description":"Used for 503 error page when server is down.","publish":1}</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -10058,7 +10117,7 @@
         <v>{"id":44,"title":"general-robot-error","group":"general","area":"common","keywords":["error","robot","exclamation","alert","exception"],"description":"Used for generic error page.","publish":1}</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -10085,7 +10144,7 @@
         <v>{"id":45,"title":"general-robot-errorcode-400","group":"general","area":"common","keywords":["error","code","400","robot","question"],"description":"Used for 400 error page bad request.","publish":1}</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -10112,7 +10171,7 @@
         <v>{"id":46,"title":"general-robot-errorcode-401","group":"general","area":"common","keywords":["error","code","401","robot","unauthorized"],"description":"Used for 401 error page unauthorized.","publish":1}</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -10139,7 +10198,7 @@
         <v>{"id":47,"title":"general-robot-errorcode-403","group":"general","area":"common","keywords":["error","code","403","robot","forbidden","permission","access"],"description":"Used for 403 error page the user does not have access.","publish":1}</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -10166,7 +10225,7 @@
         <v>{"id":48,"title":"general-robot-errorcode-404","group":"general","area":"common","keywords":["error","code","404","robot","not","found"],"description":"Used for 404 error page.","publish":1}</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -10193,7 +10252,7 @@
         <v>{"id":49,"title":"general-robot-errorcode-500","group":"general","area":"common","keywords":["error","code","500","robot","server","internal"],"description":"Used for 500 error page server error.","publish":1}</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -10220,7 +10279,7 @@
         <v>{"id":50,"title":"zerodata-no-assessments","group":"zerodata","area":"compliance","keywords":["assessments","compliance","analysis","laptop","magnifier","clipboard","chart"],"description":"For assessments page zero data state.","publish":1}</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -10247,7 +10306,7 @@
         <v>{"id":51,"title":"zerodata-initializing-test-results","group":"zerodata","area":"test","keywords":["test","initialize","result","beaker","lab","flask","clock","wait","loading"],"description":"Waiting screen image when test result is being loaded.","publish":1}</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -10274,7 +10333,7 @@
         <v>{"id":52,"title":"zerodata-no-work-scheduled","group":"zerodata","area":"work","keywords":["work","plan","planner","calendar","journal","schedule","notebook","pencil"],"description":"No work planned in current sprint.","publish":1}</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -10301,7 +10360,7 @@
         <v>{"id":53,"title":"zerodata-sprint-drag-n-drop","group":"zerodata","area":"work","keywords":["drag","drop","work","item","list","move"],"description":"Used on the Sprint page left panel to indicate there is no work item in the left panel yet.","publish":1}</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -10328,7 +10387,7 @@
         <v>{"id":54,"title":"swimlane-seamless-debugging-with-symbols","group":"vscom","area":"swimlane","keywords":["symbol","code","tag","label","identifier","file"],"description":"Used for Enable seamless debugging with symbols swimlane.","publish":1}</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="5">
         <v>55</v>
       </c>
@@ -10355,7 +10414,7 @@
         <v>{"id":55,"title":"swimlane-xamarin-cross-platform","group":"dotnet","area":"swimlane","keywords":["xamarin","cross","platform","computer","laptop","tablet","phone"],"description":"Xamarin.Mac allows user to create native iOS, Android and Mac apps.","publish":1}</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="5">
         <v>56</v>
       </c>
@@ -10382,7 +10441,7 @@
         <v>{"id":56,"title":"swimlane-azure-machine-learning","group":"dotnet","area":"swimlane","keywords":["azure","machine","learning","process","cloud","lightbulb","clock","analytics","magnifier","charts"],"description":"Azure Machine Learning.","publish":1}</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="5">
         <v>57</v>
       </c>
@@ -10409,7 +10468,7 @@
         <v>{"id":57,"title":"swimlane-cognitive-services","group":"dotnet","area":"swimlane","keywords":["cognitive","services","vision","sound","voice","speech","microphone","input","speaker","bubble","eye","magnifier"],"description":"Cognitive services such as voice recognition, vision detection, language processing, etc.","publish":1}</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="5">
         <v>58</v>
       </c>
@@ -10436,7 +10495,7 @@
         <v>{"id":58,"title":"swimlane-congratulations-finished-setup","group":"dotnet","area":"swimlane","keywords":["finish","complete","race","car","monitor","flag","people"],"description":"Used on a screen when user successfully finishes setup.","publish":1}</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="5">
         <v>59</v>
       </c>
@@ -10463,7 +10522,7 @@
         <v>{"id":59,"title":"swimlane-cross-platform","group":"dotnet","area":"swimlane","keywords":["cross","platform","windows","mac","linux","computer","laptop","mobile","phone"],"description":"Used to represent multiple Oss and devices.","publish":1}</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="5">
         <v>60</v>
       </c>
@@ -10490,7 +10549,7 @@
         <v>{"id":60,"title":"swimlane-cryengine-game-development","group":"dotnet","area":"swimlane","keywords":["cryengine","video","game","development","computer","monitor","keyboard","mouse","3d"],"description":"An example 3d game screen created with CRYENGINE.","publish":1}</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="5">
         <v>61</v>
       </c>
@@ -10517,7 +10576,7 @@
         <v>{"id":61,"title":"swimlane-developer-meetup","group":"dotnet","area":"swimlane","keywords":["meetup","people","chat","discussion","idea","light","bulb"],"description":"Three people talking about ideas.","publish":1}</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="5">
         <v>62</v>
       </c>
@@ -10544,7 +10603,7 @@
         <v>{"id":62,"title":"swimlane-dotnet-core","group":"dotnet","area":"swimlane","keywords":["developer","people","computer","laptop","work","office","team","startup"],"description":"A small team of developers working together.","publish":1}</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="5">
         <v>63</v>
       </c>
@@ -10571,7 +10630,7 @@
         <v>{"id":63,"title":"swimlane-dotnet-enterprise","group":"dotnet","area":"swimlane","keywords":["developer","people","enterprise","building","company","laptop","computer","work","office"],"description":"A developer working in an enterprise scale environment.","publish":1}</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="5">
         <v>64</v>
       </c>
@@ -10598,7 +10657,7 @@
         <v>{"id":64,"title":"swimlane-download-target","group":"dotnet","area":"swimlane","keywords":["people","download","welcome","computer","table","chair"],"description":"A generic download landing screen.","publish":1}</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="5">
         <v>65</v>
       </c>
@@ -10625,7 +10684,7 @@
         <v>{"id":65,"title":"swimlane-enterprise-customer-stories","group":"dotnet","area":"swimlane","keywords":["building","company","team","people","enterprise"],"description":"Enterprise user stories.","publish":1}</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="5">
         <v>66</v>
       </c>
@@ -10652,7 +10711,7 @@
         <v>{"id":66,"title":"swimlane-feedback-survey","group":"dotnet","area":"swimlane","keywords":["feedback","people","survey","listen","paper","cup"],"description":"A person listening user feedback with paper cup telephone.","publish":1}</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="5">
         <v>67</v>
       </c>
@@ -10679,7 +10738,7 @@
         <v>{"id":67,"title":"swimlane-fsharp-data-science","group":"dotnet","area":"swimlane","keywords":["data","science","lab","test","tube","beaker","chart","analytics","laptop","scientist"],"description":"A data scientist working in the lab.","publish":1}</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="5">
         <v>68</v>
       </c>
@@ -10706,7 +10765,7 @@
         <v>{"id":68,"title":"swimlane-machine-learning-library","group":"dotnet","area":"swimlane","keywords":["machine","learning","library","ai","test","beaker","book"],"description":"Used for machine learning AI library.","publish":1}</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="5">
         <v>69</v>
       </c>
@@ -10733,7 +10792,7 @@
         <v>{"id":69,"title":"swimlane-one-consistent-api","group":"dotnet","area":"swimlane","keywords":["one","api","consistent","people","tool","library","book","light","bulb","idea","ui","code"],"description":"A person surrounded by multiple developer tools.","publish":1}</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="5">
         <v>70</v>
       </c>
@@ -10760,7 +10819,7 @@
         <v>{"id":70,"title":"swimlane-package-library","group":"dotnet","area":"swimlane","keywords":["package","box","circuit"],"description":"A few packages soldered on a circuit.","publish":1}</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="5">
         <v>71</v>
       </c>
@@ -10787,7 +10846,7 @@
         <v>{"id":71,"title":"swimlane-programming-languages","group":"dotnet","area":"swimlane","keywords":["developer","programming","language","keyboard","c#","VB","F#"],"description":"Developers of different programming languages.","publish":1}</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="5">
         <v>72</v>
       </c>
@@ -10814,7 +10873,7 @@
         <v>{"id":72,"title":"swimlane-thank-you-for-downloading","group":"dotnet","area":"swimlane","keywords":["download","cloud","document","file"],"description":"A generic download screen after download started/finished.","publish":1}</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="5">
         <v>73</v>
       </c>
@@ -10841,7 +10900,7 @@
         <v>{"id":73,"title":"swimlane-unity-game-development","group":"dotnet","area":"swimlane","keywords":["2d","3d","video","game","castle","unity"],"description":"An example 3d game screen created with Unity.","publish":1}</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="5">
         <v>74</v>
       </c>
@@ -10868,7 +10927,7 @@
         <v>{"id":74,"title":"swimlane-universal-windows-platform","group":"dotnet","area":"swimlane","keywords":["uwp","universal","windows","platform","octopus","hololens","iot","surface","phone","tablet","band","game","controller","drone"],"description":"A octopus holding and wearing many devices built with UWP.","publish":1}</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="5">
         <v>75</v>
       </c>
@@ -10895,7 +10954,7 @@
         <v>{"id":75,"title":"swimlane-uwp-iot-core","group":"dotnet","area":"swimlane","keywords":["iot","core","drone","security","camera","microwave","thermometer","smart","home"],"description":"Common smart devices built with UWP IoT Core.","publish":1}</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="5">
         <v>76</v>
       </c>
@@ -10922,7 +10981,7 @@
         <v>{"id":76,"title":"swimlane-winform","group":"dotnet","area":"swimlane","keywords":["winform","drag","drop","designer","pencil","ruler","dialog","ui"],"description":"Drag and drop designer for building Winform applications.","publish":1}</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="5">
         <v>77</v>
       </c>
@@ -10949,7 +11008,7 @@
         <v>{"id":77,"title":"swimlane-wpf","group":"dotnet","area":"swimlane","keywords":["wpf","windows","presentation","foundation","ui","design","code","screen","monitor","computer"],"description":"A code and designer view used to represent WPF.","publish":1}</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="5">
         <v>78</v>
       </c>
@@ -10976,7 +11035,7 @@
         <v>{"id":78,"title":"swimlane-xamarin","group":"dotnet","area":"swimlane","keywords":["xamarin","mobile","cross","platform","development","phone","laptop","code"],"description":"Build cross-platform apps with Xamarin and one code base.","publish":1}</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="5">
         <v>79</v>
       </c>
@@ -11003,7 +11062,7 @@
         <v>{"id":79,"title":"swimlane-dotnet-perf-diagram","group":"dotnet","area":"swimlane","keywords":[".net","diagram","bar","chart"],"description":"A bar chart comparing requests per second of three frameworks.","publish":0}</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="5">
         <v>80</v>
       </c>
@@ -11030,7 +11089,7 @@
         <v>{"id":80,"title":"hero-snapshot-debugger","group":"vscom","area":"hero","keywords":["snapshot","debugger","debug","bug","magnifier","code","cloud"],"description":"Debugging code on the cloud.","publish":1}</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="5">
         <v>81</v>
       </c>
@@ -11057,7 +11116,7 @@
         <v>{"id":81,"title":"swimlane-collaborative-debugging","group":"vscode","area":"swimlane","keywords":["collaborate","debug","teamwork","hands","plan","draw","ruler","design","pen","triangle","bug","magnifier","lightbulb"],"description":"Collaborative debugging.","publish":1}</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="5">
         <v>82</v>
       </c>
@@ -11080,11 +11139,11 @@
         <v>1</v>
       </c>
       <c r="I83" s="2" t="str">
-        <f t="shared" ref="I83:I89" si="1">SUBSTITUTE(_xlfn.CONCAT("{'id':",A83,",'title':'",C83,"','group':'",D83,"','area':'",E83,"','keywords':['",SUBSTITUTE(F83," ","','"),"'],'description':'",G83,"','publish':",H83,"}"),"'","""")</f>
+        <f t="shared" ref="I83:I90" si="1">SUBSTITUTE(_xlfn.CONCAT("{'id':",A83,",'title':'",C83,"','group':'",D83,"','area':'",E83,"','keywords':['",SUBSTITUTE(F83," ","','"),"'],'description':'",G83,"','publish':",H83,"}"),"'","""")</f>
         <v>{"id":82,"title":"swimlane-collaborative-editing","group":"vscode","area":"swimlane","keywords":["collaborate","editor","code","people"],"description":"Collaborative code editing.","publish":1}</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="5">
         <v>83</v>
       </c>
@@ -11111,7 +11170,7 @@
         <v>{"id":83,"title":"swimlane-shared-full-context","group":"vscode","area":"swimlane","keywords":["share","context","code","editor","environment","computer","laptop"],"description":"Share code and full context.","publish":1}</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="5">
         <v>84</v>
       </c>
@@ -11138,7 +11197,7 @@
         <v>{"id":84,"title":"swimlane-real-time-sharing","group":"vscode","area":"swimlane","keywords":["people","work","team","office","real","time","code","developer","clock"],"description":"Real-time sharing with your tools.","publish":1}</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="5">
         <v>85</v>
       </c>
@@ -11165,7 +11224,7 @@
         <v>{"id":85,"title":"blog-rocket-launch-timeline","group":"vscode","area":"blog","keywords":["rocket","release","launch","cloud","timeline"],"description":"Rocket launch timeline.","publish":1}</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="5">
         <v>86</v>
       </c>
@@ -11192,7 +11251,7 @@
         <v>{"id":86,"title":"blog-vscode-metrics","group":"vscom","area":"blog","keywords":["metrics"],"description":"Download and install metrics of Visual Studio Code.","publish":1}</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="5">
         <v>87</v>
       </c>
@@ -11219,7 +11278,7 @@
         <v>{"id":87,"title":"blog-vscode-roadmap","group":"vscom","area":"blog","keywords":["roadmap","car","road","milestone","pin","timeline"],"description":"A roadmap showing Visual Studio Code major release milestones","publish":1}</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="5">
         <v>88</v>
       </c>
@@ -11244,6 +11303,33 @@
       <c r="I89" s="2" t="str">
         <f t="shared" si="1"/>
         <v>{"id":88,"title":"swimlane-monogame-game-development","group":"dotnet","area":"swimlane","keywords":["monogame","game","development","screen","platform","psvita","windows","mac","video","game"],"description":"Cross platform game development with MonoGame engine.","publish":1}</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A90" s="5">
+        <v>89</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="D90" t="s">
+        <v>246</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="G90" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="H90" s="2">
+        <v>1</v>
+      </c>
+      <c r="I90" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>{"id":89,"title":"zerodata-you-have-no-project","group":"zerodata","area":"account","keywords":["project","plan","work","briefcase","pencil","document","triangle","ruler"],"description":"Used in account page when you have no projects yet.","publish":1}</v>
       </c>
     </row>
   </sheetData>
@@ -11267,22 +11353,22 @@
       <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="38.140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.83984375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.83984375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="38.15625" style="2" customWidth="1"/>
     <col min="4" max="4" width="17" style="2" customWidth="1"/>
     <col min="5" max="5" width="18" style="2" customWidth="1"/>
-    <col min="6" max="6" width="33.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" style="2" customWidth="1"/>
-    <col min="8" max="9" width="24.140625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="33.140625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="66.42578125" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="2"/>
+    <col min="6" max="6" width="33.68359375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="20.68359375" style="2" customWidth="1"/>
+    <col min="8" max="9" width="24.15625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="33.15625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="66.41796875" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="9.15625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="3" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>73</v>
       </c>
@@ -11317,7 +11403,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -11351,7 +11437,7 @@
         <v>{"id":1,"title":"AzureToolsForVS","category":"VSCOM","keywords":["free","hosting","bug","tools","platforms","testing","beaker","wrench","azure","logo"],"description":"Azure developer tools for Visual Studio with free hosting.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -11385,7 +11471,7 @@
         <v>{"id":2,"title":"CloudPattern","category":"Pattern","keywords":["technology","nature","cloud","sky"],"description":"Clouds on blue sky pattern.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -11419,7 +11505,7 @@
         <v>{"id":3,"title":"CollaborationChatBubbles","category":"Diagram","keywords":["work","chat","bubble","conversation","communication","collaboration","team","men","women","people"],"description":"Several chat bubbles with people inside.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -11453,7 +11539,7 @@
         <v>{"id":4,"title":"CollaborationNetwork","category":"Diagram","keywords":["man","woman","network","hub","collaboration","connection","web","idea","lightbulb","gear","cloud","chat","bubble","work"],"description":"A network of people and objects connected together.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -11487,7 +11573,7 @@
         <v>{"id":5,"title":"CommunityTranslation1","category":"VSCOM","keywords":["hand","phone","hello","word","balloon","languages"],"description":"Translate world languages with smartphone.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -11521,7 +11607,7 @@
         <v>{"id":6,"title":"CommunityTranslation2","category":"VSCOM","keywords":["group","people","tablet","languages"],"description":"People from around the world using translation app on smart device to say hello.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -11555,7 +11641,7 @@
         <v>{"id":7,"title":"CommunityTranslation3","category":"VSCOM","keywords":["group","people","tablet","languages"],"description":"People from around the world using translation app on smart device to say hello.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -11589,7 +11675,7 @@
         <v>{"id":8,"title":"CordovaToolsTwitterBanner","category":"Web","keywords":["crane","cloud","tools","tree","build","construction"],"description":"Cordova Tools Twitter account banner. Construction crane and build tools on cloud.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -11623,7 +11709,7 @@
         <v>{"id":9,"title":"DesktopComputerPattern","category":"Pattern","keywords":["desktop","computer","monitor","pc","technology"],"description":"Desktop computer pattern.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -11657,7 +11743,7 @@
         <v>{"id":10,"title":"DevEssentials1","category":"VSCOM","keywords":["download","arrow","magnifying","glass","monitor","laptop","data","graphs","gears","newsletter"],"description":"Data visualization related elements on a cloud.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -11691,7 +11777,7 @@
         <v>{"id":11,"title":"DevEssentials2","category":"VSCOM","keywords":["download","arrow","magnifying","glass","monitor","laptop","data","graphs","gears","toolbox","newsletter"],"description":"Data visualization related elements on a cloud.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -11725,7 +11811,7 @@
         <v>{"id":12,"title":"DevicesPattern","category":"Pattern","keywords":["laptop","phone","tablet","smartphone","technology"],"description":"Mixed devices pattern.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -11759,7 +11845,7 @@
         <v>{"id":13,"title":"DevOpsLifecycle","category":"Diagram","keywords":["handshake","planning","continuous","delivery","dev","test","analytics","mobius","infinity","loop"],"description":"DevOps lifecycle.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -11793,7 +11879,7 @@
         <v>{"id":14,"title":"FeedbackCommentsDiscussion","category":"Email","keywords":["chat","bubble","question","exclaimation","conversation","discussion"],"description":"Feedback comment discussion.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -11827,7 +11913,7 @@
         <v>{"id":15,"title":"FeedbackPattern","category":"Pattern","keywords":["feedback","chat","bubble","conversation","question","exclaimation","problem","comment","talk"],"description":"Chat bubble feedback pattern.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -11861,7 +11947,7 @@
         <v>{"id":16,"title":"FoodCollection","category":"Elements","keywords":["food","meal","nutrition","soup","bread","spoon","tomato","broccli","vegetable","fish","crab","seafood","meat","poultry","steak","chicken","turkey","cake","pie","dessert","measuring","cup","egg","beater","cooking","utencils","drink","cocktail","glass","toast","cracker","cheese","burger","hotdog","salad","appetizer","entree"],"description":"A collection of food icons.","style":["color","sketchy"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -11895,7 +11981,7 @@
         <v>{"id":17,"title":"IdeaFactory","category":"Web","keywords":["factory","building","gear","lightbulb","database","arrow","document","gauge","lift","truck"],"description":"Ideas being manufactured in a factory.","style":["monotone"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -11929,7 +12015,7 @@
         <v>{"id":18,"title":"IntegratedDevelopmentLoop","category":"Email","keywords":["loop","cycle","edit","pencil","script","scroll","bug","arrow","device","phone","mobile","cloud"],"description":"Lifecycle of code, debug and deployment.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -11963,7 +12049,7 @@
         <v>{"id":19,"title":"InternetOfThings","category":"Diagram","keywords":["internet","iot","globe","router","smart","phone","laptop","light","bulb","printer","desktop","media","player","car","smart","home","smart","watch","mobile","payment","device","software","development"],"description":"The Internet of Things (IoT) is the network of physical objects or things embedded with electronics, software, sensors, and network connectivity, which enables these objects to collect and exchange data.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -11997,7 +12083,7 @@
         <v>{"id":20,"title":"ManufacturingIdeas","category":"Misc","keywords":["machine","tool","lightbulb"],"description":"Ideas being manufactured by a machine.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -12031,7 +12117,7 @@
         <v>{"id":21,"title":"MicrosoftWelcomeCenter","category":"Print","keywords":["microsoft","company","building","welcome","logo","work","business"],"description":"Microsoft logo and office buildings.","style":["color","3d"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -12065,7 +12151,7 @@
         <v>{"id":22,"title":"MobileAppDevelopmentPlatform","category":"VSCOM","keywords":["building","city","cloud","billboard","people","device","laptop","phone","database","security","lock","presentation","chart","development","platform","enterprise","business"],"description":"Mobile app development platform.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -12099,7 +12185,7 @@
         <v>{"id":23,"title":"MobileAppDevelopmentWithVisualStudio","category":"VSCOM","keywords":["laptop","phone","iphone","android","windows","app","development","visual","studio"],"description":"Cross platform mobile app development with Visual Studio.","style":["color","photo","monotone"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -12133,7 +12219,7 @@
         <v>{"id":24,"title":"MultiDeviceTwitterBanner","category":"Web","keywords":["cloud","sky","field","grass","phone","smartphone","tablet","computer","desktop","pc","monitor","tv","television","microsoft","logo","technology","developer"],"description":"Cordova Tools Twitter account banner. Four device icons overlay on top of cloud and field backgournd.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -12167,7 +12253,7 @@
         <v>{"id":25,"title":"NETCoreWebsiteBanner","category":"Web","keywords":["visual","studio","html5","css3","javascript"],"description":".NET Core website banner.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -12201,7 +12287,7 @@
         <v>{"id":26,"title":"OneToolForEverything","category":"Email","keywords":["tool","laptop","mobile","phone","cloud"],"description":"One tool for all platform.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -12235,7 +12321,7 @@
         <v>{"id":27,"title":"OpenSourceComputer","category":"Web","keywords":["laptop","code","arrow","exchange"],"description":"Two laptop exchanging code.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -12269,7 +12355,7 @@
         <v>{"id":28,"title":"OpenSourceExchangeCode","category":"Diagram","keywords":["code","man","woman","laptop","desktop","exchange","share","arrow"],"description":"Developers exchange open source code.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -12303,7 +12389,7 @@
         <v>{"id":29,"title":"PlaceholderFlowers","category":"VSTS","keywords":["flower"],"description":"Placeholder images.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -12337,7 +12423,7 @@
         <v>{"id":30,"title":"PublishAndDeploy","category":"Email","keywords":["rocket","document","arrow","exchange"],"description":"Publish and deploy code.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -12371,7 +12457,7 @@
         <v>{"id":31,"title":"PushNotifications","category":"Web","keywords":["mobile","phone","tablet","android","windows","ios","chat","bubble","notification"],"description":"Push notifications on multiple platforms.","style":["monotone"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -12405,7 +12491,7 @@
         <v>{"id":32,"title":"PythonToolsForVS","category":"VSCOM","keywords":["man","laptop","woman","gears","bug","code","phone","python","logo","magnifying","glass"],"description":"Python tools for Visual Studio.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -12439,7 +12525,7 @@
         <v>{"id":33,"title":"QuickstartFastSpeed","category":"Email","keywords":["stopwatch","run","man","time","fast","quick","speed"],"description":"Quick start","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -12473,7 +12559,7 @@
         <v>{"id":34,"title":"RocketMulticolor","category":"Elements","keywords":["rocket","launch","deployment"],"description":"Rocket","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -12507,7 +12593,7 @@
         <v>{"id":35,"title":"RocketWithCloudPattern","category":"Print","keywords":["rocket","cloud","sky"],"description":"Rocket on sky background","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -12541,7 +12627,7 @@
         <v>{"id":36,"title":"SeattlePostcard","category":"Print","keywords":["seattle","space","needle","cloud","city"],"description":"Seattle space needle postcard","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -12575,7 +12661,7 @@
         <v>{"id":37,"title":"SeattleSkyline","category":"Web","keywords":["seattle","space","needle","cloud","city","skyline","building","mount","rainier"],"description":"Seattle city skyline","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -12609,7 +12695,7 @@
         <v>{"id":38,"title":"SeattleSkylineFerrisWheel","category":"Web","keywords":["seattle","space","needle","ferris","wheel","waterfront","port"],"description":"Seattle city skyline","style":["monotone"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -12643,7 +12729,7 @@
         <v>{"id":39,"title":"SilhouetteAirportElements","category":"Elements","keywords":["airport","pilot","flight","attendant","uniform","causeway","airplane","sign","direction","loudge","coffee","terminal","seat","life"],"description":"A collection of airport related elements.","style":["silhuoette"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -12677,7 +12763,7 @@
         <v>{"id":40,"title":"SilhouetteBriefcasesAndDocuments","category":"Elements","keywords":["document","file","paper","briefcase","suitcase","handbag","work","object","business"],"description":" A collection of briefcases.","style":["silhuoette"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -12711,7 +12797,7 @@
         <v>{"id":41,"title":"SilhouetteCharacters","category":"Elements","keywords":["man","confuse","suit","woman","chair","desk","laptop","computer","office","work","business"],"description":"A collection of characters in work environment.","style":[" ","silhuoette"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -12745,7 +12831,7 @@
         <v>{"id":42,"title":"SilhouetteHandGenstures","category":"Elements","keywords":["hand","gesture","pick","grip","pinch","touch","web","press","technology"],"description":"Hand gestures.","style":["silhuoette"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -12779,7 +12865,7 @@
         <v>{"id":43,"title":"SilhouetteTabletAndPhones","category":"Elements","keywords":["technology","work","tablet","smartphone","phone","mobile","phone","pen","stylus","windows","phone","android","phone","surface","tablet"],"description":"Tablet and smartphones.","style":["silhuoette"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -12813,7 +12899,7 @@
         <v>{"id":44,"title":"SilhouetteToolCollection","category":"Pattern","keywords":["wrench","screwdriver","saw","plier","hammer","knife","c","clamp","clamp","pipe","wrench","filer","triangle","ruler","object"],"description":"A collection of hand tools.","style":["silhouette"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -12847,7 +12933,7 @@
         <v>{"id":45,"title":"SilhouetteWeatherReportElements","category":"Elements","keywords":["life","newspaper","radio","magezine","clock","news","weather","forcast","tv","sun","sunny","cloud","lightning","thunder","cloud","cloudy","rain","tripical","palm","tree","beach","table","vacation","beach","chair","hawaii","man","relax","drink"],"description":"A collection of weather related illustrations.","style":["silhuoette"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -12881,7 +12967,7 @@
         <v>{"id":46,"title":"SoftwareToolsSampleKit","category":"Email","keywords":["toolbox","hammer","checklist","wrench","cloud"],"description":"Software development toolkit","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -12915,7 +13001,7 @@
         <v>{"id":47,"title":"TeamworkStairs","category":"Web","keywords":["people","man","stairs","team"],"description":"People holding hands climbing up stairs as a team.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -12949,7 +13035,7 @@
         <v>{"id":48,"title":"Testing","category":"Email","keywords":["test","flask","lab","beaker","stopwatch","pie","chart","checklist"],"description":"Testing","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -12983,7 +13069,7 @@
         <v>{"id":49,"title":"VSBuildALMIntegration","category":"VSCOM","keywords":["people","working","man","computer","clipboard","debug","tools","gear","bug"],"description":"ALM (Application Lifecycle Management) debug integration.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -13017,7 +13103,7 @@
         <v>{"id":50,"title":"VSBuildCloudHostedTools","category":"VSCOM","keywords":["people","laptops","desk","workers","monitors","laptops","cross","platforms","linux","windows","ios"],"description":"Developers come from different platforms and technology stacks working together.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -13051,7 +13137,7 @@
         <v>{"id":51,"title":"VSBuildContinuousIntegration","category":"VSCOM","keywords":["monitor","laptop","test","tubes","gears","checkmark"],"description":"Build continuous integration cycle with cloud.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -13085,7 +13171,7 @@
         <v>{"id":52,"title":"VSBuildContinuousIntegrationWhite","category":"VSCOM","keywords":["cross","platforms","maven","git","apache","ant","junit","gradle","xunit","mtm","test","building"],"description":"Common tools and technologies for cross-platform development.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -13119,7 +13205,7 @@
         <v>{"id":53,"title":"VSBuildCrossPlatform","category":"VSCOM","keywords":["pillars","cross","platforms","buildings","crane","java",".net","xcode","github","ios","android","windows","git"],"description":"Common tools and technologies for cross-platform development.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -13153,7 +13239,7 @@
         <v>{"id":54,"title":"VSBuildOverview","category":"VSCOM","keywords":["cross","platforms","laptop","tablet","phone","ios","android","visual","studio","cloud"],"description":"Visual Studio for building cross-platform applications.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -13187,7 +13273,7 @@
         <v>{"id":55,"title":"VSBuildTraceability","category":"VSCOM","keywords":["blueprint","document","man","beaker","tools","clipboard","timeline","printer","download","test","tubes","gears","magnifying","glass","graphs"],"description":"Build timeline and tracebility.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -13221,7 +13307,7 @@
         <v>{"id":56,"title":"VSDownload1","category":"VSCOM","keywords":["group","people","visual","studio","logo","flags","man","woman"],"description":"Visual Studio for everyone.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -13255,7 +13341,7 @@
         <v>{"id":57,"title":"VSDownload2","category":"VSCOM","keywords":["man","monitors","download","down","arrow","computer","table"],"description":"Visual Studio tools for multiplatform.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -13289,302 +13375,302 @@
         <v>{"id":58,"title":"XamarinCrossPlatformDevelopment","category":"VSCOM","keywords":["screenshot","ios","android","windows","mobile","phone","app","development","shared","code","cross-platform","xamarin"],"description":"Xamarin for developing cross-platform application.","style":["color","photo"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="2">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="2">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="2">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="2">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="2">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="2">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="2">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="2">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="2">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="2">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="2">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="2">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="2">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="2">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="2">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="2">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="2">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="2">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="2">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="2">
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="2">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="2">
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="2">
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="2">
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="2">
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="2">
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="2">
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="2">
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="2">
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="2">
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="2">
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="2">
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="2">
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="2">
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="2">
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="2">
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="2">
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="2">
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="2">
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="2">
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="2">
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="2">
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="2">
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="2">
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="2">
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="2">
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="2">
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="2">
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="2">
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="2">
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="2">
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="2">
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="2">
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="2">
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="2">
         <v>114</v>
       </c>
     </row>
-    <row r="116" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="2">
         <v>115</v>
       </c>
     </row>
-    <row r="117" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" s="2">
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="2">
         <v>117</v>
       </c>
     </row>
-    <row r="119" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="2">
         <v>118</v>
       </c>
@@ -13619,9 +13705,9 @@
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="1" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
updated nav; added two new illustrations
</commit_message>
<xml_diff>
--- a/src/assets/data.xlsx
+++ b/src/assets/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chryw\Dropbox\Code\vsimages\src\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwang\Dropbox\Code\vsimages\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="498">
   <si>
     <t>SeattleSkyline</t>
   </si>
@@ -1514,6 +1514,15 @@
   </si>
   <si>
     <t>Used in account page when you have no projects yet.</t>
+  </si>
+  <si>
+    <t>hero-vsts-join-our-team</t>
+  </si>
+  <si>
+    <t>vsts team work ui join us people chart dialog gear</t>
+  </si>
+  <si>
+    <t>Used in VSTS jobs page hero section.</t>
   </si>
 </sst>
 </file>
@@ -6045,6 +6054,56 @@
         <a:xfrm>
           <a:off x="1169895" y="111897460"/>
           <a:ext cx="2030505" cy="1087770"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>134471</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>33618</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2313278</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>1232647</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="68" name="Picture 67">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33AA3F92-C714-4E49-BC43-1B66F6BD62C4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId91" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1019736" y="112910471"/>
+          <a:ext cx="2178807" cy="1199029"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8876,31 +8935,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I90"/>
+  <dimension ref="A1:I91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C90" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B88" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F91" sqref="F91"/>
+      <selection pane="bottomRight" activeCell="I91" sqref="I91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="100" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.26171875" style="7" customWidth="1"/>
-    <col min="2" max="2" width="35.83984375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="38.15625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="35.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="38.140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
     <col min="5" max="5" width="18" style="2" customWidth="1"/>
-    <col min="6" max="6" width="33.68359375" style="2" customWidth="1"/>
-    <col min="7" max="8" width="20.68359375" style="2" customWidth="1"/>
-    <col min="9" max="10" width="24.15625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="33.15625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="66.41796875" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="9.15625" style="2"/>
+    <col min="6" max="6" width="33.7109375" style="2" customWidth="1"/>
+    <col min="7" max="8" width="20.7109375" style="2" customWidth="1"/>
+    <col min="9" max="10" width="24.140625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="33.140625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="66.42578125" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>201</v>
       </c>
@@ -8929,7 +8988,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -8956,7 +9015,7 @@
         <v>{"id":1,"title":"general-something-wrong-on-server","group":"general","area":"common","keywords":["server","computer","tower","error","disconnect","problem"],"description":"One of three servers is down. Indicates that there is something wrong on the server side.","publish":1}</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -8983,7 +9042,7 @@
         <v>{"id":2,"title":"widget-you-dont-have-permission","group":"widget","area":"dashboard","keywords":["permission","access","man","lock","error","problem"],"description":"A man holding a lock sign. Indicates that you do not have permission to the content.","publish":1}</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -9010,7 +9069,7 @@
         <v>{"id":3,"title":"zerodata-charting-not-supported","group":"zerodata","area":"work","keywords":["chart","hierachy","error","warning","support","tree","exclamation","diagram"],"description":"Hierachy diagram with a warning sign. Indicates that charting is not supported for hierachical query. Users need to change to flat list query to use charting feature.","publish":1}</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -9037,7 +9096,7 @@
         <v>{"id":4,"title":"zerodata-custom-rules","group":"zerodata","area":"policies","keywords":["custom","build","car","arm","customization","vehicle","parts","hook","transportation"],"description":"Robot arms building a customized car. Used in Rules area to represent custom rules.","publish":1}</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -9064,7 +9123,7 @@
         <v>{"id":5,"title":"zerodata-get-back-to-recent-work","group":"zerodata","area":"account","keywords":["history","back","rewind","clock","recent","previous","arrow","time"],"description":"Backward clock. Represents recent work.","publish":1}</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -9091,7 +9150,7 @@
         <v>{"id":6,"title":"zerodata-invalid-workitem-type","group":"zerodata","area":"work","keywords":["plug","disconnect"],"description":"Plugs of two different standards that are not compatible with each other. Used when users try to create a work item which type does not exist in the current project.","publish":1}</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -9118,7 +9177,7 @@
         <v>{"id":7,"title":"zerodata-keep-an-eye-on-important-work","group":"zerodata","area":"account","keywords":["man","people","mail","message","idea","code","envelope","lightbulb","chat","bubble","brackets"],"description":"A man looking at some workspace tools. Used to represent all relevant works can be found in one place.","publish":1}</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -9145,7 +9204,7 @@
         <v>{"id":8,"title":"zerodata-mention-someone","group":"zerodata","area":"account","keywords":["mention","at","@","message","chat","conversation","discussion","people","avatar","woman","man"],"description":"A conversation between two users with an @ in the chat bubble that mimics the mention feature.","publish":1}</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -9172,7 +9231,7 @@
         <v>{"id":9,"title":"zerodata-no-charts","group":"zerodata","area":"work","keywords":["chart","pie","bar","area"],"description":"Several common chart types. Used in Work hub analytics when there is no data to create chart.","publish":1}</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -9199,7 +9258,7 @@
         <v>{"id":10,"title":"zerodata-unsaved-query","group":"zerodata","area":"work","keywords":["chart","dotted","line","invisible","temporary","save","floppy","disk","pie","bar"],"description":"Dotted line charts with save icon. Indicates that charting is not available until you save query.","publish":1}</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -9226,7 +9285,7 @@
         <v>{"id":11,"title":"zerodata-workitem-not-found","group":"zerodata","area":"work","keywords":["tools","hammer","drill","saw","plier","missing","dotted","line"],"description":"A hammer missing from a set of tools. Indicates that work item is not found or you do not have permission to view it.","publish":1}</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -9253,7 +9312,7 @@
         <v>{"id":12,"title":"zerodata-your-work-in-one-place","group":"zerodata","area":"account","keywords":["woman","avatar","people"],"description":"A woman avatar in circle. Used in Account page when you do not have works assigned to you yet.","publish":1}</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -9280,7 +9339,7 @@
         <v>{"id":13,"title":"zerodata-get-started-with-sprint","group":"zerodata","area":"work","keywords":["sprint","people"],"description":"3 people discussing sprint work. Used in Work Sprint page when there is no sprint in the current project.","publish":1}</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -9307,7 +9366,7 @@
         <v>{"id":14,"title":"zerodata-add-a-feed","group":"zerodata","area":"package","keywords":["cloud","host","package","feed","box","people","ladder"],"description":"A person standing on a ladder and putting a virtual box up on the cloud. Used in the Package page when there is no package feed set up for the current project.","publish":1}</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -9334,7 +9393,7 @@
         <v>{"id":15,"title":"zerodata-connect-to-feed","group":"zerodata","area":"package","keywords":["cloud","host","package","feed","arrow","connect","box","plug"],"description":"A solid box connected to a remote virtual box on the cloud. Used in Package page when there is no packages connected to a feed.","publish":1}</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -9361,7 +9420,7 @@
         <v>{"id":16,"title":"general-no-results-found","group":"general","area":"common","keywords":["person","telescope","explore","find","search"],"description":"A person looking through a telescope. Used for no results match/found pattern.","publish":1}</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -9388,7 +9447,7 @@
         <v>{"id":17,"title":"hero-extend-vside","group":"vscom","area":"hero","keywords":["monitor","computer","code","ide","extension","build","extend","vside","robot","arm","tools","construction"],"description":"Robot arms building extensions into Visual Studio IDE.","publish":1}</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -9415,7 +9474,7 @@
         <v>{"id":18,"title":"swimlane-create-your-own-extension","group":"vscom","area":"swimlane","keywords":["tools","toolbox","hammer","wrench","pen","work","cloud","clipboard"],"description":"A toolbox with some tools and a cloud.","publish":1}</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -9442,7 +9501,7 @@
         <v>{"id":19,"title":"swimlane-marketplace","group":"vscom","area":"swimlane","keywords":["marketplace","store","shop","market","storefront"],"description":"Used to represent Visual Studio Marketplace.","publish":1}</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -9469,7 +9528,7 @@
         <v>{"id":20,"title":"swimlane-partner-program","group":"vscom","area":"swimlane","keywords":["team","collaboration","people","bike","bicycle","engineer","businessmen","doctor","man","woman","developer","hardhat","lab","coat"],"description":"Four people riding on a bike. Used for Visual Studio Partner Program.","publish":1}</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -9496,7 +9555,7 @@
         <v>{"id":21,"title":"swimlane-what-are-extensions","group":"vscom","area":"swimlane","keywords":["extension","plugin","plug","puzzle","extend","addon","people","woman","man","ladder","gear","chart","clipboard","task"],"description":"People putting plugins together. Used to represent Visual Studio extensions.","publish":1}</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -9523,7 +9582,7 @@
         <v>{"id":22,"title":"zerodata-add-product","group":"zerodata","area":"compliance","keywords":["product","box","woman","package","label"],"description":"A woman putting shipping label on a product box. Used to represent add a product.","publish":1}</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -9550,7 +9609,7 @@
         <v>{"id":23,"title":"zerodata-configure-component-governance","group":"zerodata","area":"compliance","keywords":["product","box","scan","xray","package","compliance","screen","component","governance"],"description":"A product box going through x-ray scan. Used to represent configure component governance.","publish":1}</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -9577,7 +9636,7 @@
         <v>{"id":24,"title":"zerodata-release-management","group":"zerodata","area":"build","keywords":["rocket","release","launch","cloud"],"description":"A rocket on a launch pad. Used for release management.","publish":1}</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -9604,7 +9663,7 @@
         <v>{"id":25,"title":"zerodata-this-repository-has-no-tags-yet","group":"zerodata","area":"code","keywords":["folder","tag","repository"],"description":"A dotted line tag on a folder. Used to represent there is no tag on this repository.","publish":1}</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -9631,7 +9690,7 @@
         <v>{"id":26,"title":"zerodata-add-deployment-group","group":"zerodata","area":"build","keywords":["server","pin","computer","deployment","group","target"],"description":"A map pin on a server. Used to represent targeted deployment group.","publish":1}</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -9658,7 +9717,7 @@
         <v>{"id":27,"title":"zerodata-automate-build-definitions","group":"zerodata","area":"build","keywords":["build","robot","arm","box","construction"],"description":"A robot arm lifting building blocks. Used to represent build.","publish":1}</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -9685,7 +9744,7 @@
         <v>{"id":28,"title":"zerodata-choose-a-template","group":"zerodata","area":"build","keywords":["template","shape","cookie","cutter","star","arrow","diamond","hexagon"],"description":"A template with several shapes. Used in Build area for selecting templates.","publish":1}</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -9712,7 +9771,7 @@
         <v>{"id":29,"title":"zerodata-cloud-based-load-testing","group":"zerodata","area":"test","keywords":["cloud","gauge","stress","test","performance","load","test"],"description":"A gauge on a cloud. Used for cloud based load testing.","publish":1}</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -9739,7 +9798,7 @@
         <v>{"id":30,"title":"zerodata-favorites","group":"zerodata","area":"common","keywords":["favorite","star","box","folder","question","chat","work","bullet","list"],"description":"Favorite star on frequently used work objects.","publish":1}</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -9766,7 +9825,7 @@
         <v>{"id":31,"title":"zerodata-get-everyone-on-same-page","group":"zerodata","area":"wiki","keywords":["wiki","page","book","people","team","knowledge","share","man","woman"],"description":"People sharing knowledge via wiki.","publish":1}</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -9793,7 +9852,7 @@
         <v>{"id":32,"title":"zerodata-no-plan","group":"zerodata","area":"work","keywords":["plan","draft","collaborate","hands","paper","triangle","tool","ruler","magnifier","pen"],"description":"Four hands holding tools and working on a drafting paper. Used when there is no plan for the current project.","publish":1}</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -9820,7 +9879,7 @@
         <v>{"id":33,"title":"zerodata-no-variable-groups","group":"zerodata","area":"build","keywords":["variable","group","(x)","box","stack"],"description":"Stacked blocks with variables. Used when there is no variable group.","publish":1}</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -9847,7 +9906,7 @@
         <v>{"id":34,"title":"zerodata-pull-request","group":"zerodata","area":"code","keywords":["code","pull","request","people","team"],"description":"A person making pull request and asking for code review.","publish":1}</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -9874,7 +9933,7 @@
         <v>{"id":35,"title":"hero-swiss-army-knife","group":"vscom","area":"hero","keywords":["swiss","army","knife","tools","extension","productivity","wrench","scissors","screwdriver"],"description":"A Swiss Army knife representing a bundle of developer tools. Used on Visual Studio pricing page for comparing different levels of subscription.","publish":1}</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -9901,7 +9960,7 @@
         <v>{"id":36,"title":"swimlane-all-your-code-hosted-free","group":"vscom","area":"swimlane","keywords":["team","people","work","desk","office","man","woman","developer","cloud","git","version","control","host","laptop","chair"],"description":"Unlimited Git repository support for individuals and up to four team members. Used on Git page.","publish":1}</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -9928,7 +9987,7 @@
         <v>{"id":37,"title":"swimlane-any-client-any-platform","group":"vscom","area":"swimlane","keywords":["laptop","computer","desktop","monitor","windows","mac","osx","linux","ubuntu","cross","platform","device"],"description":"Three computers with typical Windows, Mac OS and Linux screens. Used to indicate Git support on any platform and any client on Git page.","publish":1}</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -9955,7 +10014,7 @@
         <v>{"id":38,"title":"swimlane-but-wait-theres-more","group":"vscom","area":"swimlane","keywords":["tree","node","branch","woman","people","feature","laptop","computer","smartphone","control","panel","tools","document","rocket","chart"],"description":"A woman standing on a tree of features. Used on VS Enterprise page.","publish":1}</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -9982,7 +10041,7 @@
         <v>{"id":39,"title":"swimlane-pricing","group":"vscom","area":"swimlane","keywords":["pricing","calculator","pen","laptop"],"description":"Used on pricing pages.","publish":1}</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -10009,7 +10068,7 @@
         <v>{"id":40,"title":"swimlane-were-in-your-neighborhood","group":"vscom","area":"swimlane","keywords":["globe","world","map","woman"],"description":"A woman standing in front of a world map. Used to represent data center available around the world.","publish":1}</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -10036,7 +10095,7 @@
         <v>{"id":41,"title":"hero-pricing-calculator","group":"vscom","area":"hero","keywords":["pricing","calculator","pen","laptop"],"description":"Used on pricing pages. Bottom shadow removed. Use this version on dark background.","publish":1}</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -10063,7 +10122,7 @@
         <v>{"id":42,"title":"zerodata-you-have-no-organizations-yet","group":"nuget","area":"zerodata","keywords":["empty","organization","team","office","desk","clock","chair"],"description":"An office space with empty chairs. Used for zero data state when users have not created organizations.","publish":1}</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -10090,7 +10149,7 @@
         <v>{"id":43,"title":"general-robot-errorcode-503","group":"general","area":"common","keywords":["error","code","503","robot","server","down","broken","offline"],"description":"Used for 503 error page when server is down.","publish":1}</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -10117,7 +10176,7 @@
         <v>{"id":44,"title":"general-robot-error","group":"general","area":"common","keywords":["error","robot","exclamation","alert","exception"],"description":"Used for generic error page.","publish":1}</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -10144,7 +10203,7 @@
         <v>{"id":45,"title":"general-robot-errorcode-400","group":"general","area":"common","keywords":["error","code","400","robot","question"],"description":"Used for 400 error page bad request.","publish":1}</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -10171,7 +10230,7 @@
         <v>{"id":46,"title":"general-robot-errorcode-401","group":"general","area":"common","keywords":["error","code","401","robot","unauthorized"],"description":"Used for 401 error page unauthorized.","publish":1}</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -10198,7 +10257,7 @@
         <v>{"id":47,"title":"general-robot-errorcode-403","group":"general","area":"common","keywords":["error","code","403","robot","forbidden","permission","access"],"description":"Used for 403 error page the user does not have access.","publish":1}</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -10225,7 +10284,7 @@
         <v>{"id":48,"title":"general-robot-errorcode-404","group":"general","area":"common","keywords":["error","code","404","robot","not","found"],"description":"Used for 404 error page.","publish":1}</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -10252,7 +10311,7 @@
         <v>{"id":49,"title":"general-robot-errorcode-500","group":"general","area":"common","keywords":["error","code","500","robot","server","internal"],"description":"Used for 500 error page server error.","publish":1}</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -10279,7 +10338,7 @@
         <v>{"id":50,"title":"zerodata-no-assessments","group":"zerodata","area":"compliance","keywords":["assessments","compliance","analysis","laptop","magnifier","clipboard","chart"],"description":"For assessments page zero data state.","publish":1}</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -10306,7 +10365,7 @@
         <v>{"id":51,"title":"zerodata-initializing-test-results","group":"zerodata","area":"test","keywords":["test","initialize","result","beaker","lab","flask","clock","wait","loading"],"description":"Waiting screen image when test result is being loaded.","publish":1}</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -10333,7 +10392,7 @@
         <v>{"id":52,"title":"zerodata-no-work-scheduled","group":"zerodata","area":"work","keywords":["work","plan","planner","calendar","journal","schedule","notebook","pencil"],"description":"No work planned in current sprint.","publish":1}</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -10360,7 +10419,7 @@
         <v>{"id":53,"title":"zerodata-sprint-drag-n-drop","group":"zerodata","area":"work","keywords":["drag","drop","work","item","list","move"],"description":"Used on the Sprint page left panel to indicate there is no work item in the left panel yet.","publish":1}</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -10387,7 +10446,7 @@
         <v>{"id":54,"title":"swimlane-seamless-debugging-with-symbols","group":"vscom","area":"swimlane","keywords":["symbol","code","tag","label","identifier","file"],"description":"Used for Enable seamless debugging with symbols swimlane.","publish":1}</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>55</v>
       </c>
@@ -10414,7 +10473,7 @@
         <v>{"id":55,"title":"swimlane-xamarin-cross-platform","group":"dotnet","area":"swimlane","keywords":["xamarin","cross","platform","computer","laptop","tablet","phone"],"description":"Xamarin.Mac allows user to create native iOS, Android and Mac apps.","publish":1}</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>56</v>
       </c>
@@ -10441,7 +10500,7 @@
         <v>{"id":56,"title":"swimlane-azure-machine-learning","group":"dotnet","area":"swimlane","keywords":["azure","machine","learning","process","cloud","lightbulb","clock","analytics","magnifier","charts"],"description":"Azure Machine Learning.","publish":1}</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>57</v>
       </c>
@@ -10468,7 +10527,7 @@
         <v>{"id":57,"title":"swimlane-cognitive-services","group":"dotnet","area":"swimlane","keywords":["cognitive","services","vision","sound","voice","speech","microphone","input","speaker","bubble","eye","magnifier"],"description":"Cognitive services such as voice recognition, vision detection, language processing, etc.","publish":1}</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>58</v>
       </c>
@@ -10495,7 +10554,7 @@
         <v>{"id":58,"title":"swimlane-congratulations-finished-setup","group":"dotnet","area":"swimlane","keywords":["finish","complete","race","car","monitor","flag","people"],"description":"Used on a screen when user successfully finishes setup.","publish":1}</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>59</v>
       </c>
@@ -10522,7 +10581,7 @@
         <v>{"id":59,"title":"swimlane-cross-platform","group":"dotnet","area":"swimlane","keywords":["cross","platform","windows","mac","linux","computer","laptop","mobile","phone"],"description":"Used to represent multiple Oss and devices.","publish":1}</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <v>60</v>
       </c>
@@ -10549,7 +10608,7 @@
         <v>{"id":60,"title":"swimlane-cryengine-game-development","group":"dotnet","area":"swimlane","keywords":["cryengine","video","game","development","computer","monitor","keyboard","mouse","3d"],"description":"An example 3d game screen created with CRYENGINE.","publish":1}</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
         <v>61</v>
       </c>
@@ -10576,7 +10635,7 @@
         <v>{"id":61,"title":"swimlane-developer-meetup","group":"dotnet","area":"swimlane","keywords":["meetup","people","chat","discussion","idea","light","bulb"],"description":"Three people talking about ideas.","publish":1}</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
         <v>62</v>
       </c>
@@ -10603,7 +10662,7 @@
         <v>{"id":62,"title":"swimlane-dotnet-core","group":"dotnet","area":"swimlane","keywords":["developer","people","computer","laptop","work","office","team","startup"],"description":"A small team of developers working together.","publish":1}</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
         <v>63</v>
       </c>
@@ -10630,7 +10689,7 @@
         <v>{"id":63,"title":"swimlane-dotnet-enterprise","group":"dotnet","area":"swimlane","keywords":["developer","people","enterprise","building","company","laptop","computer","work","office"],"description":"A developer working in an enterprise scale environment.","publish":1}</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
         <v>64</v>
       </c>
@@ -10657,7 +10716,7 @@
         <v>{"id":64,"title":"swimlane-download-target","group":"dotnet","area":"swimlane","keywords":["people","download","welcome","computer","table","chair"],"description":"A generic download landing screen.","publish":1}</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
         <v>65</v>
       </c>
@@ -10684,7 +10743,7 @@
         <v>{"id":65,"title":"swimlane-enterprise-customer-stories","group":"dotnet","area":"swimlane","keywords":["building","company","team","people","enterprise"],"description":"Enterprise user stories.","publish":1}</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
         <v>66</v>
       </c>
@@ -10711,7 +10770,7 @@
         <v>{"id":66,"title":"swimlane-feedback-survey","group":"dotnet","area":"swimlane","keywords":["feedback","people","survey","listen","paper","cup"],"description":"A person listening user feedback with paper cup telephone.","publish":1}</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
         <v>67</v>
       </c>
@@ -10738,7 +10797,7 @@
         <v>{"id":67,"title":"swimlane-fsharp-data-science","group":"dotnet","area":"swimlane","keywords":["data","science","lab","test","tube","beaker","chart","analytics","laptop","scientist"],"description":"A data scientist working in the lab.","publish":1}</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
         <v>68</v>
       </c>
@@ -10765,7 +10824,7 @@
         <v>{"id":68,"title":"swimlane-machine-learning-library","group":"dotnet","area":"swimlane","keywords":["machine","learning","library","ai","test","beaker","book"],"description":"Used for machine learning AI library.","publish":1}</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
         <v>69</v>
       </c>
@@ -10792,7 +10851,7 @@
         <v>{"id":69,"title":"swimlane-one-consistent-api","group":"dotnet","area":"swimlane","keywords":["one","api","consistent","people","tool","library","book","light","bulb","idea","ui","code"],"description":"A person surrounded by multiple developer tools.","publish":1}</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
         <v>70</v>
       </c>
@@ -10819,7 +10878,7 @@
         <v>{"id":70,"title":"swimlane-package-library","group":"dotnet","area":"swimlane","keywords":["package","box","circuit"],"description":"A few packages soldered on a circuit.","publish":1}</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
         <v>71</v>
       </c>
@@ -10846,7 +10905,7 @@
         <v>{"id":71,"title":"swimlane-programming-languages","group":"dotnet","area":"swimlane","keywords":["developer","programming","language","keyboard","c#","VB","F#"],"description":"Developers of different programming languages.","publish":1}</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="5">
         <v>72</v>
       </c>
@@ -10873,7 +10932,7 @@
         <v>{"id":72,"title":"swimlane-thank-you-for-downloading","group":"dotnet","area":"swimlane","keywords":["download","cloud","document","file"],"description":"A generic download screen after download started/finished.","publish":1}</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
         <v>73</v>
       </c>
@@ -10900,7 +10959,7 @@
         <v>{"id":73,"title":"swimlane-unity-game-development","group":"dotnet","area":"swimlane","keywords":["2d","3d","video","game","castle","unity"],"description":"An example 3d game screen created with Unity.","publish":1}</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="5">
         <v>74</v>
       </c>
@@ -10927,7 +10986,7 @@
         <v>{"id":74,"title":"swimlane-universal-windows-platform","group":"dotnet","area":"swimlane","keywords":["uwp","universal","windows","platform","octopus","hololens","iot","surface","phone","tablet","band","game","controller","drone"],"description":"A octopus holding and wearing many devices built with UWP.","publish":1}</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="5">
         <v>75</v>
       </c>
@@ -10954,7 +11013,7 @@
         <v>{"id":75,"title":"swimlane-uwp-iot-core","group":"dotnet","area":"swimlane","keywords":["iot","core","drone","security","camera","microwave","thermometer","smart","home"],"description":"Common smart devices built with UWP IoT Core.","publish":1}</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="5">
         <v>76</v>
       </c>
@@ -10981,7 +11040,7 @@
         <v>{"id":76,"title":"swimlane-winform","group":"dotnet","area":"swimlane","keywords":["winform","drag","drop","designer","pencil","ruler","dialog","ui"],"description":"Drag and drop designer for building Winform applications.","publish":1}</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="5">
         <v>77</v>
       </c>
@@ -11008,7 +11067,7 @@
         <v>{"id":77,"title":"swimlane-wpf","group":"dotnet","area":"swimlane","keywords":["wpf","windows","presentation","foundation","ui","design","code","screen","monitor","computer"],"description":"A code and designer view used to represent WPF.","publish":1}</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="5">
         <v>78</v>
       </c>
@@ -11035,7 +11094,7 @@
         <v>{"id":78,"title":"swimlane-xamarin","group":"dotnet","area":"swimlane","keywords":["xamarin","mobile","cross","platform","development","phone","laptop","code"],"description":"Build cross-platform apps with Xamarin and one code base.","publish":1}</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="5">
         <v>79</v>
       </c>
@@ -11062,7 +11121,7 @@
         <v>{"id":79,"title":"swimlane-dotnet-perf-diagram","group":"dotnet","area":"swimlane","keywords":[".net","diagram","bar","chart"],"description":"A bar chart comparing requests per second of three frameworks.","publish":0}</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="5">
         <v>80</v>
       </c>
@@ -11089,7 +11148,7 @@
         <v>{"id":80,"title":"hero-snapshot-debugger","group":"vscom","area":"hero","keywords":["snapshot","debugger","debug","bug","magnifier","code","cloud"],"description":"Debugging code on the cloud.","publish":1}</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="5">
         <v>81</v>
       </c>
@@ -11116,7 +11175,7 @@
         <v>{"id":81,"title":"swimlane-collaborative-debugging","group":"vscode","area":"swimlane","keywords":["collaborate","debug","teamwork","hands","plan","draw","ruler","design","pen","triangle","bug","magnifier","lightbulb"],"description":"Collaborative debugging.","publish":1}</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="5">
         <v>82</v>
       </c>
@@ -11139,11 +11198,11 @@
         <v>1</v>
       </c>
       <c r="I83" s="2" t="str">
-        <f t="shared" ref="I83:I90" si="1">SUBSTITUTE(_xlfn.CONCAT("{'id':",A83,",'title':'",C83,"','group':'",D83,"','area':'",E83,"','keywords':['",SUBSTITUTE(F83," ","','"),"'],'description':'",G83,"','publish':",H83,"}"),"'","""")</f>
+        <f t="shared" ref="I83:I91" si="1">SUBSTITUTE(_xlfn.CONCAT("{'id':",A83,",'title':'",C83,"','group':'",D83,"','area':'",E83,"','keywords':['",SUBSTITUTE(F83," ","','"),"'],'description':'",G83,"','publish':",H83,"}"),"'","""")</f>
         <v>{"id":82,"title":"swimlane-collaborative-editing","group":"vscode","area":"swimlane","keywords":["collaborate","editor","code","people"],"description":"Collaborative code editing.","publish":1}</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="5">
         <v>83</v>
       </c>
@@ -11170,7 +11229,7 @@
         <v>{"id":83,"title":"swimlane-shared-full-context","group":"vscode","area":"swimlane","keywords":["share","context","code","editor","environment","computer","laptop"],"description":"Share code and full context.","publish":1}</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="5">
         <v>84</v>
       </c>
@@ -11197,7 +11256,7 @@
         <v>{"id":84,"title":"swimlane-real-time-sharing","group":"vscode","area":"swimlane","keywords":["people","work","team","office","real","time","code","developer","clock"],"description":"Real-time sharing with your tools.","publish":1}</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="5">
         <v>85</v>
       </c>
@@ -11224,7 +11283,7 @@
         <v>{"id":85,"title":"blog-rocket-launch-timeline","group":"vscode","area":"blog","keywords":["rocket","release","launch","cloud","timeline"],"description":"Rocket launch timeline.","publish":1}</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="5">
         <v>86</v>
       </c>
@@ -11251,7 +11310,7 @@
         <v>{"id":86,"title":"blog-vscode-metrics","group":"vscom","area":"blog","keywords":["metrics"],"description":"Download and install metrics of Visual Studio Code.","publish":1}</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="5">
         <v>87</v>
       </c>
@@ -11278,7 +11337,7 @@
         <v>{"id":87,"title":"blog-vscode-roadmap","group":"vscom","area":"blog","keywords":["roadmap","car","road","milestone","pin","timeline"],"description":"A roadmap showing Visual Studio Code major release milestones","publish":1}</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="5">
         <v>88</v>
       </c>
@@ -11305,7 +11364,7 @@
         <v>{"id":88,"title":"swimlane-monogame-game-development","group":"dotnet","area":"swimlane","keywords":["monogame","game","development","screen","platform","psvita","windows","mac","video","game"],"description":"Cross platform game development with MonoGame engine.","publish":1}</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="5">
         <v>89</v>
       </c>
@@ -11330,6 +11389,33 @@
       <c r="I90" s="2" t="str">
         <f t="shared" si="1"/>
         <v>{"id":89,"title":"zerodata-you-have-no-project","group":"zerodata","area":"account","keywords":["project","plan","work","briefcase","pencil","document","triangle","ruler"],"description":"Used in account page when you have no projects yet.","publish":1}</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="5">
+        <v>90</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="D91" t="s">
+        <v>270</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="G91" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="H91" s="2">
+        <v>1</v>
+      </c>
+      <c r="I91" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>{"id":90,"title":"hero-vsts-join-our-team","group":"vscom","area":"hero","keywords":["vsts","team","work","ui","join","us","people","chart","dialog","gear"],"description":"Used in VSTS jobs page hero section.","publish":1}</v>
       </c>
     </row>
   </sheetData>
@@ -11353,22 +11439,22 @@
       <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83984375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.83984375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="38.15625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="38.140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="17" style="2" customWidth="1"/>
     <col min="5" max="5" width="18" style="2" customWidth="1"/>
-    <col min="6" max="6" width="33.68359375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="20.68359375" style="2" customWidth="1"/>
-    <col min="8" max="9" width="24.15625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="33.15625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="66.41796875" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="9.15625" style="2"/>
+    <col min="6" max="6" width="33.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" style="2" customWidth="1"/>
+    <col min="8" max="9" width="24.140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="33.140625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="66.42578125" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" s="3" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>73</v>
       </c>
@@ -11403,7 +11489,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -11437,7 +11523,7 @@
         <v>{"id":1,"title":"AzureToolsForVS","category":"VSCOM","keywords":["free","hosting","bug","tools","platforms","testing","beaker","wrench","azure","logo"],"description":"Azure developer tools for Visual Studio with free hosting.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -11471,7 +11557,7 @@
         <v>{"id":2,"title":"CloudPattern","category":"Pattern","keywords":["technology","nature","cloud","sky"],"description":"Clouds on blue sky pattern.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -11505,7 +11591,7 @@
         <v>{"id":3,"title":"CollaborationChatBubbles","category":"Diagram","keywords":["work","chat","bubble","conversation","communication","collaboration","team","men","women","people"],"description":"Several chat bubbles with people inside.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -11539,7 +11625,7 @@
         <v>{"id":4,"title":"CollaborationNetwork","category":"Diagram","keywords":["man","woman","network","hub","collaboration","connection","web","idea","lightbulb","gear","cloud","chat","bubble","work"],"description":"A network of people and objects connected together.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -11573,7 +11659,7 @@
         <v>{"id":5,"title":"CommunityTranslation1","category":"VSCOM","keywords":["hand","phone","hello","word","balloon","languages"],"description":"Translate world languages with smartphone.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -11607,7 +11693,7 @@
         <v>{"id":6,"title":"CommunityTranslation2","category":"VSCOM","keywords":["group","people","tablet","languages"],"description":"People from around the world using translation app on smart device to say hello.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -11641,7 +11727,7 @@
         <v>{"id":7,"title":"CommunityTranslation3","category":"VSCOM","keywords":["group","people","tablet","languages"],"description":"People from around the world using translation app on smart device to say hello.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -11675,7 +11761,7 @@
         <v>{"id":8,"title":"CordovaToolsTwitterBanner","category":"Web","keywords":["crane","cloud","tools","tree","build","construction"],"description":"Cordova Tools Twitter account banner. Construction crane and build tools on cloud.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -11709,7 +11795,7 @@
         <v>{"id":9,"title":"DesktopComputerPattern","category":"Pattern","keywords":["desktop","computer","monitor","pc","technology"],"description":"Desktop computer pattern.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -11743,7 +11829,7 @@
         <v>{"id":10,"title":"DevEssentials1","category":"VSCOM","keywords":["download","arrow","magnifying","glass","monitor","laptop","data","graphs","gears","newsletter"],"description":"Data visualization related elements on a cloud.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -11777,7 +11863,7 @@
         <v>{"id":11,"title":"DevEssentials2","category":"VSCOM","keywords":["download","arrow","magnifying","glass","monitor","laptop","data","graphs","gears","toolbox","newsletter"],"description":"Data visualization related elements on a cloud.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -11811,7 +11897,7 @@
         <v>{"id":12,"title":"DevicesPattern","category":"Pattern","keywords":["laptop","phone","tablet","smartphone","technology"],"description":"Mixed devices pattern.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -11845,7 +11931,7 @@
         <v>{"id":13,"title":"DevOpsLifecycle","category":"Diagram","keywords":["handshake","planning","continuous","delivery","dev","test","analytics","mobius","infinity","loop"],"description":"DevOps lifecycle.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -11879,7 +11965,7 @@
         <v>{"id":14,"title":"FeedbackCommentsDiscussion","category":"Email","keywords":["chat","bubble","question","exclaimation","conversation","discussion"],"description":"Feedback comment discussion.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -11913,7 +11999,7 @@
         <v>{"id":15,"title":"FeedbackPattern","category":"Pattern","keywords":["feedback","chat","bubble","conversation","question","exclaimation","problem","comment","talk"],"description":"Chat bubble feedback pattern.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -11947,7 +12033,7 @@
         <v>{"id":16,"title":"FoodCollection","category":"Elements","keywords":["food","meal","nutrition","soup","bread","spoon","tomato","broccli","vegetable","fish","crab","seafood","meat","poultry","steak","chicken","turkey","cake","pie","dessert","measuring","cup","egg","beater","cooking","utencils","drink","cocktail","glass","toast","cracker","cheese","burger","hotdog","salad","appetizer","entree"],"description":"A collection of food icons.","style":["color","sketchy"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -11981,7 +12067,7 @@
         <v>{"id":17,"title":"IdeaFactory","category":"Web","keywords":["factory","building","gear","lightbulb","database","arrow","document","gauge","lift","truck"],"description":"Ideas being manufactured in a factory.","style":["monotone"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -12015,7 +12101,7 @@
         <v>{"id":18,"title":"IntegratedDevelopmentLoop","category":"Email","keywords":["loop","cycle","edit","pencil","script","scroll","bug","arrow","device","phone","mobile","cloud"],"description":"Lifecycle of code, debug and deployment.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -12049,7 +12135,7 @@
         <v>{"id":19,"title":"InternetOfThings","category":"Diagram","keywords":["internet","iot","globe","router","smart","phone","laptop","light","bulb","printer","desktop","media","player","car","smart","home","smart","watch","mobile","payment","device","software","development"],"description":"The Internet of Things (IoT) is the network of physical objects or things embedded with electronics, software, sensors, and network connectivity, which enables these objects to collect and exchange data.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -12083,7 +12169,7 @@
         <v>{"id":20,"title":"ManufacturingIdeas","category":"Misc","keywords":["machine","tool","lightbulb"],"description":"Ideas being manufactured by a machine.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -12117,7 +12203,7 @@
         <v>{"id":21,"title":"MicrosoftWelcomeCenter","category":"Print","keywords":["microsoft","company","building","welcome","logo","work","business"],"description":"Microsoft logo and office buildings.","style":["color","3d"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -12151,7 +12237,7 @@
         <v>{"id":22,"title":"MobileAppDevelopmentPlatform","category":"VSCOM","keywords":["building","city","cloud","billboard","people","device","laptop","phone","database","security","lock","presentation","chart","development","platform","enterprise","business"],"description":"Mobile app development platform.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -12185,7 +12271,7 @@
         <v>{"id":23,"title":"MobileAppDevelopmentWithVisualStudio","category":"VSCOM","keywords":["laptop","phone","iphone","android","windows","app","development","visual","studio"],"description":"Cross platform mobile app development with Visual Studio.","style":["color","photo","monotone"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -12219,7 +12305,7 @@
         <v>{"id":24,"title":"MultiDeviceTwitterBanner","category":"Web","keywords":["cloud","sky","field","grass","phone","smartphone","tablet","computer","desktop","pc","monitor","tv","television","microsoft","logo","technology","developer"],"description":"Cordova Tools Twitter account banner. Four device icons overlay on top of cloud and field backgournd.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -12253,7 +12339,7 @@
         <v>{"id":25,"title":"NETCoreWebsiteBanner","category":"Web","keywords":["visual","studio","html5","css3","javascript"],"description":".NET Core website banner.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -12287,7 +12373,7 @@
         <v>{"id":26,"title":"OneToolForEverything","category":"Email","keywords":["tool","laptop","mobile","phone","cloud"],"description":"One tool for all platform.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -12321,7 +12407,7 @@
         <v>{"id":27,"title":"OpenSourceComputer","category":"Web","keywords":["laptop","code","arrow","exchange"],"description":"Two laptop exchanging code.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -12355,7 +12441,7 @@
         <v>{"id":28,"title":"OpenSourceExchangeCode","category":"Diagram","keywords":["code","man","woman","laptop","desktop","exchange","share","arrow"],"description":"Developers exchange open source code.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -12389,7 +12475,7 @@
         <v>{"id":29,"title":"PlaceholderFlowers","category":"VSTS","keywords":["flower"],"description":"Placeholder images.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -12423,7 +12509,7 @@
         <v>{"id":30,"title":"PublishAndDeploy","category":"Email","keywords":["rocket","document","arrow","exchange"],"description":"Publish and deploy code.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -12457,7 +12543,7 @@
         <v>{"id":31,"title":"PushNotifications","category":"Web","keywords":["mobile","phone","tablet","android","windows","ios","chat","bubble","notification"],"description":"Push notifications on multiple platforms.","style":["monotone"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -12491,7 +12577,7 @@
         <v>{"id":32,"title":"PythonToolsForVS","category":"VSCOM","keywords":["man","laptop","woman","gears","bug","code","phone","python","logo","magnifying","glass"],"description":"Python tools for Visual Studio.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -12525,7 +12611,7 @@
         <v>{"id":33,"title":"QuickstartFastSpeed","category":"Email","keywords":["stopwatch","run","man","time","fast","quick","speed"],"description":"Quick start","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -12559,7 +12645,7 @@
         <v>{"id":34,"title":"RocketMulticolor","category":"Elements","keywords":["rocket","launch","deployment"],"description":"Rocket","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -12593,7 +12679,7 @@
         <v>{"id":35,"title":"RocketWithCloudPattern","category":"Print","keywords":["rocket","cloud","sky"],"description":"Rocket on sky background","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -12627,7 +12713,7 @@
         <v>{"id":36,"title":"SeattlePostcard","category":"Print","keywords":["seattle","space","needle","cloud","city"],"description":"Seattle space needle postcard","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -12661,7 +12747,7 @@
         <v>{"id":37,"title":"SeattleSkyline","category":"Web","keywords":["seattle","space","needle","cloud","city","skyline","building","mount","rainier"],"description":"Seattle city skyline","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -12695,7 +12781,7 @@
         <v>{"id":38,"title":"SeattleSkylineFerrisWheel","category":"Web","keywords":["seattle","space","needle","ferris","wheel","waterfront","port"],"description":"Seattle city skyline","style":["monotone"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -12729,7 +12815,7 @@
         <v>{"id":39,"title":"SilhouetteAirportElements","category":"Elements","keywords":["airport","pilot","flight","attendant","uniform","causeway","airplane","sign","direction","loudge","coffee","terminal","seat","life"],"description":"A collection of airport related elements.","style":["silhuoette"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -12763,7 +12849,7 @@
         <v>{"id":40,"title":"SilhouetteBriefcasesAndDocuments","category":"Elements","keywords":["document","file","paper","briefcase","suitcase","handbag","work","object","business"],"description":" A collection of briefcases.","style":["silhuoette"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -12797,7 +12883,7 @@
         <v>{"id":41,"title":"SilhouetteCharacters","category":"Elements","keywords":["man","confuse","suit","woman","chair","desk","laptop","computer","office","work","business"],"description":"A collection of characters in work environment.","style":[" ","silhuoette"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -12831,7 +12917,7 @@
         <v>{"id":42,"title":"SilhouetteHandGenstures","category":"Elements","keywords":["hand","gesture","pick","grip","pinch","touch","web","press","technology"],"description":"Hand gestures.","style":["silhuoette"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -12865,7 +12951,7 @@
         <v>{"id":43,"title":"SilhouetteTabletAndPhones","category":"Elements","keywords":["technology","work","tablet","smartphone","phone","mobile","phone","pen","stylus","windows","phone","android","phone","surface","tablet"],"description":"Tablet and smartphones.","style":["silhuoette"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -12899,7 +12985,7 @@
         <v>{"id":44,"title":"SilhouetteToolCollection","category":"Pattern","keywords":["wrench","screwdriver","saw","plier","hammer","knife","c","clamp","clamp","pipe","wrench","filer","triangle","ruler","object"],"description":"A collection of hand tools.","style":["silhouette"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -12933,7 +13019,7 @@
         <v>{"id":45,"title":"SilhouetteWeatherReportElements","category":"Elements","keywords":["life","newspaper","radio","magezine","clock","news","weather","forcast","tv","sun","sunny","cloud","lightning","thunder","cloud","cloudy","rain","tripical","palm","tree","beach","table","vacation","beach","chair","hawaii","man","relax","drink"],"description":"A collection of weather related illustrations.","style":["silhuoette"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -12967,7 +13053,7 @@
         <v>{"id":46,"title":"SoftwareToolsSampleKit","category":"Email","keywords":["toolbox","hammer","checklist","wrench","cloud"],"description":"Software development toolkit","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -13001,7 +13087,7 @@
         <v>{"id":47,"title":"TeamworkStairs","category":"Web","keywords":["people","man","stairs","team"],"description":"People holding hands climbing up stairs as a team.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -13035,7 +13121,7 @@
         <v>{"id":48,"title":"Testing","category":"Email","keywords":["test","flask","lab","beaker","stopwatch","pie","chart","checklist"],"description":"Testing","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -13069,7 +13155,7 @@
         <v>{"id":49,"title":"VSBuildALMIntegration","category":"VSCOM","keywords":["people","working","man","computer","clipboard","debug","tools","gear","bug"],"description":"ALM (Application Lifecycle Management) debug integration.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -13103,7 +13189,7 @@
         <v>{"id":50,"title":"VSBuildCloudHostedTools","category":"VSCOM","keywords":["people","laptops","desk","workers","monitors","laptops","cross","platforms","linux","windows","ios"],"description":"Developers come from different platforms and technology stacks working together.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -13137,7 +13223,7 @@
         <v>{"id":51,"title":"VSBuildContinuousIntegration","category":"VSCOM","keywords":["monitor","laptop","test","tubes","gears","checkmark"],"description":"Build continuous integration cycle with cloud.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -13171,7 +13257,7 @@
         <v>{"id":52,"title":"VSBuildContinuousIntegrationWhite","category":"VSCOM","keywords":["cross","platforms","maven","git","apache","ant","junit","gradle","xunit","mtm","test","building"],"description":"Common tools and technologies for cross-platform development.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -13205,7 +13291,7 @@
         <v>{"id":53,"title":"VSBuildCrossPlatform","category":"VSCOM","keywords":["pillars","cross","platforms","buildings","crane","java",".net","xcode","github","ios","android","windows","git"],"description":"Common tools and technologies for cross-platform development.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -13239,7 +13325,7 @@
         <v>{"id":54,"title":"VSBuildOverview","category":"VSCOM","keywords":["cross","platforms","laptop","tablet","phone","ios","android","visual","studio","cloud"],"description":"Visual Studio for building cross-platform applications.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -13273,7 +13359,7 @@
         <v>{"id":55,"title":"VSBuildTraceability","category":"VSCOM","keywords":["blueprint","document","man","beaker","tools","clipboard","timeline","printer","download","test","tubes","gears","magnifying","glass","graphs"],"description":"Build timeline and tracebility.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -13307,7 +13393,7 @@
         <v>{"id":56,"title":"VSDownload1","category":"VSCOM","keywords":["group","people","visual","studio","logo","flags","man","woman"],"description":"Visual Studio for everyone.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -13341,7 +13427,7 @@
         <v>{"id":57,"title":"VSDownload2","category":"VSCOM","keywords":["man","monitors","download","down","arrow","computer","table"],"description":"Visual Studio tools for multiplatform.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -13375,302 +13461,302 @@
         <v>{"id":58,"title":"XamarinCrossPlatformDevelopment","category":"VSCOM","keywords":["screenshot","ios","android","windows","mobile","phone","app","development","shared","code","cross-platform","xamarin"],"description":"Xamarin for developing cross-platform application.","style":["color","photo"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>114</v>
       </c>
     </row>
-    <row r="116" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <v>115</v>
       </c>
     </row>
-    <row r="117" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>117</v>
       </c>
     </row>
-    <row r="119" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>118</v>
       </c>
@@ -13705,9 +13791,9 @@
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="1" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Added design element illustrations
</commit_message>
<xml_diff>
--- a/src/assets/data.xlsx
+++ b/src/assets/data.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="522">
   <si>
     <t>SeattleSkyline</t>
   </si>
@@ -1523,6 +1523,78 @@
   </si>
   <si>
     <t>Used in VSTS jobs page hero section.</t>
+  </si>
+  <si>
+    <t>elements-vehicles-3</t>
+  </si>
+  <si>
+    <t>elements-devices-1</t>
+  </si>
+  <si>
+    <t>elements-devices-2</t>
+  </si>
+  <si>
+    <t>elements-robots-1</t>
+  </si>
+  <si>
+    <t>elements-robots-2</t>
+  </si>
+  <si>
+    <t>elements-tools-1</t>
+  </si>
+  <si>
+    <t>elements-tools-2</t>
+  </si>
+  <si>
+    <t>elements-vehicles-1</t>
+  </si>
+  <si>
+    <t>elements-vehicles-2</t>
+  </si>
+  <si>
+    <t>elements</t>
+  </si>
+  <si>
+    <t>devices computer laptop desktop monitor phone tablet iot chip xbox console video game controller hololens vr</t>
+  </si>
+  <si>
+    <t>A collection of devices.</t>
+  </si>
+  <si>
+    <t>A collection of robots.</t>
+  </si>
+  <si>
+    <t>A collection of tools.</t>
+  </si>
+  <si>
+    <t>devices computer laptop desktop monitor</t>
+  </si>
+  <si>
+    <t>robot gesture alien ufo treadmill telescope construction investigate magnifire repaire maintanance</t>
+  </si>
+  <si>
+    <t>robot gesture error question unknown</t>
+  </si>
+  <si>
+    <t>tool utility wrench screwdriver lightbulb drill ruler measure swiss knife hammer plier book journal note calendar calculator pen pencil magnifier</t>
+  </si>
+  <si>
+    <t>A collection of vehicles.</t>
+  </si>
+  <si>
+    <t>toolbox tool utility hammer wrench maginfier cloud pen pencil screwdriver clipboard drill ruler measure</t>
+  </si>
+  <si>
+    <t>A collection of tools in toolboxes.</t>
+  </si>
+  <si>
+    <t>vehicle car transportation motor bike scooter mini sedan van truck bus</t>
+  </si>
+  <si>
+    <t>vehicle car transportation van towing lifting truck trolley crane construction industry</t>
+  </si>
+  <si>
+    <t>vehicle car bike rocket racing team collaboration people manufacture assemble customize launch start release machanics</t>
   </si>
 </sst>
 </file>
@@ -6104,6 +6176,456 @@
         <a:xfrm>
           <a:off x="1019736" y="112910471"/>
           <a:ext cx="2178807" cy="1199029"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>347382</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>11206</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2005852</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>1255059</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="76" name="Picture 75">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A89C626-3923-47E7-B35F-637953800402}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId92" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1232647" y="114154324"/>
+          <a:ext cx="1658470" cy="1243853"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>257735</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1882588</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>1263464</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="84" name="Picture 83">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0564AE8-5E23-4B3E-A5BD-0FA71CE79B11}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId93" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1143000" y="115454206"/>
+          <a:ext cx="1624853" cy="1218640"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>22412</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1837764</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>1257860</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="88" name="Picture 87">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE0CA465-F274-4571-B1E3-57775F4B5A22}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId94" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1075765" y="116698059"/>
+          <a:ext cx="1647264" cy="1235448"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>22412</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1815353</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>1241052</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="95" name="Picture 94">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{843130E4-61D7-4415-B1A6-706D74095005}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId95" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1075765" y="117964324"/>
+          <a:ext cx="1624853" cy="1218640"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1692088</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>2801</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="98" name="Picture 97">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3E87860-D03F-443E-80B8-D459D047B64D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId96" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="885265" y="119208176"/>
+          <a:ext cx="1692088" cy="1269066"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>123264</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>2</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1714499</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>1193428</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="100" name="Picture 99">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8031B57E-4187-43C6-B35A-7BAD87CCAA43}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId97" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1008529" y="120474443"/>
+          <a:ext cx="1591235" cy="1193426"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1714500</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>19610</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="104" name="Picture 103">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BCE43B5D-B3F2-4A68-930C-ECD1FADAE8C6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId98" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="885265" y="121740706"/>
+          <a:ext cx="1714500" cy="1285875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1714500</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>19611</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="108" name="Picture 107">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EB367E9-2697-4398-9E57-F09915177333}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId99" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="885265" y="123006971"/>
+          <a:ext cx="1714500" cy="1285875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1658470</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>1243853</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="111" name="Picture 110">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{501CF239-D412-4B5B-B305-D84CD1A6A7A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId100" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="885265" y="124273235"/>
+          <a:ext cx="1658470" cy="1243853"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8935,13 +9457,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I91"/>
+  <dimension ref="A1:I100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B88" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B96" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I91" sqref="I91"/>
+      <selection pane="bottomRight" activeCell="I92" sqref="I92:I100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -11198,7 +11720,7 @@
         <v>1</v>
       </c>
       <c r="I83" s="2" t="str">
-        <f t="shared" ref="I83:I91" si="1">SUBSTITUTE(_xlfn.CONCAT("{'id':",A83,",'title':'",C83,"','group':'",D83,"','area':'",E83,"','keywords':['",SUBSTITUTE(F83," ","','"),"'],'description':'",G83,"','publish':",H83,"}"),"'","""")</f>
+        <f t="shared" ref="I83:I100" si="1">SUBSTITUTE(_xlfn.CONCAT("{'id':",A83,",'title':'",C83,"','group':'",D83,"','area':'",E83,"','keywords':['",SUBSTITUTE(F83," ","','"),"'],'description':'",G83,"','publish':",H83,"}"),"'","""")</f>
         <v>{"id":82,"title":"swimlane-collaborative-editing","group":"vscode","area":"swimlane","keywords":["collaborate","editor","code","people"],"description":"Collaborative code editing.","publish":1}</v>
       </c>
     </row>
@@ -11418,9 +11940,252 @@
         <v>{"id":90,"title":"hero-vsts-join-our-team","group":"vscom","area":"hero","keywords":["vsts","team","work","ui","join","us","people","chart","dialog","gear"],"description":"Used in VSTS jobs page hero section.","publish":1}</v>
       </c>
     </row>
+    <row r="92" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="5">
+        <v>91</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="D92" t="s">
+        <v>507</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="G92" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H92" s="2">
+        <v>1</v>
+      </c>
+      <c r="I92" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>{"id":91,"title":"elements-devices-1","group":"elements","area":"elements","keywords":["devices","computer","laptop","desktop","monitor","phone","tablet","iot","chip","xbox","console","video","game","controller","hololens","vr"],"description":"A collection of devices.","publish":1}</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="5">
+        <v>92</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="D93" t="s">
+        <v>507</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="G93" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H93" s="2">
+        <v>1</v>
+      </c>
+      <c r="I93" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>{"id":92,"title":"elements-devices-2","group":"elements","area":"elements","keywords":["devices","computer","laptop","desktop","monitor"],"description":"A collection of devices.","publish":1}</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="5">
+        <v>93</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="D94" t="s">
+        <v>507</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="G94" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="H94" s="2">
+        <v>1</v>
+      </c>
+      <c r="I94" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>{"id":93,"title":"elements-robots-1","group":"elements","area":"elements","keywords":["robot","gesture","alien","ufo","treadmill","telescope","construction","investigate","magnifire","repaire","maintanance"],"description":"A collection of robots.","publish":1}</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="5">
+        <v>94</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="D95" t="s">
+        <v>507</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="G95" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="H95" s="2">
+        <v>1</v>
+      </c>
+      <c r="I95" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>{"id":94,"title":"elements-robots-2","group":"elements","area":"elements","keywords":["robot","gesture","error","question","unknown"],"description":"A collection of robots.","publish":1}</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="5">
+        <v>95</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="D96" t="s">
+        <v>507</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="G96" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="H96" s="2">
+        <v>1</v>
+      </c>
+      <c r="I96" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>{"id":95,"title":"elements-tools-1","group":"elements","area":"elements","keywords":["tool","utility","wrench","screwdriver","lightbulb","drill","ruler","measure","swiss","knife","hammer","plier","book","journal","note","calendar","calculator","pen","pencil","magnifier"],"description":"A collection of tools.","publish":1}</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="5">
+        <v>96</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="D97" t="s">
+        <v>507</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="G97" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="H97" s="2">
+        <v>1</v>
+      </c>
+      <c r="I97" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>{"id":96,"title":"elements-tools-2","group":"elements","area":"elements","keywords":["toolbox","tool","utility","hammer","wrench","maginfier","cloud","pen","pencil","screwdriver","clipboard","drill","ruler","measure"],"description":"A collection of tools in toolboxes.","publish":1}</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="5">
+        <v>97</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="D98" t="s">
+        <v>507</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="G98" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="H98" s="2">
+        <v>1</v>
+      </c>
+      <c r="I98" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>{"id":97,"title":"elements-vehicles-1","group":"elements","area":"elements","keywords":["vehicle","car","transportation","motor","bike","scooter","mini","sedan","van","truck","bus"],"description":"A collection of vehicles.","publish":1}</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="5">
+        <v>98</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="D99" t="s">
+        <v>507</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="G99" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="H99" s="2">
+        <v>1</v>
+      </c>
+      <c r="I99" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>{"id":98,"title":"elements-vehicles-2","group":"elements","area":"elements","keywords":["vehicle","car","transportation","van","towing","lifting","truck","trolley","crane","construction","industry"],"description":"A collection of vehicles.","publish":1}</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="5">
+        <v>99</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="D100" t="s">
+        <v>507</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="H100" s="2">
+        <v>1</v>
+      </c>
+      <c r="I100" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>{"id":99,"title":"elements-vehicles-3","group":"elements","area":"elements","keywords":["vehicle","car","bike","rocket","racing","team","collaboration","people","manufacture","assemble","customize","launch","start","release","machanics"],"description":"A collection of vehicles.","publish":1}</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:G13">
-    <sortCondition ref="C1"/>
+  <sortState ref="C92:C100">
+    <sortCondition ref="C92"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
fix by linter and added new assets
</commit_message>
<xml_diff>
--- a/src/assets/data.xlsx
+++ b/src/assets/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\Code\vsimages\src\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F50AD7-5B43-46B3-9547-15261725B20A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14C3449E-D7FA-460C-8160-CC1A32C4D8B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,12 +26,18 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1546" uniqueCount="876">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1556" uniqueCount="882">
   <si>
     <t>SeattleSkyline</t>
   </si>
@@ -2659,6 +2665,24 @@
   </si>
   <si>
     <t>Used for Azure Lab Services empty state when there is no VM in the lab.</t>
+  </si>
+  <si>
+    <t>als-waiting-beaker</t>
+  </si>
+  <si>
+    <t>als-take-notes</t>
+  </si>
+  <si>
+    <t>azure lab vm beaker waiting</t>
+  </si>
+  <si>
+    <t>azure lab vm note sticky pencil write credential</t>
+  </si>
+  <si>
+    <t>Used for Azure Lab Services waiting screens.</t>
+  </si>
+  <si>
+    <t>Used for Azure Lab Services take notes of credentials wizard.</t>
   </si>
 </sst>
 </file>
@@ -5564,13 +5588,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K230"/>
+  <dimension ref="A1:K232"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C227" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B229" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I230" sqref="I230"/>
+      <selection pane="bottomRight" activeCell="D229" sqref="D229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12035,7 +12059,7 @@
         <v>1</v>
       </c>
       <c r="I208" s="2" t="str">
-        <f t="shared" ref="I208:I230" si="7">SUBSTITUTE(_xlfn.CONCAT("{'id':",A208,",'title':'",C208,"','group':'",D208,"','area':'",E208,"','keywords':['",SUBSTITUTE(F208," ","','"),"'],'description':'",G208,"','publish':",H208,"}"),"'","""")</f>
+        <f t="shared" ref="I208:I232" si="7">SUBSTITUTE(_xlfn.CONCAT("{'id':",A208,",'title':'",C208,"','group':'",D208,"','area':'",E208,"','keywords':['",SUBSTITUTE(F208," ","','"),"'],'description':'",G208,"','publish':",H208,"}"),"'","""")</f>
         <v>{"id":207,"title":"wizard-upgrade-from-xml-to-inheritance","group":"wizard","area":"agile","keywords":["inheritance","xml","file","document","instance","dotted","line"],"description":"Upgrade from XML defined process to inheritance type.","publish":1}</v>
       </c>
       <c r="J208" s="2" t="str">
@@ -12637,8 +12661,62 @@
         <v>{"id":230,"title":"als-lab-empty-state","group":"als","area":"zerodata","keywords":["azure","lab","vm","virtual","machine","empty","dotted","line","woman","people","question","mark","computer"],"description":"Used for Azure Lab Services empty state when there is no VM in the lab.","publish":1}</v>
       </c>
     </row>
+    <row r="231" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A231" s="5">
+        <v>231</v>
+      </c>
+      <c r="C231" s="2" t="s">
+        <v>876</v>
+      </c>
+      <c r="D231" t="s">
+        <v>826</v>
+      </c>
+      <c r="E231" s="2" t="s">
+        <v>807</v>
+      </c>
+      <c r="F231" s="2" t="s">
+        <v>878</v>
+      </c>
+      <c r="G231" s="2" t="s">
+        <v>880</v>
+      </c>
+      <c r="H231" s="2">
+        <v>1</v>
+      </c>
+      <c r="I231" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>{"id":231,"title":"als-waiting-beaker","group":"als","area":"wizard","keywords":["azure","lab","vm","beaker","waiting"],"description":"Used for Azure Lab Services waiting screens.","publish":1}</v>
+      </c>
+    </row>
+    <row r="232" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A232" s="5">
+        <v>232</v>
+      </c>
+      <c r="C232" s="2" t="s">
+        <v>877</v>
+      </c>
+      <c r="D232" t="s">
+        <v>826</v>
+      </c>
+      <c r="E232" s="2" t="s">
+        <v>807</v>
+      </c>
+      <c r="F232" s="2" t="s">
+        <v>879</v>
+      </c>
+      <c r="G232" s="2" t="s">
+        <v>881</v>
+      </c>
+      <c r="H232" s="2">
+        <v>1</v>
+      </c>
+      <c r="I232" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>{"id":232,"title":"als-take-notes","group":"als","area":"wizard","keywords":["azure","lab","vm","note","sticky","pencil","write","credential"],"description":"Used for Azure Lab Services take notes of credentials wizard.","publish":1}</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="C92:C100">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C92:C100">
     <sortCondition ref="C92"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15148,7 +15226,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:H59">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H59">
     <sortCondition ref="C2:C59"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added new illustrations; fixed some svg
</commit_message>
<xml_diff>
--- a/src/assets/data.xlsx
+++ b/src/assets/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7778807B-9D1D-4E9E-BE63-81A75D710285}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F7D325-15AC-42EE-AB7C-4065126A9DA2}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1581" uniqueCount="897">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1601" uniqueCount="907">
   <si>
     <t>SeattleSkyline</t>
   </si>
@@ -2728,6 +2727,36 @@
   </si>
   <si>
     <t>swimlane-one-consistent-api-purple</t>
+  </si>
+  <si>
+    <t>hero-azure-notebooks</t>
+  </si>
+  <si>
+    <t>spot-azure-accessible-everywhere</t>
+  </si>
+  <si>
+    <t>spot-scientist-developer-student</t>
+  </si>
+  <si>
+    <t>notebooks</t>
+  </si>
+  <si>
+    <t>spot</t>
+  </si>
+  <si>
+    <t>azure notebooks</t>
+  </si>
+  <si>
+    <t>globe</t>
+  </si>
+  <si>
+    <t>spot-notebooks-languages</t>
+  </si>
+  <si>
+    <t>notebooks language</t>
+  </si>
+  <si>
+    <t>people</t>
   </si>
 </sst>
 </file>
@@ -5633,13 +5662,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K237"/>
+  <dimension ref="A1:K241"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B230" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J2" sqref="I2:J237"/>
+      <selection pane="bottomRight" activeCell="I241" sqref="I2:I241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12864,7 +12893,7 @@
         <v>1</v>
       </c>
       <c r="I236" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f>SUBSTITUTE(_xlfn.CONCAT("{'id':",A236,",'title':'",C236,"','group':'",D236,"','area':'",E236,"','keywords':['",SUBSTITUTE(F236," ","','"),"'],'description':'",G236,"','publish':",H236,"}"),"'","""")</f>
         <v>{"id":236,"title":"swimlane-embed-github-snippet","group":"dotnet","area":"swimlane","keywords":["embed","github","snippet","code","browser"],"description":"Load GitHub gists with Try .NET to edit code in browser.","publish":1}</v>
       </c>
     </row>
@@ -12891,12 +12920,120 @@
         <v>1</v>
       </c>
       <c r="I237" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f>SUBSTITUTE(_xlfn.CONCAT("{'id':",A237,",'title':'",C237,"','group':'",D237,"','area':'",E237,"','keywords':['",SUBSTITUTE(F237," ","','"),"'],'description':'",G237,"','publish':",H237,"}"),"'","""")</f>
         <v>{"id":237,"title":"swimlane-feature-tree-with-people","group":"dotnet","area":"swimlane","keywords":["tree","branch","node","feature","people"],"description":"See what people are creating with Try .NET.","publish":1}</v>
       </c>
     </row>
+    <row r="238" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A238" s="5">
+        <v>238</v>
+      </c>
+      <c r="C238" s="2" t="s">
+        <v>897</v>
+      </c>
+      <c r="D238" t="s">
+        <v>900</v>
+      </c>
+      <c r="E238" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="F238" s="2" t="s">
+        <v>902</v>
+      </c>
+      <c r="G238" s="2" t="s">
+        <v>902</v>
+      </c>
+      <c r="H238" s="2">
+        <v>1</v>
+      </c>
+      <c r="I238" s="2" t="str">
+        <f t="shared" ref="I238:I241" si="8">SUBSTITUTE(_xlfn.CONCAT("{'id':",A238,",'title':'",C238,"','group':'",D238,"','area':'",E238,"','keywords':['",SUBSTITUTE(F238," ","','"),"'],'description':'",G238,"','publish':",H238,"}"),"'","""")</f>
+        <v>{"id":238,"title":"hero-azure-notebooks","group":"notebooks","area":"hero","keywords":["azure","notebooks"],"description":"azure notebooks","publish":1}</v>
+      </c>
+    </row>
+    <row r="239" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A239" s="5">
+        <v>239</v>
+      </c>
+      <c r="C239" s="2" t="s">
+        <v>898</v>
+      </c>
+      <c r="D239" t="s">
+        <v>900</v>
+      </c>
+      <c r="E239" s="2" t="s">
+        <v>901</v>
+      </c>
+      <c r="F239" s="2" t="s">
+        <v>903</v>
+      </c>
+      <c r="G239" s="2" t="s">
+        <v>903</v>
+      </c>
+      <c r="H239" s="2">
+        <v>1</v>
+      </c>
+      <c r="I239" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v>{"id":239,"title":"spot-azure-accessible-everywhere","group":"notebooks","area":"spot","keywords":["globe"],"description":"globe","publish":1}</v>
+      </c>
+    </row>
+    <row r="240" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A240" s="5">
+        <v>240</v>
+      </c>
+      <c r="C240" s="2" t="s">
+        <v>904</v>
+      </c>
+      <c r="D240" t="s">
+        <v>900</v>
+      </c>
+      <c r="E240" s="2" t="s">
+        <v>901</v>
+      </c>
+      <c r="F240" s="2" t="s">
+        <v>905</v>
+      </c>
+      <c r="G240" s="2" t="s">
+        <v>905</v>
+      </c>
+      <c r="H240" s="2">
+        <v>1</v>
+      </c>
+      <c r="I240" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v>{"id":240,"title":"spot-notebooks-languages","group":"notebooks","area":"spot","keywords":["notebooks","language"],"description":"notebooks language","publish":1}</v>
+      </c>
+    </row>
+    <row r="241" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A241" s="5">
+        <v>241</v>
+      </c>
+      <c r="C241" s="2" t="s">
+        <v>899</v>
+      </c>
+      <c r="D241" t="s">
+        <v>900</v>
+      </c>
+      <c r="E241" s="2" t="s">
+        <v>901</v>
+      </c>
+      <c r="F241" s="2" t="s">
+        <v>906</v>
+      </c>
+      <c r="G241" s="2" t="s">
+        <v>906</v>
+      </c>
+      <c r="H241" s="2">
+        <v>1</v>
+      </c>
+      <c r="I241" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v>{"id":241,"title":"spot-scientist-developer-student","group":"notebooks","area":"spot","keywords":["people"],"description":"people","publish":1}</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C92:C100">
+  <sortState ref="C92:C100">
     <sortCondition ref="C92"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15406,7 +15543,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H59">
+  <sortState ref="A2:H59">
     <sortCondition ref="C2:C59"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added new illustrations for .NET Cloud App page
</commit_message>
<xml_diff>
--- a/src/assets/data.xlsx
+++ b/src/assets/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F7D325-15AC-42EE-AB7C-4065126A9DA2}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5590A4C0-C8DD-40F9-B183-B3ECE52367BA}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="group">cv!$A$2:$A$6</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,6 +29,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1601" uniqueCount="907">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1631" uniqueCount="929">
   <si>
     <t>SeattleSkyline</t>
   </si>
@@ -2744,19 +2745,85 @@
     <t>spot</t>
   </si>
   <si>
-    <t>azure notebooks</t>
-  </si>
-  <si>
-    <t>globe</t>
-  </si>
-  <si>
     <t>spot-notebooks-languages</t>
   </si>
   <si>
     <t>notebooks language</t>
   </si>
   <si>
-    <t>people</t>
+    <t>swimlane-migrate-to-azure</t>
+  </si>
+  <si>
+    <t>swimlane-serverless-computing</t>
+  </si>
+  <si>
+    <t>swimlane-web-app-tools-library</t>
+  </si>
+  <si>
+    <t>swimlane-build-cloud-apps</t>
+  </si>
+  <si>
+    <t>swimlane-docker-container-support</t>
+  </si>
+  <si>
+    <t>swimlane-global-data-storage</t>
+  </si>
+  <si>
+    <t>migrate azure cloud helicopter move transfer</t>
+  </si>
+  <si>
+    <t>Migrate existing .NET apps to Azure.</t>
+  </si>
+  <si>
+    <t>serverless computing unplug network cloud computer device laptop desktop pc web</t>
+  </si>
+  <si>
+    <t>Serverless computing with .NET</t>
+  </si>
+  <si>
+    <t>toolbox tool hammer utility wrench pencil clipboard book library</t>
+  </si>
+  <si>
+    <t>Blue toolbox and books.</t>
+  </si>
+  <si>
+    <t>build forklift box container cloud scalable people</t>
+  </si>
+  <si>
+    <t>Build modern scalable cloud apps with .NET</t>
+  </si>
+  <si>
+    <t>docker cloud container ship port city skyline computer laptop</t>
+  </si>
+  <si>
+    <t>Ship with containers to represent Docker containers.</t>
+  </si>
+  <si>
+    <t>data storage database globe duplicate world</t>
+  </si>
+  <si>
+    <t>Data storage accessible from everywhere in the world.</t>
+  </si>
+  <si>
+    <t>azure notebooks data science charts people lab</t>
+  </si>
+  <si>
+    <t>An open notebook with people working on different domains of data science.</t>
+  </si>
+  <si>
+    <t>azure globe cloud</t>
+  </si>
+  <si>
+    <t>Azure Cloud Services accessible from anywhere in the world.</t>
+  </si>
+  <si>
+    <t>Azure Notebooks supports multiple languages.</t>
+  </si>
+  <si>
+    <t>people scientist developer student lab microscope tool engineering cap education</t>
+  </si>
+  <si>
+    <t>Use Azure Notebooks for many workspaces and scenarios.</t>
   </si>
 </sst>
 </file>
@@ -5662,13 +5729,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K241"/>
+  <dimension ref="A1:K247"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I241" sqref="I2:I241"/>
+      <selection pane="bottomRight" activeCell="I247" sqref="I2:I247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12133,7 +12200,7 @@
         <v>1</v>
       </c>
       <c r="I208" s="2" t="str">
-        <f t="shared" ref="I208:I237" si="7">SUBSTITUTE(_xlfn.CONCAT("{'id':",A208,",'title':'",C208,"','group':'",D208,"','area':'",E208,"','keywords':['",SUBSTITUTE(F208," ","','"),"'],'description':'",G208,"','publish':",H208,"}"),"'","""")</f>
+        <f t="shared" ref="I208:I235" si="7">SUBSTITUTE(_xlfn.CONCAT("{'id':",A208,",'title':'",C208,"','group':'",D208,"','area':'",E208,"','keywords':['",SUBSTITUTE(F208," ","','"),"'],'description':'",G208,"','publish':",H208,"}"),"'","""")</f>
         <v>{"id":207,"title":"wizard-upgrade-from-xml-to-inheritance","group":"wizard","area":"agile","keywords":["inheritance","xml","file","document","instance","dotted","line"],"description":"Upgrade from XML defined process to inheritance type.","publish":1}</v>
       </c>
       <c r="J208" s="2" t="str">
@@ -12938,17 +13005,17 @@
         <v>271</v>
       </c>
       <c r="F238" s="2" t="s">
-        <v>902</v>
+        <v>922</v>
       </c>
       <c r="G238" s="2" t="s">
-        <v>902</v>
+        <v>923</v>
       </c>
       <c r="H238" s="2">
         <v>1</v>
       </c>
       <c r="I238" s="2" t="str">
-        <f t="shared" ref="I238:I241" si="8">SUBSTITUTE(_xlfn.CONCAT("{'id':",A238,",'title':'",C238,"','group':'",D238,"','area':'",E238,"','keywords':['",SUBSTITUTE(F238," ","','"),"'],'description':'",G238,"','publish':",H238,"}"),"'","""")</f>
-        <v>{"id":238,"title":"hero-azure-notebooks","group":"notebooks","area":"hero","keywords":["azure","notebooks"],"description":"azure notebooks","publish":1}</v>
+        <f t="shared" ref="I238:I247" si="8">SUBSTITUTE(_xlfn.CONCAT("{'id':",A238,",'title':'",C238,"','group':'",D238,"','area':'",E238,"','keywords':['",SUBSTITUTE(F238," ","','"),"'],'description':'",G238,"','publish':",H238,"}"),"'","""")</f>
+        <v>{"id":238,"title":"hero-azure-notebooks","group":"notebooks","area":"hero","keywords":["azure","notebooks","data","science","charts","people","lab"],"description":"An open notebook with people working on different domains of data science.","publish":1}</v>
       </c>
     </row>
     <row r="239" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -12965,17 +13032,17 @@
         <v>901</v>
       </c>
       <c r="F239" s="2" t="s">
-        <v>903</v>
+        <v>924</v>
       </c>
       <c r="G239" s="2" t="s">
-        <v>903</v>
+        <v>925</v>
       </c>
       <c r="H239" s="2">
         <v>1</v>
       </c>
       <c r="I239" s="2" t="str">
         <f t="shared" si="8"/>
-        <v>{"id":239,"title":"spot-azure-accessible-everywhere","group":"notebooks","area":"spot","keywords":["globe"],"description":"globe","publish":1}</v>
+        <v>{"id":239,"title":"spot-azure-accessible-everywhere","group":"notebooks","area":"spot","keywords":["azure","globe","cloud"],"description":"Azure Cloud Services accessible from anywhere in the world.","publish":1}</v>
       </c>
     </row>
     <row r="240" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -12983,7 +13050,7 @@
         <v>240</v>
       </c>
       <c r="C240" s="2" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="D240" t="s">
         <v>900</v>
@@ -12992,17 +13059,17 @@
         <v>901</v>
       </c>
       <c r="F240" s="2" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="G240" s="2" t="s">
-        <v>905</v>
+        <v>926</v>
       </c>
       <c r="H240" s="2">
         <v>1</v>
       </c>
       <c r="I240" s="2" t="str">
         <f t="shared" si="8"/>
-        <v>{"id":240,"title":"spot-notebooks-languages","group":"notebooks","area":"spot","keywords":["notebooks","language"],"description":"notebooks language","publish":1}</v>
+        <v>{"id":240,"title":"spot-notebooks-languages","group":"notebooks","area":"spot","keywords":["notebooks","language"],"description":"Azure Notebooks supports multiple languages.","publish":1}</v>
       </c>
     </row>
     <row r="241" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -13019,21 +13086,183 @@
         <v>901</v>
       </c>
       <c r="F241" s="2" t="s">
-        <v>906</v>
+        <v>927</v>
       </c>
       <c r="G241" s="2" t="s">
-        <v>906</v>
+        <v>928</v>
       </c>
       <c r="H241" s="2">
         <v>1</v>
       </c>
       <c r="I241" s="2" t="str">
         <f t="shared" si="8"/>
-        <v>{"id":241,"title":"spot-scientist-developer-student","group":"notebooks","area":"spot","keywords":["people"],"description":"people","publish":1}</v>
+        <v>{"id":241,"title":"spot-scientist-developer-student","group":"notebooks","area":"spot","keywords":["people","scientist","developer","student","lab","microscope","tool","engineering","cap","education"],"description":"Use Azure Notebooks for many workspaces and scenarios.","publish":1}</v>
+      </c>
+    </row>
+    <row r="242" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A242" s="5">
+        <v>242</v>
+      </c>
+      <c r="C242" s="2" t="s">
+        <v>904</v>
+      </c>
+      <c r="D242" t="s">
+        <v>387</v>
+      </c>
+      <c r="E242" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F242" s="2" t="s">
+        <v>910</v>
+      </c>
+      <c r="G242" s="2" t="s">
+        <v>911</v>
+      </c>
+      <c r="H242" s="2">
+        <v>1</v>
+      </c>
+      <c r="I242" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v>{"id":242,"title":"swimlane-migrate-to-azure","group":"dotnet","area":"swimlane","keywords":["migrate","azure","cloud","helicopter","move","transfer"],"description":"Migrate existing .NET apps to Azure.","publish":1}</v>
+      </c>
+    </row>
+    <row r="243" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A243" s="5">
+        <v>243</v>
+      </c>
+      <c r="C243" s="2" t="s">
+        <v>905</v>
+      </c>
+      <c r="D243" t="s">
+        <v>387</v>
+      </c>
+      <c r="E243" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F243" s="2" t="s">
+        <v>912</v>
+      </c>
+      <c r="G243" s="2" t="s">
+        <v>913</v>
+      </c>
+      <c r="H243" s="2">
+        <v>1</v>
+      </c>
+      <c r="I243" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v>{"id":243,"title":"swimlane-serverless-computing","group":"dotnet","area":"swimlane","keywords":["serverless","computing","unplug","network","cloud","computer","device","laptop","desktop","pc","web"],"description":"Serverless computing with .NET","publish":1}</v>
+      </c>
+    </row>
+    <row r="244" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A244" s="5">
+        <v>244</v>
+      </c>
+      <c r="C244" s="2" t="s">
+        <v>906</v>
+      </c>
+      <c r="D244" t="s">
+        <v>387</v>
+      </c>
+      <c r="E244" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F244" s="2" t="s">
+        <v>914</v>
+      </c>
+      <c r="G244" s="2" t="s">
+        <v>915</v>
+      </c>
+      <c r="H244" s="2">
+        <v>1</v>
+      </c>
+      <c r="I244" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v>{"id":244,"title":"swimlane-web-app-tools-library","group":"dotnet","area":"swimlane","keywords":["toolbox","tool","hammer","utility","wrench","pencil","clipboard","book","library"],"description":"Blue toolbox and books.","publish":1}</v>
+      </c>
+    </row>
+    <row r="245" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A245" s="5">
+        <v>245</v>
+      </c>
+      <c r="C245" s="2" t="s">
+        <v>907</v>
+      </c>
+      <c r="D245" t="s">
+        <v>387</v>
+      </c>
+      <c r="E245" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F245" s="2" t="s">
+        <v>916</v>
+      </c>
+      <c r="G245" s="2" t="s">
+        <v>917</v>
+      </c>
+      <c r="H245" s="2">
+        <v>1</v>
+      </c>
+      <c r="I245" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v>{"id":245,"title":"swimlane-build-cloud-apps","group":"dotnet","area":"swimlane","keywords":["build","forklift","box","container","cloud","scalable","people"],"description":"Build modern scalable cloud apps with .NET","publish":1}</v>
+      </c>
+    </row>
+    <row r="246" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A246" s="5">
+        <v>246</v>
+      </c>
+      <c r="C246" s="2" t="s">
+        <v>908</v>
+      </c>
+      <c r="D246" t="s">
+        <v>387</v>
+      </c>
+      <c r="E246" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F246" s="2" t="s">
+        <v>918</v>
+      </c>
+      <c r="G246" s="2" t="s">
+        <v>919</v>
+      </c>
+      <c r="H246" s="2">
+        <v>1</v>
+      </c>
+      <c r="I246" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v>{"id":246,"title":"swimlane-docker-container-support","group":"dotnet","area":"swimlane","keywords":["docker","cloud","container","ship","port","city","skyline","computer","laptop"],"description":"Ship with containers to represent Docker containers.","publish":1}</v>
+      </c>
+    </row>
+    <row r="247" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A247" s="5">
+        <v>247</v>
+      </c>
+      <c r="C247" s="2" t="s">
+        <v>909</v>
+      </c>
+      <c r="D247" t="s">
+        <v>387</v>
+      </c>
+      <c r="E247" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F247" s="2" t="s">
+        <v>920</v>
+      </c>
+      <c r="G247" s="2" t="s">
+        <v>921</v>
+      </c>
+      <c r="H247" s="2">
+        <v>1</v>
+      </c>
+      <c r="I247" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v>{"id":247,"title":"swimlane-global-data-storage","group":"dotnet","area":"swimlane","keywords":["data","storage","database","globe","duplicate","world"],"description":"Data storage accessible from everywhere in the world.","publish":1}</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="C92:C100">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C92:C100">
     <sortCondition ref="C92"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15543,7 +15772,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:H59">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H59">
     <sortCondition ref="C2:C59"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added new illustrations for ASP.NET web apps page
</commit_message>
<xml_diff>
--- a/src/assets/data.xlsx
+++ b/src/assets/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cherr\Dropbox\Code\vsimages\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5590A4C0-C8DD-40F9-B183-B3ECE52367BA}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C93A08A1-4710-461A-AD3D-49068D11FA42}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12318" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="5" r:id="rId1"/>
@@ -29,7 +29,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1631" uniqueCount="929">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1656" uniqueCount="944">
   <si>
     <t>SeattleSkyline</t>
   </si>
@@ -2824,6 +2823,51 @@
   </si>
   <si>
     <t>Use Azure Notebooks for many workspaces and scenarios.</t>
+  </si>
+  <si>
+    <t>swimlane-security</t>
+  </si>
+  <si>
+    <t>swimlane-angular-react-spa</t>
+  </si>
+  <si>
+    <t>swimlane-build-scalable-web-apps</t>
+  </si>
+  <si>
+    <t>swimlane-model-view-controller</t>
+  </si>
+  <si>
+    <t>swimlane-seamless-data-integration</t>
+  </si>
+  <si>
+    <t>security guard camera safe secure</t>
+  </si>
+  <si>
+    <t>A safety guard protecting a safe.</t>
+  </si>
+  <si>
+    <t>angular react spa single page application website</t>
+  </si>
+  <si>
+    <t>React and Angular logo and single page web app.</t>
+  </si>
+  <si>
+    <t>build scalable web app page truck box people</t>
+  </si>
+  <si>
+    <t>A worker loading boxes from truck to a web page.</t>
+  </si>
+  <si>
+    <t>mvc model view controller data gear presentation theme paint bucket brush design frontend backend stack</t>
+  </si>
+  <si>
+    <t>MVC illustration.</t>
+  </si>
+  <si>
+    <t>data database orbit</t>
+  </si>
+  <si>
+    <t>Seamless data integration.</t>
   </si>
 </sst>
 </file>
@@ -5729,31 +5773,31 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K247"/>
+  <dimension ref="A1:K252"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B248" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I247" sqref="I2:I247"/>
+      <selection pane="bottomRight" activeCell="D249" sqref="D249"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="100" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="35.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="38.140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="13.26171875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="35.83984375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="38.15625" style="2" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
     <col min="5" max="5" width="18" style="2" customWidth="1"/>
-    <col min="6" max="6" width="33.7109375" style="2" customWidth="1"/>
-    <col min="7" max="8" width="20.7109375" style="2" customWidth="1"/>
-    <col min="9" max="10" width="24.140625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="33.140625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="66.42578125" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="2"/>
+    <col min="6" max="6" width="33.68359375" style="2" customWidth="1"/>
+    <col min="7" max="8" width="20.68359375" style="2" customWidth="1"/>
+    <col min="9" max="10" width="24.15625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="33.15625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="66.41796875" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="9.15625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
         <v>201</v>
       </c>
@@ -5788,7 +5832,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -5822,7 +5866,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -5853,7 +5897,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\widget-you-dont-have-permission.svg</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -5884,7 +5928,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-charting-not-supported.svg</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -5915,7 +5959,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-custom-rules.svg</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -5946,7 +5990,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-get-back-to-recent-work.svg</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -5977,7 +6021,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-invalid-workitem-type.svg</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -6008,7 +6052,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-keep-an-eye-on-important-work.svg</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -6039,7 +6083,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-mention-someone.svg</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -6070,7 +6114,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-no-charts.svg</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -6101,7 +6145,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-unsaved-query.svg</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -6132,7 +6176,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-workitem-not-found.svg</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -6163,7 +6207,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-your-work-in-one-place.svg</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -6194,7 +6238,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-get-started-with-sprint.svg</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -6225,7 +6269,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-add-a-feed.svg</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -6256,7 +6300,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-connect-to-feed.svg</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -6287,7 +6331,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\general-no-results-found.svg</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -6318,7 +6362,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\hero-extend-vside.svg</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -6349,7 +6393,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-create-your-own-extension.svg</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -6380,7 +6424,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-marketplace.svg</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -6411,7 +6455,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-partner-program.svg</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -6442,7 +6486,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-what-are-extensions.svg</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -6473,7 +6517,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-add-product.svg</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -6504,7 +6548,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-configure-component-governance.svg</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -6535,7 +6579,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-release-management.svg</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -6566,7 +6610,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-this-repository-has-no-tags-yet.svg</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -6597,7 +6641,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-add-deployment-group.svg</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -6628,7 +6672,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-automate-build-definitions.svg</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -6659,7 +6703,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-choose-a-template.svg</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -6690,7 +6734,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-cloud-based-load-testing.svg</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -6721,7 +6765,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-favorites.svg</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -6752,7 +6796,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-get-everyone-on-same-page.svg</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -6783,7 +6827,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-no-plan.svg</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -6814,7 +6858,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-no-variable-groups.svg</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -6845,7 +6889,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-pull-request.svg</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -6876,7 +6920,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\hero-swiss-army-knife.svg</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -6907,7 +6951,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-all-your-code-hosted-free.svg</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -6938,7 +6982,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-any-client-any-platform.svg</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -6969,7 +7013,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-but-wait-theres-more.svg</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -7000,7 +7044,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-pricing.svg</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -7031,7 +7075,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-were-in-your-neighborhood.svg</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -7062,7 +7106,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\hero-pricing-calculator.svg</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -7093,7 +7137,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-you-have-no-organizations-yet.svg</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -7124,7 +7168,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\general-robot-errorcode-503.svg</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -7155,7 +7199,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\general-robot-error.svg</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -7186,7 +7230,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\general-robot-errorcode-400.svg</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -7217,7 +7261,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\general-robot-errorcode-401.svg</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -7248,7 +7292,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\general-robot-errorcode-403.svg</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -7279,7 +7323,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\general-robot-errorcode-404.svg</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -7310,7 +7354,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\general-robot-errorcode-500.svg</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -7341,7 +7385,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-no-assessments.svg</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -7372,7 +7416,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-initializing-test-results.svg</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -7403,7 +7447,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-no-work-scheduled.svg</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -7434,7 +7478,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-sprint-drag-n-drop.svg</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -7465,7 +7509,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-seamless-debugging-with-symbols.svg</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="5">
         <v>55</v>
       </c>
@@ -7496,7 +7540,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-xamarin-cross-platform.svg</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="5">
         <v>56</v>
       </c>
@@ -7527,7 +7571,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-azure-machine-learning.svg</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="5">
         <v>57</v>
       </c>
@@ -7558,7 +7602,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-cognitive-services.svg</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="5">
         <v>58</v>
       </c>
@@ -7589,7 +7633,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-congratulations-finished-setup.svg</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="5">
         <v>59</v>
       </c>
@@ -7620,7 +7664,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-cross-platform.svg</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="5">
         <v>60</v>
       </c>
@@ -7651,7 +7695,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-cryengine-game-development.svg</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="5">
         <v>61</v>
       </c>
@@ -7682,7 +7726,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-developer-meetup.svg</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="5">
         <v>62</v>
       </c>
@@ -7713,7 +7757,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-dotnet-core.svg</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="5">
         <v>63</v>
       </c>
@@ -7744,7 +7788,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-dotnet-enterprise.svg</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="5">
         <v>64</v>
       </c>
@@ -7775,7 +7819,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-download-target.svg</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="5">
         <v>65</v>
       </c>
@@ -7806,7 +7850,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-enterprise-customer-stories.svg</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="5">
         <v>66</v>
       </c>
@@ -7837,7 +7881,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-feedback-survey.svg</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="5">
         <v>67</v>
       </c>
@@ -7868,7 +7912,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-fsharp-data-science.svg</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="5">
         <v>68</v>
       </c>
@@ -7899,7 +7943,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-machine-learning-library.svg</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="5">
         <v>69</v>
       </c>
@@ -7930,7 +7974,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-one-consistent-api.svg</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="5">
         <v>70</v>
       </c>
@@ -7961,7 +8005,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-package-library.svg</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="5">
         <v>71</v>
       </c>
@@ -7992,7 +8036,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-programming-languages.svg</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="5">
         <v>72</v>
       </c>
@@ -8023,7 +8067,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-thank-you-for-downloading.svg</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="5">
         <v>73</v>
       </c>
@@ -8054,7 +8098,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-unity-game-development.svg</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="5">
         <v>74</v>
       </c>
@@ -8085,7 +8129,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-universal-windows-platform.svg</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="5">
         <v>75</v>
       </c>
@@ -8116,7 +8160,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-uwp-iot-core.svg</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="5">
         <v>76</v>
       </c>
@@ -8147,7 +8191,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-winform.svg</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="5">
         <v>77</v>
       </c>
@@ -8178,7 +8222,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-wpf.svg</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="5">
         <v>78</v>
       </c>
@@ -8209,7 +8253,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-xamarin.svg</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="5">
         <v>79</v>
       </c>
@@ -8240,7 +8284,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-dotnet-perf-diagram.svg</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="5">
         <v>80</v>
       </c>
@@ -8271,7 +8315,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\hero-snapshot-debugger.svg</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="5">
         <v>81</v>
       </c>
@@ -8302,7 +8346,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-collaborative-debugging.svg</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="5">
         <v>82</v>
       </c>
@@ -8333,7 +8377,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-collaborative-editing.svg</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="5">
         <v>83</v>
       </c>
@@ -8364,7 +8408,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-shared-full-context.svg</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="5">
         <v>84</v>
       </c>
@@ -8395,7 +8439,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-real-time-sharing.svg</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="5">
         <v>85</v>
       </c>
@@ -8426,7 +8470,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\blog-rocket-launch-timeline.svg</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="5">
         <v>86</v>
       </c>
@@ -8457,7 +8501,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\blog-vscode-metrics.svg</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="5">
         <v>87</v>
       </c>
@@ -8488,7 +8532,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\blog-vscode-roadmap.svg</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="5">
         <v>88</v>
       </c>
@@ -8519,7 +8563,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-monogame-game-development.svg</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="5">
         <v>89</v>
       </c>
@@ -8550,7 +8594,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-you-have-no-project.svg</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="5">
         <v>90</v>
       </c>
@@ -8581,7 +8625,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\hero-vsts-join-our-team.svg</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="5">
         <v>91</v>
       </c>
@@ -8612,7 +8656,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\elements-devices-1.svg</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="5">
         <v>92</v>
       </c>
@@ -8643,7 +8687,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\elements-devices-2.svg</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="5">
         <v>93</v>
       </c>
@@ -8674,7 +8718,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\elements-robots-1.svg</v>
       </c>
     </row>
-    <row r="95" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="5">
         <v>94</v>
       </c>
@@ -8705,7 +8749,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\elements-robots-2.svg</v>
       </c>
     </row>
-    <row r="96" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="5">
         <v>95</v>
       </c>
@@ -8736,7 +8780,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\elements-tools-1.svg</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="5">
         <v>96</v>
       </c>
@@ -8767,7 +8811,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\elements-tools-2.svg</v>
       </c>
     </row>
-    <row r="98" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="5">
         <v>97</v>
       </c>
@@ -8798,7 +8842,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\elements-vehicles-1.svg</v>
       </c>
     </row>
-    <row r="99" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="5">
         <v>98</v>
       </c>
@@ -8829,7 +8873,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\elements-vehicles-2.svg</v>
       </c>
     </row>
-    <row r="100" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="5">
         <v>99</v>
       </c>
@@ -8860,7 +8904,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\elements-vehicles-3.svg</v>
       </c>
     </row>
-    <row r="101" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="5">
         <v>100</v>
       </c>
@@ -8891,7 +8935,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-verify-analytics-views.svg</v>
       </c>
     </row>
-    <row r="102" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="5">
         <v>101</v>
       </c>
@@ -8922,7 +8966,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-analytics-views-error.svg</v>
       </c>
     </row>
-    <row r="103" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="5">
         <v>102</v>
       </c>
@@ -8953,7 +8997,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-analytics-views-valid.svg</v>
       </c>
     </row>
-    <row r="104" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="5">
         <v>103</v>
       </c>
@@ -8984,7 +9028,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-no-analytics-views.svg</v>
       </c>
     </row>
-    <row r="105" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="5">
         <v>104</v>
       </c>
@@ -9015,7 +9059,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-preparing-data.svg</v>
       </c>
     </row>
-    <row r="106" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="5">
         <v>105</v>
       </c>
@@ -9046,7 +9090,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\socialmedia-devops-youtube-header.svg</v>
       </c>
     </row>
-    <row r="107" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="5">
         <v>106</v>
       </c>
@@ -9077,7 +9121,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\socialmedia-devops-avatar.svg</v>
       </c>
     </row>
-    <row r="108" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="5">
         <v>107</v>
       </c>
@@ -9108,7 +9152,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\tile-self-hosted-server.svg</v>
       </c>
     </row>
-    <row r="109" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="5">
         <v>108</v>
       </c>
@@ -9139,7 +9183,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\tile-cloud-hosted-server.svg</v>
       </c>
     </row>
-    <row r="110" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="5">
         <v>109</v>
       </c>
@@ -9170,7 +9214,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\tile-integrate-with-cloud-services.svg</v>
       </c>
     </row>
-    <row r="111" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="5">
         <v>110</v>
       </c>
@@ -9201,7 +9245,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\general-folder.svg</v>
       </c>
     </row>
-    <row r="112" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="5">
         <v>111</v>
       </c>
@@ -9232,7 +9276,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-speed-gauge-comparison.svg</v>
       </c>
     </row>
-    <row r="113" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="5">
         <v>112</v>
       </c>
@@ -9263,7 +9307,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-speed-gauge-comparison-withtext.svg</v>
       </c>
     </row>
-    <row r="114" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="5">
         <v>113</v>
       </c>
@@ -9294,7 +9338,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-vside-lightbulb-intellisense.svg</v>
       </c>
     </row>
-    <row r="115" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="5">
         <v>114</v>
       </c>
@@ -9325,7 +9369,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-async-await-runners.svg</v>
       </c>
     </row>
-    <row r="116" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="5">
         <v>115</v>
       </c>
@@ -9356,7 +9400,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-barchart-skyline.svg</v>
       </c>
     </row>
-    <row r="117" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" s="5">
         <v>116</v>
       </c>
@@ -9387,7 +9431,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-barchart-skyline-withtext.svg</v>
       </c>
     </row>
-    <row r="118" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="5">
         <v>117</v>
       </c>
@@ -9418,7 +9462,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-contributors-around-world.svg</v>
       </c>
     </row>
-    <row r="119" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="5">
         <v>118</v>
       </c>
@@ -9449,7 +9493,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-contributors-around-world-withtext.svg</v>
       </c>
     </row>
-    <row r="120" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="5">
         <v>119</v>
       </c>
@@ -9480,7 +9524,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-dotnet-node-table.svg</v>
       </c>
     </row>
-    <row r="121" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="5">
         <v>120</v>
       </c>
@@ -9511,7 +9555,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-one-vs-many-tools.svg</v>
       </c>
     </row>
-    <row r="122" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="5">
         <v>121</v>
       </c>
@@ -9542,7 +9586,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-any-language.svg</v>
       </c>
     </row>
-    <row r="123" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="5">
         <v>122</v>
       </c>
@@ -9573,7 +9617,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-deploy-cross-platform.svg</v>
       </c>
     </row>
-    <row r="124" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" s="5">
         <v>123</v>
       </c>
@@ -9604,7 +9648,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-swiss-army-knife.svg</v>
       </c>
     </row>
-    <row r="125" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" s="5">
         <v>124</v>
       </c>
@@ -9635,7 +9679,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\hero-devops-conductor.svg</v>
       </c>
     </row>
-    <row r="126" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="5">
         <v>125</v>
       </c>
@@ -9666,7 +9710,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\blog-package-upstream-diagram-1.svg</v>
       </c>
     </row>
-    <row r="127" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="5">
         <v>126</v>
       </c>
@@ -9697,7 +9741,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\blog-package-upstream-diagram-2.svg</v>
       </c>
     </row>
-    <row r="128" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" s="5">
         <v>127</v>
       </c>
@@ -9728,7 +9772,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\blog-package-upstream-diagram-3.svg</v>
       </c>
     </row>
-    <row r="129" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" s="5">
         <v>128</v>
       </c>
@@ -9759,7 +9803,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\blog-package-upstream-diagram-4.svg</v>
       </c>
     </row>
-    <row r="130" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="5">
         <v>129</v>
       </c>
@@ -9790,7 +9834,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\willow-car-racing-get-ready.svg</v>
       </c>
     </row>
-    <row r="131" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="5">
         <v>130</v>
       </c>
@@ -9821,7 +9865,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\willow-rocket-get-ready.svg</v>
       </c>
     </row>
-    <row r="132" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" s="5">
         <v>131</v>
       </c>
@@ -9852,7 +9896,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\willow-bike-adventure.svg</v>
       </c>
     </row>
-    <row r="133" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" s="5">
         <v>132</v>
       </c>
@@ -9883,7 +9927,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\willow-bike-adventure-issue.svg</v>
       </c>
     </row>
-    <row r="134" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" s="5">
         <v>133</v>
       </c>
@@ -9914,7 +9958,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-no-dashboard.svg</v>
       </c>
     </row>
-    <row r="135" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" s="5">
         <v>134</v>
       </c>
@@ -9945,7 +9989,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\docs-gvfs-architecture.svg</v>
       </c>
     </row>
-    <row r="136" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" s="5">
         <v>135</v>
       </c>
@@ -9976,7 +10020,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\hero-vs-tools-for-azure.svg</v>
       </c>
     </row>
-    <row r="137" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" s="5">
         <v>136</v>
       </c>
@@ -10007,7 +10051,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-build-release-pipeline.svg</v>
       </c>
     </row>
-    <row r="138" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" s="5">
         <v>137</v>
       </c>
@@ -10038,7 +10082,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-build-release-monitor-activities.svg</v>
       </c>
     </row>
-    <row r="139" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" s="5">
         <v>138</v>
       </c>
@@ -10069,7 +10113,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-data-009.svg</v>
       </c>
     </row>
-    <row r="140" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" s="5">
         <v>139</v>
       </c>
@@ -10100,7 +10144,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-agriculture-001.svg</v>
       </c>
     </row>
-    <row r="141" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" s="5">
         <v>140</v>
       </c>
@@ -10131,7 +10175,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-001.svg</v>
       </c>
     </row>
-    <row r="142" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" s="5">
         <v>141</v>
       </c>
@@ -10162,7 +10206,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-002.svg</v>
       </c>
     </row>
-    <row r="143" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" s="5">
         <v>142</v>
       </c>
@@ -10193,7 +10237,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-003.svg</v>
       </c>
     </row>
-    <row r="144" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" s="5">
         <v>143</v>
       </c>
@@ -10224,7 +10268,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-004.svg</v>
       </c>
     </row>
-    <row r="145" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" s="5">
         <v>144</v>
       </c>
@@ -10255,7 +10299,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-005.svg</v>
       </c>
     </row>
-    <row r="146" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" s="5">
         <v>145</v>
       </c>
@@ -10286,7 +10330,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-006.svg</v>
       </c>
     </row>
-    <row r="147" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" s="5">
         <v>146</v>
       </c>
@@ -10317,7 +10361,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-007.svg</v>
       </c>
     </row>
-    <row r="148" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" s="5">
         <v>147</v>
       </c>
@@ -10348,7 +10392,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-008.svg</v>
       </c>
     </row>
-    <row r="149" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" s="5">
         <v>148</v>
       </c>
@@ -10379,7 +10423,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-009.svg</v>
       </c>
     </row>
-    <row r="150" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" s="5">
         <v>149</v>
       </c>
@@ -10410,7 +10454,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-010.svg</v>
       </c>
     </row>
-    <row r="151" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" s="5">
         <v>150</v>
       </c>
@@ -10441,7 +10485,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-011.svg</v>
       </c>
     </row>
-    <row r="152" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" s="5">
         <v>151</v>
       </c>
@@ -10472,7 +10516,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-012.svg</v>
       </c>
     </row>
-    <row r="153" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" s="5">
         <v>152</v>
       </c>
@@ -10503,7 +10547,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-013.svg</v>
       </c>
     </row>
-    <row r="154" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" s="5">
         <v>153</v>
       </c>
@@ -10534,7 +10578,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-014.svg</v>
       </c>
     </row>
-    <row r="155" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" s="5">
         <v>154</v>
       </c>
@@ -10565,7 +10609,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-015.svg</v>
       </c>
     </row>
-    <row r="156" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" s="5">
         <v>155</v>
       </c>
@@ -10596,7 +10640,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-016.svg</v>
       </c>
     </row>
-    <row r="157" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" s="5">
         <v>156</v>
       </c>
@@ -10627,7 +10671,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-017.svg</v>
       </c>
     </row>
-    <row r="158" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" s="5">
         <v>157</v>
       </c>
@@ -10658,7 +10702,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-001.svg</v>
       </c>
     </row>
-    <row r="159" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" s="5">
         <v>158</v>
       </c>
@@ -10689,7 +10733,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-002.svg</v>
       </c>
     </row>
-    <row r="160" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" s="5">
         <v>159</v>
       </c>
@@ -10720,7 +10764,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-003.svg</v>
       </c>
     </row>
-    <row r="161" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" s="5">
         <v>160</v>
       </c>
@@ -10751,7 +10795,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-004.svg</v>
       </c>
     </row>
-    <row r="162" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A162" s="5">
         <v>161</v>
       </c>
@@ -10782,7 +10826,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-005.svg</v>
       </c>
     </row>
-    <row r="163" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A163" s="5">
         <v>162</v>
       </c>
@@ -10813,7 +10857,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-006.svg</v>
       </c>
     </row>
-    <row r="164" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" s="5">
         <v>163</v>
       </c>
@@ -10844,7 +10888,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-007.svg</v>
       </c>
     </row>
-    <row r="165" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A165" s="5">
         <v>164</v>
       </c>
@@ -10875,7 +10919,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-008.svg</v>
       </c>
     </row>
-    <row r="166" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" s="5">
         <v>165</v>
       </c>
@@ -10906,7 +10950,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-009.svg</v>
       </c>
     </row>
-    <row r="167" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" s="5">
         <v>166</v>
       </c>
@@ -10937,7 +10981,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-010.svg</v>
       </c>
     </row>
-    <row r="168" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A168" s="5">
         <v>167</v>
       </c>
@@ -10968,7 +11012,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-011.svg</v>
       </c>
     </row>
-    <row r="169" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" s="5">
         <v>168</v>
       </c>
@@ -10999,7 +11043,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-012.svg</v>
       </c>
     </row>
-    <row r="170" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" s="5">
         <v>169</v>
       </c>
@@ -11030,7 +11074,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-013.svg</v>
       </c>
     </row>
-    <row r="171" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" s="5">
         <v>170</v>
       </c>
@@ -11061,7 +11105,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-collaboration-001.svg</v>
       </c>
     </row>
-    <row r="172" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A172" s="5">
         <v>171</v>
       </c>
@@ -11092,7 +11136,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-collaboration-002.svg</v>
       </c>
     </row>
-    <row r="173" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" s="5">
         <v>172</v>
       </c>
@@ -11123,7 +11167,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-collaboration-003.svg</v>
       </c>
     </row>
-    <row r="174" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A174" s="5">
         <v>173</v>
       </c>
@@ -11154,7 +11198,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-collaboration-005.svg</v>
       </c>
     </row>
-    <row r="175" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A175" s="5">
         <v>174</v>
       </c>
@@ -11185,7 +11229,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-collaboration-006.svg</v>
       </c>
     </row>
-    <row r="176" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A176" s="5">
         <v>175</v>
       </c>
@@ -11216,7 +11260,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-collaboration-007.svg</v>
       </c>
     </row>
-    <row r="177" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" s="5">
         <v>176</v>
       </c>
@@ -11247,7 +11291,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-collaboration-008.svg</v>
       </c>
     </row>
-    <row r="178" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A178" s="5">
         <v>177</v>
       </c>
@@ -11278,7 +11322,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-collaboration-009.svg</v>
       </c>
     </row>
-    <row r="179" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" s="5">
         <v>178</v>
       </c>
@@ -11309,7 +11353,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-collaboration-010.svg</v>
       </c>
     </row>
-    <row r="180" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" s="5">
         <v>179</v>
       </c>
@@ -11340,7 +11384,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-collaboration-011.svg</v>
       </c>
     </row>
-    <row r="181" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A181" s="5">
         <v>180</v>
       </c>
@@ -11371,7 +11415,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-communication-001.svg</v>
       </c>
     </row>
-    <row r="182" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" s="5">
         <v>181</v>
       </c>
@@ -11402,7 +11446,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-communication-002.svg</v>
       </c>
     </row>
-    <row r="183" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A183" s="5">
         <v>182</v>
       </c>
@@ -11433,7 +11477,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-consumer-001.svg</v>
       </c>
     </row>
-    <row r="184" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A184" s="5">
         <v>183</v>
       </c>
@@ -11464,7 +11508,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-consumer-002.svg</v>
       </c>
     </row>
-    <row r="185" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A185" s="5">
         <v>184</v>
       </c>
@@ -11495,7 +11539,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-data-001.svg</v>
       </c>
     </row>
-    <row r="186" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A186" s="5">
         <v>185</v>
       </c>
@@ -11526,7 +11570,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-data-002.svg</v>
       </c>
     </row>
-    <row r="187" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A187" s="5">
         <v>186</v>
       </c>
@@ -11557,7 +11601,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-data-003.svg</v>
       </c>
     </row>
-    <row r="188" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A188" s="5">
         <v>187</v>
       </c>
@@ -11588,7 +11632,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-data-004.svg</v>
       </c>
     </row>
-    <row r="189" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A189" s="5">
         <v>188</v>
       </c>
@@ -11619,7 +11663,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-data-005.svg</v>
       </c>
     </row>
-    <row r="190" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A190" s="5">
         <v>189</v>
       </c>
@@ -11650,7 +11694,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-data-006.svg</v>
       </c>
     </row>
-    <row r="191" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A191" s="5">
         <v>190</v>
       </c>
@@ -11681,7 +11725,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-data-007.svg</v>
       </c>
     </row>
-    <row r="192" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A192" s="5">
         <v>191</v>
       </c>
@@ -11712,7 +11756,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-data-008.svg</v>
       </c>
     </row>
-    <row r="193" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A193" s="5">
         <v>192</v>
       </c>
@@ -11743,7 +11787,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-feature-not-configured.svg</v>
       </c>
     </row>
-    <row r="194" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A194" s="5">
         <v>193</v>
       </c>
@@ -11774,7 +11818,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-boxes-and-devices.svg</v>
       </c>
     </row>
-    <row r="195" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A195" s="5">
         <v>194</v>
       </c>
@@ -11805,7 +11849,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-butler-ide.svg</v>
       </c>
     </row>
-    <row r="196" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A196" s="5">
         <v>195</v>
       </c>
@@ -11836,7 +11880,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-code-or-gui.svg</v>
       </c>
     </row>
-    <row r="197" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A197" s="5">
         <v>196</v>
       </c>
@@ -11867,7 +11911,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-data-analytics-pipeline.svg</v>
       </c>
     </row>
-    <row r="198" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A198" s="5">
         <v>197</v>
       </c>
@@ -11898,7 +11942,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-developer-scenarios.svg</v>
       </c>
     </row>
-    <row r="199" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A199" s="5">
         <v>198</v>
       </c>
@@ -11929,7 +11973,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-machine-learning-books-lab.svg</v>
       </c>
     </row>
-    <row r="200" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A200" s="5">
         <v>199</v>
       </c>
@@ -11960,7 +12004,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-machine-learning-extensible.svg</v>
       </c>
     </row>
-    <row r="201" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A201" s="5">
         <v>200</v>
       </c>
@@ -11991,7 +12035,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-machine-learning-lightbulb-hand.svg</v>
       </c>
     </row>
-    <row r="202" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A202" s="5">
         <v>201</v>
       </c>
@@ -12022,7 +12066,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-necessary-learner-tools.svg</v>
       </c>
     </row>
-    <row r="203" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A203" s="5">
         <v>202</v>
       </c>
@@ -12053,7 +12097,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-share-code-snippets.svg</v>
       </c>
     </row>
-    <row r="204" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A204" s="5">
         <v>203</v>
       </c>
@@ -12084,7 +12128,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-machine-learning-proven-extensible.svg</v>
       </c>
     </row>
-    <row r="205" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A205" s="5">
         <v>204</v>
       </c>
@@ -12115,7 +12159,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-machine-learning-pipeline.svg</v>
       </c>
     </row>
-    <row r="206" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A206" s="5">
         <v>205</v>
       </c>
@@ -12146,7 +12190,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-machine-learning-for-dotnet.svg</v>
       </c>
     </row>
-    <row r="207" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A207" s="5">
         <v>206</v>
       </c>
@@ -12177,7 +12221,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-machine-learning-brain-lightbulb.svg</v>
       </c>
     </row>
-    <row r="208" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A208" s="5">
         <v>207</v>
       </c>
@@ -12208,7 +12252,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\wizard-upgrade-from-xml-to-inheritance.svg</v>
       </c>
     </row>
-    <row r="209" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A209" s="5">
         <v>208</v>
       </c>
@@ -12235,7 +12279,7 @@
         <v>{"id":208,"title":"als-confirm-vm-specs","group":"als","area":"dashboard","keywords":["azure","lab","services","vm","virtual","machine","computer","gear","magnifier"],"description":"Used in Azure Lab Services classroom scenario onboarding UI.","publish":1}</v>
       </c>
     </row>
-    <row r="210" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A210" s="5">
         <v>209</v>
       </c>
@@ -12262,7 +12306,7 @@
         <v>{"id":209,"title":"als-install-artifacts-to-vm","group":"als","area":"dashboard","keywords":["azure","lab","services","vm","virtual","machine","install","app","package","cube","box","hook"],"description":"Used in Azure Lab Services classroom scenario onboarding UI.","publish":1}</v>
       </c>
     </row>
-    <row r="211" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A211" s="5">
         <v>210</v>
       </c>
@@ -12289,7 +12333,7 @@
         <v>{"id":210,"title":"als-decide-user-count","group":"als","area":"dashboard","keywords":["azure","lab","services","vm","virtual","machine","user","count","computer"],"description":"Used in Azure Lab Services classroom scenario onboarding UI.","publish":1}</v>
       </c>
     </row>
-    <row r="212" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A212" s="5">
         <v>211</v>
       </c>
@@ -12316,7 +12360,7 @@
         <v>{"id":211,"title":"als-set-policy-schedule","group":"als","area":"dashboard","keywords":["azure","lab","services","vm","virtual","machine","schedule","time","date","calendar","usage","analytics","chart"],"description":"Used in Azure Lab Services classroom scenario onboarding UI.","publish":1}</v>
       </c>
     </row>
-    <row r="213" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A213" s="5">
         <v>212</v>
       </c>
@@ -12343,7 +12387,7 @@
         <v>{"id":212,"title":"als-publish-vm","group":"als","area":"dashboard","keywords":["azure","lab","services","vm","virtual","machine","publish","url","send","computer","paper","plane"],"description":"Used in Azure Lab Services classroom scenario onboarding UI.","publish":1}</v>
       </c>
     </row>
-    <row r="214" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A214" s="5">
         <v>213</v>
       </c>
@@ -12370,7 +12414,7 @@
         <v>{"id":213,"title":"als-get-azure-subscription","group":"als","area":"frontdoor","keywords":["azure","lab","services","sign","up","subscription"],"description":"Get an Azure subscription.","publish":1}</v>
       </c>
     </row>
-    <row r="215" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A215" s="5">
         <v>214</v>
       </c>
@@ -12397,7 +12441,7 @@
         <v>{"id":214,"title":"als-add-lab-account","group":"als","area":"frontdoor","keywords":["azure","lab","services","cloud","add","lab","beaker"],"description":"Add lab account to Azure subscription.","publish":1}</v>
       </c>
     </row>
-    <row r="216" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A216" s="5">
         <v>215</v>
       </c>
@@ -12424,7 +12468,7 @@
         <v>{"id":215,"title":"als-create-lab","group":"als","area":"frontdoor","keywords":["azure","lab","services","add","computer","beaker","create"],"description":"Create your lab of VMs.","publish":1}</v>
       </c>
     </row>
-    <row r="217" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A217" s="5">
         <v>217</v>
       </c>
@@ -12451,7 +12495,7 @@
         <v>{"id":217,"title":"swimlane-ml-load-data","group":"dotnet","area":"swimlane","keywords":["machine","learning","load","data","import","funnel","raw"],"description":"Raw data being loaded into the pipeline.","publish":1}</v>
       </c>
     </row>
-    <row r="218" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A218" s="5">
         <v>218</v>
       </c>
@@ -12478,7 +12522,7 @@
         <v>{"id":218,"title":"swimlane-ml-transform-data","group":"dotnet","area":"swimlane","keywords":["machine","learning","transform","data","output","funnel","organize"],"description":"Data is being transformed and organized.","publish":1}</v>
       </c>
     </row>
-    <row r="219" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A219" s="5">
         <v>219</v>
       </c>
@@ -12505,7 +12549,7 @@
         <v>{"id":219,"title":"swimlane-ml-choose-algorithms","group":"dotnet","area":"swimlane","keywords":["machine","learning","fit","model","algorithm","grid","data"],"description":"Choose algorithms to fit data and develop models.","publish":1}</v>
       </c>
     </row>
-    <row r="220" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A220" s="5">
         <v>220</v>
       </c>
@@ -12532,7 +12576,7 @@
         <v>{"id":220,"title":"swimlane-ml-train-model","group":"dotnet","area":"swimlane","keywords":["machine","learning","data","train","model","prediction"],"description":"Train models to make prediction.","publish":1}</v>
       </c>
     </row>
-    <row r="221" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A221" s="5">
         <v>221</v>
       </c>
@@ -12559,7 +12603,7 @@
         <v>{"id":221,"title":"swimlane-ml-evaluate-model","group":"dotnet","area":"swimlane","keywords":["machine","learning","evaluate","model","measure","magnifier"],"description":"Evaluate and validate the model.","publish":1}</v>
       </c>
     </row>
-    <row r="222" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A222" s="5">
         <v>222</v>
       </c>
@@ -12586,7 +12630,7 @@
         <v>{"id":222,"title":"swimlane-ml-deploy-model","group":"dotnet","area":"swimlane","keywords":["machine","learning","deploy","model","parachute"],"description":"Use the model in applications.","publish":1}</v>
       </c>
     </row>
-    <row r="223" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A223" s="5">
         <v>223</v>
       </c>
@@ -12613,7 +12657,7 @@
         <v>{"id":223,"title":"swimlane-functional-programming-machine","group":"dotnet","area":"swimlane","keywords":["functional","programming","machine","fx","input","output"],"description":"Input going through a machine and output comes out. Used to represent functional programming.","publish":1}</v>
       </c>
     </row>
-    <row r="224" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A224" s="5">
         <v>224</v>
       </c>
@@ -12640,7 +12684,7 @@
         <v>{"id":224,"title":"swimlane-one-consistent-api-purple","group":"dotnet","area":"swimlane","keywords":["one","api","consistent","people","tool","library","book","light","bulb","idea","ui","code"],"description":"A person surrounded by multiple developer tools.","publish":1}</v>
       </c>
     </row>
-    <row r="225" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A225" s="5">
         <v>225</v>
       </c>
@@ -12667,7 +12711,7 @@
         <v>{"id":225,"title":"swimlane-teamwork-climb-mountain","group":"dotnet","area":"swimlane","keywords":["team","people","teamwork","collaboration","climb","mountain","outdoor"],"description":"A team climbing mountain together.","publish":1}</v>
       </c>
     </row>
-    <row r="226" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A226" s="5">
         <v>226</v>
       </c>
@@ -12694,7 +12738,7 @@
         <v>{"id":226,"title":"swimlane-toolchest-with-power-drill","group":"dotnet","area":"swimlane","keywords":["tools","sdk","toolbox","toolchest","power","drill","wrench","plier"],"description":"A toolchest stuffed with tools.","publish":1}</v>
       </c>
     </row>
-    <row r="227" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A227" s="5">
         <v>227</v>
       </c>
@@ -12721,7 +12765,7 @@
         <v>{"id":227,"title":"swimlane-tools-for-all-platforms","group":"dotnet","area":"swimlane","keywords":["tools","cross","platform","people","man","mac","windows","linux"],"description":"A developer and devices running Mac, Windows and Linux platforms.","publish":1}</v>
       </c>
     </row>
-    <row r="228" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A228" s="5">
         <v>228</v>
       </c>
@@ -12748,7 +12792,7 @@
         <v>{"id":228,"title":"swimlane-welcome-to-the-community","group":"dotnet","area":"swimlane","keywords":["people","person","man","woman","community","developer","welcome","join","open","source","team","work"],"description":"Developer community working together and welcoming new memebers.","publish":1}</v>
       </c>
     </row>
-    <row r="229" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A229" s="5">
         <v>229</v>
       </c>
@@ -12775,7 +12819,7 @@
         <v>{"id":229,"title":"devblog-mobile-app-center","group":"devblog","area":"thumbnail","keywords":["mobile","development","app","center","cloud","device","phone","laptop","xamarin","visual","studio","code"],"description":"Using Visual Studio and App Center for mobile development.","publish":1}</v>
       </c>
     </row>
-    <row r="230" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A230" s="5">
         <v>230</v>
       </c>
@@ -12802,7 +12846,7 @@
         <v>{"id":230,"title":"als-lab-empty-state","group":"als","area":"zerodata","keywords":["azure","lab","vm","virtual","machine","empty","dotted","line","woman","people","question","mark","computer"],"description":"Used for Azure Lab Services empty state when there is no VM in the lab.","publish":1}</v>
       </c>
     </row>
-    <row r="231" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A231" s="5">
         <v>231</v>
       </c>
@@ -12829,7 +12873,7 @@
         <v>{"id":231,"title":"als-waiting-beaker","group":"als","area":"wizard","keywords":["azure","lab","vm","beaker","waiting"],"description":"Used for Azure Lab Services waiting screens.","publish":1}</v>
       </c>
     </row>
-    <row r="232" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A232" s="5">
         <v>232</v>
       </c>
@@ -12856,7 +12900,7 @@
         <v>{"id":232,"title":"als-take-notes","group":"als","area":"wizard","keywords":["azure","lab","vm","note","sticky","pencil","write","credential"],"description":"Used for Azure Lab Services take notes of credentials wizard.","publish":1}</v>
       </c>
     </row>
-    <row r="233" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A233" s="5">
         <v>233</v>
       </c>
@@ -12883,7 +12927,7 @@
         <v>{"id":233,"title":"devblog-debug","group":"devblog","area":"thumbnail","keywords":["debug","magnifier","bug","code"],"description":"A magnifier looking for bugs in code.","publish":1}</v>
       </c>
     </row>
-    <row r="234" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A234" s="5">
         <v>234</v>
       </c>
@@ -12910,7 +12954,7 @@
         <v>{"id":234,"title":"swimlane-try-dotnet-features","group":"dotnet","area":"swimlane","keywords":["features","javascript","github","editor","code","theme","customize","paint","color","lightbulb","woman","people"],"description":"Try .NET features GitHub integration, customizable theme and JavaScript support.","publish":1}</v>
       </c>
     </row>
-    <row r="235" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A235" s="5">
         <v>235</v>
       </c>
@@ -12937,7 +12981,7 @@
         <v>{"id":235,"title":"swimlane-customize-editor-theme","group":"dotnet","area":"swimlane","keywords":["customize","editor","paint","brush","color","theme"],"description":"Customize Try .NET editor theme.","publish":1}</v>
       </c>
     </row>
-    <row r="236" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A236" s="5">
         <v>236</v>
       </c>
@@ -12964,7 +13008,7 @@
         <v>{"id":236,"title":"swimlane-embed-github-snippet","group":"dotnet","area":"swimlane","keywords":["embed","github","snippet","code","browser"],"description":"Load GitHub gists with Try .NET to edit code in browser.","publish":1}</v>
       </c>
     </row>
-    <row r="237" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A237" s="5">
         <v>237</v>
       </c>
@@ -12991,7 +13035,7 @@
         <v>{"id":237,"title":"swimlane-feature-tree-with-people","group":"dotnet","area":"swimlane","keywords":["tree","branch","node","feature","people"],"description":"See what people are creating with Try .NET.","publish":1}</v>
       </c>
     </row>
-    <row r="238" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A238" s="5">
         <v>238</v>
       </c>
@@ -13018,7 +13062,7 @@
         <v>{"id":238,"title":"hero-azure-notebooks","group":"notebooks","area":"hero","keywords":["azure","notebooks","data","science","charts","people","lab"],"description":"An open notebook with people working on different domains of data science.","publish":1}</v>
       </c>
     </row>
-    <row r="239" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A239" s="5">
         <v>239</v>
       </c>
@@ -13045,7 +13089,7 @@
         <v>{"id":239,"title":"spot-azure-accessible-everywhere","group":"notebooks","area":"spot","keywords":["azure","globe","cloud"],"description":"Azure Cloud Services accessible from anywhere in the world.","publish":1}</v>
       </c>
     </row>
-    <row r="240" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A240" s="5">
         <v>240</v>
       </c>
@@ -13072,7 +13116,7 @@
         <v>{"id":240,"title":"spot-notebooks-languages","group":"notebooks","area":"spot","keywords":["notebooks","language"],"description":"Azure Notebooks supports multiple languages.","publish":1}</v>
       </c>
     </row>
-    <row r="241" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A241" s="5">
         <v>241</v>
       </c>
@@ -13099,7 +13143,7 @@
         <v>{"id":241,"title":"spot-scientist-developer-student","group":"notebooks","area":"spot","keywords":["people","scientist","developer","student","lab","microscope","tool","engineering","cap","education"],"description":"Use Azure Notebooks for many workspaces and scenarios.","publish":1}</v>
       </c>
     </row>
-    <row r="242" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A242" s="5">
         <v>242</v>
       </c>
@@ -13126,7 +13170,7 @@
         <v>{"id":242,"title":"swimlane-migrate-to-azure","group":"dotnet","area":"swimlane","keywords":["migrate","azure","cloud","helicopter","move","transfer"],"description":"Migrate existing .NET apps to Azure.","publish":1}</v>
       </c>
     </row>
-    <row r="243" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A243" s="5">
         <v>243</v>
       </c>
@@ -13153,7 +13197,7 @@
         <v>{"id":243,"title":"swimlane-serverless-computing","group":"dotnet","area":"swimlane","keywords":["serverless","computing","unplug","network","cloud","computer","device","laptop","desktop","pc","web"],"description":"Serverless computing with .NET","publish":1}</v>
       </c>
     </row>
-    <row r="244" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A244" s="5">
         <v>244</v>
       </c>
@@ -13180,7 +13224,7 @@
         <v>{"id":244,"title":"swimlane-web-app-tools-library","group":"dotnet","area":"swimlane","keywords":["toolbox","tool","hammer","utility","wrench","pencil","clipboard","book","library"],"description":"Blue toolbox and books.","publish":1}</v>
       </c>
     </row>
-    <row r="245" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A245" s="5">
         <v>245</v>
       </c>
@@ -13207,7 +13251,7 @@
         <v>{"id":245,"title":"swimlane-build-cloud-apps","group":"dotnet","area":"swimlane","keywords":["build","forklift","box","container","cloud","scalable","people"],"description":"Build modern scalable cloud apps with .NET","publish":1}</v>
       </c>
     </row>
-    <row r="246" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A246" s="5">
         <v>246</v>
       </c>
@@ -13234,7 +13278,7 @@
         <v>{"id":246,"title":"swimlane-docker-container-support","group":"dotnet","area":"swimlane","keywords":["docker","cloud","container","ship","port","city","skyline","computer","laptop"],"description":"Ship with containers to represent Docker containers.","publish":1}</v>
       </c>
     </row>
-    <row r="247" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A247" s="5">
         <v>247</v>
       </c>
@@ -13261,8 +13305,143 @@
         <v>{"id":247,"title":"swimlane-global-data-storage","group":"dotnet","area":"swimlane","keywords":["data","storage","database","globe","duplicate","world"],"description":"Data storage accessible from everywhere in the world.","publish":1}</v>
       </c>
     </row>
+    <row r="248" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A248" s="5">
+        <v>248</v>
+      </c>
+      <c r="C248" s="2" t="s">
+        <v>929</v>
+      </c>
+      <c r="D248" t="s">
+        <v>387</v>
+      </c>
+      <c r="E248" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F248" s="2" t="s">
+        <v>934</v>
+      </c>
+      <c r="G248" s="2" t="s">
+        <v>935</v>
+      </c>
+      <c r="H248" s="2">
+        <v>1</v>
+      </c>
+      <c r="I248" s="2" t="str">
+        <f t="shared" ref="I248:I252" si="9">SUBSTITUTE(_xlfn.CONCAT("{'id':",A248,",'title':'",C248,"','group':'",D248,"','area':'",E248,"','keywords':['",SUBSTITUTE(F248," ","','"),"'],'description':'",G248,"','publish':",H248,"}"),"'","""")</f>
+        <v>{"id":248,"title":"swimlane-security","group":"dotnet","area":"swimlane","keywords":["security","guard","camera","safe","secure"],"description":"A safety guard protecting a safe.","publish":1}</v>
+      </c>
+    </row>
+    <row r="249" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A249" s="5">
+        <v>249</v>
+      </c>
+      <c r="C249" s="2" t="s">
+        <v>930</v>
+      </c>
+      <c r="D249" t="s">
+        <v>387</v>
+      </c>
+      <c r="E249" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F249" s="2" t="s">
+        <v>936</v>
+      </c>
+      <c r="G249" s="2" t="s">
+        <v>937</v>
+      </c>
+      <c r="H249" s="2">
+        <v>1</v>
+      </c>
+      <c r="I249" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>{"id":249,"title":"swimlane-angular-react-spa","group":"dotnet","area":"swimlane","keywords":["angular","react","spa","single","page","application","website"],"description":"React and Angular logo and single page web app.","publish":1}</v>
+      </c>
+    </row>
+    <row r="250" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A250" s="5">
+        <v>250</v>
+      </c>
+      <c r="C250" s="2" t="s">
+        <v>931</v>
+      </c>
+      <c r="D250" t="s">
+        <v>387</v>
+      </c>
+      <c r="E250" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F250" s="2" t="s">
+        <v>938</v>
+      </c>
+      <c r="G250" s="2" t="s">
+        <v>939</v>
+      </c>
+      <c r="H250" s="2">
+        <v>1</v>
+      </c>
+      <c r="I250" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>{"id":250,"title":"swimlane-build-scalable-web-apps","group":"dotnet","area":"swimlane","keywords":["build","scalable","web","app","page","truck","box","people"],"description":"A worker loading boxes from truck to a web page.","publish":1}</v>
+      </c>
+    </row>
+    <row r="251" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A251" s="5">
+        <v>251</v>
+      </c>
+      <c r="C251" s="2" t="s">
+        <v>932</v>
+      </c>
+      <c r="D251" t="s">
+        <v>387</v>
+      </c>
+      <c r="E251" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F251" s="2" t="s">
+        <v>940</v>
+      </c>
+      <c r="G251" s="2" t="s">
+        <v>941</v>
+      </c>
+      <c r="H251" s="2">
+        <v>1</v>
+      </c>
+      <c r="I251" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>{"id":251,"title":"swimlane-model-view-controller","group":"dotnet","area":"swimlane","keywords":["mvc","model","view","controller","data","gear","presentation","theme","paint","bucket","brush","design","frontend","backend","stack"],"description":"MVC illustration.","publish":1}</v>
+      </c>
+    </row>
+    <row r="252" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A252" s="5">
+        <v>252</v>
+      </c>
+      <c r="C252" s="2" t="s">
+        <v>933</v>
+      </c>
+      <c r="D252" t="s">
+        <v>387</v>
+      </c>
+      <c r="E252" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F252" s="2" t="s">
+        <v>942</v>
+      </c>
+      <c r="G252" s="2" t="s">
+        <v>943</v>
+      </c>
+      <c r="H252" s="2">
+        <v>1</v>
+      </c>
+      <c r="I252" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>{"id":252,"title":"swimlane-seamless-data-integration","group":"dotnet","area":"swimlane","keywords":["data","database","orbit"],"description":"Seamless data integration.","publish":1}</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C92:C100">
+  <sortState ref="C92:C100">
     <sortCondition ref="C92"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13279,154 +13458,154 @@
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>685</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>686</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>687</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>688</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>686</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>686</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>689</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>690</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>691</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>692</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>693</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>695</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>696</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>697</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>698</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>699</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>700</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>701</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>702</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>703</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>704</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>706</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>707</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>708</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>710</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>711</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>712</v>
       </c>
@@ -13449,22 +13628,22 @@
       <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="38.140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.83984375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.83984375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="38.15625" style="2" customWidth="1"/>
     <col min="4" max="4" width="17" style="2" customWidth="1"/>
     <col min="5" max="5" width="18" style="2" customWidth="1"/>
-    <col min="6" max="6" width="33.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" style="2" customWidth="1"/>
-    <col min="8" max="9" width="24.140625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="33.140625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="66.42578125" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="2"/>
+    <col min="6" max="6" width="33.68359375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="20.68359375" style="2" customWidth="1"/>
+    <col min="8" max="9" width="24.15625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="33.15625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="66.41796875" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="9.15625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="3" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>73</v>
       </c>
@@ -13499,7 +13678,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -13533,7 +13712,7 @@
         <v>{"id":1,"title":"AzureToolsForVS","category":"VSCOM","keywords":["free","hosting","bug","tools","platforms","testing","beaker","wrench","azure","logo"],"description":"Azure developer tools for Visual Studio with free hosting.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -13567,7 +13746,7 @@
         <v>{"id":2,"title":"CloudPattern","category":"Pattern","keywords":["technology","nature","cloud","sky"],"description":"Clouds on blue sky pattern.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -13601,7 +13780,7 @@
         <v>{"id":3,"title":"CollaborationChatBubbles","category":"Diagram","keywords":["work","chat","bubble","conversation","communication","collaboration","team","men","women","people"],"description":"Several chat bubbles with people inside.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -13635,7 +13814,7 @@
         <v>{"id":4,"title":"CollaborationNetwork","category":"Diagram","keywords":["man","woman","network","hub","collaboration","connection","web","idea","lightbulb","gear","cloud","chat","bubble","work"],"description":"A network of people and objects connected together.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -13669,7 +13848,7 @@
         <v>{"id":5,"title":"CommunityTranslation1","category":"VSCOM","keywords":["hand","phone","hello","word","balloon","languages"],"description":"Translate world languages with smartphone.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -13703,7 +13882,7 @@
         <v>{"id":6,"title":"CommunityTranslation2","category":"VSCOM","keywords":["group","people","tablet","languages"],"description":"People from around the world using translation app on smart device to say hello.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -13737,7 +13916,7 @@
         <v>{"id":7,"title":"CommunityTranslation3","category":"VSCOM","keywords":["group","people","tablet","languages"],"description":"People from around the world using translation app on smart device to say hello.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -13771,7 +13950,7 @@
         <v>{"id":8,"title":"CordovaToolsTwitterBanner","category":"Web","keywords":["crane","cloud","tools","tree","build","construction"],"description":"Cordova Tools Twitter account banner. Construction crane and build tools on cloud.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -13805,7 +13984,7 @@
         <v>{"id":9,"title":"DesktopComputerPattern","category":"Pattern","keywords":["desktop","computer","monitor","pc","technology"],"description":"Desktop computer pattern.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -13839,7 +14018,7 @@
         <v>{"id":10,"title":"DevEssentials1","category":"VSCOM","keywords":["download","arrow","magnifying","glass","monitor","laptop","data","graphs","gears","newsletter"],"description":"Data visualization related elements on a cloud.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -13873,7 +14052,7 @@
         <v>{"id":11,"title":"DevEssentials2","category":"VSCOM","keywords":["download","arrow","magnifying","glass","monitor","laptop","data","graphs","gears","toolbox","newsletter"],"description":"Data visualization related elements on a cloud.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -13907,7 +14086,7 @@
         <v>{"id":12,"title":"DevicesPattern","category":"Pattern","keywords":["laptop","phone","tablet","smartphone","technology"],"description":"Mixed devices pattern.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -13941,7 +14120,7 @@
         <v>{"id":13,"title":"DevOpsLifecycle","category":"Diagram","keywords":["handshake","planning","continuous","delivery","dev","test","analytics","mobius","infinity","loop"],"description":"DevOps lifecycle.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -13975,7 +14154,7 @@
         <v>{"id":14,"title":"FeedbackCommentsDiscussion","category":"Email","keywords":["chat","bubble","question","exclaimation","conversation","discussion"],"description":"Feedback comment discussion.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -14009,7 +14188,7 @@
         <v>{"id":15,"title":"FeedbackPattern","category":"Pattern","keywords":["feedback","chat","bubble","conversation","question","exclaimation","problem","comment","talk"],"description":"Chat bubble feedback pattern.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -14043,7 +14222,7 @@
         <v>{"id":16,"title":"FoodCollection","category":"Elements","keywords":["food","meal","nutrition","soup","bread","spoon","tomato","broccli","vegetable","fish","crab","seafood","meat","poultry","steak","chicken","turkey","cake","pie","dessert","measuring","cup","egg","beater","cooking","utencils","drink","cocktail","glass","toast","cracker","cheese","burger","hotdog","salad","appetizer","entree"],"description":"A collection of food icons.","style":["color","sketchy"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -14077,7 +14256,7 @@
         <v>{"id":17,"title":"IdeaFactory","category":"Web","keywords":["factory","building","gear","lightbulb","database","arrow","document","gauge","lift","truck"],"description":"Ideas being manufactured in a factory.","style":["monotone"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -14111,7 +14290,7 @@
         <v>{"id":18,"title":"IntegratedDevelopmentLoop","category":"Email","keywords":["loop","cycle","edit","pencil","script","scroll","bug","arrow","device","phone","mobile","cloud"],"description":"Lifecycle of code, debug and deployment.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -14145,7 +14324,7 @@
         <v>{"id":19,"title":"InternetOfThings","category":"Diagram","keywords":["internet","iot","globe","router","smart","phone","laptop","light","bulb","printer","desktop","media","player","car","smart","home","smart","watch","mobile","payment","device","software","development"],"description":"The Internet of Things (IoT) is the network of physical objects or things embedded with electronics, software, sensors, and network connectivity, which enables these objects to collect and exchange data.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -14179,7 +14358,7 @@
         <v>{"id":20,"title":"ManufacturingIdeas","category":"Misc","keywords":["machine","tool","lightbulb"],"description":"Ideas being manufactured by a machine.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -14213,7 +14392,7 @@
         <v>{"id":21,"title":"MicrosoftWelcomeCenter","category":"Print","keywords":["microsoft","company","building","welcome","logo","work","business"],"description":"Microsoft logo and office buildings.","style":["color","3d"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -14247,7 +14426,7 @@
         <v>{"id":22,"title":"MobileAppDevelopmentPlatform","category":"VSCOM","keywords":["building","city","cloud","billboard","people","device","laptop","phone","database","security","lock","presentation","chart","development","platform","enterprise","business"],"description":"Mobile app development platform.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -14281,7 +14460,7 @@
         <v>{"id":23,"title":"MobileAppDevelopmentWithVisualStudio","category":"VSCOM","keywords":["laptop","phone","iphone","android","windows","app","development","visual","studio"],"description":"Cross platform mobile app development with Visual Studio.","style":["color","photo","monotone"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -14315,7 +14494,7 @@
         <v>{"id":24,"title":"MultiDeviceTwitterBanner","category":"Web","keywords":["cloud","sky","field","grass","phone","smartphone","tablet","computer","desktop","pc","monitor","tv","television","microsoft","logo","technology","developer"],"description":"Cordova Tools Twitter account banner. Four device icons overlay on top of cloud and field backgournd.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -14349,7 +14528,7 @@
         <v>{"id":25,"title":"NETCoreWebsiteBanner","category":"Web","keywords":["visual","studio","html5","css3","javascript"],"description":".NET Core website banner.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -14383,7 +14562,7 @@
         <v>{"id":26,"title":"OneToolForEverything","category":"Email","keywords":["tool","laptop","mobile","phone","cloud"],"description":"One tool for all platform.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -14417,7 +14596,7 @@
         <v>{"id":27,"title":"OpenSourceComputer","category":"Web","keywords":["laptop","code","arrow","exchange"],"description":"Two laptop exchanging code.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -14451,7 +14630,7 @@
         <v>{"id":28,"title":"OpenSourceExchangeCode","category":"Diagram","keywords":["code","man","woman","laptop","desktop","exchange","share","arrow"],"description":"Developers exchange open source code.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -14485,7 +14664,7 @@
         <v>{"id":29,"title":"PlaceholderFlowers","category":"VSTS","keywords":["flower"],"description":"Placeholder images.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -14519,7 +14698,7 @@
         <v>{"id":30,"title":"PublishAndDeploy","category":"Email","keywords":["rocket","document","arrow","exchange"],"description":"Publish and deploy code.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -14553,7 +14732,7 @@
         <v>{"id":31,"title":"PushNotifications","category":"Web","keywords":["mobile","phone","tablet","android","windows","ios","chat","bubble","notification"],"description":"Push notifications on multiple platforms.","style":["monotone"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -14587,7 +14766,7 @@
         <v>{"id":32,"title":"PythonToolsForVS","category":"VSCOM","keywords":["man","laptop","woman","gears","bug","code","phone","python","logo","magnifying","glass"],"description":"Python tools for Visual Studio.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -14621,7 +14800,7 @@
         <v>{"id":33,"title":"QuickstartFastSpeed","category":"Email","keywords":["stopwatch","run","man","time","fast","quick","speed"],"description":"Quick start","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -14655,7 +14834,7 @@
         <v>{"id":34,"title":"RocketMulticolor","category":"Elements","keywords":["rocket","launch","deployment"],"description":"Rocket","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -14689,7 +14868,7 @@
         <v>{"id":35,"title":"RocketWithCloudPattern","category":"Print","keywords":["rocket","cloud","sky"],"description":"Rocket on sky background","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -14723,7 +14902,7 @@
         <v>{"id":36,"title":"SeattlePostcard","category":"Print","keywords":["seattle","space","needle","cloud","city"],"description":"Seattle space needle postcard","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -14757,7 +14936,7 @@
         <v>{"id":37,"title":"SeattleSkyline","category":"Web","keywords":["seattle","space","needle","cloud","city","skyline","building","mount","rainier"],"description":"Seattle city skyline","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -14791,7 +14970,7 @@
         <v>{"id":38,"title":"SeattleSkylineFerrisWheel","category":"Web","keywords":["seattle","space","needle","ferris","wheel","waterfront","port"],"description":"Seattle city skyline","style":["monotone"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -14825,7 +15004,7 @@
         <v>{"id":39,"title":"SilhouetteAirportElements","category":"Elements","keywords":["airport","pilot","flight","attendant","uniform","causeway","airplane","sign","direction","loudge","coffee","terminal","seat","life"],"description":"A collection of airport related elements.","style":["silhuoette"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -14859,7 +15038,7 @@
         <v>{"id":40,"title":"SilhouetteBriefcasesAndDocuments","category":"Elements","keywords":["document","file","paper","briefcase","suitcase","handbag","work","object","business"],"description":" A collection of briefcases.","style":["silhuoette"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -14893,7 +15072,7 @@
         <v>{"id":41,"title":"SilhouetteCharacters","category":"Elements","keywords":["man","confuse","suit","woman","chair","desk","laptop","computer","office","work","business"],"description":"A collection of characters in work environment.","style":[" ","silhuoette"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -14927,7 +15106,7 @@
         <v>{"id":42,"title":"SilhouetteHandGenstures","category":"Elements","keywords":["hand","gesture","pick","grip","pinch","touch","web","press","technology"],"description":"Hand gestures.","style":["silhuoette"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -14961,7 +15140,7 @@
         <v>{"id":43,"title":"SilhouetteTabletAndPhones","category":"Elements","keywords":["technology","work","tablet","smartphone","phone","mobile","phone","pen","stylus","windows","phone","android","phone","surface","tablet"],"description":"Tablet and smartphones.","style":["silhuoette"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -14995,7 +15174,7 @@
         <v>{"id":44,"title":"SilhouetteToolCollection","category":"Pattern","keywords":["wrench","screwdriver","saw","plier","hammer","knife","c","clamp","clamp","pipe","wrench","filer","triangle","ruler","object"],"description":"A collection of hand tools.","style":["silhouette"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -15029,7 +15208,7 @@
         <v>{"id":45,"title":"SilhouetteWeatherReportElements","category":"Elements","keywords":["life","newspaper","radio","magezine","clock","news","weather","forcast","tv","sun","sunny","cloud","lightning","thunder","cloud","cloudy","rain","tripical","palm","tree","beach","table","vacation","beach","chair","hawaii","man","relax","drink"],"description":"A collection of weather related illustrations.","style":["silhuoette"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -15063,7 +15242,7 @@
         <v>{"id":46,"title":"SoftwareToolsSampleKit","category":"Email","keywords":["toolbox","hammer","checklist","wrench","cloud"],"description":"Software development toolkit","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -15097,7 +15276,7 @@
         <v>{"id":47,"title":"TeamworkStairs","category":"Web","keywords":["people","man","stairs","team"],"description":"People holding hands climbing up stairs as a team.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -15131,7 +15310,7 @@
         <v>{"id":48,"title":"Testing","category":"Email","keywords":["test","flask","lab","beaker","stopwatch","pie","chart","checklist"],"description":"Testing","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -15165,7 +15344,7 @@
         <v>{"id":49,"title":"VSBuildALMIntegration","category":"VSCOM","keywords":["people","working","man","computer","clipboard","debug","tools","gear","bug"],"description":"ALM (Application Lifecycle Management) debug integration.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -15199,7 +15378,7 @@
         <v>{"id":50,"title":"VSBuildCloudHostedTools","category":"VSCOM","keywords":["people","laptops","desk","workers","monitors","laptops","cross","platforms","linux","windows","ios"],"description":"Developers come from different platforms and technology stacks working together.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -15233,7 +15412,7 @@
         <v>{"id":51,"title":"VSBuildContinuousIntegration","category":"VSCOM","keywords":["monitor","laptop","test","tubes","gears","checkmark"],"description":"Build continuous integration cycle with cloud.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -15267,7 +15446,7 @@
         <v>{"id":52,"title":"VSBuildContinuousIntegrationWhite","category":"VSCOM","keywords":["cross","platforms","maven","git","apache","ant","junit","gradle","xunit","mtm","test","building"],"description":"Common tools and technologies for cross-platform development.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -15301,7 +15480,7 @@
         <v>{"id":53,"title":"VSBuildCrossPlatform","category":"VSCOM","keywords":["pillars","cross","platforms","buildings","crane","java",".net","xcode","github","ios","android","windows","git"],"description":"Common tools and technologies for cross-platform development.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -15335,7 +15514,7 @@
         <v>{"id":54,"title":"VSBuildOverview","category":"VSCOM","keywords":["cross","platforms","laptop","tablet","phone","ios","android","visual","studio","cloud"],"description":"Visual Studio for building cross-platform applications.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -15369,7 +15548,7 @@
         <v>{"id":55,"title":"VSBuildTraceability","category":"VSCOM","keywords":["blueprint","document","man","beaker","tools","clipboard","timeline","printer","download","test","tubes","gears","magnifying","glass","graphs"],"description":"Build timeline and tracebility.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -15403,7 +15582,7 @@
         <v>{"id":56,"title":"VSDownload1","category":"VSCOM","keywords":["group","people","visual","studio","logo","flags","man","woman"],"description":"Visual Studio for everyone.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -15437,7 +15616,7 @@
         <v>{"id":57,"title":"VSDownload2","category":"VSCOM","keywords":["man","monitors","download","down","arrow","computer","table"],"description":"Visual Studio tools for multiplatform.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -15471,308 +15650,308 @@
         <v>{"id":58,"title":"XamarinCrossPlatformDevelopment","category":"VSCOM","keywords":["screenshot","ios","android","windows","mobile","phone","app","development","shared","code","cross-platform","xamarin"],"description":"Xamarin for developing cross-platform application.","style":["color","photo"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="2">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="2">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="2">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="2">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="2">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="2">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="2">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="2">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="2">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="2">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="2">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="2">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="2">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="2">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="2">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="2">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="2">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="2">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="2">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="2">
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="2">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="2">
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="2">
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="2">
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="2">
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="2">
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="2">
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="2">
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="2">
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="2">
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="2">
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="2">
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="2">
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="2">
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="2">
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="2">
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="2">
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="2">
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="2">
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="2">
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="2">
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="2">
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="2">
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="2">
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="2">
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="2">
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="2">
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="2">
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="2">
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="2">
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="2">
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="2">
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="2">
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="2">
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="2">
         <v>114</v>
       </c>
     </row>
-    <row r="116" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="2">
         <v>115</v>
       </c>
     </row>
-    <row r="117" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" s="2">
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="2">
         <v>117</v>
       </c>
     </row>
-    <row r="119" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="2">
         <v>118</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H59">
+  <sortState ref="A2:H59">
     <sortCondition ref="C2:C59"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15802,9 +15981,9 @@
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="1" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Added new illustrations for API page
</commit_message>
<xml_diff>
--- a/src/assets/data.xlsx
+++ b/src/assets/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cherr\Dropbox\Code\vsimages\src\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\Code\vsimages\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C93A08A1-4710-461A-AD3D-49068D11FA42}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1716BF1E-4F84-4E8D-9411-14B7F1EA42AF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12318" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="5" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1656" uniqueCount="944">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1671" uniqueCount="953">
   <si>
     <t>SeattleSkyline</t>
   </si>
@@ -2868,6 +2868,33 @@
   </si>
   <si>
     <t>Seamless data integration.</t>
+  </si>
+  <si>
+    <t>swimlane-authentication-authorization</t>
+  </si>
+  <si>
+    <t>swimlane-rest-api</t>
+  </si>
+  <si>
+    <t>swimlane-secure-chat-app</t>
+  </si>
+  <si>
+    <t>authentication authorization password login key lock badge access key chain</t>
+  </si>
+  <si>
+    <t>A key chain with several authentication objects.</t>
+  </si>
+  <si>
+    <t>rest restful api json bracket data database interface connect device platform</t>
+  </si>
+  <si>
+    <t>Used to represent REST api.</t>
+  </si>
+  <si>
+    <t>lock secure chat people avatar message</t>
+  </si>
+  <si>
+    <t>An IM app with encrypted conversation.</t>
   </si>
 </sst>
 </file>
@@ -5773,31 +5800,31 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K252"/>
+  <dimension ref="A1:K255"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B248" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B251" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D249" sqref="D249"/>
+      <selection pane="bottomRight" activeCell="F257" sqref="F257"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="100" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.26171875" style="7" customWidth="1"/>
-    <col min="2" max="2" width="35.83984375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="38.15625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="35.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="38.140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
     <col min="5" max="5" width="18" style="2" customWidth="1"/>
-    <col min="6" max="6" width="33.68359375" style="2" customWidth="1"/>
-    <col min="7" max="8" width="20.68359375" style="2" customWidth="1"/>
-    <col min="9" max="10" width="24.15625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="33.15625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="66.41796875" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="9.15625" style="2"/>
+    <col min="6" max="6" width="33.7109375" style="2" customWidth="1"/>
+    <col min="7" max="8" width="20.7109375" style="2" customWidth="1"/>
+    <col min="9" max="10" width="24.140625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="33.140625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="66.42578125" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>201</v>
       </c>
@@ -5832,7 +5859,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -5866,7 +5893,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -5897,7 +5924,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\widget-you-dont-have-permission.svg</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -5928,7 +5955,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-charting-not-supported.svg</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -5959,7 +5986,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-custom-rules.svg</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -5990,7 +6017,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-get-back-to-recent-work.svg</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -6021,7 +6048,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-invalid-workitem-type.svg</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -6052,7 +6079,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-keep-an-eye-on-important-work.svg</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -6083,7 +6110,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-mention-someone.svg</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -6114,7 +6141,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-no-charts.svg</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -6145,7 +6172,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-unsaved-query.svg</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -6176,7 +6203,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-workitem-not-found.svg</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -6207,7 +6234,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-your-work-in-one-place.svg</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -6238,7 +6265,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-get-started-with-sprint.svg</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -6269,7 +6296,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-add-a-feed.svg</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -6300,7 +6327,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-connect-to-feed.svg</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -6331,7 +6358,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\general-no-results-found.svg</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -6362,7 +6389,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\hero-extend-vside.svg</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -6393,7 +6420,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-create-your-own-extension.svg</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -6424,7 +6451,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-marketplace.svg</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -6455,7 +6482,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-partner-program.svg</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -6486,7 +6513,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-what-are-extensions.svg</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -6517,7 +6544,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-add-product.svg</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -6548,7 +6575,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-configure-component-governance.svg</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -6579,7 +6606,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-release-management.svg</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -6610,7 +6637,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-this-repository-has-no-tags-yet.svg</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -6641,7 +6668,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-add-deployment-group.svg</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -6672,7 +6699,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-automate-build-definitions.svg</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -6703,7 +6730,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-choose-a-template.svg</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -6734,7 +6761,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-cloud-based-load-testing.svg</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -6765,7 +6792,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-favorites.svg</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -6796,7 +6823,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-get-everyone-on-same-page.svg</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -6827,7 +6854,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-no-plan.svg</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -6858,7 +6885,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-no-variable-groups.svg</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -6889,7 +6916,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-pull-request.svg</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -6920,7 +6947,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\hero-swiss-army-knife.svg</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -6951,7 +6978,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-all-your-code-hosted-free.svg</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -6982,7 +7009,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-any-client-any-platform.svg</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -7013,7 +7040,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-but-wait-theres-more.svg</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -7044,7 +7071,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-pricing.svg</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -7075,7 +7102,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-were-in-your-neighborhood.svg</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -7106,7 +7133,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\hero-pricing-calculator.svg</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -7137,7 +7164,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-you-have-no-organizations-yet.svg</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -7168,7 +7195,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\general-robot-errorcode-503.svg</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -7199,7 +7226,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\general-robot-error.svg</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -7230,7 +7257,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\general-robot-errorcode-400.svg</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -7261,7 +7288,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\general-robot-errorcode-401.svg</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -7292,7 +7319,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\general-robot-errorcode-403.svg</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -7323,7 +7350,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\general-robot-errorcode-404.svg</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -7354,7 +7381,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\general-robot-errorcode-500.svg</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -7385,7 +7412,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-no-assessments.svg</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -7416,7 +7443,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-initializing-test-results.svg</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -7447,7 +7474,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-no-work-scheduled.svg</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -7478,7 +7505,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-sprint-drag-n-drop.svg</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -7509,7 +7536,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-seamless-debugging-with-symbols.svg</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>55</v>
       </c>
@@ -7540,7 +7567,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-xamarin-cross-platform.svg</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>56</v>
       </c>
@@ -7571,7 +7598,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-azure-machine-learning.svg</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>57</v>
       </c>
@@ -7602,7 +7629,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-cognitive-services.svg</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>58</v>
       </c>
@@ -7633,7 +7660,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-congratulations-finished-setup.svg</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>59</v>
       </c>
@@ -7664,7 +7691,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-cross-platform.svg</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <v>60</v>
       </c>
@@ -7695,7 +7722,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-cryengine-game-development.svg</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
         <v>61</v>
       </c>
@@ -7726,7 +7753,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-developer-meetup.svg</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
         <v>62</v>
       </c>
@@ -7757,7 +7784,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-dotnet-core.svg</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
         <v>63</v>
       </c>
@@ -7788,7 +7815,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-dotnet-enterprise.svg</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
         <v>64</v>
       </c>
@@ -7819,7 +7846,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-download-target.svg</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
         <v>65</v>
       </c>
@@ -7850,7 +7877,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-enterprise-customer-stories.svg</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
         <v>66</v>
       </c>
@@ -7881,7 +7908,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-feedback-survey.svg</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
         <v>67</v>
       </c>
@@ -7912,7 +7939,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-fsharp-data-science.svg</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
         <v>68</v>
       </c>
@@ -7943,7 +7970,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-machine-learning-library.svg</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
         <v>69</v>
       </c>
@@ -7974,7 +8001,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-one-consistent-api.svg</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
         <v>70</v>
       </c>
@@ -8005,7 +8032,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-package-library.svg</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
         <v>71</v>
       </c>
@@ -8036,7 +8063,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-programming-languages.svg</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="5">
         <v>72</v>
       </c>
@@ -8067,7 +8094,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-thank-you-for-downloading.svg</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
         <v>73</v>
       </c>
@@ -8098,7 +8125,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-unity-game-development.svg</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="5">
         <v>74</v>
       </c>
@@ -8129,7 +8156,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-universal-windows-platform.svg</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="5">
         <v>75</v>
       </c>
@@ -8160,7 +8187,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-uwp-iot-core.svg</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="5">
         <v>76</v>
       </c>
@@ -8191,7 +8218,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-winform.svg</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="5">
         <v>77</v>
       </c>
@@ -8222,7 +8249,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-wpf.svg</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="5">
         <v>78</v>
       </c>
@@ -8253,7 +8280,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-xamarin.svg</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="5">
         <v>79</v>
       </c>
@@ -8284,7 +8311,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-dotnet-perf-diagram.svg</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="5">
         <v>80</v>
       </c>
@@ -8315,7 +8342,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\hero-snapshot-debugger.svg</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="5">
         <v>81</v>
       </c>
@@ -8346,7 +8373,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-collaborative-debugging.svg</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="5">
         <v>82</v>
       </c>
@@ -8377,7 +8404,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-collaborative-editing.svg</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="5">
         <v>83</v>
       </c>
@@ -8408,7 +8435,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-shared-full-context.svg</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="5">
         <v>84</v>
       </c>
@@ -8439,7 +8466,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-real-time-sharing.svg</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="5">
         <v>85</v>
       </c>
@@ -8470,7 +8497,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\blog-rocket-launch-timeline.svg</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="5">
         <v>86</v>
       </c>
@@ -8501,7 +8528,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\blog-vscode-metrics.svg</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="5">
         <v>87</v>
       </c>
@@ -8532,7 +8559,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\blog-vscode-roadmap.svg</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="5">
         <v>88</v>
       </c>
@@ -8563,7 +8590,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-monogame-game-development.svg</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="5">
         <v>89</v>
       </c>
@@ -8594,7 +8621,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-you-have-no-project.svg</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="5">
         <v>90</v>
       </c>
@@ -8625,7 +8652,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\hero-vsts-join-our-team.svg</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="5">
         <v>91</v>
       </c>
@@ -8656,7 +8683,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\elements-devices-1.svg</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="5">
         <v>92</v>
       </c>
@@ -8687,7 +8714,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\elements-devices-2.svg</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="5">
         <v>93</v>
       </c>
@@ -8718,7 +8745,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\elements-robots-1.svg</v>
       </c>
     </row>
-    <row r="95" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="5">
         <v>94</v>
       </c>
@@ -8749,7 +8776,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\elements-robots-2.svg</v>
       </c>
     </row>
-    <row r="96" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="5">
         <v>95</v>
       </c>
@@ -8780,7 +8807,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\elements-tools-1.svg</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="5">
         <v>96</v>
       </c>
@@ -8811,7 +8838,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\elements-tools-2.svg</v>
       </c>
     </row>
-    <row r="98" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="5">
         <v>97</v>
       </c>
@@ -8842,7 +8869,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\elements-vehicles-1.svg</v>
       </c>
     </row>
-    <row r="99" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="5">
         <v>98</v>
       </c>
@@ -8873,7 +8900,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\elements-vehicles-2.svg</v>
       </c>
     </row>
-    <row r="100" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="5">
         <v>99</v>
       </c>
@@ -8904,7 +8931,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\elements-vehicles-3.svg</v>
       </c>
     </row>
-    <row r="101" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="5">
         <v>100</v>
       </c>
@@ -8935,7 +8962,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-verify-analytics-views.svg</v>
       </c>
     </row>
-    <row r="102" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="5">
         <v>101</v>
       </c>
@@ -8966,7 +8993,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-analytics-views-error.svg</v>
       </c>
     </row>
-    <row r="103" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="5">
         <v>102</v>
       </c>
@@ -8997,7 +9024,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-analytics-views-valid.svg</v>
       </c>
     </row>
-    <row r="104" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="5">
         <v>103</v>
       </c>
@@ -9028,7 +9055,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-no-analytics-views.svg</v>
       </c>
     </row>
-    <row r="105" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="5">
         <v>104</v>
       </c>
@@ -9059,7 +9086,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-preparing-data.svg</v>
       </c>
     </row>
-    <row r="106" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="5">
         <v>105</v>
       </c>
@@ -9090,7 +9117,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\socialmedia-devops-youtube-header.svg</v>
       </c>
     </row>
-    <row r="107" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="5">
         <v>106</v>
       </c>
@@ -9121,7 +9148,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\socialmedia-devops-avatar.svg</v>
       </c>
     </row>
-    <row r="108" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="5">
         <v>107</v>
       </c>
@@ -9152,7 +9179,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\tile-self-hosted-server.svg</v>
       </c>
     </row>
-    <row r="109" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="5">
         <v>108</v>
       </c>
@@ -9183,7 +9210,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\tile-cloud-hosted-server.svg</v>
       </c>
     </row>
-    <row r="110" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="5">
         <v>109</v>
       </c>
@@ -9214,7 +9241,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\tile-integrate-with-cloud-services.svg</v>
       </c>
     </row>
-    <row r="111" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="5">
         <v>110</v>
       </c>
@@ -9245,7 +9272,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\general-folder.svg</v>
       </c>
     </row>
-    <row r="112" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="5">
         <v>111</v>
       </c>
@@ -9276,7 +9303,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-speed-gauge-comparison.svg</v>
       </c>
     </row>
-    <row r="113" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="5">
         <v>112</v>
       </c>
@@ -9307,7 +9334,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-speed-gauge-comparison-withtext.svg</v>
       </c>
     </row>
-    <row r="114" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="5">
         <v>113</v>
       </c>
@@ -9338,7 +9365,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-vside-lightbulb-intellisense.svg</v>
       </c>
     </row>
-    <row r="115" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="5">
         <v>114</v>
       </c>
@@ -9369,7 +9396,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-async-await-runners.svg</v>
       </c>
     </row>
-    <row r="116" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="5">
         <v>115</v>
       </c>
@@ -9400,7 +9427,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-barchart-skyline.svg</v>
       </c>
     </row>
-    <row r="117" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="5">
         <v>116</v>
       </c>
@@ -9431,7 +9458,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-barchart-skyline-withtext.svg</v>
       </c>
     </row>
-    <row r="118" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="5">
         <v>117</v>
       </c>
@@ -9462,7 +9489,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-contributors-around-world.svg</v>
       </c>
     </row>
-    <row r="119" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="5">
         <v>118</v>
       </c>
@@ -9493,7 +9520,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-contributors-around-world-withtext.svg</v>
       </c>
     </row>
-    <row r="120" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="5">
         <v>119</v>
       </c>
@@ -9524,7 +9551,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-dotnet-node-table.svg</v>
       </c>
     </row>
-    <row r="121" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="5">
         <v>120</v>
       </c>
@@ -9555,7 +9582,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-one-vs-many-tools.svg</v>
       </c>
     </row>
-    <row r="122" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="5">
         <v>121</v>
       </c>
@@ -9586,7 +9613,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-any-language.svg</v>
       </c>
     </row>
-    <row r="123" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="5">
         <v>122</v>
       </c>
@@ -9617,7 +9644,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-deploy-cross-platform.svg</v>
       </c>
     </row>
-    <row r="124" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="5">
         <v>123</v>
       </c>
@@ -9648,7 +9675,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-swiss-army-knife.svg</v>
       </c>
     </row>
-    <row r="125" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="5">
         <v>124</v>
       </c>
@@ -9679,7 +9706,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\hero-devops-conductor.svg</v>
       </c>
     </row>
-    <row r="126" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="5">
         <v>125</v>
       </c>
@@ -9710,7 +9737,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\blog-package-upstream-diagram-1.svg</v>
       </c>
     </row>
-    <row r="127" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="5">
         <v>126</v>
       </c>
@@ -9741,7 +9768,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\blog-package-upstream-diagram-2.svg</v>
       </c>
     </row>
-    <row r="128" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="5">
         <v>127</v>
       </c>
@@ -9772,7 +9799,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\blog-package-upstream-diagram-3.svg</v>
       </c>
     </row>
-    <row r="129" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="5">
         <v>128</v>
       </c>
@@ -9803,7 +9830,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\blog-package-upstream-diagram-4.svg</v>
       </c>
     </row>
-    <row r="130" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="5">
         <v>129</v>
       </c>
@@ -9834,7 +9861,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\willow-car-racing-get-ready.svg</v>
       </c>
     </row>
-    <row r="131" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="5">
         <v>130</v>
       </c>
@@ -9865,7 +9892,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\willow-rocket-get-ready.svg</v>
       </c>
     </row>
-    <row r="132" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="5">
         <v>131</v>
       </c>
@@ -9896,7 +9923,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\willow-bike-adventure.svg</v>
       </c>
     </row>
-    <row r="133" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="5">
         <v>132</v>
       </c>
@@ -9927,7 +9954,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\willow-bike-adventure-issue.svg</v>
       </c>
     </row>
-    <row r="134" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="5">
         <v>133</v>
       </c>
@@ -9958,7 +9985,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-no-dashboard.svg</v>
       </c>
     </row>
-    <row r="135" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="5">
         <v>134</v>
       </c>
@@ -9989,7 +10016,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\docs-gvfs-architecture.svg</v>
       </c>
     </row>
-    <row r="136" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="5">
         <v>135</v>
       </c>
@@ -10020,7 +10047,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\hero-vs-tools-for-azure.svg</v>
       </c>
     </row>
-    <row r="137" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="5">
         <v>136</v>
       </c>
@@ -10051,7 +10078,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-build-release-pipeline.svg</v>
       </c>
     </row>
-    <row r="138" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="5">
         <v>137</v>
       </c>
@@ -10082,7 +10109,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-build-release-monitor-activities.svg</v>
       </c>
     </row>
-    <row r="139" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="5">
         <v>138</v>
       </c>
@@ -10113,7 +10140,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-data-009.svg</v>
       </c>
     </row>
-    <row r="140" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="5">
         <v>139</v>
       </c>
@@ -10144,7 +10171,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-agriculture-001.svg</v>
       </c>
     </row>
-    <row r="141" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="5">
         <v>140</v>
       </c>
@@ -10175,7 +10202,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-001.svg</v>
       </c>
     </row>
-    <row r="142" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="5">
         <v>141</v>
       </c>
@@ -10206,7 +10233,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-002.svg</v>
       </c>
     </row>
-    <row r="143" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="5">
         <v>142</v>
       </c>
@@ -10237,7 +10264,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-003.svg</v>
       </c>
     </row>
-    <row r="144" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="5">
         <v>143</v>
       </c>
@@ -10268,7 +10295,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-004.svg</v>
       </c>
     </row>
-    <row r="145" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="145" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="5">
         <v>144</v>
       </c>
@@ -10299,7 +10326,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-005.svg</v>
       </c>
     </row>
-    <row r="146" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="146" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="5">
         <v>145</v>
       </c>
@@ -10330,7 +10357,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-006.svg</v>
       </c>
     </row>
-    <row r="147" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="147" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="5">
         <v>146</v>
       </c>
@@ -10361,7 +10388,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-007.svg</v>
       </c>
     </row>
-    <row r="148" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="148" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="5">
         <v>147</v>
       </c>
@@ -10392,7 +10419,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-008.svg</v>
       </c>
     </row>
-    <row r="149" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="149" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="5">
         <v>148</v>
       </c>
@@ -10423,7 +10450,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-009.svg</v>
       </c>
     </row>
-    <row r="150" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="150" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="5">
         <v>149</v>
       </c>
@@ -10454,7 +10481,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-010.svg</v>
       </c>
     </row>
-    <row r="151" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="151" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="5">
         <v>150</v>
       </c>
@@ -10485,7 +10512,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-011.svg</v>
       </c>
     </row>
-    <row r="152" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="152" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="5">
         <v>151</v>
       </c>
@@ -10516,7 +10543,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-012.svg</v>
       </c>
     </row>
-    <row r="153" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="153" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="5">
         <v>152</v>
       </c>
@@ -10547,7 +10574,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-013.svg</v>
       </c>
     </row>
-    <row r="154" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="154" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="5">
         <v>153</v>
       </c>
@@ -10578,7 +10605,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-014.svg</v>
       </c>
     </row>
-    <row r="155" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="155" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="5">
         <v>154</v>
       </c>
@@ -10609,7 +10636,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-015.svg</v>
       </c>
     </row>
-    <row r="156" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="156" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="5">
         <v>155</v>
       </c>
@@ -10640,7 +10667,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-016.svg</v>
       </c>
     </row>
-    <row r="157" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="157" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="5">
         <v>156</v>
       </c>
@@ -10671,7 +10698,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-017.svg</v>
       </c>
     </row>
-    <row r="158" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="158" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="5">
         <v>157</v>
       </c>
@@ -10702,7 +10729,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-001.svg</v>
       </c>
     </row>
-    <row r="159" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="159" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="5">
         <v>158</v>
       </c>
@@ -10733,7 +10760,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-002.svg</v>
       </c>
     </row>
-    <row r="160" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="160" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="5">
         <v>159</v>
       </c>
@@ -10764,7 +10791,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-003.svg</v>
       </c>
     </row>
-    <row r="161" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="161" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="5">
         <v>160</v>
       </c>
@@ -10795,7 +10822,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-004.svg</v>
       </c>
     </row>
-    <row r="162" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="162" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="5">
         <v>161</v>
       </c>
@@ -10826,7 +10853,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-005.svg</v>
       </c>
     </row>
-    <row r="163" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="163" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="5">
         <v>162</v>
       </c>
@@ -10857,7 +10884,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-006.svg</v>
       </c>
     </row>
-    <row r="164" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="164" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="5">
         <v>163</v>
       </c>
@@ -10888,7 +10915,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-007.svg</v>
       </c>
     </row>
-    <row r="165" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="165" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="5">
         <v>164</v>
       </c>
@@ -10919,7 +10946,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-008.svg</v>
       </c>
     </row>
-    <row r="166" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="166" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="5">
         <v>165</v>
       </c>
@@ -10950,7 +10977,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-009.svg</v>
       </c>
     </row>
-    <row r="167" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="167" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="5">
         <v>166</v>
       </c>
@@ -10981,7 +11008,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-010.svg</v>
       </c>
     </row>
-    <row r="168" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="168" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="5">
         <v>167</v>
       </c>
@@ -11012,7 +11039,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-011.svg</v>
       </c>
     </row>
-    <row r="169" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="169" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="5">
         <v>168</v>
       </c>
@@ -11043,7 +11070,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-012.svg</v>
       </c>
     </row>
-    <row r="170" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="170" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="5">
         <v>169</v>
       </c>
@@ -11074,7 +11101,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-013.svg</v>
       </c>
     </row>
-    <row r="171" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="171" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="5">
         <v>170</v>
       </c>
@@ -11105,7 +11132,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-collaboration-001.svg</v>
       </c>
     </row>
-    <row r="172" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="172" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="5">
         <v>171</v>
       </c>
@@ -11136,7 +11163,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-collaboration-002.svg</v>
       </c>
     </row>
-    <row r="173" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="173" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="5">
         <v>172</v>
       </c>
@@ -11167,7 +11194,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-collaboration-003.svg</v>
       </c>
     </row>
-    <row r="174" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="174" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="5">
         <v>173</v>
       </c>
@@ -11198,7 +11225,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-collaboration-005.svg</v>
       </c>
     </row>
-    <row r="175" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="175" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="5">
         <v>174</v>
       </c>
@@ -11229,7 +11256,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-collaboration-006.svg</v>
       </c>
     </row>
-    <row r="176" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="176" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="5">
         <v>175</v>
       </c>
@@ -11260,7 +11287,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-collaboration-007.svg</v>
       </c>
     </row>
-    <row r="177" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="177" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="5">
         <v>176</v>
       </c>
@@ -11291,7 +11318,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-collaboration-008.svg</v>
       </c>
     </row>
-    <row r="178" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="178" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="5">
         <v>177</v>
       </c>
@@ -11322,7 +11349,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-collaboration-009.svg</v>
       </c>
     </row>
-    <row r="179" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="179" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="5">
         <v>178</v>
       </c>
@@ -11353,7 +11380,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-collaboration-010.svg</v>
       </c>
     </row>
-    <row r="180" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="180" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="5">
         <v>179</v>
       </c>
@@ -11384,7 +11411,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-collaboration-011.svg</v>
       </c>
     </row>
-    <row r="181" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="181" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="5">
         <v>180</v>
       </c>
@@ -11415,7 +11442,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-communication-001.svg</v>
       </c>
     </row>
-    <row r="182" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="182" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="5">
         <v>181</v>
       </c>
@@ -11446,7 +11473,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-communication-002.svg</v>
       </c>
     </row>
-    <row r="183" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="183" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="5">
         <v>182</v>
       </c>
@@ -11477,7 +11504,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-consumer-001.svg</v>
       </c>
     </row>
-    <row r="184" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="184" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="5">
         <v>183</v>
       </c>
@@ -11508,7 +11535,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-consumer-002.svg</v>
       </c>
     </row>
-    <row r="185" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="185" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="5">
         <v>184</v>
       </c>
@@ -11539,7 +11566,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-data-001.svg</v>
       </c>
     </row>
-    <row r="186" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="186" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="5">
         <v>185</v>
       </c>
@@ -11570,7 +11597,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-data-002.svg</v>
       </c>
     </row>
-    <row r="187" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="187" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="5">
         <v>186</v>
       </c>
@@ -11601,7 +11628,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-data-003.svg</v>
       </c>
     </row>
-    <row r="188" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="188" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="5">
         <v>187</v>
       </c>
@@ -11632,7 +11659,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-data-004.svg</v>
       </c>
     </row>
-    <row r="189" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="189" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="5">
         <v>188</v>
       </c>
@@ -11663,7 +11690,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-data-005.svg</v>
       </c>
     </row>
-    <row r="190" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="190" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="5">
         <v>189</v>
       </c>
@@ -11694,7 +11721,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-data-006.svg</v>
       </c>
     </row>
-    <row r="191" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="191" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="5">
         <v>190</v>
       </c>
@@ -11725,7 +11752,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-data-007.svg</v>
       </c>
     </row>
-    <row r="192" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="192" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="5">
         <v>191</v>
       </c>
@@ -11756,7 +11783,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-data-008.svg</v>
       </c>
     </row>
-    <row r="193" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="193" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="5">
         <v>192</v>
       </c>
@@ -11787,7 +11814,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-feature-not-configured.svg</v>
       </c>
     </row>
-    <row r="194" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="194" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="5">
         <v>193</v>
       </c>
@@ -11818,7 +11845,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-boxes-and-devices.svg</v>
       </c>
     </row>
-    <row r="195" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="195" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="5">
         <v>194</v>
       </c>
@@ -11849,7 +11876,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-butler-ide.svg</v>
       </c>
     </row>
-    <row r="196" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="196" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="5">
         <v>195</v>
       </c>
@@ -11880,7 +11907,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-code-or-gui.svg</v>
       </c>
     </row>
-    <row r="197" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="197" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="5">
         <v>196</v>
       </c>
@@ -11911,7 +11938,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-data-analytics-pipeline.svg</v>
       </c>
     </row>
-    <row r="198" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="198" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="5">
         <v>197</v>
       </c>
@@ -11942,7 +11969,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-developer-scenarios.svg</v>
       </c>
     </row>
-    <row r="199" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="199" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="5">
         <v>198</v>
       </c>
@@ -11973,7 +12000,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-machine-learning-books-lab.svg</v>
       </c>
     </row>
-    <row r="200" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="200" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="5">
         <v>199</v>
       </c>
@@ -12004,7 +12031,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-machine-learning-extensible.svg</v>
       </c>
     </row>
-    <row r="201" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="201" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="5">
         <v>200</v>
       </c>
@@ -12035,7 +12062,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-machine-learning-lightbulb-hand.svg</v>
       </c>
     </row>
-    <row r="202" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="202" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="5">
         <v>201</v>
       </c>
@@ -12066,7 +12093,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-necessary-learner-tools.svg</v>
       </c>
     </row>
-    <row r="203" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="203" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="5">
         <v>202</v>
       </c>
@@ -12097,7 +12124,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-share-code-snippets.svg</v>
       </c>
     </row>
-    <row r="204" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="204" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="5">
         <v>203</v>
       </c>
@@ -12128,7 +12155,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-machine-learning-proven-extensible.svg</v>
       </c>
     </row>
-    <row r="205" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="205" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="5">
         <v>204</v>
       </c>
@@ -12159,7 +12186,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-machine-learning-pipeline.svg</v>
       </c>
     </row>
-    <row r="206" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="206" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="5">
         <v>205</v>
       </c>
@@ -12190,7 +12217,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-machine-learning-for-dotnet.svg</v>
       </c>
     </row>
-    <row r="207" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="207" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="5">
         <v>206</v>
       </c>
@@ -12221,7 +12248,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-machine-learning-brain-lightbulb.svg</v>
       </c>
     </row>
-    <row r="208" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="208" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="5">
         <v>207</v>
       </c>
@@ -12252,7 +12279,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\wizard-upgrade-from-xml-to-inheritance.svg</v>
       </c>
     </row>
-    <row r="209" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="209" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="5">
         <v>208</v>
       </c>
@@ -12279,7 +12306,7 @@
         <v>{"id":208,"title":"als-confirm-vm-specs","group":"als","area":"dashboard","keywords":["azure","lab","services","vm","virtual","machine","computer","gear","magnifier"],"description":"Used in Azure Lab Services classroom scenario onboarding UI.","publish":1}</v>
       </c>
     </row>
-    <row r="210" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="210" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="5">
         <v>209</v>
       </c>
@@ -12306,7 +12333,7 @@
         <v>{"id":209,"title":"als-install-artifacts-to-vm","group":"als","area":"dashboard","keywords":["azure","lab","services","vm","virtual","machine","install","app","package","cube","box","hook"],"description":"Used in Azure Lab Services classroom scenario onboarding UI.","publish":1}</v>
       </c>
     </row>
-    <row r="211" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="211" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="5">
         <v>210</v>
       </c>
@@ -12333,7 +12360,7 @@
         <v>{"id":210,"title":"als-decide-user-count","group":"als","area":"dashboard","keywords":["azure","lab","services","vm","virtual","machine","user","count","computer"],"description":"Used in Azure Lab Services classroom scenario onboarding UI.","publish":1}</v>
       </c>
     </row>
-    <row r="212" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="212" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="5">
         <v>211</v>
       </c>
@@ -12360,7 +12387,7 @@
         <v>{"id":211,"title":"als-set-policy-schedule","group":"als","area":"dashboard","keywords":["azure","lab","services","vm","virtual","machine","schedule","time","date","calendar","usage","analytics","chart"],"description":"Used in Azure Lab Services classroom scenario onboarding UI.","publish":1}</v>
       </c>
     </row>
-    <row r="213" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="213" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="5">
         <v>212</v>
       </c>
@@ -12387,7 +12414,7 @@
         <v>{"id":212,"title":"als-publish-vm","group":"als","area":"dashboard","keywords":["azure","lab","services","vm","virtual","machine","publish","url","send","computer","paper","plane"],"description":"Used in Azure Lab Services classroom scenario onboarding UI.","publish":1}</v>
       </c>
     </row>
-    <row r="214" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="214" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="5">
         <v>213</v>
       </c>
@@ -12414,7 +12441,7 @@
         <v>{"id":213,"title":"als-get-azure-subscription","group":"als","area":"frontdoor","keywords":["azure","lab","services","sign","up","subscription"],"description":"Get an Azure subscription.","publish":1}</v>
       </c>
     </row>
-    <row r="215" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="215" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="5">
         <v>214</v>
       </c>
@@ -12441,7 +12468,7 @@
         <v>{"id":214,"title":"als-add-lab-account","group":"als","area":"frontdoor","keywords":["azure","lab","services","cloud","add","lab","beaker"],"description":"Add lab account to Azure subscription.","publish":1}</v>
       </c>
     </row>
-    <row r="216" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="216" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="5">
         <v>215</v>
       </c>
@@ -12468,7 +12495,7 @@
         <v>{"id":215,"title":"als-create-lab","group":"als","area":"frontdoor","keywords":["azure","lab","services","add","computer","beaker","create"],"description":"Create your lab of VMs.","publish":1}</v>
       </c>
     </row>
-    <row r="217" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="217" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="5">
         <v>217</v>
       </c>
@@ -12495,7 +12522,7 @@
         <v>{"id":217,"title":"swimlane-ml-load-data","group":"dotnet","area":"swimlane","keywords":["machine","learning","load","data","import","funnel","raw"],"description":"Raw data being loaded into the pipeline.","publish":1}</v>
       </c>
     </row>
-    <row r="218" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="218" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="5">
         <v>218</v>
       </c>
@@ -12522,7 +12549,7 @@
         <v>{"id":218,"title":"swimlane-ml-transform-data","group":"dotnet","area":"swimlane","keywords":["machine","learning","transform","data","output","funnel","organize"],"description":"Data is being transformed and organized.","publish":1}</v>
       </c>
     </row>
-    <row r="219" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="219" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="5">
         <v>219</v>
       </c>
@@ -12549,7 +12576,7 @@
         <v>{"id":219,"title":"swimlane-ml-choose-algorithms","group":"dotnet","area":"swimlane","keywords":["machine","learning","fit","model","algorithm","grid","data"],"description":"Choose algorithms to fit data and develop models.","publish":1}</v>
       </c>
     </row>
-    <row r="220" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="220" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="5">
         <v>220</v>
       </c>
@@ -12576,7 +12603,7 @@
         <v>{"id":220,"title":"swimlane-ml-train-model","group":"dotnet","area":"swimlane","keywords":["machine","learning","data","train","model","prediction"],"description":"Train models to make prediction.","publish":1}</v>
       </c>
     </row>
-    <row r="221" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="221" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="5">
         <v>221</v>
       </c>
@@ -12603,7 +12630,7 @@
         <v>{"id":221,"title":"swimlane-ml-evaluate-model","group":"dotnet","area":"swimlane","keywords":["machine","learning","evaluate","model","measure","magnifier"],"description":"Evaluate and validate the model.","publish":1}</v>
       </c>
     </row>
-    <row r="222" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="222" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="5">
         <v>222</v>
       </c>
@@ -12630,7 +12657,7 @@
         <v>{"id":222,"title":"swimlane-ml-deploy-model","group":"dotnet","area":"swimlane","keywords":["machine","learning","deploy","model","parachute"],"description":"Use the model in applications.","publish":1}</v>
       </c>
     </row>
-    <row r="223" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="223" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="5">
         <v>223</v>
       </c>
@@ -12657,7 +12684,7 @@
         <v>{"id":223,"title":"swimlane-functional-programming-machine","group":"dotnet","area":"swimlane","keywords":["functional","programming","machine","fx","input","output"],"description":"Input going through a machine and output comes out. Used to represent functional programming.","publish":1}</v>
       </c>
     </row>
-    <row r="224" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="224" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="5">
         <v>224</v>
       </c>
@@ -12684,7 +12711,7 @@
         <v>{"id":224,"title":"swimlane-one-consistent-api-purple","group":"dotnet","area":"swimlane","keywords":["one","api","consistent","people","tool","library","book","light","bulb","idea","ui","code"],"description":"A person surrounded by multiple developer tools.","publish":1}</v>
       </c>
     </row>
-    <row r="225" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="225" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="5">
         <v>225</v>
       </c>
@@ -12711,7 +12738,7 @@
         <v>{"id":225,"title":"swimlane-teamwork-climb-mountain","group":"dotnet","area":"swimlane","keywords":["team","people","teamwork","collaboration","climb","mountain","outdoor"],"description":"A team climbing mountain together.","publish":1}</v>
       </c>
     </row>
-    <row r="226" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="226" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="5">
         <v>226</v>
       </c>
@@ -12738,7 +12765,7 @@
         <v>{"id":226,"title":"swimlane-toolchest-with-power-drill","group":"dotnet","area":"swimlane","keywords":["tools","sdk","toolbox","toolchest","power","drill","wrench","plier"],"description":"A toolchest stuffed with tools.","publish":1}</v>
       </c>
     </row>
-    <row r="227" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="227" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="5">
         <v>227</v>
       </c>
@@ -12765,7 +12792,7 @@
         <v>{"id":227,"title":"swimlane-tools-for-all-platforms","group":"dotnet","area":"swimlane","keywords":["tools","cross","platform","people","man","mac","windows","linux"],"description":"A developer and devices running Mac, Windows and Linux platforms.","publish":1}</v>
       </c>
     </row>
-    <row r="228" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="228" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="5">
         <v>228</v>
       </c>
@@ -12792,7 +12819,7 @@
         <v>{"id":228,"title":"swimlane-welcome-to-the-community","group":"dotnet","area":"swimlane","keywords":["people","person","man","woman","community","developer","welcome","join","open","source","team","work"],"description":"Developer community working together and welcoming new memebers.","publish":1}</v>
       </c>
     </row>
-    <row r="229" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="229" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="5">
         <v>229</v>
       </c>
@@ -12819,7 +12846,7 @@
         <v>{"id":229,"title":"devblog-mobile-app-center","group":"devblog","area":"thumbnail","keywords":["mobile","development","app","center","cloud","device","phone","laptop","xamarin","visual","studio","code"],"description":"Using Visual Studio and App Center for mobile development.","publish":1}</v>
       </c>
     </row>
-    <row r="230" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="230" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="5">
         <v>230</v>
       </c>
@@ -12846,7 +12873,7 @@
         <v>{"id":230,"title":"als-lab-empty-state","group":"als","area":"zerodata","keywords":["azure","lab","vm","virtual","machine","empty","dotted","line","woman","people","question","mark","computer"],"description":"Used for Azure Lab Services empty state when there is no VM in the lab.","publish":1}</v>
       </c>
     </row>
-    <row r="231" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="231" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="5">
         <v>231</v>
       </c>
@@ -12873,7 +12900,7 @@
         <v>{"id":231,"title":"als-waiting-beaker","group":"als","area":"wizard","keywords":["azure","lab","vm","beaker","waiting"],"description":"Used for Azure Lab Services waiting screens.","publish":1}</v>
       </c>
     </row>
-    <row r="232" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="232" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="5">
         <v>232</v>
       </c>
@@ -12900,7 +12927,7 @@
         <v>{"id":232,"title":"als-take-notes","group":"als","area":"wizard","keywords":["azure","lab","vm","note","sticky","pencil","write","credential"],"description":"Used for Azure Lab Services take notes of credentials wizard.","publish":1}</v>
       </c>
     </row>
-    <row r="233" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="233" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="5">
         <v>233</v>
       </c>
@@ -12927,7 +12954,7 @@
         <v>{"id":233,"title":"devblog-debug","group":"devblog","area":"thumbnail","keywords":["debug","magnifier","bug","code"],"description":"A magnifier looking for bugs in code.","publish":1}</v>
       </c>
     </row>
-    <row r="234" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="234" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="5">
         <v>234</v>
       </c>
@@ -12954,7 +12981,7 @@
         <v>{"id":234,"title":"swimlane-try-dotnet-features","group":"dotnet","area":"swimlane","keywords":["features","javascript","github","editor","code","theme","customize","paint","color","lightbulb","woman","people"],"description":"Try .NET features GitHub integration, customizable theme and JavaScript support.","publish":1}</v>
       </c>
     </row>
-    <row r="235" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="235" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="5">
         <v>235</v>
       </c>
@@ -12981,7 +13008,7 @@
         <v>{"id":235,"title":"swimlane-customize-editor-theme","group":"dotnet","area":"swimlane","keywords":["customize","editor","paint","brush","color","theme"],"description":"Customize Try .NET editor theme.","publish":1}</v>
       </c>
     </row>
-    <row r="236" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="236" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="5">
         <v>236</v>
       </c>
@@ -13008,7 +13035,7 @@
         <v>{"id":236,"title":"swimlane-embed-github-snippet","group":"dotnet","area":"swimlane","keywords":["embed","github","snippet","code","browser"],"description":"Load GitHub gists with Try .NET to edit code in browser.","publish":1}</v>
       </c>
     </row>
-    <row r="237" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="237" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="5">
         <v>237</v>
       </c>
@@ -13035,7 +13062,7 @@
         <v>{"id":237,"title":"swimlane-feature-tree-with-people","group":"dotnet","area":"swimlane","keywords":["tree","branch","node","feature","people"],"description":"See what people are creating with Try .NET.","publish":1}</v>
       </c>
     </row>
-    <row r="238" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="238" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" s="5">
         <v>238</v>
       </c>
@@ -13062,7 +13089,7 @@
         <v>{"id":238,"title":"hero-azure-notebooks","group":"notebooks","area":"hero","keywords":["azure","notebooks","data","science","charts","people","lab"],"description":"An open notebook with people working on different domains of data science.","publish":1}</v>
       </c>
     </row>
-    <row r="239" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="239" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="5">
         <v>239</v>
       </c>
@@ -13089,7 +13116,7 @@
         <v>{"id":239,"title":"spot-azure-accessible-everywhere","group":"notebooks","area":"spot","keywords":["azure","globe","cloud"],"description":"Azure Cloud Services accessible from anywhere in the world.","publish":1}</v>
       </c>
     </row>
-    <row r="240" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="240" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="5">
         <v>240</v>
       </c>
@@ -13116,7 +13143,7 @@
         <v>{"id":240,"title":"spot-notebooks-languages","group":"notebooks","area":"spot","keywords":["notebooks","language"],"description":"Azure Notebooks supports multiple languages.","publish":1}</v>
       </c>
     </row>
-    <row r="241" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="241" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="5">
         <v>241</v>
       </c>
@@ -13143,7 +13170,7 @@
         <v>{"id":241,"title":"spot-scientist-developer-student","group":"notebooks","area":"spot","keywords":["people","scientist","developer","student","lab","microscope","tool","engineering","cap","education"],"description":"Use Azure Notebooks for many workspaces and scenarios.","publish":1}</v>
       </c>
     </row>
-    <row r="242" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="242" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242" s="5">
         <v>242</v>
       </c>
@@ -13170,7 +13197,7 @@
         <v>{"id":242,"title":"swimlane-migrate-to-azure","group":"dotnet","area":"swimlane","keywords":["migrate","azure","cloud","helicopter","move","transfer"],"description":"Migrate existing .NET apps to Azure.","publish":1}</v>
       </c>
     </row>
-    <row r="243" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="243" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="5">
         <v>243</v>
       </c>
@@ -13197,7 +13224,7 @@
         <v>{"id":243,"title":"swimlane-serverless-computing","group":"dotnet","area":"swimlane","keywords":["serverless","computing","unplug","network","cloud","computer","device","laptop","desktop","pc","web"],"description":"Serverless computing with .NET","publish":1}</v>
       </c>
     </row>
-    <row r="244" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="244" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244" s="5">
         <v>244</v>
       </c>
@@ -13224,7 +13251,7 @@
         <v>{"id":244,"title":"swimlane-web-app-tools-library","group":"dotnet","area":"swimlane","keywords":["toolbox","tool","hammer","utility","wrench","pencil","clipboard","book","library"],"description":"Blue toolbox and books.","publish":1}</v>
       </c>
     </row>
-    <row r="245" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="245" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="5">
         <v>245</v>
       </c>
@@ -13251,7 +13278,7 @@
         <v>{"id":245,"title":"swimlane-build-cloud-apps","group":"dotnet","area":"swimlane","keywords":["build","forklift","box","container","cloud","scalable","people"],"description":"Build modern scalable cloud apps with .NET","publish":1}</v>
       </c>
     </row>
-    <row r="246" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="246" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="5">
         <v>246</v>
       </c>
@@ -13278,7 +13305,7 @@
         <v>{"id":246,"title":"swimlane-docker-container-support","group":"dotnet","area":"swimlane","keywords":["docker","cloud","container","ship","port","city","skyline","computer","laptop"],"description":"Ship with containers to represent Docker containers.","publish":1}</v>
       </c>
     </row>
-    <row r="247" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="247" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A247" s="5">
         <v>247</v>
       </c>
@@ -13305,7 +13332,7 @@
         <v>{"id":247,"title":"swimlane-global-data-storage","group":"dotnet","area":"swimlane","keywords":["data","storage","database","globe","duplicate","world"],"description":"Data storage accessible from everywhere in the world.","publish":1}</v>
       </c>
     </row>
-    <row r="248" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="248" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="5">
         <v>248</v>
       </c>
@@ -13332,7 +13359,7 @@
         <v>{"id":248,"title":"swimlane-security","group":"dotnet","area":"swimlane","keywords":["security","guard","camera","safe","secure"],"description":"A safety guard protecting a safe.","publish":1}</v>
       </c>
     </row>
-    <row r="249" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="249" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="5">
         <v>249</v>
       </c>
@@ -13359,7 +13386,7 @@
         <v>{"id":249,"title":"swimlane-angular-react-spa","group":"dotnet","area":"swimlane","keywords":["angular","react","spa","single","page","application","website"],"description":"React and Angular logo and single page web app.","publish":1}</v>
       </c>
     </row>
-    <row r="250" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="250" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="5">
         <v>250</v>
       </c>
@@ -13386,7 +13413,7 @@
         <v>{"id":250,"title":"swimlane-build-scalable-web-apps","group":"dotnet","area":"swimlane","keywords":["build","scalable","web","app","page","truck","box","people"],"description":"A worker loading boxes from truck to a web page.","publish":1}</v>
       </c>
     </row>
-    <row r="251" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="251" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="5">
         <v>251</v>
       </c>
@@ -13413,7 +13440,7 @@
         <v>{"id":251,"title":"swimlane-model-view-controller","group":"dotnet","area":"swimlane","keywords":["mvc","model","view","controller","data","gear","presentation","theme","paint","bucket","brush","design","frontend","backend","stack"],"description":"MVC illustration.","publish":1}</v>
       </c>
     </row>
-    <row r="252" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="252" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="5">
         <v>252</v>
       </c>
@@ -13438,6 +13465,87 @@
       <c r="I252" s="2" t="str">
         <f t="shared" si="9"/>
         <v>{"id":252,"title":"swimlane-seamless-data-integration","group":"dotnet","area":"swimlane","keywords":["data","database","orbit"],"description":"Seamless data integration.","publish":1}</v>
+      </c>
+    </row>
+    <row r="253" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A253" s="5">
+        <v>253</v>
+      </c>
+      <c r="C253" s="2" t="s">
+        <v>944</v>
+      </c>
+      <c r="D253" t="s">
+        <v>387</v>
+      </c>
+      <c r="E253" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F253" s="2" t="s">
+        <v>947</v>
+      </c>
+      <c r="G253" s="2" t="s">
+        <v>948</v>
+      </c>
+      <c r="H253" s="2">
+        <v>1</v>
+      </c>
+      <c r="I253" s="2" t="str">
+        <f t="shared" ref="I253:I255" si="10">SUBSTITUTE(_xlfn.CONCAT("{'id':",A253,",'title':'",C253,"','group':'",D253,"','area':'",E253,"','keywords':['",SUBSTITUTE(F253," ","','"),"'],'description':'",G253,"','publish':",H253,"}"),"'","""")</f>
+        <v>{"id":253,"title":"swimlane-authentication-authorization","group":"dotnet","area":"swimlane","keywords":["authentication","authorization","password","login","key","lock","badge","access","key","chain"],"description":"A key chain with several authentication objects.","publish":1}</v>
+      </c>
+    </row>
+    <row r="254" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A254" s="5">
+        <v>254</v>
+      </c>
+      <c r="C254" s="2" t="s">
+        <v>945</v>
+      </c>
+      <c r="D254" t="s">
+        <v>387</v>
+      </c>
+      <c r="E254" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F254" s="2" t="s">
+        <v>949</v>
+      </c>
+      <c r="G254" s="2" t="s">
+        <v>950</v>
+      </c>
+      <c r="H254" s="2">
+        <v>1</v>
+      </c>
+      <c r="I254" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>{"id":254,"title":"swimlane-rest-api","group":"dotnet","area":"swimlane","keywords":["rest","restful","api","json","bracket","data","database","interface","connect","device","platform"],"description":"Used to represent REST api.","publish":1}</v>
+      </c>
+    </row>
+    <row r="255" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A255" s="5">
+        <v>255</v>
+      </c>
+      <c r="C255" s="2" t="s">
+        <v>946</v>
+      </c>
+      <c r="D255" t="s">
+        <v>387</v>
+      </c>
+      <c r="E255" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F255" s="2" t="s">
+        <v>951</v>
+      </c>
+      <c r="G255" s="2" t="s">
+        <v>952</v>
+      </c>
+      <c r="H255" s="2">
+        <v>1</v>
+      </c>
+      <c r="I255" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>{"id":255,"title":"swimlane-secure-chat-app","group":"dotnet","area":"swimlane","keywords":["lock","secure","chat","people","avatar","message"],"description":"An IM app with encrypted conversation.","publish":1}</v>
       </c>
     </row>
   </sheetData>
@@ -13458,154 +13566,154 @@
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>685</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>686</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>687</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>688</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>686</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>686</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>689</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>690</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>691</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>692</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>693</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>695</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>696</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>697</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>698</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>699</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>700</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>701</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>702</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>703</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>704</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>706</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>707</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>708</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>710</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>711</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>712</v>
       </c>
@@ -13628,22 +13736,22 @@
       <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83984375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.83984375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="38.15625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="38.140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="17" style="2" customWidth="1"/>
     <col min="5" max="5" width="18" style="2" customWidth="1"/>
-    <col min="6" max="6" width="33.68359375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="20.68359375" style="2" customWidth="1"/>
-    <col min="8" max="9" width="24.15625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="33.15625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="66.41796875" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="9.15625" style="2"/>
+    <col min="6" max="6" width="33.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" style="2" customWidth="1"/>
+    <col min="8" max="9" width="24.140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="33.140625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="66.42578125" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" s="3" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>73</v>
       </c>
@@ -13678,7 +13786,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -13712,7 +13820,7 @@
         <v>{"id":1,"title":"AzureToolsForVS","category":"VSCOM","keywords":["free","hosting","bug","tools","platforms","testing","beaker","wrench","azure","logo"],"description":"Azure developer tools for Visual Studio with free hosting.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -13746,7 +13854,7 @@
         <v>{"id":2,"title":"CloudPattern","category":"Pattern","keywords":["technology","nature","cloud","sky"],"description":"Clouds on blue sky pattern.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -13780,7 +13888,7 @@
         <v>{"id":3,"title":"CollaborationChatBubbles","category":"Diagram","keywords":["work","chat","bubble","conversation","communication","collaboration","team","men","women","people"],"description":"Several chat bubbles with people inside.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -13814,7 +13922,7 @@
         <v>{"id":4,"title":"CollaborationNetwork","category":"Diagram","keywords":["man","woman","network","hub","collaboration","connection","web","idea","lightbulb","gear","cloud","chat","bubble","work"],"description":"A network of people and objects connected together.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -13848,7 +13956,7 @@
         <v>{"id":5,"title":"CommunityTranslation1","category":"VSCOM","keywords":["hand","phone","hello","word","balloon","languages"],"description":"Translate world languages with smartphone.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -13882,7 +13990,7 @@
         <v>{"id":6,"title":"CommunityTranslation2","category":"VSCOM","keywords":["group","people","tablet","languages"],"description":"People from around the world using translation app on smart device to say hello.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -13916,7 +14024,7 @@
         <v>{"id":7,"title":"CommunityTranslation3","category":"VSCOM","keywords":["group","people","tablet","languages"],"description":"People from around the world using translation app on smart device to say hello.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -13950,7 +14058,7 @@
         <v>{"id":8,"title":"CordovaToolsTwitterBanner","category":"Web","keywords":["crane","cloud","tools","tree","build","construction"],"description":"Cordova Tools Twitter account banner. Construction crane and build tools on cloud.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -13984,7 +14092,7 @@
         <v>{"id":9,"title":"DesktopComputerPattern","category":"Pattern","keywords":["desktop","computer","monitor","pc","technology"],"description":"Desktop computer pattern.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -14018,7 +14126,7 @@
         <v>{"id":10,"title":"DevEssentials1","category":"VSCOM","keywords":["download","arrow","magnifying","glass","monitor","laptop","data","graphs","gears","newsletter"],"description":"Data visualization related elements on a cloud.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -14052,7 +14160,7 @@
         <v>{"id":11,"title":"DevEssentials2","category":"VSCOM","keywords":["download","arrow","magnifying","glass","monitor","laptop","data","graphs","gears","toolbox","newsletter"],"description":"Data visualization related elements on a cloud.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -14086,7 +14194,7 @@
         <v>{"id":12,"title":"DevicesPattern","category":"Pattern","keywords":["laptop","phone","tablet","smartphone","technology"],"description":"Mixed devices pattern.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -14120,7 +14228,7 @@
         <v>{"id":13,"title":"DevOpsLifecycle","category":"Diagram","keywords":["handshake","planning","continuous","delivery","dev","test","analytics","mobius","infinity","loop"],"description":"DevOps lifecycle.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -14154,7 +14262,7 @@
         <v>{"id":14,"title":"FeedbackCommentsDiscussion","category":"Email","keywords":["chat","bubble","question","exclaimation","conversation","discussion"],"description":"Feedback comment discussion.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -14188,7 +14296,7 @@
         <v>{"id":15,"title":"FeedbackPattern","category":"Pattern","keywords":["feedback","chat","bubble","conversation","question","exclaimation","problem","comment","talk"],"description":"Chat bubble feedback pattern.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -14222,7 +14330,7 @@
         <v>{"id":16,"title":"FoodCollection","category":"Elements","keywords":["food","meal","nutrition","soup","bread","spoon","tomato","broccli","vegetable","fish","crab","seafood","meat","poultry","steak","chicken","turkey","cake","pie","dessert","measuring","cup","egg","beater","cooking","utencils","drink","cocktail","glass","toast","cracker","cheese","burger","hotdog","salad","appetizer","entree"],"description":"A collection of food icons.","style":["color","sketchy"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -14256,7 +14364,7 @@
         <v>{"id":17,"title":"IdeaFactory","category":"Web","keywords":["factory","building","gear","lightbulb","database","arrow","document","gauge","lift","truck"],"description":"Ideas being manufactured in a factory.","style":["monotone"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -14290,7 +14398,7 @@
         <v>{"id":18,"title":"IntegratedDevelopmentLoop","category":"Email","keywords":["loop","cycle","edit","pencil","script","scroll","bug","arrow","device","phone","mobile","cloud"],"description":"Lifecycle of code, debug and deployment.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -14324,7 +14432,7 @@
         <v>{"id":19,"title":"InternetOfThings","category":"Diagram","keywords":["internet","iot","globe","router","smart","phone","laptop","light","bulb","printer","desktop","media","player","car","smart","home","smart","watch","mobile","payment","device","software","development"],"description":"The Internet of Things (IoT) is the network of physical objects or things embedded with electronics, software, sensors, and network connectivity, which enables these objects to collect and exchange data.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -14358,7 +14466,7 @@
         <v>{"id":20,"title":"ManufacturingIdeas","category":"Misc","keywords":["machine","tool","lightbulb"],"description":"Ideas being manufactured by a machine.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -14392,7 +14500,7 @@
         <v>{"id":21,"title":"MicrosoftWelcomeCenter","category":"Print","keywords":["microsoft","company","building","welcome","logo","work","business"],"description":"Microsoft logo and office buildings.","style":["color","3d"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -14426,7 +14534,7 @@
         <v>{"id":22,"title":"MobileAppDevelopmentPlatform","category":"VSCOM","keywords":["building","city","cloud","billboard","people","device","laptop","phone","database","security","lock","presentation","chart","development","platform","enterprise","business"],"description":"Mobile app development platform.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -14460,7 +14568,7 @@
         <v>{"id":23,"title":"MobileAppDevelopmentWithVisualStudio","category":"VSCOM","keywords":["laptop","phone","iphone","android","windows","app","development","visual","studio"],"description":"Cross platform mobile app development with Visual Studio.","style":["color","photo","monotone"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -14494,7 +14602,7 @@
         <v>{"id":24,"title":"MultiDeviceTwitterBanner","category":"Web","keywords":["cloud","sky","field","grass","phone","smartphone","tablet","computer","desktop","pc","monitor","tv","television","microsoft","logo","technology","developer"],"description":"Cordova Tools Twitter account banner. Four device icons overlay on top of cloud and field backgournd.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -14528,7 +14636,7 @@
         <v>{"id":25,"title":"NETCoreWebsiteBanner","category":"Web","keywords":["visual","studio","html5","css3","javascript"],"description":".NET Core website banner.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -14562,7 +14670,7 @@
         <v>{"id":26,"title":"OneToolForEverything","category":"Email","keywords":["tool","laptop","mobile","phone","cloud"],"description":"One tool for all platform.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -14596,7 +14704,7 @@
         <v>{"id":27,"title":"OpenSourceComputer","category":"Web","keywords":["laptop","code","arrow","exchange"],"description":"Two laptop exchanging code.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -14630,7 +14738,7 @@
         <v>{"id":28,"title":"OpenSourceExchangeCode","category":"Diagram","keywords":["code","man","woman","laptop","desktop","exchange","share","arrow"],"description":"Developers exchange open source code.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -14664,7 +14772,7 @@
         <v>{"id":29,"title":"PlaceholderFlowers","category":"VSTS","keywords":["flower"],"description":"Placeholder images.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -14698,7 +14806,7 @@
         <v>{"id":30,"title":"PublishAndDeploy","category":"Email","keywords":["rocket","document","arrow","exchange"],"description":"Publish and deploy code.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -14732,7 +14840,7 @@
         <v>{"id":31,"title":"PushNotifications","category":"Web","keywords":["mobile","phone","tablet","android","windows","ios","chat","bubble","notification"],"description":"Push notifications on multiple platforms.","style":["monotone"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -14766,7 +14874,7 @@
         <v>{"id":32,"title":"PythonToolsForVS","category":"VSCOM","keywords":["man","laptop","woman","gears","bug","code","phone","python","logo","magnifying","glass"],"description":"Python tools for Visual Studio.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -14800,7 +14908,7 @@
         <v>{"id":33,"title":"QuickstartFastSpeed","category":"Email","keywords":["stopwatch","run","man","time","fast","quick","speed"],"description":"Quick start","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -14834,7 +14942,7 @@
         <v>{"id":34,"title":"RocketMulticolor","category":"Elements","keywords":["rocket","launch","deployment"],"description":"Rocket","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -14868,7 +14976,7 @@
         <v>{"id":35,"title":"RocketWithCloudPattern","category":"Print","keywords":["rocket","cloud","sky"],"description":"Rocket on sky background","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -14902,7 +15010,7 @@
         <v>{"id":36,"title":"SeattlePostcard","category":"Print","keywords":["seattle","space","needle","cloud","city"],"description":"Seattle space needle postcard","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -14936,7 +15044,7 @@
         <v>{"id":37,"title":"SeattleSkyline","category":"Web","keywords":["seattle","space","needle","cloud","city","skyline","building","mount","rainier"],"description":"Seattle city skyline","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -14970,7 +15078,7 @@
         <v>{"id":38,"title":"SeattleSkylineFerrisWheel","category":"Web","keywords":["seattle","space","needle","ferris","wheel","waterfront","port"],"description":"Seattle city skyline","style":["monotone"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -15004,7 +15112,7 @@
         <v>{"id":39,"title":"SilhouetteAirportElements","category":"Elements","keywords":["airport","pilot","flight","attendant","uniform","causeway","airplane","sign","direction","loudge","coffee","terminal","seat","life"],"description":"A collection of airport related elements.","style":["silhuoette"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -15038,7 +15146,7 @@
         <v>{"id":40,"title":"SilhouetteBriefcasesAndDocuments","category":"Elements","keywords":["document","file","paper","briefcase","suitcase","handbag","work","object","business"],"description":" A collection of briefcases.","style":["silhuoette"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -15072,7 +15180,7 @@
         <v>{"id":41,"title":"SilhouetteCharacters","category":"Elements","keywords":["man","confuse","suit","woman","chair","desk","laptop","computer","office","work","business"],"description":"A collection of characters in work environment.","style":[" ","silhuoette"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -15106,7 +15214,7 @@
         <v>{"id":42,"title":"SilhouetteHandGenstures","category":"Elements","keywords":["hand","gesture","pick","grip","pinch","touch","web","press","technology"],"description":"Hand gestures.","style":["silhuoette"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -15140,7 +15248,7 @@
         <v>{"id":43,"title":"SilhouetteTabletAndPhones","category":"Elements","keywords":["technology","work","tablet","smartphone","phone","mobile","phone","pen","stylus","windows","phone","android","phone","surface","tablet"],"description":"Tablet and smartphones.","style":["silhuoette"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -15174,7 +15282,7 @@
         <v>{"id":44,"title":"SilhouetteToolCollection","category":"Pattern","keywords":["wrench","screwdriver","saw","plier","hammer","knife","c","clamp","clamp","pipe","wrench","filer","triangle","ruler","object"],"description":"A collection of hand tools.","style":["silhouette"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -15208,7 +15316,7 @@
         <v>{"id":45,"title":"SilhouetteWeatherReportElements","category":"Elements","keywords":["life","newspaper","radio","magezine","clock","news","weather","forcast","tv","sun","sunny","cloud","lightning","thunder","cloud","cloudy","rain","tripical","palm","tree","beach","table","vacation","beach","chair","hawaii","man","relax","drink"],"description":"A collection of weather related illustrations.","style":["silhuoette"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -15242,7 +15350,7 @@
         <v>{"id":46,"title":"SoftwareToolsSampleKit","category":"Email","keywords":["toolbox","hammer","checklist","wrench","cloud"],"description":"Software development toolkit","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -15276,7 +15384,7 @@
         <v>{"id":47,"title":"TeamworkStairs","category":"Web","keywords":["people","man","stairs","team"],"description":"People holding hands climbing up stairs as a team.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -15310,7 +15418,7 @@
         <v>{"id":48,"title":"Testing","category":"Email","keywords":["test","flask","lab","beaker","stopwatch","pie","chart","checklist"],"description":"Testing","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -15344,7 +15452,7 @@
         <v>{"id":49,"title":"VSBuildALMIntegration","category":"VSCOM","keywords":["people","working","man","computer","clipboard","debug","tools","gear","bug"],"description":"ALM (Application Lifecycle Management) debug integration.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -15378,7 +15486,7 @@
         <v>{"id":50,"title":"VSBuildCloudHostedTools","category":"VSCOM","keywords":["people","laptops","desk","workers","monitors","laptops","cross","platforms","linux","windows","ios"],"description":"Developers come from different platforms and technology stacks working together.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -15412,7 +15520,7 @@
         <v>{"id":51,"title":"VSBuildContinuousIntegration","category":"VSCOM","keywords":["monitor","laptop","test","tubes","gears","checkmark"],"description":"Build continuous integration cycle with cloud.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -15446,7 +15554,7 @@
         <v>{"id":52,"title":"VSBuildContinuousIntegrationWhite","category":"VSCOM","keywords":["cross","platforms","maven","git","apache","ant","junit","gradle","xunit","mtm","test","building"],"description":"Common tools and technologies for cross-platform development.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -15480,7 +15588,7 @@
         <v>{"id":53,"title":"VSBuildCrossPlatform","category":"VSCOM","keywords":["pillars","cross","platforms","buildings","crane","java",".net","xcode","github","ios","android","windows","git"],"description":"Common tools and technologies for cross-platform development.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -15514,7 +15622,7 @@
         <v>{"id":54,"title":"VSBuildOverview","category":"VSCOM","keywords":["cross","platforms","laptop","tablet","phone","ios","android","visual","studio","cloud"],"description":"Visual Studio for building cross-platform applications.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -15548,7 +15656,7 @@
         <v>{"id":55,"title":"VSBuildTraceability","category":"VSCOM","keywords":["blueprint","document","man","beaker","tools","clipboard","timeline","printer","download","test","tubes","gears","magnifying","glass","graphs"],"description":"Build timeline and tracebility.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -15582,7 +15690,7 @@
         <v>{"id":56,"title":"VSDownload1","category":"VSCOM","keywords":["group","people","visual","studio","logo","flags","man","woman"],"description":"Visual Studio for everyone.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -15616,7 +15724,7 @@
         <v>{"id":57,"title":"VSDownload2","category":"VSCOM","keywords":["man","monitors","download","down","arrow","computer","table"],"description":"Visual Studio tools for multiplatform.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -15650,302 +15758,302 @@
         <v>{"id":58,"title":"XamarinCrossPlatformDevelopment","category":"VSCOM","keywords":["screenshot","ios","android","windows","mobile","phone","app","development","shared","code","cross-platform","xamarin"],"description":"Xamarin for developing cross-platform application.","style":["color","photo"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>114</v>
       </c>
     </row>
-    <row r="116" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <v>115</v>
       </c>
     </row>
-    <row r="117" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>117</v>
       </c>
     </row>
-    <row r="119" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>118</v>
       </c>
@@ -15981,9 +16089,9 @@
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="1" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Added new illustrations for .NET
</commit_message>
<xml_diff>
--- a/src/assets/data.xlsx
+++ b/src/assets/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\Code\vsimages\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1716BF1E-4F84-4E8D-9411-14B7F1EA42AF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B58C37FC-53E6-44D5-92B1-D116DEEB2ED3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,6 +29,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1671" uniqueCount="953">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1706" uniqueCount="974">
   <si>
     <t>SeattleSkyline</t>
   </si>
@@ -2895,6 +2896,69 @@
   </si>
   <si>
     <t>An IM app with encrypted conversation.</t>
+  </si>
+  <si>
+    <t>swimlane-multiplayer-game</t>
+  </si>
+  <si>
+    <t>swimlane-mvc-scenario</t>
+  </si>
+  <si>
+    <t>swimlane-real-time-chat-app</t>
+  </si>
+  <si>
+    <t>swimlane-signalr-hub</t>
+  </si>
+  <si>
+    <t>swimlane-azure-signalr-logo</t>
+  </si>
+  <si>
+    <t>swimlane-chat-app-multiplatform</t>
+  </si>
+  <si>
+    <t>swimlane-fast-performance-gauge</t>
+  </si>
+  <si>
+    <t>game multi player people xbox tv</t>
+  </si>
+  <si>
+    <t>model view controller mvc layer tier stack web app design data people</t>
+  </si>
+  <si>
+    <t>real time chat app people tablet device</t>
+  </si>
+  <si>
+    <t>signalr hub server device phone mobile tablet browser computer laptop</t>
+  </si>
+  <si>
+    <t>azure signalr logo</t>
+  </si>
+  <si>
+    <t>chat app multi platform device people</t>
+  </si>
+  <si>
+    <t>performance race car gauge speed fast</t>
+  </si>
+  <si>
+    <t>A man playing real-time multiplayer video game with a woman.</t>
+  </si>
+  <si>
+    <t>Model-View-Controller explained with illustrated example.</t>
+  </si>
+  <si>
+    <t>A woman using a laptop to chat with a man using tablet.</t>
+  </si>
+  <si>
+    <t>A server hub with connectors to multiple devices.</t>
+  </si>
+  <si>
+    <t>Azure SignalR brand icon.</t>
+  </si>
+  <si>
+    <t>A woman using the same chat app available on multiple devices.</t>
+  </si>
+  <si>
+    <t>A car racing themed background with a speed gauge.</t>
   </si>
 </sst>
 </file>
@@ -5800,13 +5864,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K255"/>
+  <dimension ref="A1:K262"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B251" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B258" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F257" sqref="F257"/>
+      <selection pane="bottomRight" activeCell="I256" sqref="I256:I262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -13548,8 +13612,197 @@
         <v>{"id":255,"title":"swimlane-secure-chat-app","group":"dotnet","area":"swimlane","keywords":["lock","secure","chat","people","avatar","message"],"description":"An IM app with encrypted conversation.","publish":1}</v>
       </c>
     </row>
+    <row r="256" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A256" s="5">
+        <v>256</v>
+      </c>
+      <c r="C256" s="2" t="s">
+        <v>953</v>
+      </c>
+      <c r="D256" t="s">
+        <v>387</v>
+      </c>
+      <c r="E256" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F256" s="2" t="s">
+        <v>960</v>
+      </c>
+      <c r="G256" s="2" t="s">
+        <v>967</v>
+      </c>
+      <c r="H256" s="2">
+        <v>1</v>
+      </c>
+      <c r="I256" s="2" t="str">
+        <f t="shared" ref="I256:I262" si="11">SUBSTITUTE(_xlfn.CONCAT("{'id':",A256,",'title':'",C256,"','group':'",D256,"','area':'",E256,"','keywords':['",SUBSTITUTE(F256," ","','"),"'],'description':'",G256,"','publish':",H256,"}"),"'","""")</f>
+        <v>{"id":256,"title":"swimlane-multiplayer-game","group":"dotnet","area":"swimlane","keywords":["game","multi","player","people","xbox","tv"],"description":"A man playing real-time multiplayer video game with a woman.","publish":1}</v>
+      </c>
+    </row>
+    <row r="257" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A257" s="5">
+        <v>257</v>
+      </c>
+      <c r="C257" s="2" t="s">
+        <v>954</v>
+      </c>
+      <c r="D257" t="s">
+        <v>387</v>
+      </c>
+      <c r="E257" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F257" s="2" t="s">
+        <v>961</v>
+      </c>
+      <c r="G257" s="2" t="s">
+        <v>968</v>
+      </c>
+      <c r="H257" s="2">
+        <v>1</v>
+      </c>
+      <c r="I257" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>{"id":257,"title":"swimlane-mvc-scenario","group":"dotnet","area":"swimlane","keywords":["model","view","controller","mvc","layer","tier","stack","web","app","design","data","people"],"description":"Model-View-Controller explained with illustrated example.","publish":1}</v>
+      </c>
+    </row>
+    <row r="258" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A258" s="5">
+        <v>258</v>
+      </c>
+      <c r="C258" s="2" t="s">
+        <v>955</v>
+      </c>
+      <c r="D258" t="s">
+        <v>387</v>
+      </c>
+      <c r="E258" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F258" s="2" t="s">
+        <v>962</v>
+      </c>
+      <c r="G258" s="2" t="s">
+        <v>969</v>
+      </c>
+      <c r="H258" s="2">
+        <v>1</v>
+      </c>
+      <c r="I258" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>{"id":258,"title":"swimlane-real-time-chat-app","group":"dotnet","area":"swimlane","keywords":["real","time","chat","app","people","tablet","device"],"description":"A woman using a laptop to chat with a man using tablet.","publish":1}</v>
+      </c>
+    </row>
+    <row r="259" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A259" s="5">
+        <v>259</v>
+      </c>
+      <c r="C259" s="2" t="s">
+        <v>956</v>
+      </c>
+      <c r="D259" t="s">
+        <v>387</v>
+      </c>
+      <c r="E259" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F259" s="2" t="s">
+        <v>963</v>
+      </c>
+      <c r="G259" s="2" t="s">
+        <v>970</v>
+      </c>
+      <c r="H259" s="2">
+        <v>1</v>
+      </c>
+      <c r="I259" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>{"id":259,"title":"swimlane-signalr-hub","group":"dotnet","area":"swimlane","keywords":["signalr","hub","server","device","phone","mobile","tablet","browser","computer","laptop"],"description":"A server hub with connectors to multiple devices.","publish":1}</v>
+      </c>
+    </row>
+    <row r="260" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A260" s="5">
+        <v>260</v>
+      </c>
+      <c r="C260" s="2" t="s">
+        <v>957</v>
+      </c>
+      <c r="D260" t="s">
+        <v>387</v>
+      </c>
+      <c r="E260" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F260" s="2" t="s">
+        <v>964</v>
+      </c>
+      <c r="G260" s="2" t="s">
+        <v>971</v>
+      </c>
+      <c r="H260" s="2">
+        <v>1</v>
+      </c>
+      <c r="I260" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>{"id":260,"title":"swimlane-azure-signalr-logo","group":"dotnet","area":"swimlane","keywords":["azure","signalr","logo"],"description":"Azure SignalR brand icon.","publish":1}</v>
+      </c>
+    </row>
+    <row r="261" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A261" s="5">
+        <v>261</v>
+      </c>
+      <c r="C261" s="2" t="s">
+        <v>958</v>
+      </c>
+      <c r="D261" t="s">
+        <v>387</v>
+      </c>
+      <c r="E261" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F261" s="2" t="s">
+        <v>965</v>
+      </c>
+      <c r="G261" s="2" t="s">
+        <v>972</v>
+      </c>
+      <c r="H261" s="2">
+        <v>1</v>
+      </c>
+      <c r="I261" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>{"id":261,"title":"swimlane-chat-app-multiplatform","group":"dotnet","area":"swimlane","keywords":["chat","app","multi","platform","device","people"],"description":"A woman using the same chat app available on multiple devices.","publish":1}</v>
+      </c>
+    </row>
+    <row r="262" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A262" s="5">
+        <v>262</v>
+      </c>
+      <c r="C262" s="2" t="s">
+        <v>959</v>
+      </c>
+      <c r="D262" t="s">
+        <v>387</v>
+      </c>
+      <c r="E262" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F262" s="2" t="s">
+        <v>966</v>
+      </c>
+      <c r="G262" s="2" t="s">
+        <v>973</v>
+      </c>
+      <c r="H262" s="2">
+        <v>1</v>
+      </c>
+      <c r="I262" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>{"id":262,"title":"swimlane-fast-performance-gauge","group":"dotnet","area":"swimlane","keywords":["performance","race","car","gauge","speed","fast"],"description":"A car racing themed background with a speed gauge.","publish":1}</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="C92:C100">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C92:C100">
     <sortCondition ref="C92"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16059,7 +16312,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:H59">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H59">
     <sortCondition ref="C2:C59"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added vsmac installer screen illustration
</commit_message>
<xml_diff>
--- a/src/assets/data.xlsx
+++ b/src/assets/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\Code\vsimages\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B58C37FC-53E6-44D5-92B1-D116DEEB2ED3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E66255-9EF5-4416-AA54-B1A53E7E0766}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1706" uniqueCount="974">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1711" uniqueCount="979">
   <si>
     <t>SeattleSkyline</t>
   </si>
@@ -2959,6 +2959,21 @@
   </si>
   <si>
     <t>A car racing themed background with a speed gauge.</t>
+  </si>
+  <si>
+    <t>vsmac-installer-screen</t>
+  </si>
+  <si>
+    <t>vsmac</t>
+  </si>
+  <si>
+    <t>splashscreen</t>
+  </si>
+  <si>
+    <t>space galaxy cloud people work desk install download waiting</t>
+  </si>
+  <si>
+    <t>Two people playing with paper plane while waiting for installation. Space theme background.</t>
   </si>
 </sst>
 </file>
@@ -5864,13 +5879,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K262"/>
+  <dimension ref="A1:K263"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B258" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I256" sqref="I256:I262"/>
+      <selection pane="bottomRight" activeCell="I263" sqref="I263"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -13635,7 +13650,7 @@
         <v>1</v>
       </c>
       <c r="I256" s="2" t="str">
-        <f t="shared" ref="I256:I262" si="11">SUBSTITUTE(_xlfn.CONCAT("{'id':",A256,",'title':'",C256,"','group':'",D256,"','area':'",E256,"','keywords':['",SUBSTITUTE(F256," ","','"),"'],'description':'",G256,"','publish':",H256,"}"),"'","""")</f>
+        <f t="shared" ref="I256:I263" si="11">SUBSTITUTE(_xlfn.CONCAT("{'id':",A256,",'title':'",C256,"','group':'",D256,"','area':'",E256,"','keywords':['",SUBSTITUTE(F256," ","','"),"'],'description':'",G256,"','publish':",H256,"}"),"'","""")</f>
         <v>{"id":256,"title":"swimlane-multiplayer-game","group":"dotnet","area":"swimlane","keywords":["game","multi","player","people","xbox","tv"],"description":"A man playing real-time multiplayer video game with a woman.","publish":1}</v>
       </c>
     </row>
@@ -13799,6 +13814,33 @@
       <c r="I262" s="2" t="str">
         <f t="shared" si="11"/>
         <v>{"id":262,"title":"swimlane-fast-performance-gauge","group":"dotnet","area":"swimlane","keywords":["performance","race","car","gauge","speed","fast"],"description":"A car racing themed background with a speed gauge.","publish":1}</v>
+      </c>
+    </row>
+    <row r="263" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A263" s="5">
+        <v>263</v>
+      </c>
+      <c r="C263" s="2" t="s">
+        <v>974</v>
+      </c>
+      <c r="D263" t="s">
+        <v>975</v>
+      </c>
+      <c r="E263" s="2" t="s">
+        <v>976</v>
+      </c>
+      <c r="F263" s="2" t="s">
+        <v>977</v>
+      </c>
+      <c r="G263" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="H263" s="2">
+        <v>1</v>
+      </c>
+      <c r="I263" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>{"id":263,"title":"vsmac-installer-screen","group":"vsmac","area":"splashscreen","keywords":["space","galaxy","cloud","people","work","desk","install","download","waiting"],"description":"Two people playing with paper plane while waiting for installation. Space theme background.","publish":1}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added illustrations for .NET Microservices page
</commit_message>
<xml_diff>
--- a/src/assets/data.xlsx
+++ b/src/assets/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\Code\vsimages\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3190CA-7FAC-4992-8D8C-A20481A271A9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F3051C-A87D-46D5-9C98-244B6CA2C43A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1726" uniqueCount="988">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1756" uniqueCount="1006">
   <si>
     <t>SeattleSkyline</t>
   </si>
@@ -3001,6 +3001,60 @@
   </si>
   <si>
     <t>Big enterprise mass producing rockets.</t>
+  </si>
+  <si>
+    <t>swimlane-build-scalable-apps</t>
+  </si>
+  <si>
+    <t>swimlane-docker-three-platforms</t>
+  </si>
+  <si>
+    <t>swimlane-dotnet-compatible-with-other-tools</t>
+  </si>
+  <si>
+    <t>swimlane-microservices-build</t>
+  </si>
+  <si>
+    <t>swimlane-microservices-modules</t>
+  </si>
+  <si>
+    <t>swimlane-brand-docker</t>
+  </si>
+  <si>
+    <t>build scalable building crane construction scalability stack city tree</t>
+  </si>
+  <si>
+    <t>A construction crane loading stacks to build a skyscraper.</t>
+  </si>
+  <si>
+    <t>docker platform os windows linux macos ship container</t>
+  </si>
+  <si>
+    <t>A freight ship with containers running on Windows, Linux and macOS.</t>
+  </si>
+  <si>
+    <t>dotnet module microservices cube plug compatible side by side tools stacks people</t>
+  </si>
+  <si>
+    <t>.NET works side-by-side with other technology stacks.</t>
+  </si>
+  <si>
+    <t>microservices build module truck people load blocks</t>
+  </si>
+  <si>
+    <t>People integrating microservice modules to make complete products.</t>
+  </si>
+  <si>
+    <t>microservices building blocks modules cubes plug connect integrate</t>
+  </si>
+  <si>
+    <t>Microservices building blocks.</t>
+  </si>
+  <si>
+    <t>docker brand logo</t>
+  </si>
+  <si>
+    <t>Docker logo</t>
   </si>
 </sst>
 </file>
@@ -5906,13 +5960,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K266"/>
+  <dimension ref="A1:K272"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B260" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B272" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G264" sqref="G264"/>
+      <selection pane="bottomRight" activeCell="E273" sqref="E273"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -13949,6 +14003,168 @@
       <c r="I266" s="2" t="str">
         <f t="shared" si="12"/>
         <v>{"id":266,"title":"hero-vs-community-sku","group":"vscom","area":"hero","keywords":["enterprise","company","large","scale","buildings","process","rocket","workflow","truck"],"description":"Big enterprise mass producing rockets.","publish":1}</v>
+      </c>
+    </row>
+    <row r="267" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A267" s="5">
+        <v>267</v>
+      </c>
+      <c r="C267" s="2" t="s">
+        <v>988</v>
+      </c>
+      <c r="D267" t="s">
+        <v>387</v>
+      </c>
+      <c r="E267" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F267" s="2" t="s">
+        <v>994</v>
+      </c>
+      <c r="G267" s="2" t="s">
+        <v>995</v>
+      </c>
+      <c r="H267" s="2">
+        <v>1</v>
+      </c>
+      <c r="I267" s="2" t="str">
+        <f t="shared" ref="I267:I272" si="13">SUBSTITUTE(_xlfn.CONCAT("{'id':",A267,",'title':'",C267,"','group':'",D267,"','area':'",E267,"','keywords':['",SUBSTITUTE(F267," ","','"),"'],'description':'",G267,"','publish':",H267,"}"),"'","""")</f>
+        <v>{"id":267,"title":"swimlane-build-scalable-apps","group":"dotnet","area":"swimlane","keywords":["build","scalable","building","crane","construction","scalability","stack","city","tree"],"description":"A construction crane loading stacks to build a skyscraper.","publish":1}</v>
+      </c>
+    </row>
+    <row r="268" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A268" s="5">
+        <v>268</v>
+      </c>
+      <c r="C268" s="2" t="s">
+        <v>989</v>
+      </c>
+      <c r="D268" t="s">
+        <v>387</v>
+      </c>
+      <c r="E268" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F268" s="2" t="s">
+        <v>996</v>
+      </c>
+      <c r="G268" s="2" t="s">
+        <v>997</v>
+      </c>
+      <c r="H268" s="2">
+        <v>1</v>
+      </c>
+      <c r="I268" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>{"id":268,"title":"swimlane-docker-three-platforms","group":"dotnet","area":"swimlane","keywords":["docker","platform","os","windows","linux","macos","ship","container"],"description":"A freight ship with containers running on Windows, Linux and macOS.","publish":1}</v>
+      </c>
+    </row>
+    <row r="269" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A269" s="5">
+        <v>269</v>
+      </c>
+      <c r="C269" s="2" t="s">
+        <v>990</v>
+      </c>
+      <c r="D269" t="s">
+        <v>387</v>
+      </c>
+      <c r="E269" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F269" s="2" t="s">
+        <v>998</v>
+      </c>
+      <c r="G269" s="2" t="s">
+        <v>999</v>
+      </c>
+      <c r="H269" s="2">
+        <v>1</v>
+      </c>
+      <c r="I269" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>{"id":269,"title":"swimlane-dotnet-compatible-with-other-tools","group":"dotnet","area":"swimlane","keywords":["dotnet","module","microservices","cube","plug","compatible","side","by","side","tools","stacks","people"],"description":".NET works side-by-side with other technology stacks.","publish":1}</v>
+      </c>
+    </row>
+    <row r="270" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A270" s="5">
+        <v>270</v>
+      </c>
+      <c r="C270" s="2" t="s">
+        <v>991</v>
+      </c>
+      <c r="D270" t="s">
+        <v>387</v>
+      </c>
+      <c r="E270" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F270" s="2" t="s">
+        <v>1000</v>
+      </c>
+      <c r="G270" s="2" t="s">
+        <v>1001</v>
+      </c>
+      <c r="H270" s="2">
+        <v>1</v>
+      </c>
+      <c r="I270" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>{"id":270,"title":"swimlane-microservices-build","group":"dotnet","area":"swimlane","keywords":["microservices","build","module","truck","people","load","blocks"],"description":"People integrating microservice modules to make complete products.","publish":1}</v>
+      </c>
+    </row>
+    <row r="271" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A271" s="5">
+        <v>271</v>
+      </c>
+      <c r="C271" s="2" t="s">
+        <v>992</v>
+      </c>
+      <c r="D271" t="s">
+        <v>387</v>
+      </c>
+      <c r="E271" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F271" s="2" t="s">
+        <v>1002</v>
+      </c>
+      <c r="G271" s="2" t="s">
+        <v>1003</v>
+      </c>
+      <c r="H271" s="2">
+        <v>1</v>
+      </c>
+      <c r="I271" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>{"id":271,"title":"swimlane-microservices-modules","group":"dotnet","area":"swimlane","keywords":["microservices","building","blocks","modules","cubes","plug","connect","integrate"],"description":"Microservices building blocks.","publish":1}</v>
+      </c>
+    </row>
+    <row r="272" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A272" s="5">
+        <v>272</v>
+      </c>
+      <c r="C272" s="2" t="s">
+        <v>993</v>
+      </c>
+      <c r="D272" t="s">
+        <v>387</v>
+      </c>
+      <c r="E272" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F272" s="2" t="s">
+        <v>1004</v>
+      </c>
+      <c r="G272" s="2" t="s">
+        <v>1005</v>
+      </c>
+      <c r="H272" s="2">
+        <v>1</v>
+      </c>
+      <c r="I272" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>{"id":272,"title":"swimlane-brand-docker","group":"dotnet","area":"swimlane","keywords":["docker","brand","logo"],"description":"Docker logo","publish":1}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added ASP.NET webforms page illustrations
</commit_message>
<xml_diff>
--- a/src/assets/data.xlsx
+++ b/src/assets/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\Code\vsimages\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F3051C-A87D-46D5-9C98-244B6CA2C43A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0437381C-E5DD-450C-B498-7783A5BFF277}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1756" uniqueCount="1006">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1781" uniqueCount="1021">
   <si>
     <t>SeattleSkyline</t>
   </si>
@@ -3055,6 +3055,51 @@
   </si>
   <si>
     <t>Docker logo</t>
+  </si>
+  <si>
+    <t>swimlane-event-driven-programming</t>
+  </si>
+  <si>
+    <t>swimlane-razor-cross-platform</t>
+  </si>
+  <si>
+    <t>swimlane-webform</t>
+  </si>
+  <si>
+    <t>swimlane-webform-control-library</t>
+  </si>
+  <si>
+    <t>swimlane-webform-data-integration</t>
+  </si>
+  <si>
+    <t>winform event trigger click button control sync server gear</t>
+  </si>
+  <si>
+    <t>Event triggered in the presentation tier and passed to server.</t>
+  </si>
+  <si>
+    <t>razor @ html cross platform windows linux macos coffee mugs cups tea</t>
+  </si>
+  <si>
+    <t>Razor pages works across multiple platforms.</t>
+  </si>
+  <si>
+    <t>webform control drag drop pencil button window dialog</t>
+  </si>
+  <si>
+    <t>Drag and drop designer for building Webform applications.</t>
+  </si>
+  <si>
+    <t>webform control button dropdown textbox radio button checkbox</t>
+  </si>
+  <si>
+    <t>A large library of webform controls.</t>
+  </si>
+  <si>
+    <t>data integration webform dropdown input table database connect</t>
+  </si>
+  <si>
+    <t>Simple data integration with .NET web forms.</t>
   </si>
 </sst>
 </file>
@@ -5960,13 +6005,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K272"/>
+  <dimension ref="A1:K277"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B272" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B274" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E273" sqref="E273"/>
+      <selection pane="bottomRight" activeCell="G278" sqref="G278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14165,6 +14210,141 @@
       <c r="I272" s="2" t="str">
         <f t="shared" si="13"/>
         <v>{"id":272,"title":"swimlane-brand-docker","group":"dotnet","area":"swimlane","keywords":["docker","brand","logo"],"description":"Docker logo","publish":1}</v>
+      </c>
+    </row>
+    <row r="273" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A273" s="5">
+        <v>273</v>
+      </c>
+      <c r="C273" s="2" t="s">
+        <v>1006</v>
+      </c>
+      <c r="D273" t="s">
+        <v>387</v>
+      </c>
+      <c r="E273" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F273" s="2" t="s">
+        <v>1011</v>
+      </c>
+      <c r="G273" s="2" t="s">
+        <v>1012</v>
+      </c>
+      <c r="H273" s="2">
+        <v>1</v>
+      </c>
+      <c r="I273" s="2" t="str">
+        <f t="shared" ref="I273:I277" si="14">SUBSTITUTE(_xlfn.CONCAT("{'id':",A273,",'title':'",C273,"','group':'",D273,"','area':'",E273,"','keywords':['",SUBSTITUTE(F273," ","','"),"'],'description':'",G273,"','publish':",H273,"}"),"'","""")</f>
+        <v>{"id":273,"title":"swimlane-event-driven-programming","group":"dotnet","area":"swimlane","keywords":["winform","event","trigger","click","button","control","sync","server","gear"],"description":"Event triggered in the presentation tier and passed to server.","publish":1}</v>
+      </c>
+    </row>
+    <row r="274" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A274" s="5">
+        <v>274</v>
+      </c>
+      <c r="C274" s="2" t="s">
+        <v>1007</v>
+      </c>
+      <c r="D274" t="s">
+        <v>387</v>
+      </c>
+      <c r="E274" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F274" s="2" t="s">
+        <v>1013</v>
+      </c>
+      <c r="G274" s="2" t="s">
+        <v>1014</v>
+      </c>
+      <c r="H274" s="2">
+        <v>1</v>
+      </c>
+      <c r="I274" s="2" t="str">
+        <f t="shared" si="14"/>
+        <v>{"id":274,"title":"swimlane-razor-cross-platform","group":"dotnet","area":"swimlane","keywords":["razor","@","html","cross","platform","windows","linux","macos","coffee","mugs","cups","tea"],"description":"Razor pages works across multiple platforms.","publish":1}</v>
+      </c>
+    </row>
+    <row r="275" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A275" s="5">
+        <v>275</v>
+      </c>
+      <c r="C275" s="2" t="s">
+        <v>1008</v>
+      </c>
+      <c r="D275" t="s">
+        <v>387</v>
+      </c>
+      <c r="E275" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F275" s="2" t="s">
+        <v>1015</v>
+      </c>
+      <c r="G275" s="2" t="s">
+        <v>1016</v>
+      </c>
+      <c r="H275" s="2">
+        <v>1</v>
+      </c>
+      <c r="I275" s="2" t="str">
+        <f t="shared" si="14"/>
+        <v>{"id":275,"title":"swimlane-webform","group":"dotnet","area":"swimlane","keywords":["webform","control","drag","drop","pencil","button","window","dialog"],"description":"Drag and drop designer for building Webform applications.","publish":1}</v>
+      </c>
+    </row>
+    <row r="276" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A276" s="5">
+        <v>276</v>
+      </c>
+      <c r="C276" s="2" t="s">
+        <v>1009</v>
+      </c>
+      <c r="D276" t="s">
+        <v>387</v>
+      </c>
+      <c r="E276" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F276" s="2" t="s">
+        <v>1017</v>
+      </c>
+      <c r="G276" s="2" t="s">
+        <v>1018</v>
+      </c>
+      <c r="H276" s="2">
+        <v>1</v>
+      </c>
+      <c r="I276" s="2" t="str">
+        <f t="shared" si="14"/>
+        <v>{"id":276,"title":"swimlane-webform-control-library","group":"dotnet","area":"swimlane","keywords":["webform","control","button","dropdown","textbox","radio","button","checkbox"],"description":"A large library of webform controls.","publish":1}</v>
+      </c>
+    </row>
+    <row r="277" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A277" s="5">
+        <v>277</v>
+      </c>
+      <c r="C277" s="2" t="s">
+        <v>1010</v>
+      </c>
+      <c r="D277" t="s">
+        <v>387</v>
+      </c>
+      <c r="E277" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F277" s="2" t="s">
+        <v>1019</v>
+      </c>
+      <c r="G277" s="2" t="s">
+        <v>1020</v>
+      </c>
+      <c r="H277" s="2">
+        <v>1</v>
+      </c>
+      <c r="I277" s="2" t="str">
+        <f t="shared" si="14"/>
+        <v>{"id":277,"title":"swimlane-webform-data-integration","group":"dotnet","area":"swimlane","keywords":["data","integration","webform","dropdown","input","table","database","connect"],"description":"Simple data integration with .NET web forms.","publish":1}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added .NET and Open Source illustrations
</commit_message>
<xml_diff>
--- a/src/assets/data.xlsx
+++ b/src/assets/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\Code\vsimages\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0437381C-E5DD-450C-B498-7783A5BFF277}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{995FC15E-5B4D-421D-A758-64F831C02894}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1781" uniqueCount="1021">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1801" uniqueCount="1033">
   <si>
     <t>SeattleSkyline</t>
   </si>
@@ -3100,6 +3100,42 @@
   </si>
   <si>
     <t>Simple data integration with .NET web forms.</t>
+  </si>
+  <si>
+    <t>swimlane-community-documentation</t>
+  </si>
+  <si>
+    <t>swimlane-license-certificates</t>
+  </si>
+  <si>
+    <t>swimlane-brand-dotnet-foundation</t>
+  </si>
+  <si>
+    <t>swimlane-brand-github-octocat</t>
+  </si>
+  <si>
+    <t>community people collaboration documentation open source hands paper pencil team</t>
+  </si>
+  <si>
+    <t>Active developer community and up to date documentation.</t>
+  </si>
+  <si>
+    <t>license certificate ribbon copyright</t>
+  </si>
+  <si>
+    <t>License certificates.</t>
+  </si>
+  <si>
+    <t>brand dotnet foundation logo</t>
+  </si>
+  <si>
+    <t>.NET Foundation logo.</t>
+  </si>
+  <si>
+    <t>brand github octocat mascot</t>
+  </si>
+  <si>
+    <t>GitHub Octocat.</t>
   </si>
 </sst>
 </file>
@@ -6005,13 +6041,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K277"/>
+  <dimension ref="A1:K281"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B274" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B116" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G278" sqref="G278"/>
+      <selection pane="bottomRight" activeCell="H118" sqref="H118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14345,6 +14381,114 @@
       <c r="I277" s="2" t="str">
         <f t="shared" si="14"/>
         <v>{"id":277,"title":"swimlane-webform-data-integration","group":"dotnet","area":"swimlane","keywords":["data","integration","webform","dropdown","input","table","database","connect"],"description":"Simple data integration with .NET web forms.","publish":1}</v>
+      </c>
+    </row>
+    <row r="278" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A278" s="5">
+        <v>278</v>
+      </c>
+      <c r="C278" s="2" t="s">
+        <v>1021</v>
+      </c>
+      <c r="D278" t="s">
+        <v>387</v>
+      </c>
+      <c r="E278" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F278" s="2" t="s">
+        <v>1025</v>
+      </c>
+      <c r="G278" s="2" t="s">
+        <v>1026</v>
+      </c>
+      <c r="H278" s="2">
+        <v>1</v>
+      </c>
+      <c r="I278" s="2" t="str">
+        <f t="shared" ref="I278:I281" si="15">SUBSTITUTE(_xlfn.CONCAT("{'id':",A278,",'title':'",C278,"','group':'",D278,"','area':'",E278,"','keywords':['",SUBSTITUTE(F278," ","','"),"'],'description':'",G278,"','publish':",H278,"}"),"'","""")</f>
+        <v>{"id":278,"title":"swimlane-community-documentation","group":"dotnet","area":"swimlane","keywords":["community","people","collaboration","documentation","open","source","hands","paper","pencil","team"],"description":"Active developer community and up to date documentation.","publish":1}</v>
+      </c>
+    </row>
+    <row r="279" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A279" s="5">
+        <v>279</v>
+      </c>
+      <c r="C279" s="2" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D279" t="s">
+        <v>387</v>
+      </c>
+      <c r="E279" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F279" s="2" t="s">
+        <v>1027</v>
+      </c>
+      <c r="G279" s="2" t="s">
+        <v>1028</v>
+      </c>
+      <c r="H279" s="2">
+        <v>1</v>
+      </c>
+      <c r="I279" s="2" t="str">
+        <f t="shared" si="15"/>
+        <v>{"id":279,"title":"swimlane-license-certificates","group":"dotnet","area":"swimlane","keywords":["license","certificate","ribbon","copyright"],"description":"License certificates.","publish":1}</v>
+      </c>
+    </row>
+    <row r="280" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A280" s="5">
+        <v>280</v>
+      </c>
+      <c r="C280" s="2" t="s">
+        <v>1023</v>
+      </c>
+      <c r="D280" t="s">
+        <v>387</v>
+      </c>
+      <c r="E280" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F280" s="2" t="s">
+        <v>1029</v>
+      </c>
+      <c r="G280" s="2" t="s">
+        <v>1030</v>
+      </c>
+      <c r="H280" s="2">
+        <v>1</v>
+      </c>
+      <c r="I280" s="2" t="str">
+        <f t="shared" si="15"/>
+        <v>{"id":280,"title":"swimlane-brand-dotnet-foundation","group":"dotnet","area":"swimlane","keywords":["brand","dotnet","foundation","logo"],"description":".NET Foundation logo.","publish":1}</v>
+      </c>
+    </row>
+    <row r="281" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A281" s="5">
+        <v>281</v>
+      </c>
+      <c r="C281" s="2" t="s">
+        <v>1024</v>
+      </c>
+      <c r="D281" t="s">
+        <v>387</v>
+      </c>
+      <c r="E281" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F281" s="2" t="s">
+        <v>1031</v>
+      </c>
+      <c r="G281" s="2" t="s">
+        <v>1032</v>
+      </c>
+      <c r="H281" s="2">
+        <v>1</v>
+      </c>
+      <c r="I281" s="2" t="str">
+        <f t="shared" si="15"/>
+        <v>{"id":281,"title":"swimlane-brand-github-octocat","group":"dotnet","area":"swimlane","keywords":["brand","github","octocat","mascot"],"description":"GitHub Octocat.","publish":1}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new illustrations; fixed json
</commit_message>
<xml_diff>
--- a/src/assets/data.xlsx
+++ b/src/assets/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\Code\vsimages\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{995FC15E-5B4D-421D-A758-64F831C02894}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40EAACA-3EDA-4568-86CF-A0001C792B8E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1801" uniqueCount="1033">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1806" uniqueCount="1036">
   <si>
     <t>SeattleSkyline</t>
   </si>
@@ -3136,6 +3136,15 @@
   </si>
   <si>
     <t>GitHub Octocat.</t>
+  </si>
+  <si>
+    <t>swimlane-brand-microsoft</t>
+  </si>
+  <si>
+    <t>Microsoft logo.</t>
+  </si>
+  <si>
+    <t>brand microsoft logo</t>
   </si>
 </sst>
 </file>
@@ -6041,13 +6050,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K281"/>
+  <dimension ref="A1:K282"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B116" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B279" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H118" sqref="H118"/>
+      <selection pane="bottomRight" activeCell="I282" sqref="I282"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14489,6 +14498,33 @@
       <c r="I281" s="2" t="str">
         <f t="shared" si="15"/>
         <v>{"id":281,"title":"swimlane-brand-github-octocat","group":"dotnet","area":"swimlane","keywords":["brand","github","octocat","mascot"],"description":"GitHub Octocat.","publish":1}</v>
+      </c>
+    </row>
+    <row r="282" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A282" s="5">
+        <v>282</v>
+      </c>
+      <c r="C282" s="2" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D282" t="s">
+        <v>387</v>
+      </c>
+      <c r="E282" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F282" s="2" t="s">
+        <v>1035</v>
+      </c>
+      <c r="G282" s="2" t="s">
+        <v>1034</v>
+      </c>
+      <c r="H282" s="2">
+        <v>1</v>
+      </c>
+      <c r="I282" s="2" t="str">
+        <f t="shared" ref="I282" si="16">SUBSTITUTE(_xlfn.CONCAT("{'id':",A282,",'title':'",C282,"','group':'",D282,"','area':'",E282,"','keywords':['",SUBSTITUTE(F282," ","','"),"'],'description':'",G282,"','publish':",H282,"}"),"'","""")</f>
+        <v>{"id":282,"title":"swimlane-brand-microsoft","group":"dotnet","area":"swimlane","keywords":["brand","microsoft","logo"],"description":"Microsoft logo.","publish":1}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added VSCOM modal illustrations
</commit_message>
<xml_diff>
--- a/src/assets/data.xlsx
+++ b/src/assets/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\Code\vsimages\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40EAACA-3EDA-4568-86CF-A0001C792B8E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50CF9AD-DFA2-4D9D-9EF8-F57509814CB2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1806" uniqueCount="1036">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1821" uniqueCount="1046">
   <si>
     <t>SeattleSkyline</t>
   </si>
@@ -3145,6 +3145,36 @@
   </si>
   <si>
     <t>brand microsoft logo</t>
+  </si>
+  <si>
+    <t>modal-man-and-dog</t>
+  </si>
+  <si>
+    <t>modal-man-dog- rube-goldberg-machine</t>
+  </si>
+  <si>
+    <t>modal-subscribe-to-news-tips</t>
+  </si>
+  <si>
+    <t>modal</t>
+  </si>
+  <si>
+    <t>man laptop people dog work play</t>
+  </si>
+  <si>
+    <t>A man using a laptop, sitting on the ground with a dog.</t>
+  </si>
+  <si>
+    <t>man laptop people dog work play productivity rube goldberg machine</t>
+  </si>
+  <si>
+    <t>A man using a laptop, sitting on the ground with a dog. A Rube Goldberg's machine in the background.</t>
+  </si>
+  <si>
+    <t>woman people laptop subscribe email newsletter newspaper lightbulb tips envelope video tutorials</t>
+  </si>
+  <si>
+    <t>A woman using a laptop. Newsletter related icons floating around.</t>
   </si>
 </sst>
 </file>
@@ -6050,13 +6080,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K282"/>
+  <dimension ref="A1:K285"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B279" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B282" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I282" sqref="I282"/>
+      <selection pane="bottomRight" activeCell="I285" sqref="I284:I285"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14523,8 +14553,89 @@
         <v>1</v>
       </c>
       <c r="I282" s="2" t="str">
-        <f t="shared" ref="I282" si="16">SUBSTITUTE(_xlfn.CONCAT("{'id':",A282,",'title':'",C282,"','group':'",D282,"','area':'",E282,"','keywords':['",SUBSTITUTE(F282," ","','"),"'],'description':'",G282,"','publish':",H282,"}"),"'","""")</f>
+        <f t="shared" ref="I282:I283" si="16">SUBSTITUTE(_xlfn.CONCAT("{'id':",A282,",'title':'",C282,"','group':'",D282,"','area':'",E282,"','keywords':['",SUBSTITUTE(F282," ","','"),"'],'description':'",G282,"','publish':",H282,"}"),"'","""")</f>
         <v>{"id":282,"title":"swimlane-brand-microsoft","group":"dotnet","area":"swimlane","keywords":["brand","microsoft","logo"],"description":"Microsoft logo.","publish":1}</v>
+      </c>
+    </row>
+    <row r="283" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A283" s="5">
+        <v>283</v>
+      </c>
+      <c r="C283" s="2" t="s">
+        <v>1036</v>
+      </c>
+      <c r="D283" t="s">
+        <v>270</v>
+      </c>
+      <c r="E283" s="2" t="s">
+        <v>1039</v>
+      </c>
+      <c r="F283" s="2" t="s">
+        <v>1040</v>
+      </c>
+      <c r="G283" s="2" t="s">
+        <v>1041</v>
+      </c>
+      <c r="H283" s="2">
+        <v>1</v>
+      </c>
+      <c r="I283" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>{"id":283,"title":"modal-man-and-dog","group":"vscom","area":"modal","keywords":["man","laptop","people","dog","work","play"],"description":"A man using a laptop, sitting on the ground with a dog.","publish":1}</v>
+      </c>
+    </row>
+    <row r="284" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A284" s="5">
+        <v>284</v>
+      </c>
+      <c r="C284" s="2" t="s">
+        <v>1037</v>
+      </c>
+      <c r="D284" t="s">
+        <v>270</v>
+      </c>
+      <c r="E284" s="2" t="s">
+        <v>1039</v>
+      </c>
+      <c r="F284" s="2" t="s">
+        <v>1042</v>
+      </c>
+      <c r="G284" s="2" t="s">
+        <v>1043</v>
+      </c>
+      <c r="H284" s="2">
+        <v>1</v>
+      </c>
+      <c r="I284" s="2" t="str">
+        <f t="shared" ref="I284:I285" si="17">SUBSTITUTE(_xlfn.CONCAT("{'id':",A284,",'title':'",C284,"','group':'",D284,"','area':'",E284,"','keywords':['",SUBSTITUTE(F284," ","','"),"'],'description':'",G284,"','publish':",H284,"}"),"'","""")</f>
+        <v>{"id":284,"title":"modal-man-dog- rube-goldberg-machine","group":"vscom","area":"modal","keywords":["man","laptop","people","dog","work","play","productivity","rube","goldberg","machine"],"description":"A man using a laptop, sitting on the ground with a dog. A Rube Goldberg"s machine in the background.","publish":1}</v>
+      </c>
+    </row>
+    <row r="285" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A285" s="5">
+        <v>285</v>
+      </c>
+      <c r="C285" s="2" t="s">
+        <v>1038</v>
+      </c>
+      <c r="D285" t="s">
+        <v>270</v>
+      </c>
+      <c r="E285" s="2" t="s">
+        <v>1039</v>
+      </c>
+      <c r="F285" s="2" t="s">
+        <v>1044</v>
+      </c>
+      <c r="G285" s="2" t="s">
+        <v>1045</v>
+      </c>
+      <c r="H285" s="2">
+        <v>1</v>
+      </c>
+      <c r="I285" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v>{"id":285,"title":"modal-subscribe-to-news-tips","group":"vscom","area":"modal","keywords":["woman","people","laptop","subscribe","email","newsletter","newspaper","lightbulb","tips","envelope","video","tutorials"],"description":"A woman using a laptop. Newsletter related icons floating around.","publish":1}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new illustration for Live Share
</commit_message>
<xml_diff>
--- a/src/assets/data.xlsx
+++ b/src/assets/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\Code\vsimages\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC49C40-13A9-4C00-8F23-69A211FEDCF6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47AE3DAF-7454-4B72-AA6A-1BD7898A93B4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1821" uniqueCount="1046">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1826" uniqueCount="1049">
   <si>
     <t>SeattleSkyline</t>
   </si>
@@ -3175,6 +3175,15 @@
   </si>
   <si>
     <t>A man using a laptop, sitting on the ground with a dog. A Rube Goldberg machine in the background.</t>
+  </si>
+  <si>
+    <t>modal-joining-live-share-session</t>
+  </si>
+  <si>
+    <t>code developer editor collaborate share people computer monitor laptop</t>
+  </si>
+  <si>
+    <t>A developer joining a Live Share session.</t>
   </si>
 </sst>
 </file>
@@ -6080,13 +6089,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K285"/>
+  <dimension ref="A1:K286"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B282" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B283" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D285" sqref="D285"/>
+      <selection pane="bottomRight" activeCell="I286" sqref="I286"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14607,7 +14616,7 @@
         <v>1</v>
       </c>
       <c r="I284" s="2" t="str">
-        <f t="shared" ref="I284:I285" si="17">SUBSTITUTE(_xlfn.CONCAT("{'id':",A284,",'title':'",C284,"','group':'",D284,"','area':'",E284,"','keywords':['",SUBSTITUTE(F284," ","','"),"'],'description':'",G284,"','publish':",H284,"}"),"'","""")</f>
+        <f t="shared" ref="I284:I286" si="17">SUBSTITUTE(_xlfn.CONCAT("{'id':",A284,",'title':'",C284,"','group':'",D284,"','area':'",E284,"','keywords':['",SUBSTITUTE(F284," ","','"),"'],'description':'",G284,"','publish':",H284,"}"),"'","""")</f>
         <v>{"id":284,"title":"modal-man-dog- rube-goldberg-machine","group":"vscom","area":"modal","keywords":["man","laptop","people","dog","work","play","productivity","rube","goldberg","machine"],"description":"A man using a laptop, sitting on the ground with a dog. A Rube Goldberg machine in the background.","publish":1}</v>
       </c>
     </row>
@@ -14636,6 +14645,33 @@
       <c r="I285" s="2" t="str">
         <f t="shared" si="17"/>
         <v>{"id":285,"title":"modal-subscribe-to-news-tips","group":"vscom","area":"modal","keywords":["woman","people","laptop","subscribe","email","newsletter","newspaper","lightbulb","tips","envelope","video","tutorials"],"description":"A woman using a laptop. Newsletter related icons floating around.","publish":1}</v>
+      </c>
+    </row>
+    <row r="286" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A286" s="5">
+        <v>286</v>
+      </c>
+      <c r="C286" s="2" t="s">
+        <v>1046</v>
+      </c>
+      <c r="D286" t="s">
+        <v>270</v>
+      </c>
+      <c r="E286" s="2" t="s">
+        <v>1039</v>
+      </c>
+      <c r="F286" s="2" t="s">
+        <v>1047</v>
+      </c>
+      <c r="G286" s="2" t="s">
+        <v>1048</v>
+      </c>
+      <c r="H286" s="2">
+        <v>1</v>
+      </c>
+      <c r="I286" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v>{"id":286,"title":"modal-joining-live-share-session","group":"vscom","area":"modal","keywords":["code","developer","editor","collaborate","share","people","computer","monitor","laptop"],"description":"A developer joining a Live Share session.","publish":1}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new live share illustration
</commit_message>
<xml_diff>
--- a/src/assets/data.xlsx
+++ b/src/assets/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\Code\vsimages\src\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47AE3DAF-7454-4B72-AA6A-1BD7898A93B4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E356535-CCF7-426D-BC84-6FD503316111}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1826" uniqueCount="1049">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1831" uniqueCount="1052">
   <si>
     <t>SeattleSkyline</t>
   </si>
@@ -3184,6 +3184,15 @@
   </si>
   <si>
     <t>A developer joining a Live Share session.</t>
+  </si>
+  <si>
+    <t>modal-live-share-session-inactive</t>
+  </si>
+  <si>
+    <t>code developer editor collaborate share people computer monitor laptop wait inactive clock</t>
+  </si>
+  <si>
+    <t>A developer waiting to join a Live Share session but the session is inactive.</t>
   </si>
 </sst>
 </file>
@@ -6089,13 +6098,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K286"/>
+  <dimension ref="A1:K287"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B283" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I286" sqref="I286"/>
+      <selection pane="bottomRight" activeCell="F287" sqref="F287"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14672,6 +14681,33 @@
       <c r="I286" s="2" t="str">
         <f t="shared" si="17"/>
         <v>{"id":286,"title":"modal-joining-live-share-session","group":"vscom","area":"modal","keywords":["code","developer","editor","collaborate","share","people","computer","monitor","laptop"],"description":"A developer joining a Live Share session.","publish":1}</v>
+      </c>
+    </row>
+    <row r="287" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A287" s="5">
+        <v>287</v>
+      </c>
+      <c r="C287" s="2" t="s">
+        <v>1049</v>
+      </c>
+      <c r="D287" t="s">
+        <v>270</v>
+      </c>
+      <c r="E287" s="2" t="s">
+        <v>1039</v>
+      </c>
+      <c r="F287" s="2" t="s">
+        <v>1050</v>
+      </c>
+      <c r="G287" s="2" t="s">
+        <v>1051</v>
+      </c>
+      <c r="H287" s="2">
+        <v>1</v>
+      </c>
+      <c r="I287" s="2" t="str">
+        <f t="shared" ref="I287" si="18">SUBSTITUTE(_xlfn.CONCAT("{'id':",A287,",'title':'",C287,"','group':'",D287,"','area':'",E287,"','keywords':['",SUBSTITUTE(F287," ","','"),"'],'description':'",G287,"','publish':",H287,"}"),"'","""")</f>
+        <v>{"id":287,"title":"modal-live-share-session-inactive","group":"vscom","area":"modal","keywords":["code","developer","editor","collaborate","share","people","computer","monitor","laptop","wait","inactive","clock"],"description":"A developer waiting to join a Live Share session but the session is inactive.","publish":1}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added VSCOM value prop illustrations
</commit_message>
<xml_diff>
--- a/src/assets/data.xlsx
+++ b/src/assets/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cherr\Dropbox\Code\vsimages\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA345A3-AE9C-4ABB-9954-E875AE9A69A3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8F67D3-E8C6-4F6C-9E35-F43D0FE015C0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1861" uniqueCount="1066">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1876" uniqueCount="1076">
   <si>
     <t>SeattleSkyline</t>
   </si>
@@ -3235,6 +3235,36 @@
   </si>
   <si>
     <t>swimlane-subscribe-to-news-tips</t>
+  </si>
+  <si>
+    <t>prop-productive</t>
+  </si>
+  <si>
+    <t>prop-innovate</t>
+  </si>
+  <si>
+    <t>prop-modern</t>
+  </si>
+  <si>
+    <t>valueprop</t>
+  </si>
+  <si>
+    <t>Belt and gear.</t>
+  </si>
+  <si>
+    <t>A robot pressing a button.</t>
+  </si>
+  <si>
+    <t>innovative lightbulb idea insight beaker</t>
+  </si>
+  <si>
+    <t>A lightbulb and a beaker.</t>
+  </si>
+  <si>
+    <t>productivity machine belt process</t>
+  </si>
+  <si>
+    <t>modern technology robot machine</t>
   </si>
 </sst>
 </file>
@@ -6140,31 +6170,31 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K293"/>
+  <dimension ref="A1:K296"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B293" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I293" sqref="I2:I293"/>
+      <selection pane="bottomRight" activeCell="I296" sqref="I296"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="35.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="38.140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="13.265625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="35.86328125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="38.1328125" style="2" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
     <col min="5" max="5" width="18" style="2" customWidth="1"/>
-    <col min="6" max="6" width="33.7109375" style="2" customWidth="1"/>
-    <col min="7" max="8" width="20.7109375" style="2" customWidth="1"/>
-    <col min="9" max="10" width="24.140625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="33.140625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="66.42578125" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="2"/>
+    <col min="6" max="6" width="33.73046875" style="2" customWidth="1"/>
+    <col min="7" max="8" width="20.73046875" style="2" customWidth="1"/>
+    <col min="9" max="10" width="24.1328125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="33.1328125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="66.3984375" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="9.1328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="6" t="s">
         <v>201</v>
       </c>
@@ -6199,7 +6229,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -6233,7 +6263,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -6264,7 +6294,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\widget-you-dont-have-permission.svg</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -6295,7 +6325,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-charting-not-supported.svg</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -6326,7 +6356,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-custom-rules.svg</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -6357,7 +6387,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-get-back-to-recent-work.svg</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -6388,7 +6418,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-invalid-workitem-type.svg</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -6419,7 +6449,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-keep-an-eye-on-important-work.svg</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -6450,7 +6480,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-mention-someone.svg</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -6481,7 +6511,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-no-charts.svg</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -6512,7 +6542,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-unsaved-query.svg</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -6543,7 +6573,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-workitem-not-found.svg</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -6574,7 +6604,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-your-work-in-one-place.svg</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -6605,7 +6635,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-get-started-with-sprint.svg</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -6636,7 +6666,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-add-a-feed.svg</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -6667,7 +6697,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-connect-to-feed.svg</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -6698,7 +6728,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\general-no-results-found.svg</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -6729,7 +6759,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\hero-extend-vside.svg</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -6760,7 +6790,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-create-your-own-extension.svg</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -6791,7 +6821,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-marketplace.svg</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -6822,7 +6852,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-partner-program.svg</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -6853,7 +6883,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-what-are-extensions.svg</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -6884,7 +6914,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-add-product.svg</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -6915,7 +6945,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-configure-component-governance.svg</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -6946,7 +6976,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-release-management.svg</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -6977,7 +7007,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-this-repository-has-no-tags-yet.svg</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -7008,7 +7038,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-add-deployment-group.svg</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -7039,7 +7069,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-automate-build-definitions.svg</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -7070,7 +7100,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-choose-a-template.svg</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -7101,7 +7131,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-cloud-based-load-testing.svg</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -7132,7 +7162,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-favorites.svg</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -7163,7 +7193,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-get-everyone-on-same-page.svg</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -7194,7 +7224,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-no-plan.svg</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -7225,7 +7255,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-no-variable-groups.svg</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -7256,7 +7286,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-pull-request.svg</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -7287,7 +7317,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\hero-swiss-army-knife.svg</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -7318,7 +7348,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-all-your-code-hosted-free.svg</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -7349,7 +7379,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-any-client-any-platform.svg</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -7380,7 +7410,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-but-wait-theres-more.svg</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -7411,7 +7441,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-pricing.svg</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -7442,7 +7472,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-were-in-your-neighborhood.svg</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -7473,7 +7503,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\hero-pricing-calculator.svg</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -7504,7 +7534,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-you-have-no-organizations-yet.svg</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -7535,7 +7565,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\general-robot-errorcode-503.svg</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -7566,7 +7596,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\general-robot-error.svg</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -7597,7 +7627,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\general-robot-errorcode-400.svg</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -7628,7 +7658,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\general-robot-errorcode-401.svg</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -7659,7 +7689,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\general-robot-errorcode-403.svg</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -7690,7 +7720,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\general-robot-errorcode-404.svg</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -7721,7 +7751,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\general-robot-errorcode-500.svg</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -7752,7 +7782,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-no-assessments.svg</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -7783,7 +7813,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-initializing-test-results.svg</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -7814,7 +7844,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-no-work-scheduled.svg</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -7845,7 +7875,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-sprint-drag-n-drop.svg</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -7876,7 +7906,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-seamless-debugging-with-symbols.svg</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A56" s="5">
         <v>55</v>
       </c>
@@ -7907,7 +7937,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-xamarin-cross-platform.svg</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A57" s="5">
         <v>56</v>
       </c>
@@ -7938,7 +7968,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-azure-machine-learning.svg</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A58" s="5">
         <v>57</v>
       </c>
@@ -7969,7 +7999,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-cognitive-services.svg</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A59" s="5">
         <v>58</v>
       </c>
@@ -8000,7 +8030,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-congratulations-finished-setup.svg</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A60" s="5">
         <v>59</v>
       </c>
@@ -8031,7 +8061,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-cross-platform.svg</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A61" s="5">
         <v>60</v>
       </c>
@@ -8062,7 +8092,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-cryengine-game-development.svg</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A62" s="5">
         <v>61</v>
       </c>
@@ -8093,7 +8123,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-developer-meetup.svg</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A63" s="5">
         <v>62</v>
       </c>
@@ -8124,7 +8154,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-dotnet-core.svg</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A64" s="5">
         <v>63</v>
       </c>
@@ -8155,7 +8185,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-dotnet-enterprise.svg</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A65" s="5">
         <v>64</v>
       </c>
@@ -8186,7 +8216,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-download-target.svg</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A66" s="5">
         <v>65</v>
       </c>
@@ -8217,7 +8247,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-enterprise-customer-stories.svg</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A67" s="5">
         <v>66</v>
       </c>
@@ -8248,7 +8278,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-feedback-survey.svg</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A68" s="5">
         <v>67</v>
       </c>
@@ -8279,7 +8309,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-fsharp-data-science.svg</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A69" s="5">
         <v>68</v>
       </c>
@@ -8310,7 +8340,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-machine-learning-library.svg</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A70" s="5">
         <v>69</v>
       </c>
@@ -8341,7 +8371,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-one-consistent-api.svg</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A71" s="5">
         <v>70</v>
       </c>
@@ -8372,7 +8402,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-package-library.svg</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A72" s="5">
         <v>71</v>
       </c>
@@ -8403,7 +8433,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-programming-languages.svg</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A73" s="5">
         <v>72</v>
       </c>
@@ -8434,7 +8464,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-thank-you-for-downloading.svg</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A74" s="5">
         <v>73</v>
       </c>
@@ -8465,7 +8495,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-unity-game-development.svg</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A75" s="5">
         <v>74</v>
       </c>
@@ -8496,7 +8526,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-universal-windows-platform.svg</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A76" s="5">
         <v>75</v>
       </c>
@@ -8527,7 +8557,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-uwp-iot-core.svg</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A77" s="5">
         <v>76</v>
       </c>
@@ -8558,7 +8588,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-winform.svg</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A78" s="5">
         <v>77</v>
       </c>
@@ -8589,7 +8619,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-wpf.svg</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A79" s="5">
         <v>78</v>
       </c>
@@ -8620,7 +8650,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-xamarin.svg</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A80" s="5">
         <v>79</v>
       </c>
@@ -8651,7 +8681,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-dotnet-perf-diagram.svg</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A81" s="5">
         <v>80</v>
       </c>
@@ -8682,7 +8712,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\hero-snapshot-debugger.svg</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A82" s="5">
         <v>81</v>
       </c>
@@ -8713,7 +8743,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-collaborative-debugging.svg</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A83" s="5">
         <v>82</v>
       </c>
@@ -8744,7 +8774,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-collaborative-editing.svg</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A84" s="5">
         <v>83</v>
       </c>
@@ -8775,7 +8805,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-shared-full-context.svg</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A85" s="5">
         <v>84</v>
       </c>
@@ -8806,7 +8836,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-real-time-sharing.svg</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A86" s="5">
         <v>85</v>
       </c>
@@ -8837,7 +8867,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\blog-rocket-launch-timeline.svg</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A87" s="5">
         <v>86</v>
       </c>
@@ -8868,7 +8898,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\blog-vscode-metrics.svg</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A88" s="5">
         <v>87</v>
       </c>
@@ -8899,7 +8929,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\blog-vscode-roadmap.svg</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A89" s="5">
         <v>88</v>
       </c>
@@ -8930,7 +8960,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-monogame-game-development.svg</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A90" s="5">
         <v>89</v>
       </c>
@@ -8961,7 +8991,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-you-have-no-project.svg</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A91" s="5">
         <v>90</v>
       </c>
@@ -8992,7 +9022,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\hero-vsts-join-our-team.svg</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A92" s="5">
         <v>91</v>
       </c>
@@ -9023,7 +9053,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\elements-devices-1.svg</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A93" s="5">
         <v>92</v>
       </c>
@@ -9054,7 +9084,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\elements-devices-2.svg</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A94" s="5">
         <v>93</v>
       </c>
@@ -9085,7 +9115,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\elements-robots-1.svg</v>
       </c>
     </row>
-    <row r="95" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A95" s="5">
         <v>94</v>
       </c>
@@ -9116,7 +9146,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\elements-robots-2.svg</v>
       </c>
     </row>
-    <row r="96" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A96" s="5">
         <v>95</v>
       </c>
@@ -9147,7 +9177,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\elements-tools-1.svg</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A97" s="5">
         <v>96</v>
       </c>
@@ -9178,7 +9208,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\elements-tools-2.svg</v>
       </c>
     </row>
-    <row r="98" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A98" s="5">
         <v>97</v>
       </c>
@@ -9209,7 +9239,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\elements-vehicles-1.svg</v>
       </c>
     </row>
-    <row r="99" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A99" s="5">
         <v>98</v>
       </c>
@@ -9240,7 +9270,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\elements-vehicles-2.svg</v>
       </c>
     </row>
-    <row r="100" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A100" s="5">
         <v>99</v>
       </c>
@@ -9271,7 +9301,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\elements-vehicles-3.svg</v>
       </c>
     </row>
-    <row r="101" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A101" s="5">
         <v>100</v>
       </c>
@@ -9302,7 +9332,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-verify-analytics-views.svg</v>
       </c>
     </row>
-    <row r="102" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A102" s="5">
         <v>101</v>
       </c>
@@ -9333,7 +9363,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-analytics-views-error.svg</v>
       </c>
     </row>
-    <row r="103" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A103" s="5">
         <v>102</v>
       </c>
@@ -9364,7 +9394,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-analytics-views-valid.svg</v>
       </c>
     </row>
-    <row r="104" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A104" s="5">
         <v>103</v>
       </c>
@@ -9395,7 +9425,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-no-analytics-views.svg</v>
       </c>
     </row>
-    <row r="105" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A105" s="5">
         <v>104</v>
       </c>
@@ -9426,7 +9456,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-preparing-data.svg</v>
       </c>
     </row>
-    <row r="106" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A106" s="5">
         <v>105</v>
       </c>
@@ -9457,7 +9487,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\socialmedia-devops-youtube-header.svg</v>
       </c>
     </row>
-    <row r="107" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A107" s="5">
         <v>106</v>
       </c>
@@ -9488,7 +9518,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\socialmedia-devops-avatar.svg</v>
       </c>
     </row>
-    <row r="108" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A108" s="5">
         <v>107</v>
       </c>
@@ -9519,7 +9549,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\tile-self-hosted-server.svg</v>
       </c>
     </row>
-    <row r="109" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A109" s="5">
         <v>108</v>
       </c>
@@ -9550,7 +9580,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\tile-cloud-hosted-server.svg</v>
       </c>
     </row>
-    <row r="110" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A110" s="5">
         <v>109</v>
       </c>
@@ -9581,7 +9611,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\tile-integrate-with-cloud-services.svg</v>
       </c>
     </row>
-    <row r="111" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A111" s="5">
         <v>110</v>
       </c>
@@ -9612,7 +9642,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\general-folder.svg</v>
       </c>
     </row>
-    <row r="112" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A112" s="5">
         <v>111</v>
       </c>
@@ -9643,7 +9673,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-speed-gauge-comparison.svg</v>
       </c>
     </row>
-    <row r="113" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A113" s="5">
         <v>112</v>
       </c>
@@ -9674,7 +9704,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-speed-gauge-comparison-withtext.svg</v>
       </c>
     </row>
-    <row r="114" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A114" s="5">
         <v>113</v>
       </c>
@@ -9705,7 +9735,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-vside-lightbulb-intellisense.svg</v>
       </c>
     </row>
-    <row r="115" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A115" s="5">
         <v>114</v>
       </c>
@@ -9736,7 +9766,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-async-await-runners.svg</v>
       </c>
     </row>
-    <row r="116" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A116" s="5">
         <v>115</v>
       </c>
@@ -9767,7 +9797,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-barchart-skyline.svg</v>
       </c>
     </row>
-    <row r="117" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A117" s="5">
         <v>116</v>
       </c>
@@ -9798,7 +9828,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-barchart-skyline-withtext.svg</v>
       </c>
     </row>
-    <row r="118" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A118" s="5">
         <v>117</v>
       </c>
@@ -9829,7 +9859,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-contributors-around-world.svg</v>
       </c>
     </row>
-    <row r="119" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A119" s="5">
         <v>118</v>
       </c>
@@ -9860,7 +9890,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-contributors-around-world-withtext.svg</v>
       </c>
     </row>
-    <row r="120" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A120" s="5">
         <v>119</v>
       </c>
@@ -9891,7 +9921,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-dotnet-node-table.svg</v>
       </c>
     </row>
-    <row r="121" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A121" s="5">
         <v>120</v>
       </c>
@@ -9922,7 +9952,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-one-vs-many-tools.svg</v>
       </c>
     </row>
-    <row r="122" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A122" s="5">
         <v>121</v>
       </c>
@@ -9953,7 +9983,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-any-language.svg</v>
       </c>
     </row>
-    <row r="123" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A123" s="5">
         <v>122</v>
       </c>
@@ -9984,7 +10014,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-deploy-cross-platform.svg</v>
       </c>
     </row>
-    <row r="124" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A124" s="5">
         <v>123</v>
       </c>
@@ -10015,7 +10045,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-swiss-army-knife.svg</v>
       </c>
     </row>
-    <row r="125" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A125" s="5">
         <v>124</v>
       </c>
@@ -10046,7 +10076,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\hero-devops-conductor.svg</v>
       </c>
     </row>
-    <row r="126" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A126" s="5">
         <v>125</v>
       </c>
@@ -10077,7 +10107,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\blog-package-upstream-diagram-1.svg</v>
       </c>
     </row>
-    <row r="127" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A127" s="5">
         <v>126</v>
       </c>
@@ -10108,7 +10138,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\blog-package-upstream-diagram-2.svg</v>
       </c>
     </row>
-    <row r="128" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A128" s="5">
         <v>127</v>
       </c>
@@ -10139,7 +10169,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\blog-package-upstream-diagram-3.svg</v>
       </c>
     </row>
-    <row r="129" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A129" s="5">
         <v>128</v>
       </c>
@@ -10170,7 +10200,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\blog-package-upstream-diagram-4.svg</v>
       </c>
     </row>
-    <row r="130" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A130" s="5">
         <v>129</v>
       </c>
@@ -10201,7 +10231,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\willow-car-racing-get-ready.svg</v>
       </c>
     </row>
-    <row r="131" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A131" s="5">
         <v>130</v>
       </c>
@@ -10232,7 +10262,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\willow-rocket-get-ready.svg</v>
       </c>
     </row>
-    <row r="132" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A132" s="5">
         <v>131</v>
       </c>
@@ -10263,7 +10293,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\willow-bike-adventure.svg</v>
       </c>
     </row>
-    <row r="133" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A133" s="5">
         <v>132</v>
       </c>
@@ -10294,7 +10324,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\willow-bike-adventure-issue.svg</v>
       </c>
     </row>
-    <row r="134" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A134" s="5">
         <v>133</v>
       </c>
@@ -10325,7 +10355,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-no-dashboard.svg</v>
       </c>
     </row>
-    <row r="135" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A135" s="5">
         <v>134</v>
       </c>
@@ -10356,7 +10386,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\docs-gvfs-architecture.svg</v>
       </c>
     </row>
-    <row r="136" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A136" s="5">
         <v>135</v>
       </c>
@@ -10387,7 +10417,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\hero-vs-tools-for-azure.svg</v>
       </c>
     </row>
-    <row r="137" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A137" s="5">
         <v>136</v>
       </c>
@@ -10418,7 +10448,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-build-release-pipeline.svg</v>
       </c>
     </row>
-    <row r="138" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A138" s="5">
         <v>137</v>
       </c>
@@ -10449,7 +10479,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-build-release-monitor-activities.svg</v>
       </c>
     </row>
-    <row r="139" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A139" s="5">
         <v>138</v>
       </c>
@@ -10480,7 +10510,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-data-009.svg</v>
       </c>
     </row>
-    <row r="140" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A140" s="5">
         <v>139</v>
       </c>
@@ -10511,7 +10541,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-agriculture-001.svg</v>
       </c>
     </row>
-    <row r="141" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A141" s="5">
         <v>140</v>
       </c>
@@ -10542,7 +10572,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-001.svg</v>
       </c>
     </row>
-    <row r="142" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A142" s="5">
         <v>141</v>
       </c>
@@ -10573,7 +10603,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-002.svg</v>
       </c>
     </row>
-    <row r="143" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A143" s="5">
         <v>142</v>
       </c>
@@ -10604,7 +10634,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-003.svg</v>
       </c>
     </row>
-    <row r="144" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A144" s="5">
         <v>143</v>
       </c>
@@ -10635,7 +10665,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-004.svg</v>
       </c>
     </row>
-    <row r="145" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A145" s="5">
         <v>144</v>
       </c>
@@ -10666,7 +10696,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-005.svg</v>
       </c>
     </row>
-    <row r="146" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A146" s="5">
         <v>145</v>
       </c>
@@ -10697,7 +10727,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-006.svg</v>
       </c>
     </row>
-    <row r="147" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A147" s="5">
         <v>146</v>
       </c>
@@ -10728,7 +10758,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-007.svg</v>
       </c>
     </row>
-    <row r="148" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A148" s="5">
         <v>147</v>
       </c>
@@ -10759,7 +10789,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-008.svg</v>
       </c>
     </row>
-    <row r="149" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A149" s="5">
         <v>148</v>
       </c>
@@ -10790,7 +10820,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-009.svg</v>
       </c>
     </row>
-    <row r="150" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A150" s="5">
         <v>149</v>
       </c>
@@ -10821,7 +10851,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-010.svg</v>
       </c>
     </row>
-    <row r="151" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A151" s="5">
         <v>150</v>
       </c>
@@ -10852,7 +10882,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-011.svg</v>
       </c>
     </row>
-    <row r="152" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A152" s="5">
         <v>151</v>
       </c>
@@ -10883,7 +10913,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-012.svg</v>
       </c>
     </row>
-    <row r="153" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A153" s="5">
         <v>152</v>
       </c>
@@ -10914,7 +10944,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-013.svg</v>
       </c>
     </row>
-    <row r="154" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A154" s="5">
         <v>153</v>
       </c>
@@ -10945,7 +10975,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-014.svg</v>
       </c>
     </row>
-    <row r="155" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A155" s="5">
         <v>154</v>
       </c>
@@ -10976,7 +11006,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-015.svg</v>
       </c>
     </row>
-    <row r="156" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A156" s="5">
         <v>155</v>
       </c>
@@ -11007,7 +11037,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-016.svg</v>
       </c>
     </row>
-    <row r="157" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A157" s="5">
         <v>156</v>
       </c>
@@ -11038,7 +11068,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-017.svg</v>
       </c>
     </row>
-    <row r="158" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A158" s="5">
         <v>157</v>
       </c>
@@ -11069,7 +11099,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-001.svg</v>
       </c>
     </row>
-    <row r="159" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A159" s="5">
         <v>158</v>
       </c>
@@ -11100,7 +11130,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-002.svg</v>
       </c>
     </row>
-    <row r="160" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A160" s="5">
         <v>159</v>
       </c>
@@ -11131,7 +11161,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-003.svg</v>
       </c>
     </row>
-    <row r="161" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A161" s="5">
         <v>160</v>
       </c>
@@ -11162,7 +11192,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-004.svg</v>
       </c>
     </row>
-    <row r="162" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A162" s="5">
         <v>161</v>
       </c>
@@ -11193,7 +11223,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-005.svg</v>
       </c>
     </row>
-    <row r="163" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A163" s="5">
         <v>162</v>
       </c>
@@ -11224,7 +11254,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-006.svg</v>
       </c>
     </row>
-    <row r="164" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A164" s="5">
         <v>163</v>
       </c>
@@ -11255,7 +11285,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-007.svg</v>
       </c>
     </row>
-    <row r="165" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A165" s="5">
         <v>164</v>
       </c>
@@ -11286,7 +11316,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-008.svg</v>
       </c>
     </row>
-    <row r="166" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A166" s="5">
         <v>165</v>
       </c>
@@ -11317,7 +11347,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-009.svg</v>
       </c>
     </row>
-    <row r="167" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A167" s="5">
         <v>166</v>
       </c>
@@ -11348,7 +11378,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-010.svg</v>
       </c>
     </row>
-    <row r="168" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A168" s="5">
         <v>167</v>
       </c>
@@ -11379,7 +11409,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-011.svg</v>
       </c>
     </row>
-    <row r="169" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A169" s="5">
         <v>168</v>
       </c>
@@ -11410,7 +11440,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-012.svg</v>
       </c>
     </row>
-    <row r="170" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A170" s="5">
         <v>169</v>
       </c>
@@ -11441,7 +11471,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-013.svg</v>
       </c>
     </row>
-    <row r="171" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A171" s="5">
         <v>170</v>
       </c>
@@ -11472,7 +11502,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-collaboration-001.svg</v>
       </c>
     </row>
-    <row r="172" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A172" s="5">
         <v>171</v>
       </c>
@@ -11503,7 +11533,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-collaboration-002.svg</v>
       </c>
     </row>
-    <row r="173" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A173" s="5">
         <v>172</v>
       </c>
@@ -11534,7 +11564,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-collaboration-003.svg</v>
       </c>
     </row>
-    <row r="174" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A174" s="5">
         <v>173</v>
       </c>
@@ -11565,7 +11595,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-collaboration-005.svg</v>
       </c>
     </row>
-    <row r="175" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A175" s="5">
         <v>174</v>
       </c>
@@ -11596,7 +11626,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-collaboration-006.svg</v>
       </c>
     </row>
-    <row r="176" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A176" s="5">
         <v>175</v>
       </c>
@@ -11627,7 +11657,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-collaboration-007.svg</v>
       </c>
     </row>
-    <row r="177" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A177" s="5">
         <v>176</v>
       </c>
@@ -11658,7 +11688,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-collaboration-008.svg</v>
       </c>
     </row>
-    <row r="178" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A178" s="5">
         <v>177</v>
       </c>
@@ -11689,7 +11719,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-collaboration-009.svg</v>
       </c>
     </row>
-    <row r="179" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A179" s="5">
         <v>178</v>
       </c>
@@ -11720,7 +11750,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-collaboration-010.svg</v>
       </c>
     </row>
-    <row r="180" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A180" s="5">
         <v>179</v>
       </c>
@@ -11751,7 +11781,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-collaboration-011.svg</v>
       </c>
     </row>
-    <row r="181" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A181" s="5">
         <v>180</v>
       </c>
@@ -11782,7 +11812,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-communication-001.svg</v>
       </c>
     </row>
-    <row r="182" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A182" s="5">
         <v>181</v>
       </c>
@@ -11813,7 +11843,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-communication-002.svg</v>
       </c>
     </row>
-    <row r="183" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A183" s="5">
         <v>182</v>
       </c>
@@ -11844,7 +11874,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-consumer-001.svg</v>
       </c>
     </row>
-    <row r="184" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A184" s="5">
         <v>183</v>
       </c>
@@ -11875,7 +11905,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-consumer-002.svg</v>
       </c>
     </row>
-    <row r="185" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A185" s="5">
         <v>184</v>
       </c>
@@ -11906,7 +11936,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-data-001.svg</v>
       </c>
     </row>
-    <row r="186" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A186" s="5">
         <v>185</v>
       </c>
@@ -11937,7 +11967,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-data-002.svg</v>
       </c>
     </row>
-    <row r="187" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A187" s="5">
         <v>186</v>
       </c>
@@ -11968,7 +11998,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-data-003.svg</v>
       </c>
     </row>
-    <row r="188" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A188" s="5">
         <v>187</v>
       </c>
@@ -11999,7 +12029,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-data-004.svg</v>
       </c>
     </row>
-    <row r="189" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A189" s="5">
         <v>188</v>
       </c>
@@ -12030,7 +12060,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-data-005.svg</v>
       </c>
     </row>
-    <row r="190" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A190" s="5">
         <v>189</v>
       </c>
@@ -12061,7 +12091,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-data-006.svg</v>
       </c>
     </row>
-    <row r="191" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A191" s="5">
         <v>190</v>
       </c>
@@ -12092,7 +12122,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-data-007.svg</v>
       </c>
     </row>
-    <row r="192" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A192" s="5">
         <v>191</v>
       </c>
@@ -12123,7 +12153,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-data-008.svg</v>
       </c>
     </row>
-    <row r="193" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A193" s="5">
         <v>192</v>
       </c>
@@ -12154,7 +12184,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-feature-not-configured.svg</v>
       </c>
     </row>
-    <row r="194" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A194" s="5">
         <v>193</v>
       </c>
@@ -12185,7 +12215,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-boxes-and-devices.svg</v>
       </c>
     </row>
-    <row r="195" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A195" s="5">
         <v>194</v>
       </c>
@@ -12216,7 +12246,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-butler-ide.svg</v>
       </c>
     </row>
-    <row r="196" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A196" s="5">
         <v>195</v>
       </c>
@@ -12247,7 +12277,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-code-or-gui.svg</v>
       </c>
     </row>
-    <row r="197" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A197" s="5">
         <v>196</v>
       </c>
@@ -12278,7 +12308,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-data-analytics-pipeline.svg</v>
       </c>
     </row>
-    <row r="198" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A198" s="5">
         <v>197</v>
       </c>
@@ -12309,7 +12339,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-developer-scenarios.svg</v>
       </c>
     </row>
-    <row r="199" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A199" s="5">
         <v>198</v>
       </c>
@@ -12340,7 +12370,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-machine-learning-books-lab.svg</v>
       </c>
     </row>
-    <row r="200" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A200" s="5">
         <v>199</v>
       </c>
@@ -12371,7 +12401,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-machine-learning-extensible.svg</v>
       </c>
     </row>
-    <row r="201" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A201" s="5">
         <v>200</v>
       </c>
@@ -12402,7 +12432,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-machine-learning-lightbulb-hand.svg</v>
       </c>
     </row>
-    <row r="202" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A202" s="5">
         <v>201</v>
       </c>
@@ -12433,7 +12463,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-necessary-learner-tools.svg</v>
       </c>
     </row>
-    <row r="203" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A203" s="5">
         <v>202</v>
       </c>
@@ -12464,7 +12494,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-share-code-snippets.svg</v>
       </c>
     </row>
-    <row r="204" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A204" s="5">
         <v>203</v>
       </c>
@@ -12495,7 +12525,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-machine-learning-proven-extensible.svg</v>
       </c>
     </row>
-    <row r="205" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A205" s="5">
         <v>204</v>
       </c>
@@ -12526,7 +12556,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-machine-learning-pipeline.svg</v>
       </c>
     </row>
-    <row r="206" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A206" s="5">
         <v>205</v>
       </c>
@@ -12557,7 +12587,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-machine-learning-for-dotnet.svg</v>
       </c>
     </row>
-    <row r="207" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A207" s="5">
         <v>206</v>
       </c>
@@ -12588,7 +12618,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-machine-learning-brain-lightbulb.svg</v>
       </c>
     </row>
-    <row r="208" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A208" s="5">
         <v>207</v>
       </c>
@@ -12619,7 +12649,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\wizard-upgrade-from-xml-to-inheritance.svg</v>
       </c>
     </row>
-    <row r="209" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A209" s="5">
         <v>208</v>
       </c>
@@ -12646,7 +12676,7 @@
         <v>{"id":208,"title":"als-confirm-vm-specs","group":"als","area":"dashboard","keywords":["azure","lab","services","vm","virtual","machine","computer","gear","magnifier"],"description":"Used in Azure Lab Services classroom scenario onboarding UI.","publish":1}</v>
       </c>
     </row>
-    <row r="210" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A210" s="5">
         <v>209</v>
       </c>
@@ -12673,7 +12703,7 @@
         <v>{"id":209,"title":"als-install-artifacts-to-vm","group":"als","area":"dashboard","keywords":["azure","lab","services","vm","virtual","machine","install","app","package","cube","box","hook"],"description":"Used in Azure Lab Services classroom scenario onboarding UI.","publish":1}</v>
       </c>
     </row>
-    <row r="211" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A211" s="5">
         <v>210</v>
       </c>
@@ -12700,7 +12730,7 @@
         <v>{"id":210,"title":"als-decide-user-count","group":"als","area":"dashboard","keywords":["azure","lab","services","vm","virtual","machine","user","count","computer"],"description":"Used in Azure Lab Services classroom scenario onboarding UI.","publish":1}</v>
       </c>
     </row>
-    <row r="212" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A212" s="5">
         <v>211</v>
       </c>
@@ -12727,7 +12757,7 @@
         <v>{"id":211,"title":"als-set-policy-schedule","group":"als","area":"dashboard","keywords":["azure","lab","services","vm","virtual","machine","schedule","time","date","calendar","usage","analytics","chart"],"description":"Used in Azure Lab Services classroom scenario onboarding UI.","publish":1}</v>
       </c>
     </row>
-    <row r="213" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A213" s="5">
         <v>212</v>
       </c>
@@ -12754,7 +12784,7 @@
         <v>{"id":212,"title":"als-publish-vm","group":"als","area":"dashboard","keywords":["azure","lab","services","vm","virtual","machine","publish","url","send","computer","paper","plane"],"description":"Used in Azure Lab Services classroom scenario onboarding UI.","publish":1}</v>
       </c>
     </row>
-    <row r="214" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A214" s="5">
         <v>213</v>
       </c>
@@ -12781,7 +12811,7 @@
         <v>{"id":213,"title":"als-get-azure-subscription","group":"als","area":"frontdoor","keywords":["azure","lab","services","sign","up","subscription"],"description":"Get an Azure subscription.","publish":1}</v>
       </c>
     </row>
-    <row r="215" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A215" s="5">
         <v>214</v>
       </c>
@@ -12808,7 +12838,7 @@
         <v>{"id":214,"title":"als-add-lab-account","group":"als","area":"frontdoor","keywords":["azure","lab","services","cloud","add","lab","beaker"],"description":"Add lab account to Azure subscription.","publish":1}</v>
       </c>
     </row>
-    <row r="216" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A216" s="5">
         <v>215</v>
       </c>
@@ -12835,7 +12865,7 @@
         <v>{"id":215,"title":"als-create-lab","group":"als","area":"frontdoor","keywords":["azure","lab","services","add","computer","beaker","create"],"description":"Create your lab of VMs.","publish":1}</v>
       </c>
     </row>
-    <row r="217" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A217" s="5">
         <v>217</v>
       </c>
@@ -12862,7 +12892,7 @@
         <v>{"id":217,"title":"swimlane-ml-load-data","group":"dotnet","area":"swimlane","keywords":["machine","learning","load","data","import","funnel","raw"],"description":"Raw data being loaded into the pipeline.","publish":1}</v>
       </c>
     </row>
-    <row r="218" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A218" s="5">
         <v>218</v>
       </c>
@@ -12889,7 +12919,7 @@
         <v>{"id":218,"title":"swimlane-ml-transform-data","group":"dotnet","area":"swimlane","keywords":["machine","learning","transform","data","output","funnel","organize"],"description":"Data is being transformed and organized.","publish":1}</v>
       </c>
     </row>
-    <row r="219" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A219" s="5">
         <v>219</v>
       </c>
@@ -12916,7 +12946,7 @@
         <v>{"id":219,"title":"swimlane-ml-choose-algorithms","group":"dotnet","area":"swimlane","keywords":["machine","learning","fit","model","algorithm","grid","data"],"description":"Choose algorithms to fit data and develop models.","publish":1}</v>
       </c>
     </row>
-    <row r="220" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A220" s="5">
         <v>220</v>
       </c>
@@ -12943,7 +12973,7 @@
         <v>{"id":220,"title":"swimlane-ml-train-model","group":"dotnet","area":"swimlane","keywords":["machine","learning","data","train","model","prediction"],"description":"Train models to make prediction.","publish":1}</v>
       </c>
     </row>
-    <row r="221" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A221" s="5">
         <v>221</v>
       </c>
@@ -12970,7 +13000,7 @@
         <v>{"id":221,"title":"swimlane-ml-evaluate-model","group":"dotnet","area":"swimlane","keywords":["machine","learning","evaluate","model","measure","magnifier"],"description":"Evaluate and validate the model.","publish":1}</v>
       </c>
     </row>
-    <row r="222" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A222" s="5">
         <v>222</v>
       </c>
@@ -12997,7 +13027,7 @@
         <v>{"id":222,"title":"swimlane-ml-deploy-model","group":"dotnet","area":"swimlane","keywords":["machine","learning","deploy","model","parachute"],"description":"Use the model in applications.","publish":1}</v>
       </c>
     </row>
-    <row r="223" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A223" s="5">
         <v>223</v>
       </c>
@@ -13024,7 +13054,7 @@
         <v>{"id":223,"title":"swimlane-functional-programming-machine","group":"dotnet","area":"swimlane","keywords":["functional","programming","machine","fx","input","output"],"description":"Input going through a machine and output comes out. Used to represent functional programming.","publish":1}</v>
       </c>
     </row>
-    <row r="224" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A224" s="5">
         <v>224</v>
       </c>
@@ -13051,7 +13081,7 @@
         <v>{"id":224,"title":"swimlane-one-consistent-api-purple","group":"dotnet","area":"swimlane","keywords":["one","api","consistent","people","tool","library","book","light","bulb","idea","ui","code"],"description":"A person surrounded by multiple developer tools.","publish":1}</v>
       </c>
     </row>
-    <row r="225" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A225" s="5">
         <v>225</v>
       </c>
@@ -13078,7 +13108,7 @@
         <v>{"id":225,"title":"swimlane-teamwork-climb-mountain","group":"dotnet","area":"swimlane","keywords":["team","people","teamwork","collaboration","climb","mountain","outdoor"],"description":"A team climbing mountain together.","publish":1}</v>
       </c>
     </row>
-    <row r="226" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A226" s="5">
         <v>226</v>
       </c>
@@ -13105,7 +13135,7 @@
         <v>{"id":226,"title":"swimlane-toolchest-with-power-drill","group":"dotnet","area":"swimlane","keywords":["tools","sdk","toolbox","toolchest","power","drill","wrench","plier"],"description":"A toolchest stuffed with tools.","publish":1}</v>
       </c>
     </row>
-    <row r="227" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A227" s="5">
         <v>227</v>
       </c>
@@ -13132,7 +13162,7 @@
         <v>{"id":227,"title":"swimlane-tools-for-all-platforms","group":"dotnet","area":"swimlane","keywords":["tools","cross","platform","people","man","mac","windows","linux"],"description":"A developer and devices running Mac, Windows and Linux platforms.","publish":1}</v>
       </c>
     </row>
-    <row r="228" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A228" s="5">
         <v>228</v>
       </c>
@@ -13159,7 +13189,7 @@
         <v>{"id":228,"title":"swimlane-welcome-to-the-community","group":"dotnet","area":"swimlane","keywords":["people","person","man","woman","community","developer","welcome","join","open","source","team","work"],"description":"Developer community working together and welcoming new memebers.","publish":1}</v>
       </c>
     </row>
-    <row r="229" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A229" s="5">
         <v>229</v>
       </c>
@@ -13186,7 +13216,7 @@
         <v>{"id":229,"title":"devblog-mobile-app-center","group":"devblog","area":"thumbnail","keywords":["mobile","development","app","center","cloud","device","phone","laptop","xamarin","visual","studio","code"],"description":"Using Visual Studio and App Center for mobile development.","publish":1}</v>
       </c>
     </row>
-    <row r="230" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A230" s="5">
         <v>230</v>
       </c>
@@ -13213,7 +13243,7 @@
         <v>{"id":230,"title":"als-lab-empty-state","group":"als","area":"zerodata","keywords":["azure","lab","vm","virtual","machine","empty","dotted","line","woman","people","question","mark","computer"],"description":"Used for Azure Lab Services empty state when there is no VM in the lab.","publish":1}</v>
       </c>
     </row>
-    <row r="231" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A231" s="5">
         <v>231</v>
       </c>
@@ -13240,7 +13270,7 @@
         <v>{"id":231,"title":"als-waiting-beaker","group":"als","area":"wizard","keywords":["azure","lab","vm","beaker","waiting"],"description":"Used for Azure Lab Services waiting screens.","publish":1}</v>
       </c>
     </row>
-    <row r="232" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A232" s="5">
         <v>232</v>
       </c>
@@ -13267,7 +13297,7 @@
         <v>{"id":232,"title":"als-take-notes","group":"als","area":"wizard","keywords":["azure","lab","vm","note","sticky","pencil","write","credential"],"description":"Used for Azure Lab Services take notes of credentials wizard.","publish":1}</v>
       </c>
     </row>
-    <row r="233" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A233" s="5">
         <v>233</v>
       </c>
@@ -13294,7 +13324,7 @@
         <v>{"id":233,"title":"devblog-debug","group":"devblog","area":"thumbnail","keywords":["debug","magnifier","bug","code"],"description":"A magnifier looking for bugs in code.","publish":1}</v>
       </c>
     </row>
-    <row r="234" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A234" s="5">
         <v>234</v>
       </c>
@@ -13321,7 +13351,7 @@
         <v>{"id":234,"title":"swimlane-try-dotnet-features","group":"dotnet","area":"swimlane","keywords":["features","javascript","github","editor","code","theme","customize","paint","color","lightbulb","woman","people"],"description":"Try .NET features GitHub integration, customizable theme and JavaScript support.","publish":1}</v>
       </c>
     </row>
-    <row r="235" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A235" s="5">
         <v>235</v>
       </c>
@@ -13348,7 +13378,7 @@
         <v>{"id":235,"title":"swimlane-customize-editor-theme","group":"dotnet","area":"swimlane","keywords":["customize","editor","paint","brush","color","theme"],"description":"Customize Try .NET editor theme.","publish":1}</v>
       </c>
     </row>
-    <row r="236" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A236" s="5">
         <v>236</v>
       </c>
@@ -13375,7 +13405,7 @@
         <v>{"id":236,"title":"swimlane-embed-github-snippet","group":"dotnet","area":"swimlane","keywords":["embed","github","snippet","code","browser"],"description":"Load GitHub gists with Try .NET to edit code in browser.","publish":1}</v>
       </c>
     </row>
-    <row r="237" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A237" s="5">
         <v>237</v>
       </c>
@@ -13402,7 +13432,7 @@
         <v>{"id":237,"title":"swimlane-feature-tree-with-people","group":"dotnet","area":"swimlane","keywords":["tree","branch","node","feature","people"],"description":"See what people are creating with Try .NET.","publish":1}</v>
       </c>
     </row>
-    <row r="238" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A238" s="5">
         <v>238</v>
       </c>
@@ -13429,7 +13459,7 @@
         <v>{"id":238,"title":"hero-azure-notebooks","group":"notebooks","area":"hero","keywords":["azure","notebooks","data","science","charts","people","lab"],"description":"An open notebook with people working on different domains of data science.","publish":1}</v>
       </c>
     </row>
-    <row r="239" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A239" s="5">
         <v>239</v>
       </c>
@@ -13456,7 +13486,7 @@
         <v>{"id":239,"title":"spot-azure-accessible-everywhere","group":"notebooks","area":"spot","keywords":["azure","globe","cloud"],"description":"Azure Cloud Services accessible from anywhere in the world.","publish":1}</v>
       </c>
     </row>
-    <row r="240" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A240" s="5">
         <v>240</v>
       </c>
@@ -13483,7 +13513,7 @@
         <v>{"id":240,"title":"spot-notebooks-languages","group":"notebooks","area":"spot","keywords":["notebooks","language"],"description":"Azure Notebooks supports multiple languages.","publish":1}</v>
       </c>
     </row>
-    <row r="241" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A241" s="5">
         <v>241</v>
       </c>
@@ -13510,7 +13540,7 @@
         <v>{"id":241,"title":"spot-scientist-developer-student","group":"notebooks","area":"spot","keywords":["people","scientist","developer","student","lab","microscope","tool","engineering","cap","education"],"description":"Use Azure Notebooks for many workspaces and scenarios.","publish":1}</v>
       </c>
     </row>
-    <row r="242" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A242" s="5">
         <v>242</v>
       </c>
@@ -13537,7 +13567,7 @@
         <v>{"id":242,"title":"swimlane-migrate-to-azure","group":"dotnet","area":"swimlane","keywords":["migrate","azure","cloud","helicopter","move","transfer"],"description":"Migrate existing .NET apps to Azure.","publish":1}</v>
       </c>
     </row>
-    <row r="243" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A243" s="5">
         <v>243</v>
       </c>
@@ -13564,7 +13594,7 @@
         <v>{"id":243,"title":"swimlane-serverless-computing","group":"dotnet","area":"swimlane","keywords":["serverless","computing","unplug","network","cloud","computer","device","laptop","desktop","pc","web"],"description":"Serverless computing with .NET","publish":1}</v>
       </c>
     </row>
-    <row r="244" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A244" s="5">
         <v>244</v>
       </c>
@@ -13591,7 +13621,7 @@
         <v>{"id":244,"title":"swimlane-web-app-tools-library","group":"dotnet","area":"swimlane","keywords":["toolbox","tool","hammer","utility","wrench","pencil","clipboard","book","library"],"description":"Blue toolbox and books.","publish":1}</v>
       </c>
     </row>
-    <row r="245" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A245" s="5">
         <v>245</v>
       </c>
@@ -13618,7 +13648,7 @@
         <v>{"id":245,"title":"swimlane-build-cloud-apps","group":"dotnet","area":"swimlane","keywords":["build","forklift","box","container","cloud","scalable","people"],"description":"Build modern scalable cloud apps with .NET","publish":1}</v>
       </c>
     </row>
-    <row r="246" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A246" s="5">
         <v>246</v>
       </c>
@@ -13645,7 +13675,7 @@
         <v>{"id":246,"title":"swimlane-docker-container-support","group":"dotnet","area":"swimlane","keywords":["docker","cloud","container","ship","port","city","skyline","computer","laptop"],"description":"Ship with containers to represent Docker containers.","publish":1}</v>
       </c>
     </row>
-    <row r="247" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A247" s="5">
         <v>247</v>
       </c>
@@ -13672,7 +13702,7 @@
         <v>{"id":247,"title":"swimlane-global-data-storage","group":"dotnet","area":"swimlane","keywords":["data","storage","database","globe","duplicate","world"],"description":"Data storage accessible from everywhere in the world.","publish":1}</v>
       </c>
     </row>
-    <row r="248" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A248" s="5">
         <v>248</v>
       </c>
@@ -13699,7 +13729,7 @@
         <v>{"id":248,"title":"swimlane-security","group":"dotnet","area":"swimlane","keywords":["security","guard","camera","safe","secure"],"description":"A safety guard protecting a safe.","publish":1}</v>
       </c>
     </row>
-    <row r="249" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A249" s="5">
         <v>249</v>
       </c>
@@ -13726,7 +13756,7 @@
         <v>{"id":249,"title":"swimlane-angular-react-spa","group":"dotnet","area":"swimlane","keywords":["angular","react","spa","single","page","application","website"],"description":"React and Angular logo and single page web app.","publish":1}</v>
       </c>
     </row>
-    <row r="250" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A250" s="5">
         <v>250</v>
       </c>
@@ -13753,7 +13783,7 @@
         <v>{"id":250,"title":"swimlane-build-scalable-web-apps","group":"dotnet","area":"swimlane","keywords":["build","scalable","web","app","page","truck","box","people"],"description":"A worker loading boxes from truck to a web page.","publish":1}</v>
       </c>
     </row>
-    <row r="251" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A251" s="5">
         <v>251</v>
       </c>
@@ -13780,7 +13810,7 @@
         <v>{"id":251,"title":"swimlane-model-view-controller","group":"dotnet","area":"swimlane","keywords":["mvc","model","view","controller","data","gear","presentation","theme","paint","bucket","brush","design","frontend","backend","stack"],"description":"MVC illustration.","publish":1}</v>
       </c>
     </row>
-    <row r="252" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A252" s="5">
         <v>252</v>
       </c>
@@ -13807,7 +13837,7 @@
         <v>{"id":252,"title":"swimlane-seamless-data-integration","group":"dotnet","area":"swimlane","keywords":["data","database","orbit"],"description":"Seamless data integration.","publish":1}</v>
       </c>
     </row>
-    <row r="253" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A253" s="5">
         <v>253</v>
       </c>
@@ -13834,7 +13864,7 @@
         <v>{"id":253,"title":"swimlane-authentication-authorization","group":"dotnet","area":"swimlane","keywords":["authentication","authorization","password","login","key","lock","badge","access","key","chain"],"description":"A key chain with several authentication objects.","publish":1}</v>
       </c>
     </row>
-    <row r="254" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A254" s="5">
         <v>254</v>
       </c>
@@ -13861,7 +13891,7 @@
         <v>{"id":254,"title":"swimlane-rest-api","group":"dotnet","area":"swimlane","keywords":["rest","restful","api","json","bracket","data","database","interface","connect","device","platform"],"description":"Used to represent REST api.","publish":1}</v>
       </c>
     </row>
-    <row r="255" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A255" s="5">
         <v>255</v>
       </c>
@@ -13888,7 +13918,7 @@
         <v>{"id":255,"title":"swimlane-secure-chat-app","group":"dotnet","area":"swimlane","keywords":["lock","secure","chat","people","avatar","message"],"description":"An IM app with encrypted conversation.","publish":1}</v>
       </c>
     </row>
-    <row r="256" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A256" s="5">
         <v>256</v>
       </c>
@@ -13915,7 +13945,7 @@
         <v>{"id":256,"title":"swimlane-multiplayer-game","group":"dotnet","area":"swimlane","keywords":["game","multi","player","people","xbox","tv"],"description":"A man playing real-time multiplayer video game with a woman.","publish":1}</v>
       </c>
     </row>
-    <row r="257" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A257" s="5">
         <v>257</v>
       </c>
@@ -13942,7 +13972,7 @@
         <v>{"id":257,"title":"swimlane-mvc-scenario","group":"dotnet","area":"swimlane","keywords":["model","view","controller","mvc","layer","tier","stack","web","app","design","data","people"],"description":"Model-View-Controller explained with illustrated example.","publish":1}</v>
       </c>
     </row>
-    <row r="258" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A258" s="5">
         <v>258</v>
       </c>
@@ -13969,7 +13999,7 @@
         <v>{"id":258,"title":"swimlane-real-time-chat-app","group":"dotnet","area":"swimlane","keywords":["real","time","chat","app","people","tablet","device"],"description":"A woman using a laptop to chat with a man using tablet.","publish":1}</v>
       </c>
     </row>
-    <row r="259" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A259" s="5">
         <v>259</v>
       </c>
@@ -13996,7 +14026,7 @@
         <v>{"id":259,"title":"swimlane-signalr-hub","group":"dotnet","area":"swimlane","keywords":["signalr","hub","server","device","phone","mobile","tablet","browser","computer","laptop"],"description":"A server hub with connectors to multiple devices.","publish":1}</v>
       </c>
     </row>
-    <row r="260" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A260" s="5">
         <v>260</v>
       </c>
@@ -14023,7 +14053,7 @@
         <v>{"id":260,"title":"swimlane-azure-signalr-logo","group":"dotnet","area":"swimlane","keywords":["azure","signalr","logo"],"description":"Azure SignalR brand icon.","publish":1}</v>
       </c>
     </row>
-    <row r="261" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A261" s="5">
         <v>261</v>
       </c>
@@ -14050,7 +14080,7 @@
         <v>{"id":261,"title":"swimlane-chat-app-multiplatform","group":"dotnet","area":"swimlane","keywords":["chat","app","multi","platform","device","people"],"description":"A woman using the same chat app available on multiple devices.","publish":1}</v>
       </c>
     </row>
-    <row r="262" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A262" s="5">
         <v>262</v>
       </c>
@@ -14077,7 +14107,7 @@
         <v>{"id":262,"title":"swimlane-fast-performance-gauge","group":"dotnet","area":"swimlane","keywords":["performance","race","car","gauge","speed","fast"],"description":"A car racing themed background with a speed gauge.","publish":1}</v>
       </c>
     </row>
-    <row r="263" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A263" s="5">
         <v>263</v>
       </c>
@@ -14104,7 +14134,7 @@
         <v>{"id":263,"title":"vsmac-installer-screen","group":"vsmac","area":"splashscreen","keywords":["space","galaxy","cloud","people","work","desk","install","download","waiting"],"description":"Two people playing with paper plane while waiting for installation. Space theme background.","publish":1}</v>
       </c>
     </row>
-    <row r="264" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A264" s="5">
         <v>264</v>
       </c>
@@ -14131,7 +14161,7 @@
         <v>{"id":264,"title":"hero-vs-enterprise-sku","group":"vscom","area":"hero","keywords":["small","team","free","community","collaboration","rocket","sketch","blueprint","hands"],"description":"Small team designing rocket collaboratively.","publish":1}</v>
       </c>
     </row>
-    <row r="265" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A265" s="5">
         <v>265</v>
       </c>
@@ -14158,7 +14188,7 @@
         <v>{"id":265,"title":"hero-vs-professional-sku","group":"vscom","area":"hero","keywords":["medium","team","professional","build","collaboration","rocket","robot","engineer"],"description":"Medium size professional engineers building rocket.","publish":1}</v>
       </c>
     </row>
-    <row r="266" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A266" s="5">
         <v>266</v>
       </c>
@@ -14185,7 +14215,7 @@
         <v>{"id":266,"title":"hero-vs-community-sku","group":"vscom","area":"hero","keywords":["enterprise","company","large","scale","buildings","process","rocket","workflow","truck"],"description":"Big enterprise mass producing rockets.","publish":1}</v>
       </c>
     </row>
-    <row r="267" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A267" s="5">
         <v>267</v>
       </c>
@@ -14212,7 +14242,7 @@
         <v>{"id":267,"title":"swimlane-build-scalable-apps","group":"dotnet","area":"swimlane","keywords":["build","scalable","building","crane","construction","scalability","stack","city","tree"],"description":"A construction crane loading stacks to build a skyscraper.","publish":1}</v>
       </c>
     </row>
-    <row r="268" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A268" s="5">
         <v>268</v>
       </c>
@@ -14239,7 +14269,7 @@
         <v>{"id":268,"title":"swimlane-docker-three-platforms","group":"dotnet","area":"swimlane","keywords":["docker","platform","os","windows","linux","macos","ship","container"],"description":"A freight ship with containers running on Windows, Linux and macOS.","publish":1}</v>
       </c>
     </row>
-    <row r="269" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A269" s="5">
         <v>269</v>
       </c>
@@ -14266,7 +14296,7 @@
         <v>{"id":269,"title":"swimlane-dotnet-compatible-with-other-tools","group":"dotnet","area":"swimlane","keywords":["dotnet","module","microservices","cube","plug","compatible","side","by","side","tools","stacks","people"],"description":".NET works side-by-side with other technology stacks.","publish":1}</v>
       </c>
     </row>
-    <row r="270" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A270" s="5">
         <v>270</v>
       </c>
@@ -14293,7 +14323,7 @@
         <v>{"id":270,"title":"swimlane-microservices-build","group":"dotnet","area":"swimlane","keywords":["microservices","build","module","truck","people","load","blocks"],"description":"People integrating microservice modules to make complete products.","publish":1}</v>
       </c>
     </row>
-    <row r="271" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A271" s="5">
         <v>271</v>
       </c>
@@ -14320,7 +14350,7 @@
         <v>{"id":271,"title":"swimlane-microservices-modules","group":"dotnet","area":"swimlane","keywords":["microservices","building","blocks","modules","cubes","plug","connect","integrate"],"description":"Microservices building blocks.","publish":1}</v>
       </c>
     </row>
-    <row r="272" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A272" s="5">
         <v>272</v>
       </c>
@@ -14347,7 +14377,7 @@
         <v>{"id":272,"title":"swimlane-brand-docker","group":"dotnet","area":"swimlane","keywords":["docker","brand","logo"],"description":"Docker logo","publish":1}</v>
       </c>
     </row>
-    <row r="273" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A273" s="5">
         <v>273</v>
       </c>
@@ -14374,7 +14404,7 @@
         <v>{"id":273,"title":"swimlane-event-driven-programming","group":"dotnet","area":"swimlane","keywords":["winform","event","trigger","click","button","control","sync","server","gear"],"description":"Event triggered in the presentation tier and passed to server.","publish":1}</v>
       </c>
     </row>
-    <row r="274" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A274" s="5">
         <v>274</v>
       </c>
@@ -14401,7 +14431,7 @@
         <v>{"id":274,"title":"swimlane-razor-cross-platform","group":"dotnet","area":"swimlane","keywords":["razor","@","html","cross","platform","windows","linux","macos","coffee","mugs","cups","tea"],"description":"Razor pages works across multiple platforms.","publish":1}</v>
       </c>
     </row>
-    <row r="275" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A275" s="5">
         <v>275</v>
       </c>
@@ -14428,7 +14458,7 @@
         <v>{"id":275,"title":"swimlane-webform","group":"dotnet","area":"swimlane","keywords":["webform","control","drag","drop","pencil","button","window","dialog"],"description":"Drag and drop designer for building Webform applications.","publish":1}</v>
       </c>
     </row>
-    <row r="276" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A276" s="5">
         <v>276</v>
       </c>
@@ -14455,7 +14485,7 @@
         <v>{"id":276,"title":"swimlane-webform-control-library","group":"dotnet","area":"swimlane","keywords":["webform","control","button","dropdown","textbox","radio","button","checkbox"],"description":"A large library of webform controls.","publish":1}</v>
       </c>
     </row>
-    <row r="277" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A277" s="5">
         <v>277</v>
       </c>
@@ -14482,7 +14512,7 @@
         <v>{"id":277,"title":"swimlane-webform-data-integration","group":"dotnet","area":"swimlane","keywords":["data","integration","webform","dropdown","input","table","database","connect"],"description":"Simple data integration with .NET web forms.","publish":1}</v>
       </c>
     </row>
-    <row r="278" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A278" s="5">
         <v>278</v>
       </c>
@@ -14509,7 +14539,7 @@
         <v>{"id":278,"title":"swimlane-community-documentation","group":"dotnet","area":"swimlane","keywords":["community","people","collaboration","documentation","open","source","hands","paper","pencil","team"],"description":"Active developer community and up to date documentation.","publish":1}</v>
       </c>
     </row>
-    <row r="279" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A279" s="5">
         <v>279</v>
       </c>
@@ -14536,7 +14566,7 @@
         <v>{"id":279,"title":"swimlane-license-certificates","group":"dotnet","area":"swimlane","keywords":["license","certificate","ribbon","copyright"],"description":"License certificates.","publish":1}</v>
       </c>
     </row>
-    <row r="280" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A280" s="5">
         <v>280</v>
       </c>
@@ -14563,7 +14593,7 @@
         <v>{"id":280,"title":"swimlane-brand-dotnet-foundation","group":"dotnet","area":"swimlane","keywords":["brand","dotnet","foundation","logo"],"description":".NET Foundation logo.","publish":1}</v>
       </c>
     </row>
-    <row r="281" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A281" s="5">
         <v>281</v>
       </c>
@@ -14590,7 +14620,7 @@
         <v>{"id":281,"title":"swimlane-brand-github-octocat","group":"dotnet","area":"swimlane","keywords":["brand","github","octocat","mascot"],"description":"GitHub Octocat.","publish":1}</v>
       </c>
     </row>
-    <row r="282" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A282" s="5">
         <v>282</v>
       </c>
@@ -14617,7 +14647,7 @@
         <v>{"id":282,"title":"swimlane-brand-microsoft","group":"dotnet","area":"swimlane","keywords":["brand","microsoft","logo"],"description":"Microsoft logo.","publish":1}</v>
       </c>
     </row>
-    <row r="283" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A283" s="5">
         <v>283</v>
       </c>
@@ -14644,7 +14674,7 @@
         <v>{"id":283,"title":"modal-man-and-dog","group":"vscom","area":"modal","keywords":["man","laptop","people","dog","work","play"],"description":"A man using a laptop, sitting on the ground with a dog.","publish":1}</v>
       </c>
     </row>
-    <row r="284" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A284" s="5">
         <v>284</v>
       </c>
@@ -14671,7 +14701,7 @@
         <v>{"id":284,"title":"modal-man-dog- rube-goldberg-machine","group":"vscom","area":"modal","keywords":["man","laptop","people","dog","work","play","productivity","rube","goldberg","machine"],"description":"A man using a laptop, sitting on the ground with a dog. A Rube Goldberg machine in the background.","publish":1}</v>
       </c>
     </row>
-    <row r="285" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A285" s="5">
         <v>285</v>
       </c>
@@ -14698,7 +14728,7 @@
         <v>{"id":285,"title":"modal-subscribe-to-news-tips","group":"vscom","area":"modal","keywords":["woman","people","laptop","subscribe","email","newsletter","newspaper","lightbulb","tips","envelope","video","tutorials"],"description":"A woman using a laptop. Newsletter related icons floating around.","publish":1}</v>
       </c>
     </row>
-    <row r="286" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A286" s="5">
         <v>286</v>
       </c>
@@ -14725,7 +14755,7 @@
         <v>{"id":286,"title":"modal-joining-live-share-session","group":"vscom","area":"modal","keywords":["code","developer","editor","collaborate","share","people","computer","monitor","laptop"],"description":"A developer joining a Live Share session.","publish":1}</v>
       </c>
     </row>
-    <row r="287" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A287" s="5">
         <v>287</v>
       </c>
@@ -14752,7 +14782,7 @@
         <v>{"id":287,"title":"modal-live-share-session-inactive","group":"vscom","area":"modal","keywords":["code","developer","editor","collaborate","share","people","computer","monitor","laptop","wait","inactive","clock"],"description":"A developer waiting to join a Live Share session but the session is inactive.","publish":1}</v>
       </c>
     </row>
-    <row r="288" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A288" s="5">
         <v>288</v>
       </c>
@@ -14779,7 +14809,7 @@
         <v>{"id":288,"title":"swimlane-dotnet-platform","group":"dotnet","area":"swimlane","keywords":["platform","tools","library","utility","framework","drill","wrench","screwdriver","ruler","pencil","book"],"description":"A workbench with varies tools.","publish":1}</v>
       </c>
     </row>
-    <row r="289" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A289" s="5">
         <v>289</v>
       </c>
@@ -14806,7 +14836,7 @@
         <v>{"id":289,"title":"swimlane-pages-realtime-apis-microservices","group":"dotnet","area":"swimlane","keywords":["page","realtime","api","microservice","scroll","puzzle","clock","cube","block","module","people","tree"],"description":"A man standing under a feature tree.","publish":1}</v>
       </c>
     </row>
-    <row r="290" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A290" s="5">
         <v>290</v>
       </c>
@@ -14833,7 +14863,7 @@
         <v>{"id":290,"title":"swimlane-aspnet-extends-dotnet","group":"dotnet","area":"swimlane","keywords":["platform","tools","utility","framework","drill","wrench","screwdriver","ruler","pencil","hammer","plier"],"description":"A blueprint with varies tools drawing and a few tools floating.","publish":1}</v>
       </c>
     </row>
-    <row r="291" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A291" s="5">
         <v>291</v>
       </c>
@@ -14860,7 +14890,7 @@
         <v>{"id":291,"title":"swimlane-backend-code","group":"dotnet","area":"swimlane","keywords":["backend","code","programming","editor","people","gear","developer"],"description":"A code editor and two developers working on backend.","publish":1}</v>
       </c>
     </row>
-    <row r="292" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A292" s="5">
         <v>292</v>
       </c>
@@ -14883,11 +14913,11 @@
         <v>1</v>
       </c>
       <c r="I292" s="2" t="str">
-        <f t="shared" ref="I292:I293" si="20">SUBSTITUTE(_xlfn.CONCAT("{'id':",A292,",'title':'",C292,"','group':'",D292,"','area':'",E292,"','keywords':['",SUBSTITUTE(F292," ","','"),"'],'description':'",G292,"','publish':",H292,"}"),"'","""")</f>
+        <f t="shared" ref="I292:I296" si="20">SUBSTITUTE(_xlfn.CONCAT("{'id':",A292,",'title':'",C292,"','group':'",D292,"','area':'",E292,"','keywords':['",SUBSTITUTE(F292," ","','"),"'],'description':'",G292,"','publish':",H292,"}"),"'","""")</f>
         <v>{"id":292,"title":"swimlane-man-dog- rube-goldberg-machine","group":"dotnet","area":"swimlane","keywords":["man","laptop","people","dog","work","play","productivity","rube","goldberg","machine"],"description":"A man using a laptop, sitting on the ground with a dog. A Rube Goldberg machine in the background.","publish":1}</v>
       </c>
     </row>
-    <row r="293" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A293" s="5">
         <v>293</v>
       </c>
@@ -14912,6 +14942,87 @@
       <c r="I293" s="2" t="str">
         <f t="shared" si="20"/>
         <v>{"id":293,"title":"swimlane-subscribe-to-news-tips","group":"dotnet","area":"swimlane","keywords":["woman","people","laptop","subscribe","email","newsletter","newspaper","lightbulb","tips","envelope","video","tutorials"],"description":"A woman using a laptop. Newsletter related icons floating around.","publish":1}</v>
+      </c>
+    </row>
+    <row r="294" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A294" s="5">
+        <v>294</v>
+      </c>
+      <c r="C294" s="2" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D294" t="s">
+        <v>270</v>
+      </c>
+      <c r="E294" s="2" t="s">
+        <v>1069</v>
+      </c>
+      <c r="F294" s="2" t="s">
+        <v>1074</v>
+      </c>
+      <c r="G294" s="2" t="s">
+        <v>1070</v>
+      </c>
+      <c r="H294" s="2">
+        <v>1</v>
+      </c>
+      <c r="I294" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>{"id":294,"title":"prop-productive","group":"vscom","area":"valueprop","keywords":["productivity","machine","belt","process"],"description":"Belt and gear.","publish":1}</v>
+      </c>
+    </row>
+    <row r="295" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A295" s="5">
+        <v>295</v>
+      </c>
+      <c r="C295" s="2" t="s">
+        <v>1067</v>
+      </c>
+      <c r="D295" t="s">
+        <v>270</v>
+      </c>
+      <c r="E295" s="2" t="s">
+        <v>1069</v>
+      </c>
+      <c r="F295" s="2" t="s">
+        <v>1072</v>
+      </c>
+      <c r="G295" s="2" t="s">
+        <v>1073</v>
+      </c>
+      <c r="H295" s="2">
+        <v>1</v>
+      </c>
+      <c r="I295" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>{"id":295,"title":"prop-innovate","group":"vscom","area":"valueprop","keywords":["innovative","lightbulb","idea","insight","beaker"],"description":"A lightbulb and a beaker.","publish":1}</v>
+      </c>
+    </row>
+    <row r="296" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A296" s="5">
+        <v>296</v>
+      </c>
+      <c r="C296" s="2" t="s">
+        <v>1068</v>
+      </c>
+      <c r="D296" t="s">
+        <v>270</v>
+      </c>
+      <c r="E296" s="2" t="s">
+        <v>1069</v>
+      </c>
+      <c r="F296" s="2" t="s">
+        <v>1075</v>
+      </c>
+      <c r="G296" s="2" t="s">
+        <v>1071</v>
+      </c>
+      <c r="H296" s="2">
+        <v>1</v>
+      </c>
+      <c r="I296" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>{"id":296,"title":"prop-modern","group":"vscom","area":"valueprop","keywords":["modern","technology","robot","machine"],"description":"A robot pressing a button.","publish":1}</v>
       </c>
     </row>
   </sheetData>
@@ -14932,154 +15043,154 @@
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>683</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>684</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>685</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>686</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>684</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>684</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>687</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>688</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>689</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>690</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>691</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>692</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>693</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>695</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>696</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>697</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>698</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>699</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>700</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>701</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>702</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>703</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>704</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>706</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>707</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>708</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>710</v>
       </c>
@@ -15102,22 +15213,22 @@
       <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="50.1" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="38.140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.86328125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.86328125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="38.1328125" style="2" customWidth="1"/>
     <col min="4" max="4" width="17" style="2" customWidth="1"/>
     <col min="5" max="5" width="18" style="2" customWidth="1"/>
-    <col min="6" max="6" width="33.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" style="2" customWidth="1"/>
-    <col min="8" max="9" width="24.140625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="33.140625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="66.42578125" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="2"/>
+    <col min="6" max="6" width="33.73046875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="20.73046875" style="2" customWidth="1"/>
+    <col min="8" max="9" width="24.1328125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="33.1328125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="66.3984375" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="9.1328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="3" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>73</v>
       </c>
@@ -15152,7 +15263,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -15186,7 +15297,7 @@
         <v>{"id":1,"title":"AzureToolsForVS","category":"VSCOM","keywords":["free","hosting","bug","tools","platforms","testing","beaker","wrench","azure","logo"],"description":"Azure developer tools for Visual Studio with free hosting.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -15220,7 +15331,7 @@
         <v>{"id":2,"title":"CloudPattern","category":"Pattern","keywords":["technology","nature","cloud","sky"],"description":"Clouds on blue sky pattern.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -15254,7 +15365,7 @@
         <v>{"id":3,"title":"CollaborationChatBubbles","category":"Diagram","keywords":["work","chat","bubble","conversation","communication","collaboration","team","men","women","people"],"description":"Several chat bubbles with people inside.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -15288,7 +15399,7 @@
         <v>{"id":4,"title":"CollaborationNetwork","category":"Diagram","keywords":["man","woman","network","hub","collaboration","connection","web","idea","lightbulb","gear","cloud","chat","bubble","work"],"description":"A network of people and objects connected together.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -15322,7 +15433,7 @@
         <v>{"id":5,"title":"CommunityTranslation1","category":"VSCOM","keywords":["hand","phone","hello","word","balloon","languages"],"description":"Translate world languages with smartphone.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -15356,7 +15467,7 @@
         <v>{"id":6,"title":"CommunityTranslation2","category":"VSCOM","keywords":["group","people","tablet","languages"],"description":"People from around the world using translation app on smart device to say hello.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -15390,7 +15501,7 @@
         <v>{"id":7,"title":"CommunityTranslation3","category":"VSCOM","keywords":["group","people","tablet","languages"],"description":"People from around the world using translation app on smart device to say hello.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -15424,7 +15535,7 @@
         <v>{"id":8,"title":"CordovaToolsTwitterBanner","category":"Web","keywords":["crane","cloud","tools","tree","build","construction"],"description":"Cordova Tools Twitter account banner. Construction crane and build tools on cloud.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -15458,7 +15569,7 @@
         <v>{"id":9,"title":"DesktopComputerPattern","category":"Pattern","keywords":["desktop","computer","monitor","pc","technology"],"description":"Desktop computer pattern.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -15492,7 +15603,7 @@
         <v>{"id":10,"title":"DevEssentials1","category":"VSCOM","keywords":["download","arrow","magnifying","glass","monitor","laptop","data","graphs","gears","newsletter"],"description":"Data visualization related elements on a cloud.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -15526,7 +15637,7 @@
         <v>{"id":11,"title":"DevEssentials2","category":"VSCOM","keywords":["download","arrow","magnifying","glass","monitor","laptop","data","graphs","gears","toolbox","newsletter"],"description":"Data visualization related elements on a cloud.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -15560,7 +15671,7 @@
         <v>{"id":12,"title":"DevicesPattern","category":"Pattern","keywords":["laptop","phone","tablet","smartphone","technology"],"description":"Mixed devices pattern.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -15594,7 +15705,7 @@
         <v>{"id":13,"title":"DevOpsLifecycle","category":"Diagram","keywords":["handshake","planning","continuous","delivery","dev","test","analytics","mobius","infinity","loop"],"description":"DevOps lifecycle.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -15628,7 +15739,7 @@
         <v>{"id":14,"title":"FeedbackCommentsDiscussion","category":"Email","keywords":["chat","bubble","question","exclaimation","conversation","discussion"],"description":"Feedback comment discussion.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -15662,7 +15773,7 @@
         <v>{"id":15,"title":"FeedbackPattern","category":"Pattern","keywords":["feedback","chat","bubble","conversation","question","exclaimation","problem","comment","talk"],"description":"Chat bubble feedback pattern.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -15696,7 +15807,7 @@
         <v>{"id":16,"title":"FoodCollection","category":"Elements","keywords":["food","meal","nutrition","soup","bread","spoon","tomato","broccli","vegetable","fish","crab","seafood","meat","poultry","steak","chicken","turkey","cake","pie","dessert","measuring","cup","egg","beater","cooking","utencils","drink","cocktail","glass","toast","cracker","cheese","burger","hotdog","salad","appetizer","entree"],"description":"A collection of food icons.","style":["color","sketchy"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -15730,7 +15841,7 @@
         <v>{"id":17,"title":"IdeaFactory","category":"Web","keywords":["factory","building","gear","lightbulb","database","arrow","document","gauge","lift","truck"],"description":"Ideas being manufactured in a factory.","style":["monotone"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -15764,7 +15875,7 @@
         <v>{"id":18,"title":"IntegratedDevelopmentLoop","category":"Email","keywords":["loop","cycle","edit","pencil","script","scroll","bug","arrow","device","phone","mobile","cloud"],"description":"Lifecycle of code, debug and deployment.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -15798,7 +15909,7 @@
         <v>{"id":19,"title":"InternetOfThings","category":"Diagram","keywords":["internet","iot","globe","router","smart","phone","laptop","light","bulb","printer","desktop","media","player","car","smart","home","smart","watch","mobile","payment","device","software","development"],"description":"The Internet of Things (IoT) is the network of physical objects or things embedded with electronics, software, sensors, and network connectivity, which enables these objects to collect and exchange data.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -15832,7 +15943,7 @@
         <v>{"id":20,"title":"ManufacturingIdeas","category":"Misc","keywords":["machine","tool","lightbulb"],"description":"Ideas being manufactured by a machine.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -15866,7 +15977,7 @@
         <v>{"id":21,"title":"MicrosoftWelcomeCenter","category":"Print","keywords":["microsoft","company","building","welcome","logo","work","business"],"description":"Microsoft logo and office buildings.","style":["color","3d"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -15900,7 +16011,7 @@
         <v>{"id":22,"title":"MobileAppDevelopmentPlatform","category":"VSCOM","keywords":["building","city","cloud","billboard","people","device","laptop","phone","database","security","lock","presentation","chart","development","platform","enterprise","business"],"description":"Mobile app development platform.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -15934,7 +16045,7 @@
         <v>{"id":23,"title":"MobileAppDevelopmentWithVisualStudio","category":"VSCOM","keywords":["laptop","phone","iphone","android","windows","app","development","visual","studio"],"description":"Cross platform mobile app development with Visual Studio.","style":["color","photo","monotone"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -15968,7 +16079,7 @@
         <v>{"id":24,"title":"MultiDeviceTwitterBanner","category":"Web","keywords":["cloud","sky","field","grass","phone","smartphone","tablet","computer","desktop","pc","monitor","tv","television","microsoft","logo","technology","developer"],"description":"Cordova Tools Twitter account banner. Four device icons overlay on top of cloud and field backgournd.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -16002,7 +16113,7 @@
         <v>{"id":25,"title":"NETCoreWebsiteBanner","category":"Web","keywords":["visual","studio","html5","css3","javascript"],"description":".NET Core website banner.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -16036,7 +16147,7 @@
         <v>{"id":26,"title":"OneToolForEverything","category":"Email","keywords":["tool","laptop","mobile","phone","cloud"],"description":"One tool for all platform.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -16070,7 +16181,7 @@
         <v>{"id":27,"title":"OpenSourceComputer","category":"Web","keywords":["laptop","code","arrow","exchange"],"description":"Two laptop exchanging code.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -16104,7 +16215,7 @@
         <v>{"id":28,"title":"OpenSourceExchangeCode","category":"Diagram","keywords":["code","man","woman","laptop","desktop","exchange","share","arrow"],"description":"Developers exchange open source code.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -16138,7 +16249,7 @@
         <v>{"id":29,"title":"PlaceholderFlowers","category":"VSTS","keywords":["flower"],"description":"Placeholder images.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -16172,7 +16283,7 @@
         <v>{"id":30,"title":"PublishAndDeploy","category":"Email","keywords":["rocket","document","arrow","exchange"],"description":"Publish and deploy code.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -16206,7 +16317,7 @@
         <v>{"id":31,"title":"PushNotifications","category":"Web","keywords":["mobile","phone","tablet","android","windows","ios","chat","bubble","notification"],"description":"Push notifications on multiple platforms.","style":["monotone"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -16240,7 +16351,7 @@
         <v>{"id":32,"title":"PythonToolsForVS","category":"VSCOM","keywords":["man","laptop","woman","gears","bug","code","phone","python","logo","magnifying","glass"],"description":"Python tools for Visual Studio.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -16274,7 +16385,7 @@
         <v>{"id":33,"title":"QuickstartFastSpeed","category":"Email","keywords":["stopwatch","run","man","time","fast","quick","speed"],"description":"Quick start","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -16308,7 +16419,7 @@
         <v>{"id":34,"title":"RocketMulticolor","category":"Elements","keywords":["rocket","launch","deployment"],"description":"Rocket","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -16342,7 +16453,7 @@
         <v>{"id":35,"title":"RocketWithCloudPattern","category":"Print","keywords":["rocket","cloud","sky"],"description":"Rocket on sky background","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -16376,7 +16487,7 @@
         <v>{"id":36,"title":"SeattlePostcard","category":"Print","keywords":["seattle","space","needle","cloud","city"],"description":"Seattle space needle postcard","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -16410,7 +16521,7 @@
         <v>{"id":37,"title":"SeattleSkyline","category":"Web","keywords":["seattle","space","needle","cloud","city","skyline","building","mount","rainier"],"description":"Seattle city skyline","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -16444,7 +16555,7 @@
         <v>{"id":38,"title":"SeattleSkylineFerrisWheel","category":"Web","keywords":["seattle","space","needle","ferris","wheel","waterfront","port"],"description":"Seattle city skyline","style":["monotone"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -16478,7 +16589,7 @@
         <v>{"id":39,"title":"SilhouetteAirportElements","category":"Elements","keywords":["airport","pilot","flight","attendant","uniform","causeway","airplane","sign","direction","loudge","coffee","terminal","seat","life"],"description":"A collection of airport related elements.","style":["silhuoette"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -16512,7 +16623,7 @@
         <v>{"id":40,"title":"SilhouetteBriefcasesAndDocuments","category":"Elements","keywords":["document","file","paper","briefcase","suitcase","handbag","work","object","business"],"description":" A collection of briefcases.","style":["silhuoette"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -16546,7 +16657,7 @@
         <v>{"id":41,"title":"SilhouetteCharacters","category":"Elements","keywords":["man","confuse","suit","woman","chair","desk","laptop","computer","office","work","business"],"description":"A collection of characters in work environment.","style":[" ","silhuoette"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -16580,7 +16691,7 @@
         <v>{"id":42,"title":"SilhouetteHandGenstures","category":"Elements","keywords":["hand","gesture","pick","grip","pinch","touch","web","press","technology"],"description":"Hand gestures.","style":["silhuoette"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -16614,7 +16725,7 @@
         <v>{"id":43,"title":"SilhouetteTabletAndPhones","category":"Elements","keywords":["technology","work","tablet","smartphone","phone","mobile","phone","pen","stylus","windows","phone","android","phone","surface","tablet"],"description":"Tablet and smartphones.","style":["silhuoette"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -16648,7 +16759,7 @@
         <v>{"id":44,"title":"SilhouetteToolCollection","category":"Pattern","keywords":["wrench","screwdriver","saw","plier","hammer","knife","c","clamp","clamp","pipe","wrench","filer","triangle","ruler","object"],"description":"A collection of hand tools.","style":["silhouette"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -16682,7 +16793,7 @@
         <v>{"id":45,"title":"SilhouetteWeatherReportElements","category":"Elements","keywords":["life","newspaper","radio","magezine","clock","news","weather","forcast","tv","sun","sunny","cloud","lightning","thunder","cloud","cloudy","rain","tripical","palm","tree","beach","table","vacation","beach","chair","hawaii","man","relax","drink"],"description":"A collection of weather related illustrations.","style":["silhuoette"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -16716,7 +16827,7 @@
         <v>{"id":46,"title":"SoftwareToolsSampleKit","category":"Email","keywords":["toolbox","hammer","checklist","wrench","cloud"],"description":"Software development toolkit","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -16750,7 +16861,7 @@
         <v>{"id":47,"title":"TeamworkStairs","category":"Web","keywords":["people","man","stairs","team"],"description":"People holding hands climbing up stairs as a team.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -16784,7 +16895,7 @@
         <v>{"id":48,"title":"Testing","category":"Email","keywords":["test","flask","lab","beaker","stopwatch","pie","chart","checklist"],"description":"Testing","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -16818,7 +16929,7 @@
         <v>{"id":49,"title":"VSBuildALMIntegration","category":"VSCOM","keywords":["people","working","man","computer","clipboard","debug","tools","gear","bug"],"description":"ALM (Application Lifecycle Management) debug integration.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -16852,7 +16963,7 @@
         <v>{"id":50,"title":"VSBuildCloudHostedTools","category":"VSCOM","keywords":["people","laptops","desk","workers","monitors","laptops","cross","platforms","linux","windows","ios"],"description":"Developers come from different platforms and technology stacks working together.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -16886,7 +16997,7 @@
         <v>{"id":51,"title":"VSBuildContinuousIntegration","category":"VSCOM","keywords":["monitor","laptop","test","tubes","gears","checkmark"],"description":"Build continuous integration cycle with cloud.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -16920,7 +17031,7 @@
         <v>{"id":52,"title":"VSBuildContinuousIntegrationWhite","category":"VSCOM","keywords":["cross","platforms","maven","git","apache","ant","junit","gradle","xunit","mtm","test","building"],"description":"Common tools and technologies for cross-platform development.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -16954,7 +17065,7 @@
         <v>{"id":53,"title":"VSBuildCrossPlatform","category":"VSCOM","keywords":["pillars","cross","platforms","buildings","crane","java",".net","xcode","github","ios","android","windows","git"],"description":"Common tools and technologies for cross-platform development.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -16988,7 +17099,7 @@
         <v>{"id":54,"title":"VSBuildOverview","category":"VSCOM","keywords":["cross","platforms","laptop","tablet","phone","ios","android","visual","studio","cloud"],"description":"Visual Studio for building cross-platform applications.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -17022,7 +17133,7 @@
         <v>{"id":55,"title":"VSBuildTraceability","category":"VSCOM","keywords":["blueprint","document","man","beaker","tools","clipboard","timeline","printer","download","test","tubes","gears","magnifying","glass","graphs"],"description":"Build timeline and tracebility.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -17056,7 +17167,7 @@
         <v>{"id":56,"title":"VSDownload1","category":"VSCOM","keywords":["group","people","visual","studio","logo","flags","man","woman"],"description":"Visual Studio for everyone.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -17090,7 +17201,7 @@
         <v>{"id":57,"title":"VSDownload2","category":"VSCOM","keywords":["man","monitors","download","down","arrow","computer","table"],"description":"Visual Studio tools for multiplatform.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -17124,302 +17235,302 @@
         <v>{"id":58,"title":"XamarinCrossPlatformDevelopment","category":"VSCOM","keywords":["screenshot","ios","android","windows","mobile","phone","app","development","shared","code","cross-platform","xamarin"],"description":"Xamarin for developing cross-platform application.","style":["color","photo"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A60" s="2">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A61" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A62" s="2">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A63" s="2">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A64" s="2">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A65" s="2">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A66" s="2">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A67" s="2">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A68" s="2">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A69" s="2">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A70" s="2">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A71" s="2">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A72" s="2">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A73" s="2">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A74" s="2">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A75" s="2">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A76" s="2">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A77" s="2">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A78" s="2">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A79" s="2">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A80" s="2">
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A81" s="2">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A82" s="2">
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A83" s="2">
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A84" s="2">
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A85" s="2">
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A86" s="2">
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A87" s="2">
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A88" s="2">
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A89" s="2">
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A90" s="2">
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A91" s="2">
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A92" s="2">
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A93" s="2">
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A94" s="2">
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A95" s="2">
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A96" s="2">
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A97" s="2">
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A98" s="2">
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A99" s="2">
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A100" s="2">
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A101" s="2">
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A102" s="2">
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A103" s="2">
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A104" s="2">
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A105" s="2">
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A106" s="2">
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A107" s="2">
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A108" s="2">
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A109" s="2">
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A110" s="2">
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A111" s="2">
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A112" s="2">
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A113" s="2">
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A114" s="2">
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A115" s="2">
         <v>114</v>
       </c>
     </row>
-    <row r="116" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A116" s="2">
         <v>115</v>
       </c>
     </row>
-    <row r="117" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A117" s="2">
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A118" s="2">
         <v>117</v>
       </c>
     </row>
-    <row r="119" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A119" s="2">
         <v>118</v>
       </c>
@@ -17455,9 +17566,9 @@
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="1" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Added devblog banner images
</commit_message>
<xml_diff>
--- a/src/assets/data.xlsx
+++ b/src/assets/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10318"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cherrywang/Dropbox/Code/vsimages/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C538887A-3CEE-7646-82DC-E7EAB7E75C3E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1090E974-1AE4-8248-A910-A4B523B82AA8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,6 +31,7 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1926" uniqueCount="1105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2051" uniqueCount="1141">
   <si>
     <t>SeattleSkyline</t>
   </si>
@@ -3353,6 +3354,114 @@
   </si>
   <si>
     <t>developer day build seattle feedback bubble lightbulb rube goldburg machine process city sasquatch</t>
+  </si>
+  <si>
+    <t>banner-arrows-dark-blue</t>
+  </si>
+  <si>
+    <t>banner-big-code-1-purple</t>
+  </si>
+  <si>
+    <t>banner-big-code-2-purple</t>
+  </si>
+  <si>
+    <t>banner-big-code-dark-blue</t>
+  </si>
+  <si>
+    <t>banner-big-code-turquoise</t>
+  </si>
+  <si>
+    <t>banner-bugs-gray</t>
+  </si>
+  <si>
+    <t>banner-bugs-purple</t>
+  </si>
+  <si>
+    <t>banner-bugs-turquoise</t>
+  </si>
+  <si>
+    <t>banner-cloud-vectors-blue</t>
+  </si>
+  <si>
+    <t>banner-code-1-purple</t>
+  </si>
+  <si>
+    <t>banner-code-2-purple</t>
+  </si>
+  <si>
+    <t>banner-cubes-magenta</t>
+  </si>
+  <si>
+    <t>banner-devices-1-blue</t>
+  </si>
+  <si>
+    <t>banner-devices-1-purple</t>
+  </si>
+  <si>
+    <t>banner-mix-1-blue</t>
+  </si>
+  <si>
+    <t>banner-mix-1-gray</t>
+  </si>
+  <si>
+    <t>banner-outline-icons-blue</t>
+  </si>
+  <si>
+    <t>banner-outline-icons-purple</t>
+  </si>
+  <si>
+    <t>banner-particle-lines-blue</t>
+  </si>
+  <si>
+    <t>banner-people-purple</t>
+  </si>
+  <si>
+    <t>banner-small-outline-purple</t>
+  </si>
+  <si>
+    <t>banner-solid-icons-1-purple</t>
+  </si>
+  <si>
+    <t>banner-solid-icons-2-purple-dark</t>
+  </si>
+  <si>
+    <t>banner-solid-icons-2-purple</t>
+  </si>
+  <si>
+    <t>banner-triangulation-purple</t>
+  </si>
+  <si>
+    <t>banner</t>
+  </si>
+  <si>
+    <t>arrow navigation motion</t>
+  </si>
+  <si>
+    <t>bug debug</t>
+  </si>
+  <si>
+    <t>cloud</t>
+  </si>
+  <si>
+    <t>cube microservice module component</t>
+  </si>
+  <si>
+    <t>device mobile phone computer laptop</t>
+  </si>
+  <si>
+    <t>particle line</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>people</t>
+  </si>
+  <si>
+    <t>triangle shape geometry</t>
+  </si>
+  <si>
+    <t>Background images used for DevBlog banner area.</t>
   </si>
 </sst>
 </file>
@@ -6258,13 +6367,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K306"/>
+  <dimension ref="A1:K331"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B302" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B327" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I294" sqref="I294:I306"/>
+      <selection pane="bottomRight" activeCell="I307" sqref="I307:I331"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="100" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -15001,7 +15110,7 @@
         <v>1</v>
       </c>
       <c r="I292" s="2" t="str">
-        <f t="shared" ref="I292:I306" si="20">SUBSTITUTE(_xlfn.CONCAT("{'id':",A292,",'title':'",C292,"','group':'",D292,"','area':'",E292,"','keywords':['",SUBSTITUTE(F292," ","','"),"'],'description':'",G292,"','publish':",H292,"}"),"'","""")</f>
+        <f t="shared" ref="I292:I331" si="20">SUBSTITUTE(_xlfn.CONCAT("{'id':",A292,",'title':'",C292,"','group':'",D292,"','area':'",E292,"','keywords':['",SUBSTITUTE(F292," ","','"),"'],'description':'",G292,"','publish':",H292,"}"),"'","""")</f>
         <v>{"id":292,"title":"swimlane-man-dog- rube-goldberg-machine","group":"dotnet","area":"swimlane","keywords":["man","laptop","people","dog","work","play","productivity","rube","goldberg","machine"],"description":"A man using a laptop, sitting on the ground with a dog. A Rube Goldberg machine in the background.","publish":1}</v>
       </c>
     </row>
@@ -15381,6 +15490,681 @@
       <c r="I306" s="2" t="str">
         <f t="shared" si="20"/>
         <v>{"id":306,"title":"hero-developer-day-2019","group":"vscom","area":"hero","keywords":["developer","day","build","seattle","feedback","bubble","lightbulb","rube","goldburg","machine","process","city","sasquatch"],"description":"Hero image for Develoepr Day 2019","publish":1}</v>
+      </c>
+    </row>
+    <row r="307" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A307" s="5">
+        <v>307</v>
+      </c>
+      <c r="C307" s="2" t="s">
+        <v>1105</v>
+      </c>
+      <c r="D307" t="s">
+        <v>866</v>
+      </c>
+      <c r="E307" s="2" t="s">
+        <v>1130</v>
+      </c>
+      <c r="F307" s="2" t="s">
+        <v>1131</v>
+      </c>
+      <c r="G307" s="2" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H307" s="2">
+        <v>1</v>
+      </c>
+      <c r="I307" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>{"id":307,"title":"banner-arrows-dark-blue","group":"devblog","area":"banner","keywords":["arrow","navigation","motion"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
+      </c>
+    </row>
+    <row r="308" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A308" s="5">
+        <v>308</v>
+      </c>
+      <c r="C308" s="2" t="s">
+        <v>1106</v>
+      </c>
+      <c r="D308" t="s">
+        <v>866</v>
+      </c>
+      <c r="E308" s="2" t="s">
+        <v>1130</v>
+      </c>
+      <c r="F308" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="G308" s="2" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H308" s="2">
+        <v>1</v>
+      </c>
+      <c r="I308" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>{"id":308,"title":"banner-big-code-1-purple","group":"devblog","area":"banner","keywords":["code"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
+      </c>
+    </row>
+    <row r="309" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A309" s="5">
+        <v>309</v>
+      </c>
+      <c r="C309" s="2" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D309" t="s">
+        <v>866</v>
+      </c>
+      <c r="E309" s="2" t="s">
+        <v>1130</v>
+      </c>
+      <c r="F309" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="G309" s="2" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H309" s="2">
+        <v>1</v>
+      </c>
+      <c r="I309" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>{"id":309,"title":"banner-big-code-2-purple","group":"devblog","area":"banner","keywords":["code"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
+      </c>
+    </row>
+    <row r="310" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A310" s="5">
+        <v>310</v>
+      </c>
+      <c r="C310" s="2" t="s">
+        <v>1108</v>
+      </c>
+      <c r="D310" t="s">
+        <v>866</v>
+      </c>
+      <c r="E310" s="2" t="s">
+        <v>1130</v>
+      </c>
+      <c r="F310" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="G310" s="2" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H310" s="2">
+        <v>1</v>
+      </c>
+      <c r="I310" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>{"id":310,"title":"banner-big-code-dark-blue","group":"devblog","area":"banner","keywords":["code"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
+      </c>
+    </row>
+    <row r="311" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A311" s="5">
+        <v>311</v>
+      </c>
+      <c r="C311" s="2" t="s">
+        <v>1109</v>
+      </c>
+      <c r="D311" t="s">
+        <v>866</v>
+      </c>
+      <c r="E311" s="2" t="s">
+        <v>1130</v>
+      </c>
+      <c r="F311" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="G311" s="2" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H311" s="2">
+        <v>1</v>
+      </c>
+      <c r="I311" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>{"id":311,"title":"banner-big-code-turquoise","group":"devblog","area":"banner","keywords":["code"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
+      </c>
+    </row>
+    <row r="312" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A312" s="5">
+        <v>312</v>
+      </c>
+      <c r="C312" s="2" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D312" t="s">
+        <v>866</v>
+      </c>
+      <c r="E312" s="2" t="s">
+        <v>1130</v>
+      </c>
+      <c r="F312" s="2" t="s">
+        <v>1132</v>
+      </c>
+      <c r="G312" s="2" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H312" s="2">
+        <v>1</v>
+      </c>
+      <c r="I312" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>{"id":312,"title":"banner-bugs-gray","group":"devblog","area":"banner","keywords":["bug","debug"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
+      </c>
+    </row>
+    <row r="313" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A313" s="5">
+        <v>313</v>
+      </c>
+      <c r="C313" s="2" t="s">
+        <v>1111</v>
+      </c>
+      <c r="D313" t="s">
+        <v>866</v>
+      </c>
+      <c r="E313" s="2" t="s">
+        <v>1130</v>
+      </c>
+      <c r="F313" s="2" t="s">
+        <v>1132</v>
+      </c>
+      <c r="G313" s="2" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H313" s="2">
+        <v>1</v>
+      </c>
+      <c r="I313" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>{"id":313,"title":"banner-bugs-purple","group":"devblog","area":"banner","keywords":["bug","debug"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
+      </c>
+    </row>
+    <row r="314" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A314" s="5">
+        <v>314</v>
+      </c>
+      <c r="C314" s="2" t="s">
+        <v>1112</v>
+      </c>
+      <c r="D314" t="s">
+        <v>866</v>
+      </c>
+      <c r="E314" s="2" t="s">
+        <v>1130</v>
+      </c>
+      <c r="F314" s="2" t="s">
+        <v>1132</v>
+      </c>
+      <c r="G314" s="2" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H314" s="2">
+        <v>1</v>
+      </c>
+      <c r="I314" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>{"id":314,"title":"banner-bugs-turquoise","group":"devblog","area":"banner","keywords":["bug","debug"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
+      </c>
+    </row>
+    <row r="315" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A315" s="5">
+        <v>315</v>
+      </c>
+      <c r="C315" s="2" t="s">
+        <v>1113</v>
+      </c>
+      <c r="D315" t="s">
+        <v>866</v>
+      </c>
+      <c r="E315" s="2" t="s">
+        <v>1130</v>
+      </c>
+      <c r="F315" s="2" t="s">
+        <v>1133</v>
+      </c>
+      <c r="G315" s="2" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H315" s="2">
+        <v>1</v>
+      </c>
+      <c r="I315" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>{"id":315,"title":"banner-cloud-vectors-blue","group":"devblog","area":"banner","keywords":["cloud"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
+      </c>
+    </row>
+    <row r="316" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A316" s="5">
+        <v>316</v>
+      </c>
+      <c r="C316" s="2" t="s">
+        <v>1114</v>
+      </c>
+      <c r="D316" t="s">
+        <v>866</v>
+      </c>
+      <c r="E316" s="2" t="s">
+        <v>1130</v>
+      </c>
+      <c r="F316" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="G316" s="2" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H316" s="2">
+        <v>1</v>
+      </c>
+      <c r="I316" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>{"id":316,"title":"banner-code-1-purple","group":"devblog","area":"banner","keywords":["code"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
+      </c>
+    </row>
+    <row r="317" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A317" s="5">
+        <v>317</v>
+      </c>
+      <c r="C317" s="2" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D317" t="s">
+        <v>866</v>
+      </c>
+      <c r="E317" s="2" t="s">
+        <v>1130</v>
+      </c>
+      <c r="F317" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="G317" s="2" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H317" s="2">
+        <v>1</v>
+      </c>
+      <c r="I317" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>{"id":317,"title":"banner-code-2-purple","group":"devblog","area":"banner","keywords":["code"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
+      </c>
+    </row>
+    <row r="318" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A318" s="5">
+        <v>318</v>
+      </c>
+      <c r="C318" s="2" t="s">
+        <v>1116</v>
+      </c>
+      <c r="D318" t="s">
+        <v>866</v>
+      </c>
+      <c r="E318" s="2" t="s">
+        <v>1130</v>
+      </c>
+      <c r="F318" s="2" t="s">
+        <v>1134</v>
+      </c>
+      <c r="G318" s="2" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H318" s="2">
+        <v>1</v>
+      </c>
+      <c r="I318" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>{"id":318,"title":"banner-cubes-magenta","group":"devblog","area":"banner","keywords":["cube","microservice","module","component"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
+      </c>
+    </row>
+    <row r="319" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A319" s="5">
+        <v>319</v>
+      </c>
+      <c r="C319" s="2" t="s">
+        <v>1117</v>
+      </c>
+      <c r="D319" t="s">
+        <v>866</v>
+      </c>
+      <c r="E319" s="2" t="s">
+        <v>1130</v>
+      </c>
+      <c r="F319" s="2" t="s">
+        <v>1135</v>
+      </c>
+      <c r="G319" s="2" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H319" s="2">
+        <v>1</v>
+      </c>
+      <c r="I319" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>{"id":319,"title":"banner-devices-1-blue","group":"devblog","area":"banner","keywords":["device","mobile","phone","computer","laptop"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
+      </c>
+    </row>
+    <row r="320" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A320" s="5">
+        <v>320</v>
+      </c>
+      <c r="C320" s="2" t="s">
+        <v>1118</v>
+      </c>
+      <c r="D320" t="s">
+        <v>866</v>
+      </c>
+      <c r="E320" s="2" t="s">
+        <v>1130</v>
+      </c>
+      <c r="F320" s="2" t="s">
+        <v>1135</v>
+      </c>
+      <c r="G320" s="2" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H320" s="2">
+        <v>1</v>
+      </c>
+      <c r="I320" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>{"id":320,"title":"banner-devices-1-purple","group":"devblog","area":"banner","keywords":["device","mobile","phone","computer","laptop"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
+      </c>
+    </row>
+    <row r="321" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A321" s="5">
+        <v>321</v>
+      </c>
+      <c r="C321" s="2" t="s">
+        <v>1119</v>
+      </c>
+      <c r="D321" t="s">
+        <v>866</v>
+      </c>
+      <c r="E321" s="2" t="s">
+        <v>1130</v>
+      </c>
+      <c r="F321" s="2" t="s">
+        <v>1137</v>
+      </c>
+      <c r="G321" s="2" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H321" s="2">
+        <v>1</v>
+      </c>
+      <c r="I321" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>{"id":321,"title":"banner-mix-1-blue","group":"devblog","area":"banner","keywords":["icon"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
+      </c>
+    </row>
+    <row r="322" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A322" s="5">
+        <v>322</v>
+      </c>
+      <c r="C322" s="2" t="s">
+        <v>1120</v>
+      </c>
+      <c r="D322" t="s">
+        <v>866</v>
+      </c>
+      <c r="E322" s="2" t="s">
+        <v>1130</v>
+      </c>
+      <c r="F322" s="2" t="s">
+        <v>1137</v>
+      </c>
+      <c r="G322" s="2" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H322" s="2">
+        <v>1</v>
+      </c>
+      <c r="I322" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>{"id":322,"title":"banner-mix-1-gray","group":"devblog","area":"banner","keywords":["icon"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
+      </c>
+    </row>
+    <row r="323" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A323" s="5">
+        <v>323</v>
+      </c>
+      <c r="C323" s="2" t="s">
+        <v>1121</v>
+      </c>
+      <c r="D323" t="s">
+        <v>866</v>
+      </c>
+      <c r="E323" s="2" t="s">
+        <v>1130</v>
+      </c>
+      <c r="F323" s="2" t="s">
+        <v>1137</v>
+      </c>
+      <c r="G323" s="2" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H323" s="2">
+        <v>1</v>
+      </c>
+      <c r="I323" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>{"id":323,"title":"banner-outline-icons-blue","group":"devblog","area":"banner","keywords":["icon"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
+      </c>
+    </row>
+    <row r="324" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A324" s="5">
+        <v>324</v>
+      </c>
+      <c r="C324" s="2" t="s">
+        <v>1122</v>
+      </c>
+      <c r="D324" t="s">
+        <v>866</v>
+      </c>
+      <c r="E324" s="2" t="s">
+        <v>1130</v>
+      </c>
+      <c r="F324" s="2" t="s">
+        <v>1136</v>
+      </c>
+      <c r="G324" s="2" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H324" s="2">
+        <v>1</v>
+      </c>
+      <c r="I324" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>{"id":324,"title":"banner-outline-icons-purple","group":"devblog","area":"banner","keywords":["particle","line"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
+      </c>
+    </row>
+    <row r="325" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A325" s="5">
+        <v>325</v>
+      </c>
+      <c r="C325" s="2" t="s">
+        <v>1123</v>
+      </c>
+      <c r="D325" t="s">
+        <v>866</v>
+      </c>
+      <c r="E325" s="2" t="s">
+        <v>1130</v>
+      </c>
+      <c r="F325" s="2" t="s">
+        <v>1136</v>
+      </c>
+      <c r="G325" s="2" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H325" s="2">
+        <v>1</v>
+      </c>
+      <c r="I325" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>{"id":325,"title":"banner-particle-lines-blue","group":"devblog","area":"banner","keywords":["particle","line"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
+      </c>
+    </row>
+    <row r="326" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A326" s="5">
+        <v>326</v>
+      </c>
+      <c r="C326" s="2" t="s">
+        <v>1124</v>
+      </c>
+      <c r="D326" t="s">
+        <v>866</v>
+      </c>
+      <c r="E326" s="2" t="s">
+        <v>1130</v>
+      </c>
+      <c r="F326" s="2" t="s">
+        <v>1138</v>
+      </c>
+      <c r="G326" s="2" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H326" s="2">
+        <v>1</v>
+      </c>
+      <c r="I326" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>{"id":326,"title":"banner-people-purple","group":"devblog","area":"banner","keywords":["people"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
+      </c>
+    </row>
+    <row r="327" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A327" s="5">
+        <v>327</v>
+      </c>
+      <c r="C327" s="2" t="s">
+        <v>1125</v>
+      </c>
+      <c r="D327" t="s">
+        <v>866</v>
+      </c>
+      <c r="E327" s="2" t="s">
+        <v>1130</v>
+      </c>
+      <c r="F327" s="2" t="s">
+        <v>1138</v>
+      </c>
+      <c r="G327" s="2" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H327" s="2">
+        <v>1</v>
+      </c>
+      <c r="I327" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>{"id":327,"title":"banner-small-outline-purple","group":"devblog","area":"banner","keywords":["people"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
+      </c>
+    </row>
+    <row r="328" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A328" s="5">
+        <v>328</v>
+      </c>
+      <c r="C328" s="2" t="s">
+        <v>1126</v>
+      </c>
+      <c r="D328" t="s">
+        <v>866</v>
+      </c>
+      <c r="E328" s="2" t="s">
+        <v>1130</v>
+      </c>
+      <c r="F328" s="2" t="s">
+        <v>1137</v>
+      </c>
+      <c r="G328" s="2" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H328" s="2">
+        <v>1</v>
+      </c>
+      <c r="I328" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>{"id":328,"title":"banner-solid-icons-1-purple","group":"devblog","area":"banner","keywords":["icon"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
+      </c>
+    </row>
+    <row r="329" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A329" s="5">
+        <v>329</v>
+      </c>
+      <c r="C329" s="2" t="s">
+        <v>1127</v>
+      </c>
+      <c r="D329" t="s">
+        <v>866</v>
+      </c>
+      <c r="E329" s="2" t="s">
+        <v>1130</v>
+      </c>
+      <c r="F329" s="2" t="s">
+        <v>1137</v>
+      </c>
+      <c r="G329" s="2" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H329" s="2">
+        <v>1</v>
+      </c>
+      <c r="I329" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>{"id":329,"title":"banner-solid-icons-2-purple-dark","group":"devblog","area":"banner","keywords":["icon"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
+      </c>
+    </row>
+    <row r="330" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A330" s="5">
+        <v>330</v>
+      </c>
+      <c r="C330" s="2" t="s">
+        <v>1128</v>
+      </c>
+      <c r="D330" t="s">
+        <v>866</v>
+      </c>
+      <c r="E330" s="2" t="s">
+        <v>1130</v>
+      </c>
+      <c r="F330" s="2" t="s">
+        <v>1137</v>
+      </c>
+      <c r="G330" s="2" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H330" s="2">
+        <v>1</v>
+      </c>
+      <c r="I330" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>{"id":330,"title":"banner-solid-icons-2-purple","group":"devblog","area":"banner","keywords":["icon"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
+      </c>
+    </row>
+    <row r="331" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A331" s="5">
+        <v>331</v>
+      </c>
+      <c r="C331" s="2" t="s">
+        <v>1129</v>
+      </c>
+      <c r="D331" t="s">
+        <v>866</v>
+      </c>
+      <c r="E331" s="2" t="s">
+        <v>1130</v>
+      </c>
+      <c r="F331" s="2" t="s">
+        <v>1139</v>
+      </c>
+      <c r="G331" s="2" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H331" s="2">
+        <v>1</v>
+      </c>
+      <c r="I331" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>{"id":331,"title":"banner-triangulation-purple","group":"devblog","area":"banner","keywords":["triangle","shape","geometry"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new .NET illustrations
</commit_message>
<xml_diff>
--- a/src/assets/data.xlsx
+++ b/src/assets/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cherrywang/Dropbox/Code/vsimages/src/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cherr\Documents\Repos\illustration-catalog\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51DB282F-758D-0E4F-837B-4940913FA3EB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF42863-D1C1-497B-A5E6-63B0A80371CF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="5" r:id="rId1"/>
@@ -29,9 +29,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -6459,29 +6457,29 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K341"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B337" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B340" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H341" sqref="H341"/>
+      <selection pane="bottomRight" activeCell="C341" sqref="C341"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="100" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="100.05" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="13.33203125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="35.83203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="38.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="35.796875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="38.1328125" style="2" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
     <col min="5" max="5" width="18" style="2" customWidth="1"/>
     <col min="6" max="6" width="33.6640625" style="2" customWidth="1"/>
     <col min="7" max="8" width="20.6640625" style="2" customWidth="1"/>
-    <col min="9" max="10" width="24.1640625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="33.1640625" style="2" customWidth="1"/>
+    <col min="9" max="10" width="24.1328125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="33.1328125" style="2" customWidth="1"/>
     <col min="12" max="12" width="66.33203125" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="9.1640625" style="2"/>
+    <col min="13" max="16384" width="9.1328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="6" t="s">
         <v>201</v>
       </c>
@@ -6516,7 +6514,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -6550,7 +6548,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -6581,7 +6579,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\widget-you-dont-have-permission.svg</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -6612,7 +6610,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-charting-not-supported.svg</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -6643,7 +6641,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-custom-rules.svg</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -6674,7 +6672,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-get-back-to-recent-work.svg</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -6705,7 +6703,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-invalid-workitem-type.svg</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -6736,7 +6734,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-keep-an-eye-on-important-work.svg</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -6767,7 +6765,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-mention-someone.svg</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -6798,7 +6796,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-no-charts.svg</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -6829,7 +6827,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-unsaved-query.svg</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -6860,7 +6858,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-workitem-not-found.svg</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -6891,7 +6889,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-your-work-in-one-place.svg</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -6922,7 +6920,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-get-started-with-sprint.svg</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -6953,7 +6951,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-add-a-feed.svg</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -6984,7 +6982,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-connect-to-feed.svg</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -7015,7 +7013,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\general-no-results-found.svg</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -7046,7 +7044,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\hero-extend-vside.svg</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -7077,7 +7075,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-create-your-own-extension.svg</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -7108,7 +7106,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-marketplace.svg</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -7139,7 +7137,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-partner-program.svg</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -7170,7 +7168,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-what-are-extensions.svg</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -7201,7 +7199,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-add-product.svg</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -7232,7 +7230,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-configure-component-governance.svg</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -7263,7 +7261,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-release-management.svg</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -7294,7 +7292,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-this-repository-has-no-tags-yet.svg</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -7325,7 +7323,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-add-deployment-group.svg</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -7356,7 +7354,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-automate-build-definitions.svg</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -7387,7 +7385,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-choose-a-template.svg</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -7418,7 +7416,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-cloud-based-load-testing.svg</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -7449,7 +7447,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-favorites.svg</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -7480,7 +7478,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-get-everyone-on-same-page.svg</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -7511,7 +7509,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-no-plan.svg</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -7542,7 +7540,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-no-variable-groups.svg</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -7573,7 +7571,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-pull-request.svg</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -7604,7 +7602,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\hero-swiss-army-knife.svg</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -7635,7 +7633,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-all-your-code-hosted-free.svg</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -7666,7 +7664,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-any-client-any-platform.svg</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -7697,7 +7695,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-but-wait-theres-more.svg</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -7728,7 +7726,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-pricing.svg</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -7759,7 +7757,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-were-in-your-neighborhood.svg</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -7790,7 +7788,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\hero-pricing-calculator.svg</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -7821,7 +7819,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-you-have-no-organizations-yet.svg</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -7852,7 +7850,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\general-robot-errorcode-503.svg</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -7883,7 +7881,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\general-robot-error.svg</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -7914,7 +7912,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\general-robot-errorcode-400.svg</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -7945,7 +7943,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\general-robot-errorcode-401.svg</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -7976,7 +7974,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\general-robot-errorcode-403.svg</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -8007,7 +8005,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\general-robot-errorcode-404.svg</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -8038,7 +8036,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\general-robot-errorcode-500.svg</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -8069,7 +8067,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-no-assessments.svg</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -8100,7 +8098,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-initializing-test-results.svg</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -8131,7 +8129,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-no-work-scheduled.svg</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -8162,7 +8160,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-sprint-drag-n-drop.svg</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -8193,7 +8191,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-seamless-debugging-with-symbols.svg</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A56" s="5">
         <v>55</v>
       </c>
@@ -8224,7 +8222,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-xamarin-cross-platform.svg</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A57" s="5">
         <v>56</v>
       </c>
@@ -8255,7 +8253,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-azure-machine-learning.svg</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A58" s="5">
         <v>57</v>
       </c>
@@ -8286,7 +8284,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-cognitive-services.svg</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A59" s="5">
         <v>58</v>
       </c>
@@ -8317,7 +8315,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-congratulations-finished-setup.svg</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A60" s="5">
         <v>59</v>
       </c>
@@ -8348,7 +8346,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-cross-platform.svg</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A61" s="5">
         <v>60</v>
       </c>
@@ -8379,7 +8377,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-cryengine-game-development.svg</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A62" s="5">
         <v>61</v>
       </c>
@@ -8410,7 +8408,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-developer-meetup.svg</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A63" s="5">
         <v>62</v>
       </c>
@@ -8441,7 +8439,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-dotnet-core.svg</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A64" s="5">
         <v>63</v>
       </c>
@@ -8472,7 +8470,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-dotnet-enterprise.svg</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A65" s="5">
         <v>64</v>
       </c>
@@ -8503,7 +8501,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-download-target.svg</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A66" s="5">
         <v>65</v>
       </c>
@@ -8534,7 +8532,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-enterprise-customer-stories.svg</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A67" s="5">
         <v>66</v>
       </c>
@@ -8565,7 +8563,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-feedback-survey.svg</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A68" s="5">
         <v>67</v>
       </c>
@@ -8596,7 +8594,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-fsharp-data-science.svg</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A69" s="5">
         <v>68</v>
       </c>
@@ -8627,7 +8625,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-machine-learning-library.svg</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A70" s="5">
         <v>69</v>
       </c>
@@ -8658,7 +8656,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-one-consistent-api.svg</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A71" s="5">
         <v>70</v>
       </c>
@@ -8689,7 +8687,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-package-library.svg</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A72" s="5">
         <v>71</v>
       </c>
@@ -8720,7 +8718,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-programming-languages.svg</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A73" s="5">
         <v>72</v>
       </c>
@@ -8751,7 +8749,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-thank-you-for-downloading.svg</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A74" s="5">
         <v>73</v>
       </c>
@@ -8782,7 +8780,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-unity-game-development.svg</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A75" s="5">
         <v>74</v>
       </c>
@@ -8813,7 +8811,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-universal-windows-platform.svg</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A76" s="5">
         <v>75</v>
       </c>
@@ -8844,7 +8842,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-uwp-iot-core.svg</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A77" s="5">
         <v>76</v>
       </c>
@@ -8875,7 +8873,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-winform.svg</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A78" s="5">
         <v>77</v>
       </c>
@@ -8906,7 +8904,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-wpf.svg</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A79" s="5">
         <v>78</v>
       </c>
@@ -8937,7 +8935,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-xamarin.svg</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A80" s="5">
         <v>79</v>
       </c>
@@ -8968,7 +8966,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-dotnet-perf-diagram.svg</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A81" s="5">
         <v>80</v>
       </c>
@@ -8999,7 +8997,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\hero-snapshot-debugger.svg</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A82" s="5">
         <v>81</v>
       </c>
@@ -9030,7 +9028,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-collaborative-debugging.svg</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A83" s="5">
         <v>82</v>
       </c>
@@ -9061,7 +9059,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-collaborative-editing.svg</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A84" s="5">
         <v>83</v>
       </c>
@@ -9092,7 +9090,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-shared-full-context.svg</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A85" s="5">
         <v>84</v>
       </c>
@@ -9123,7 +9121,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-real-time-sharing.svg</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A86" s="5">
         <v>85</v>
       </c>
@@ -9154,7 +9152,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\blog-rocket-launch-timeline.svg</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A87" s="5">
         <v>86</v>
       </c>
@@ -9185,7 +9183,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\blog-vscode-metrics.svg</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A88" s="5">
         <v>87</v>
       </c>
@@ -9216,7 +9214,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\blog-vscode-roadmap.svg</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A89" s="5">
         <v>88</v>
       </c>
@@ -9247,7 +9245,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-monogame-game-development.svg</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A90" s="5">
         <v>89</v>
       </c>
@@ -9278,7 +9276,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-you-have-no-project.svg</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A91" s="5">
         <v>90</v>
       </c>
@@ -9309,7 +9307,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\hero-vsts-join-our-team.svg</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A92" s="5">
         <v>91</v>
       </c>
@@ -9340,7 +9338,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\elements-devices-1.svg</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A93" s="5">
         <v>92</v>
       </c>
@@ -9371,7 +9369,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\elements-devices-2.svg</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A94" s="5">
         <v>93</v>
       </c>
@@ -9402,7 +9400,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\elements-robots-1.svg</v>
       </c>
     </row>
-    <row r="95" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A95" s="5">
         <v>94</v>
       </c>
@@ -9433,7 +9431,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\elements-robots-2.svg</v>
       </c>
     </row>
-    <row r="96" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A96" s="5">
         <v>95</v>
       </c>
@@ -9464,7 +9462,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\elements-tools-1.svg</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A97" s="5">
         <v>96</v>
       </c>
@@ -9495,7 +9493,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\elements-tools-2.svg</v>
       </c>
     </row>
-    <row r="98" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A98" s="5">
         <v>97</v>
       </c>
@@ -9526,7 +9524,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\elements-vehicles-1.svg</v>
       </c>
     </row>
-    <row r="99" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A99" s="5">
         <v>98</v>
       </c>
@@ -9557,7 +9555,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\elements-vehicles-2.svg</v>
       </c>
     </row>
-    <row r="100" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A100" s="5">
         <v>99</v>
       </c>
@@ -9588,7 +9586,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\elements-vehicles-3.svg</v>
       </c>
     </row>
-    <row r="101" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A101" s="5">
         <v>100</v>
       </c>
@@ -9619,7 +9617,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-verify-analytics-views.svg</v>
       </c>
     </row>
-    <row r="102" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A102" s="5">
         <v>101</v>
       </c>
@@ -9650,7 +9648,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-analytics-views-error.svg</v>
       </c>
     </row>
-    <row r="103" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A103" s="5">
         <v>102</v>
       </c>
@@ -9681,7 +9679,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-analytics-views-valid.svg</v>
       </c>
     </row>
-    <row r="104" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A104" s="5">
         <v>103</v>
       </c>
@@ -9712,7 +9710,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-no-analytics-views.svg</v>
       </c>
     </row>
-    <row r="105" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A105" s="5">
         <v>104</v>
       </c>
@@ -9743,7 +9741,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-preparing-data.svg</v>
       </c>
     </row>
-    <row r="106" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A106" s="5">
         <v>105</v>
       </c>
@@ -9774,7 +9772,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\socialmedia-devops-youtube-header.svg</v>
       </c>
     </row>
-    <row r="107" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A107" s="5">
         <v>106</v>
       </c>
@@ -9805,7 +9803,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\socialmedia-devops-avatar.svg</v>
       </c>
     </row>
-    <row r="108" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A108" s="5">
         <v>107</v>
       </c>
@@ -9836,7 +9834,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\tile-self-hosted-server.svg</v>
       </c>
     </row>
-    <row r="109" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A109" s="5">
         <v>108</v>
       </c>
@@ -9867,7 +9865,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\tile-cloud-hosted-server.svg</v>
       </c>
     </row>
-    <row r="110" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A110" s="5">
         <v>109</v>
       </c>
@@ -9898,7 +9896,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\tile-integrate-with-cloud-services.svg</v>
       </c>
     </row>
-    <row r="111" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A111" s="5">
         <v>110</v>
       </c>
@@ -9929,7 +9927,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\general-folder.svg</v>
       </c>
     </row>
-    <row r="112" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A112" s="5">
         <v>111</v>
       </c>
@@ -9960,7 +9958,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-speed-gauge-comparison.svg</v>
       </c>
     </row>
-    <row r="113" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A113" s="5">
         <v>112</v>
       </c>
@@ -9991,7 +9989,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-speed-gauge-comparison-withtext.svg</v>
       </c>
     </row>
-    <row r="114" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A114" s="5">
         <v>113</v>
       </c>
@@ -10022,7 +10020,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-vside-lightbulb-intellisense.svg</v>
       </c>
     </row>
-    <row r="115" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A115" s="5">
         <v>114</v>
       </c>
@@ -10053,7 +10051,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-async-await-runners.svg</v>
       </c>
     </row>
-    <row r="116" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A116" s="5">
         <v>115</v>
       </c>
@@ -10084,7 +10082,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-barchart-skyline.svg</v>
       </c>
     </row>
-    <row r="117" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A117" s="5">
         <v>116</v>
       </c>
@@ -10115,7 +10113,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-barchart-skyline-withtext.svg</v>
       </c>
     </row>
-    <row r="118" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A118" s="5">
         <v>117</v>
       </c>
@@ -10146,7 +10144,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-contributors-around-world.svg</v>
       </c>
     </row>
-    <row r="119" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A119" s="5">
         <v>118</v>
       </c>
@@ -10177,7 +10175,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-contributors-around-world-withtext.svg</v>
       </c>
     </row>
-    <row r="120" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A120" s="5">
         <v>119</v>
       </c>
@@ -10208,7 +10206,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-dotnet-node-table.svg</v>
       </c>
     </row>
-    <row r="121" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A121" s="5">
         <v>120</v>
       </c>
@@ -10239,7 +10237,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-one-vs-many-tools.svg</v>
       </c>
     </row>
-    <row r="122" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A122" s="5">
         <v>121</v>
       </c>
@@ -10270,7 +10268,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-any-language.svg</v>
       </c>
     </row>
-    <row r="123" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A123" s="5">
         <v>122</v>
       </c>
@@ -10301,7 +10299,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-deploy-cross-platform.svg</v>
       </c>
     </row>
-    <row r="124" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A124" s="5">
         <v>123</v>
       </c>
@@ -10332,7 +10330,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-swiss-army-knife.svg</v>
       </c>
     </row>
-    <row r="125" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A125" s="5">
         <v>124</v>
       </c>
@@ -10363,7 +10361,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\hero-devops-conductor.svg</v>
       </c>
     </row>
-    <row r="126" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A126" s="5">
         <v>125</v>
       </c>
@@ -10394,7 +10392,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\blog-package-upstream-diagram-1.svg</v>
       </c>
     </row>
-    <row r="127" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A127" s="5">
         <v>126</v>
       </c>
@@ -10425,7 +10423,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\blog-package-upstream-diagram-2.svg</v>
       </c>
     </row>
-    <row r="128" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A128" s="5">
         <v>127</v>
       </c>
@@ -10456,7 +10454,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\blog-package-upstream-diagram-3.svg</v>
       </c>
     </row>
-    <row r="129" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A129" s="5">
         <v>128</v>
       </c>
@@ -10487,7 +10485,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\blog-package-upstream-diagram-4.svg</v>
       </c>
     </row>
-    <row r="130" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A130" s="5">
         <v>129</v>
       </c>
@@ -10518,7 +10516,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\willow-car-racing-get-ready.svg</v>
       </c>
     </row>
-    <row r="131" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A131" s="5">
         <v>130</v>
       </c>
@@ -10549,7 +10547,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\willow-rocket-get-ready.svg</v>
       </c>
     </row>
-    <row r="132" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A132" s="5">
         <v>131</v>
       </c>
@@ -10580,7 +10578,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\willow-bike-adventure.svg</v>
       </c>
     </row>
-    <row r="133" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A133" s="5">
         <v>132</v>
       </c>
@@ -10611,7 +10609,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\willow-bike-adventure-issue.svg</v>
       </c>
     </row>
-    <row r="134" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A134" s="5">
         <v>133</v>
       </c>
@@ -10642,7 +10640,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-no-dashboard.svg</v>
       </c>
     </row>
-    <row r="135" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A135" s="5">
         <v>134</v>
       </c>
@@ -10673,7 +10671,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\docs-gvfs-architecture.svg</v>
       </c>
     </row>
-    <row r="136" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A136" s="5">
         <v>135</v>
       </c>
@@ -10704,7 +10702,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\hero-vs-tools-for-azure.svg</v>
       </c>
     </row>
-    <row r="137" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A137" s="5">
         <v>136</v>
       </c>
@@ -10735,7 +10733,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-build-release-pipeline.svg</v>
       </c>
     </row>
-    <row r="138" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A138" s="5">
         <v>137</v>
       </c>
@@ -10766,7 +10764,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-build-release-monitor-activities.svg</v>
       </c>
     </row>
-    <row r="139" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A139" s="5">
         <v>138</v>
       </c>
@@ -10797,7 +10795,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-data-009.svg</v>
       </c>
     </row>
-    <row r="140" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A140" s="5">
         <v>139</v>
       </c>
@@ -10828,7 +10826,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-agriculture-001.svg</v>
       </c>
     </row>
-    <row r="141" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A141" s="5">
         <v>140</v>
       </c>
@@ -10859,7 +10857,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-001.svg</v>
       </c>
     </row>
-    <row r="142" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A142" s="5">
         <v>141</v>
       </c>
@@ -10890,7 +10888,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-002.svg</v>
       </c>
     </row>
-    <row r="143" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A143" s="5">
         <v>142</v>
       </c>
@@ -10921,7 +10919,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-003.svg</v>
       </c>
     </row>
-    <row r="144" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A144" s="5">
         <v>143</v>
       </c>
@@ -10952,7 +10950,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-004.svg</v>
       </c>
     </row>
-    <row r="145" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A145" s="5">
         <v>144</v>
       </c>
@@ -10983,7 +10981,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-005.svg</v>
       </c>
     </row>
-    <row r="146" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A146" s="5">
         <v>145</v>
       </c>
@@ -11014,7 +11012,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-006.svg</v>
       </c>
     </row>
-    <row r="147" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A147" s="5">
         <v>146</v>
       </c>
@@ -11045,7 +11043,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-007.svg</v>
       </c>
     </row>
-    <row r="148" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A148" s="5">
         <v>147</v>
       </c>
@@ -11076,7 +11074,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-008.svg</v>
       </c>
     </row>
-    <row r="149" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A149" s="5">
         <v>148</v>
       </c>
@@ -11107,7 +11105,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-009.svg</v>
       </c>
     </row>
-    <row r="150" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A150" s="5">
         <v>149</v>
       </c>
@@ -11138,7 +11136,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-010.svg</v>
       </c>
     </row>
-    <row r="151" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A151" s="5">
         <v>150</v>
       </c>
@@ -11169,7 +11167,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-011.svg</v>
       </c>
     </row>
-    <row r="152" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A152" s="5">
         <v>151</v>
       </c>
@@ -11200,7 +11198,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-012.svg</v>
       </c>
     </row>
-    <row r="153" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A153" s="5">
         <v>152</v>
       </c>
@@ -11231,7 +11229,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-013.svg</v>
       </c>
     </row>
-    <row r="154" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A154" s="5">
         <v>153</v>
       </c>
@@ -11262,7 +11260,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-014.svg</v>
       </c>
     </row>
-    <row r="155" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A155" s="5">
         <v>154</v>
       </c>
@@ -11293,7 +11291,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-015.svg</v>
       </c>
     </row>
-    <row r="156" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A156" s="5">
         <v>155</v>
       </c>
@@ -11324,7 +11322,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-016.svg</v>
       </c>
     </row>
-    <row r="157" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A157" s="5">
         <v>156</v>
       </c>
@@ -11355,7 +11353,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-business-017.svg</v>
       </c>
     </row>
-    <row r="158" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A158" s="5">
         <v>157</v>
       </c>
@@ -11386,7 +11384,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-001.svg</v>
       </c>
     </row>
-    <row r="159" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A159" s="5">
         <v>158</v>
       </c>
@@ -11417,7 +11415,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-002.svg</v>
       </c>
     </row>
-    <row r="160" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A160" s="5">
         <v>159</v>
       </c>
@@ -11448,7 +11446,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-003.svg</v>
       </c>
     </row>
-    <row r="161" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A161" s="5">
         <v>160</v>
       </c>
@@ -11479,7 +11477,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-004.svg</v>
       </c>
     </row>
-    <row r="162" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A162" s="5">
         <v>161</v>
       </c>
@@ -11510,7 +11508,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-005.svg</v>
       </c>
     </row>
-    <row r="163" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A163" s="5">
         <v>162</v>
       </c>
@@ -11541,7 +11539,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-006.svg</v>
       </c>
     </row>
-    <row r="164" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A164" s="5">
         <v>163</v>
       </c>
@@ -11572,7 +11570,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-007.svg</v>
       </c>
     </row>
-    <row r="165" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A165" s="5">
         <v>164</v>
       </c>
@@ -11603,7 +11601,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-008.svg</v>
       </c>
     </row>
-    <row r="166" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A166" s="5">
         <v>165</v>
       </c>
@@ -11634,7 +11632,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-009.svg</v>
       </c>
     </row>
-    <row r="167" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A167" s="5">
         <v>166</v>
       </c>
@@ -11665,7 +11663,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-010.svg</v>
       </c>
     </row>
-    <row r="168" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A168" s="5">
         <v>167</v>
       </c>
@@ -11696,7 +11694,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-011.svg</v>
       </c>
     </row>
-    <row r="169" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A169" s="5">
         <v>168</v>
       </c>
@@ -11727,7 +11725,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-012.svg</v>
       </c>
     </row>
-    <row r="170" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A170" s="5">
         <v>169</v>
       </c>
@@ -11758,7 +11756,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-cloud-013.svg</v>
       </c>
     </row>
-    <row r="171" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A171" s="5">
         <v>170</v>
       </c>
@@ -11789,7 +11787,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-collaboration-001.svg</v>
       </c>
     </row>
-    <row r="172" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A172" s="5">
         <v>171</v>
       </c>
@@ -11820,7 +11818,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-collaboration-002.svg</v>
       </c>
     </row>
-    <row r="173" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A173" s="5">
         <v>172</v>
       </c>
@@ -11851,7 +11849,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-collaboration-003.svg</v>
       </c>
     </row>
-    <row r="174" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A174" s="5">
         <v>173</v>
       </c>
@@ -11882,7 +11880,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-collaboration-005.svg</v>
       </c>
     </row>
-    <row r="175" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A175" s="5">
         <v>174</v>
       </c>
@@ -11913,7 +11911,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-collaboration-006.svg</v>
       </c>
     </row>
-    <row r="176" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A176" s="5">
         <v>175</v>
       </c>
@@ -11944,7 +11942,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-collaboration-007.svg</v>
       </c>
     </row>
-    <row r="177" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A177" s="5">
         <v>176</v>
       </c>
@@ -11975,7 +11973,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-collaboration-008.svg</v>
       </c>
     </row>
-    <row r="178" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A178" s="5">
         <v>177</v>
       </c>
@@ -12006,7 +12004,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-collaboration-009.svg</v>
       </c>
     </row>
-    <row r="179" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A179" s="5">
         <v>178</v>
       </c>
@@ -12037,7 +12035,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-collaboration-010.svg</v>
       </c>
     </row>
-    <row r="180" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A180" s="5">
         <v>179</v>
       </c>
@@ -12068,7 +12066,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-collaboration-011.svg</v>
       </c>
     </row>
-    <row r="181" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A181" s="5">
         <v>180</v>
       </c>
@@ -12099,7 +12097,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-communication-001.svg</v>
       </c>
     </row>
-    <row r="182" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A182" s="5">
         <v>181</v>
       </c>
@@ -12130,7 +12128,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-communication-002.svg</v>
       </c>
     </row>
-    <row r="183" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A183" s="5">
         <v>182</v>
       </c>
@@ -12161,7 +12159,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-consumer-001.svg</v>
       </c>
     </row>
-    <row r="184" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A184" s="5">
         <v>183</v>
       </c>
@@ -12192,7 +12190,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-consumer-002.svg</v>
       </c>
     </row>
-    <row r="185" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A185" s="5">
         <v>184</v>
       </c>
@@ -12223,7 +12221,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-data-001.svg</v>
       </c>
     </row>
-    <row r="186" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A186" s="5">
         <v>185</v>
       </c>
@@ -12254,7 +12252,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-data-002.svg</v>
       </c>
     </row>
-    <row r="187" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A187" s="5">
         <v>186</v>
       </c>
@@ -12285,7 +12283,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-data-003.svg</v>
       </c>
     </row>
-    <row r="188" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A188" s="5">
         <v>187</v>
       </c>
@@ -12316,7 +12314,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-data-004.svg</v>
       </c>
     </row>
-    <row r="189" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A189" s="5">
         <v>188</v>
       </c>
@@ -12347,7 +12345,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-data-005.svg</v>
       </c>
     </row>
-    <row r="190" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A190" s="5">
         <v>189</v>
       </c>
@@ -12378,7 +12376,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-data-006.svg</v>
       </c>
     </row>
-    <row r="191" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A191" s="5">
         <v>190</v>
       </c>
@@ -12409,7 +12407,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-data-007.svg</v>
       </c>
     </row>
-    <row r="192" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A192" s="5">
         <v>191</v>
       </c>
@@ -12440,7 +12438,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\MSC17-data-008.svg</v>
       </c>
     </row>
-    <row r="193" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A193" s="5">
         <v>192</v>
       </c>
@@ -12471,7 +12469,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\zerodata-feature-not-configured.svg</v>
       </c>
     </row>
-    <row r="194" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A194" s="5">
         <v>193</v>
       </c>
@@ -12502,7 +12500,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-boxes-and-devices.svg</v>
       </c>
     </row>
-    <row r="195" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A195" s="5">
         <v>194</v>
       </c>
@@ -12533,7 +12531,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-butler-ide.svg</v>
       </c>
     </row>
-    <row r="196" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A196" s="5">
         <v>195</v>
       </c>
@@ -12564,7 +12562,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-code-or-gui.svg</v>
       </c>
     </row>
-    <row r="197" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A197" s="5">
         <v>196</v>
       </c>
@@ -12595,7 +12593,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-data-analytics-pipeline.svg</v>
       </c>
     </row>
-    <row r="198" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A198" s="5">
         <v>197</v>
       </c>
@@ -12626,7 +12624,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-developer-scenarios.svg</v>
       </c>
     </row>
-    <row r="199" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A199" s="5">
         <v>198</v>
       </c>
@@ -12657,7 +12655,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-machine-learning-books-lab.svg</v>
       </c>
     </row>
-    <row r="200" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A200" s="5">
         <v>199</v>
       </c>
@@ -12688,7 +12686,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-machine-learning-extensible.svg</v>
       </c>
     </row>
-    <row r="201" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A201" s="5">
         <v>200</v>
       </c>
@@ -12719,7 +12717,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-machine-learning-lightbulb-hand.svg</v>
       </c>
     </row>
-    <row r="202" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A202" s="5">
         <v>201</v>
       </c>
@@ -12750,7 +12748,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-necessary-learner-tools.svg</v>
       </c>
     </row>
-    <row r="203" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A203" s="5">
         <v>202</v>
       </c>
@@ -12781,7 +12779,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-share-code-snippets.svg</v>
       </c>
     </row>
-    <row r="204" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A204" s="5">
         <v>203</v>
       </c>
@@ -12812,7 +12810,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-machine-learning-proven-extensible.svg</v>
       </c>
     </row>
-    <row r="205" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A205" s="5">
         <v>204</v>
       </c>
@@ -12843,7 +12841,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-machine-learning-pipeline.svg</v>
       </c>
     </row>
-    <row r="206" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A206" s="5">
         <v>205</v>
       </c>
@@ -12874,7 +12872,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-machine-learning-for-dotnet.svg</v>
       </c>
     </row>
-    <row r="207" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A207" s="5">
         <v>206</v>
       </c>
@@ -12905,7 +12903,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\swimlane-machine-learning-brain-lightbulb.svg</v>
       </c>
     </row>
-    <row r="208" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A208" s="5">
         <v>207</v>
       </c>
@@ -12936,7 +12934,7 @@
         <v>C:\Users\v-cowang\Dropbox\Code\vsimages\src\assets\illustrations\wizard-upgrade-from-xml-to-inheritance.svg</v>
       </c>
     </row>
-    <row r="209" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A209" s="5">
         <v>208</v>
       </c>
@@ -12963,7 +12961,7 @@
         <v>{"id":208,"title":"als-confirm-vm-specs","group":"als","area":"dashboard","keywords":["azure","lab","services","vm","virtual","machine","computer","gear","magnifier"],"description":"Used in Azure Lab Services classroom scenario onboarding UI.","publish":1}</v>
       </c>
     </row>
-    <row r="210" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A210" s="5">
         <v>209</v>
       </c>
@@ -12990,7 +12988,7 @@
         <v>{"id":209,"title":"als-install-artifacts-to-vm","group":"als","area":"dashboard","keywords":["azure","lab","services","vm","virtual","machine","install","app","package","cube","box","hook"],"description":"Used in Azure Lab Services classroom scenario onboarding UI.","publish":1}</v>
       </c>
     </row>
-    <row r="211" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A211" s="5">
         <v>210</v>
       </c>
@@ -13017,7 +13015,7 @@
         <v>{"id":210,"title":"als-decide-user-count","group":"als","area":"dashboard","keywords":["azure","lab","services","vm","virtual","machine","user","count","computer"],"description":"Used in Azure Lab Services classroom scenario onboarding UI.","publish":1}</v>
       </c>
     </row>
-    <row r="212" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A212" s="5">
         <v>211</v>
       </c>
@@ -13044,7 +13042,7 @@
         <v>{"id":211,"title":"als-set-policy-schedule","group":"als","area":"dashboard","keywords":["azure","lab","services","vm","virtual","machine","schedule","time","date","calendar","usage","analytics","chart"],"description":"Used in Azure Lab Services classroom scenario onboarding UI.","publish":1}</v>
       </c>
     </row>
-    <row r="213" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A213" s="5">
         <v>212</v>
       </c>
@@ -13071,7 +13069,7 @@
         <v>{"id":212,"title":"als-publish-vm","group":"als","area":"dashboard","keywords":["azure","lab","services","vm","virtual","machine","publish","url","send","computer","paper","plane"],"description":"Used in Azure Lab Services classroom scenario onboarding UI.","publish":1}</v>
       </c>
     </row>
-    <row r="214" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A214" s="5">
         <v>213</v>
       </c>
@@ -13098,7 +13096,7 @@
         <v>{"id":213,"title":"als-get-azure-subscription","group":"als","area":"frontdoor","keywords":["azure","lab","services","sign","up","subscription"],"description":"Get an Azure subscription.","publish":1}</v>
       </c>
     </row>
-    <row r="215" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A215" s="5">
         <v>214</v>
       </c>
@@ -13125,7 +13123,7 @@
         <v>{"id":214,"title":"als-add-lab-account","group":"als","area":"frontdoor","keywords":["azure","lab","services","cloud","add","lab","beaker"],"description":"Add lab account to Azure subscription.","publish":1}</v>
       </c>
     </row>
-    <row r="216" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A216" s="5">
         <v>215</v>
       </c>
@@ -13152,7 +13150,7 @@
         <v>{"id":215,"title":"als-create-lab","group":"als","area":"frontdoor","keywords":["azure","lab","services","add","computer","beaker","create"],"description":"Create your lab of VMs.","publish":1}</v>
       </c>
     </row>
-    <row r="217" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A217" s="5">
         <v>217</v>
       </c>
@@ -13179,7 +13177,7 @@
         <v>{"id":217,"title":"swimlane-ml-load-data","group":"dotnet","area":"swimlane","keywords":["machine","learning","load","data","import","funnel","raw"],"description":"Raw data being loaded into the pipeline.","publish":1}</v>
       </c>
     </row>
-    <row r="218" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A218" s="5">
         <v>218</v>
       </c>
@@ -13206,7 +13204,7 @@
         <v>{"id":218,"title":"swimlane-ml-transform-data","group":"dotnet","area":"swimlane","keywords":["machine","learning","transform","data","output","funnel","organize"],"description":"Data is being transformed and organized.","publish":1}</v>
       </c>
     </row>
-    <row r="219" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A219" s="5">
         <v>219</v>
       </c>
@@ -13233,7 +13231,7 @@
         <v>{"id":219,"title":"swimlane-ml-choose-algorithms","group":"dotnet","area":"swimlane","keywords":["machine","learning","fit","model","algorithm","grid","data"],"description":"Choose algorithms to fit data and develop models.","publish":1}</v>
       </c>
     </row>
-    <row r="220" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A220" s="5">
         <v>220</v>
       </c>
@@ -13260,7 +13258,7 @@
         <v>{"id":220,"title":"swimlane-ml-train-model","group":"dotnet","area":"swimlane","keywords":["machine","learning","data","train","model","prediction"],"description":"Train models to make prediction.","publish":1}</v>
       </c>
     </row>
-    <row r="221" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A221" s="5">
         <v>221</v>
       </c>
@@ -13287,7 +13285,7 @@
         <v>{"id":221,"title":"swimlane-ml-evaluate-model","group":"dotnet","area":"swimlane","keywords":["machine","learning","evaluate","model","measure","magnifier"],"description":"Evaluate and validate the model.","publish":1}</v>
       </c>
     </row>
-    <row r="222" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A222" s="5">
         <v>222</v>
       </c>
@@ -13314,7 +13312,7 @@
         <v>{"id":222,"title":"swimlane-ml-deploy-model","group":"dotnet","area":"swimlane","keywords":["machine","learning","deploy","model","parachute"],"description":"Use the model in applications.","publish":1}</v>
       </c>
     </row>
-    <row r="223" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A223" s="5">
         <v>223</v>
       </c>
@@ -13341,7 +13339,7 @@
         <v>{"id":223,"title":"swimlane-functional-programming-machine","group":"dotnet","area":"swimlane","keywords":["functional","programming","machine","fx","input","output"],"description":"Input going through a machine and output comes out. Used to represent functional programming.","publish":1}</v>
       </c>
     </row>
-    <row r="224" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A224" s="5">
         <v>224</v>
       </c>
@@ -13368,7 +13366,7 @@
         <v>{"id":224,"title":"swimlane-one-consistent-api-purple","group":"dotnet","area":"swimlane","keywords":["one","api","consistent","people","tool","library","book","light","bulb","idea","ui","code"],"description":"A person surrounded by multiple developer tools.","publish":1}</v>
       </c>
     </row>
-    <row r="225" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A225" s="5">
         <v>225</v>
       </c>
@@ -13395,7 +13393,7 @@
         <v>{"id":225,"title":"swimlane-teamwork-climb-mountain","group":"dotnet","area":"swimlane","keywords":["team","people","teamwork","collaboration","climb","mountain","outdoor"],"description":"A team climbing mountain together.","publish":1}</v>
       </c>
     </row>
-    <row r="226" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A226" s="5">
         <v>226</v>
       </c>
@@ -13422,7 +13420,7 @@
         <v>{"id":226,"title":"swimlane-toolchest-with-power-drill","group":"dotnet","area":"swimlane","keywords":["tools","sdk","toolbox","toolchest","power","drill","wrench","plier"],"description":"A toolchest stuffed with tools.","publish":1}</v>
       </c>
     </row>
-    <row r="227" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A227" s="5">
         <v>227</v>
       </c>
@@ -13449,7 +13447,7 @@
         <v>{"id":227,"title":"swimlane-tools-for-all-platforms","group":"dotnet","area":"swimlane","keywords":["tools","cross","platform","people","man","mac","windows","linux"],"description":"A developer and devices running Mac, Windows and Linux platforms.","publish":1}</v>
       </c>
     </row>
-    <row r="228" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A228" s="5">
         <v>228</v>
       </c>
@@ -13476,7 +13474,7 @@
         <v>{"id":228,"title":"swimlane-welcome-to-the-community","group":"dotnet","area":"swimlane","keywords":["people","person","man","woman","community","developer","welcome","join","open","source","team","work"],"description":"Developer community working together and welcoming new memebers.","publish":1}</v>
       </c>
     </row>
-    <row r="229" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A229" s="5">
         <v>229</v>
       </c>
@@ -13503,7 +13501,7 @@
         <v>{"id":229,"title":"devblog-mobile-app-center","group":"devblog","area":"thumbnail","keywords":["mobile","development","app","center","cloud","device","phone","laptop","xamarin","visual","studio","code"],"description":"Using Visual Studio and App Center for mobile development.","publish":1}</v>
       </c>
     </row>
-    <row r="230" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A230" s="5">
         <v>230</v>
       </c>
@@ -13530,7 +13528,7 @@
         <v>{"id":230,"title":"als-lab-empty-state","group":"als","area":"zerodata","keywords":["azure","lab","vm","virtual","machine","empty","dotted","line","woman","people","question","mark","computer"],"description":"Used for Azure Lab Services empty state when there is no VM in the lab.","publish":1}</v>
       </c>
     </row>
-    <row r="231" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A231" s="5">
         <v>231</v>
       </c>
@@ -13557,7 +13555,7 @@
         <v>{"id":231,"title":"als-waiting-beaker","group":"als","area":"wizard","keywords":["azure","lab","vm","beaker","waiting"],"description":"Used for Azure Lab Services waiting screens.","publish":1}</v>
       </c>
     </row>
-    <row r="232" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A232" s="5">
         <v>232</v>
       </c>
@@ -13584,7 +13582,7 @@
         <v>{"id":232,"title":"als-take-notes","group":"als","area":"wizard","keywords":["azure","lab","vm","note","sticky","pencil","write","credential"],"description":"Used for Azure Lab Services take notes of credentials wizard.","publish":1}</v>
       </c>
     </row>
-    <row r="233" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A233" s="5">
         <v>233</v>
       </c>
@@ -13611,7 +13609,7 @@
         <v>{"id":233,"title":"devblog-debug","group":"devblog","area":"thumbnail","keywords":["debug","magnifier","bug","code"],"description":"A magnifier looking for bugs in code.","publish":1}</v>
       </c>
     </row>
-    <row r="234" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A234" s="5">
         <v>234</v>
       </c>
@@ -13638,7 +13636,7 @@
         <v>{"id":234,"title":"swimlane-try-dotnet-features","group":"dotnet","area":"swimlane","keywords":["features","javascript","github","editor","code","theme","customize","paint","color","lightbulb","woman","people"],"description":"Try .NET features GitHub integration, customizable theme and JavaScript support.","publish":1}</v>
       </c>
     </row>
-    <row r="235" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A235" s="5">
         <v>235</v>
       </c>
@@ -13665,7 +13663,7 @@
         <v>{"id":235,"title":"swimlane-customize-editor-theme","group":"dotnet","area":"swimlane","keywords":["customize","editor","paint","brush","color","theme"],"description":"Customize Try .NET editor theme.","publish":1}</v>
       </c>
     </row>
-    <row r="236" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A236" s="5">
         <v>236</v>
       </c>
@@ -13692,7 +13690,7 @@
         <v>{"id":236,"title":"swimlane-embed-github-snippet","group":"dotnet","area":"swimlane","keywords":["embed","github","snippet","code","browser"],"description":"Load GitHub gists with Try .NET to edit code in browser.","publish":1}</v>
       </c>
     </row>
-    <row r="237" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A237" s="5">
         <v>237</v>
       </c>
@@ -13719,7 +13717,7 @@
         <v>{"id":237,"title":"swimlane-feature-tree-with-people","group":"dotnet","area":"swimlane","keywords":["tree","branch","node","feature","people"],"description":"See what people are creating with Try .NET.","publish":1}</v>
       </c>
     </row>
-    <row r="238" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A238" s="5">
         <v>238</v>
       </c>
@@ -13746,7 +13744,7 @@
         <v>{"id":238,"title":"hero-azure-notebooks","group":"notebooks","area":"hero","keywords":["azure","notebooks","data","science","charts","people","lab"],"description":"An open notebook with people working on different domains of data science.","publish":1}</v>
       </c>
     </row>
-    <row r="239" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A239" s="5">
         <v>239</v>
       </c>
@@ -13773,7 +13771,7 @@
         <v>{"id":239,"title":"spot-azure-accessible-everywhere","group":"notebooks","area":"spot","keywords":["azure","globe","cloud"],"description":"Azure Cloud Services accessible from anywhere in the world.","publish":1}</v>
       </c>
     </row>
-    <row r="240" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A240" s="5">
         <v>240</v>
       </c>
@@ -13800,7 +13798,7 @@
         <v>{"id":240,"title":"spot-notebooks-languages","group":"notebooks","area":"spot","keywords":["notebooks","language"],"description":"Azure Notebooks supports multiple languages.","publish":1}</v>
       </c>
     </row>
-    <row r="241" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A241" s="5">
         <v>241</v>
       </c>
@@ -13827,7 +13825,7 @@
         <v>{"id":241,"title":"spot-scientist-developer-student","group":"notebooks","area":"spot","keywords":["people","scientist","developer","student","lab","microscope","tool","engineering","cap","education"],"description":"Use Azure Notebooks for many workspaces and scenarios.","publish":1}</v>
       </c>
     </row>
-    <row r="242" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A242" s="5">
         <v>242</v>
       </c>
@@ -13854,7 +13852,7 @@
         <v>{"id":242,"title":"swimlane-migrate-to-azure","group":"dotnet","area":"swimlane","keywords":["migrate","azure","cloud","helicopter","move","transfer"],"description":"Migrate existing .NET apps to Azure.","publish":1}</v>
       </c>
     </row>
-    <row r="243" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A243" s="5">
         <v>243</v>
       </c>
@@ -13881,7 +13879,7 @@
         <v>{"id":243,"title":"swimlane-serverless-computing","group":"dotnet","area":"swimlane","keywords":["serverless","computing","unplug","network","cloud","computer","device","laptop","desktop","pc","web"],"description":"Serverless computing with .NET","publish":1}</v>
       </c>
     </row>
-    <row r="244" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A244" s="5">
         <v>244</v>
       </c>
@@ -13908,7 +13906,7 @@
         <v>{"id":244,"title":"swimlane-web-app-tools-library","group":"dotnet","area":"swimlane","keywords":["toolbox","tool","hammer","utility","wrench","pencil","clipboard","book","library"],"description":"Blue toolbox and books.","publish":1}</v>
       </c>
     </row>
-    <row r="245" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A245" s="5">
         <v>245</v>
       </c>
@@ -13935,7 +13933,7 @@
         <v>{"id":245,"title":"swimlane-build-cloud-apps","group":"dotnet","area":"swimlane","keywords":["build","forklift","box","container","cloud","scalable","people"],"description":"Build modern scalable cloud apps with .NET","publish":1}</v>
       </c>
     </row>
-    <row r="246" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A246" s="5">
         <v>246</v>
       </c>
@@ -13962,7 +13960,7 @@
         <v>{"id":246,"title":"swimlane-docker-container-support","group":"dotnet","area":"swimlane","keywords":["docker","cloud","container","ship","port","city","skyline","computer","laptop"],"description":"Ship with containers to represent Docker containers.","publish":1}</v>
       </c>
     </row>
-    <row r="247" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A247" s="5">
         <v>247</v>
       </c>
@@ -13989,7 +13987,7 @@
         <v>{"id":247,"title":"swimlane-global-data-storage","group":"dotnet","area":"swimlane","keywords":["data","storage","database","globe","duplicate","world"],"description":"Data storage accessible from everywhere in the world.","publish":1}</v>
       </c>
     </row>
-    <row r="248" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A248" s="5">
         <v>248</v>
       </c>
@@ -14016,7 +14014,7 @@
         <v>{"id":248,"title":"swimlane-security","group":"dotnet","area":"swimlane","keywords":["security","guard","camera","safe","secure"],"description":"A safety guard protecting a safe.","publish":1}</v>
       </c>
     </row>
-    <row r="249" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A249" s="5">
         <v>249</v>
       </c>
@@ -14043,7 +14041,7 @@
         <v>{"id":249,"title":"swimlane-angular-react-spa","group":"dotnet","area":"swimlane","keywords":["angular","react","spa","single","page","application","website"],"description":"React and Angular logo and single page web app.","publish":1}</v>
       </c>
     </row>
-    <row r="250" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A250" s="5">
         <v>250</v>
       </c>
@@ -14070,7 +14068,7 @@
         <v>{"id":250,"title":"swimlane-build-scalable-web-apps","group":"dotnet","area":"swimlane","keywords":["build","scalable","web","app","page","truck","box","people"],"description":"A worker loading boxes from truck to a web page.","publish":1}</v>
       </c>
     </row>
-    <row r="251" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A251" s="5">
         <v>251</v>
       </c>
@@ -14097,7 +14095,7 @@
         <v>{"id":251,"title":"swimlane-model-view-controller","group":"dotnet","area":"swimlane","keywords":["mvc","model","view","controller","data","gear","presentation","theme","paint","bucket","brush","design","frontend","backend","stack"],"description":"MVC illustration.","publish":1}</v>
       </c>
     </row>
-    <row r="252" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A252" s="5">
         <v>252</v>
       </c>
@@ -14124,7 +14122,7 @@
         <v>{"id":252,"title":"swimlane-seamless-data-integration","group":"dotnet","area":"swimlane","keywords":["data","database","orbit"],"description":"Seamless data integration.","publish":1}</v>
       </c>
     </row>
-    <row r="253" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A253" s="5">
         <v>253</v>
       </c>
@@ -14151,7 +14149,7 @@
         <v>{"id":253,"title":"swimlane-authentication-authorization","group":"dotnet","area":"swimlane","keywords":["authentication","authorization","password","login","key","lock","badge","access","key","chain"],"description":"A key chain with several authentication objects.","publish":1}</v>
       </c>
     </row>
-    <row r="254" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A254" s="5">
         <v>254</v>
       </c>
@@ -14178,7 +14176,7 @@
         <v>{"id":254,"title":"swimlane-rest-api","group":"dotnet","area":"swimlane","keywords":["rest","restful","api","json","bracket","data","database","interface","connect","device","platform"],"description":"Used to represent REST api.","publish":1}</v>
       </c>
     </row>
-    <row r="255" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A255" s="5">
         <v>255</v>
       </c>
@@ -14205,7 +14203,7 @@
         <v>{"id":255,"title":"swimlane-secure-chat-app","group":"dotnet","area":"swimlane","keywords":["lock","secure","chat","people","avatar","message"],"description":"An IM app with encrypted conversation.","publish":1}</v>
       </c>
     </row>
-    <row r="256" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A256" s="5">
         <v>256</v>
       </c>
@@ -14232,7 +14230,7 @@
         <v>{"id":256,"title":"swimlane-multiplayer-game","group":"dotnet","area":"swimlane","keywords":["game","multi","player","people","xbox","tv"],"description":"A man playing real-time multiplayer video game with a woman.","publish":1}</v>
       </c>
     </row>
-    <row r="257" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A257" s="5">
         <v>257</v>
       </c>
@@ -14259,7 +14257,7 @@
         <v>{"id":257,"title":"swimlane-mvc-scenario","group":"dotnet","area":"swimlane","keywords":["model","view","controller","mvc","layer","tier","stack","web","app","design","data","people"],"description":"Model-View-Controller explained with illustrated example.","publish":1}</v>
       </c>
     </row>
-    <row r="258" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A258" s="5">
         <v>258</v>
       </c>
@@ -14286,7 +14284,7 @@
         <v>{"id":258,"title":"swimlane-real-time-chat-app","group":"dotnet","area":"swimlane","keywords":["real","time","chat","app","people","tablet","device"],"description":"A woman using a laptop to chat with a man using tablet.","publish":1}</v>
       </c>
     </row>
-    <row r="259" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A259" s="5">
         <v>259</v>
       </c>
@@ -14313,7 +14311,7 @@
         <v>{"id":259,"title":"swimlane-signalr-hub","group":"dotnet","area":"swimlane","keywords":["signalr","hub","server","device","phone","mobile","tablet","browser","computer","laptop"],"description":"A server hub with connectors to multiple devices.","publish":1}</v>
       </c>
     </row>
-    <row r="260" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A260" s="5">
         <v>260</v>
       </c>
@@ -14340,7 +14338,7 @@
         <v>{"id":260,"title":"swimlane-azure-signalr-logo","group":"dotnet","area":"swimlane","keywords":["azure","signalr","logo"],"description":"Azure SignalR brand icon.","publish":1}</v>
       </c>
     </row>
-    <row r="261" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A261" s="5">
         <v>261</v>
       </c>
@@ -14367,7 +14365,7 @@
         <v>{"id":261,"title":"swimlane-chat-app-multiplatform","group":"dotnet","area":"swimlane","keywords":["chat","app","multi","platform","device","people"],"description":"A woman using the same chat app available on multiple devices.","publish":1}</v>
       </c>
     </row>
-    <row r="262" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A262" s="5">
         <v>262</v>
       </c>
@@ -14394,7 +14392,7 @@
         <v>{"id":262,"title":"swimlane-fast-performance-gauge","group":"dotnet","area":"swimlane","keywords":["performance","race","car","gauge","speed","fast"],"description":"A car racing themed background with a speed gauge.","publish":1}</v>
       </c>
     </row>
-    <row r="263" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A263" s="5">
         <v>263</v>
       </c>
@@ -14421,7 +14419,7 @@
         <v>{"id":263,"title":"vsmac-installer-screen","group":"vsmac","area":"splashscreen","keywords":["space","galaxy","cloud","people","work","desk","install","download","waiting"],"description":"Two people playing with paper plane while waiting for installation. Space theme background.","publish":1}</v>
       </c>
     </row>
-    <row r="264" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A264" s="5">
         <v>264</v>
       </c>
@@ -14448,7 +14446,7 @@
         <v>{"id":264,"title":"hero-vs-enterprise-sku","group":"vscom","area":"hero","keywords":["small","team","free","community","collaboration","rocket","sketch","blueprint","hands"],"description":"Small team designing rocket collaboratively.","publish":1}</v>
       </c>
     </row>
-    <row r="265" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A265" s="5">
         <v>265</v>
       </c>
@@ -14475,7 +14473,7 @@
         <v>{"id":265,"title":"hero-vs-professional-sku","group":"vscom","area":"hero","keywords":["medium","team","professional","build","collaboration","rocket","robot","engineer"],"description":"Medium size professional engineers building rocket.","publish":1}</v>
       </c>
     </row>
-    <row r="266" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A266" s="5">
         <v>266</v>
       </c>
@@ -14502,7 +14500,7 @@
         <v>{"id":266,"title":"hero-vs-community-sku","group":"vscom","area":"hero","keywords":["enterprise","company","large","scale","buildings","process","rocket","workflow","truck"],"description":"Big enterprise mass producing rockets.","publish":1}</v>
       </c>
     </row>
-    <row r="267" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A267" s="5">
         <v>267</v>
       </c>
@@ -14529,7 +14527,7 @@
         <v>{"id":267,"title":"swimlane-build-scalable-apps","group":"dotnet","area":"swimlane","keywords":["build","scalable","building","crane","construction","scalability","stack","city","tree"],"description":"A construction crane loading stacks to build a skyscraper.","publish":1}</v>
       </c>
     </row>
-    <row r="268" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A268" s="5">
         <v>268</v>
       </c>
@@ -14556,7 +14554,7 @@
         <v>{"id":268,"title":"swimlane-docker-three-platforms","group":"dotnet","area":"swimlane","keywords":["docker","platform","os","windows","linux","macos","ship","container"],"description":"A freight ship with containers running on Windows, Linux and macOS.","publish":1}</v>
       </c>
     </row>
-    <row r="269" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A269" s="5">
         <v>269</v>
       </c>
@@ -14583,7 +14581,7 @@
         <v>{"id":269,"title":"swimlane-dotnet-compatible-with-other-tools","group":"dotnet","area":"swimlane","keywords":["dotnet","module","microservices","cube","plug","compatible","side","by","side","tools","stacks","people"],"description":".NET works side-by-side with other technology stacks.","publish":1}</v>
       </c>
     </row>
-    <row r="270" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A270" s="5">
         <v>270</v>
       </c>
@@ -14610,7 +14608,7 @@
         <v>{"id":270,"title":"swimlane-microservices-build","group":"dotnet","area":"swimlane","keywords":["microservices","build","module","truck","people","load","blocks"],"description":"People integrating microservice modules to make complete products.","publish":1}</v>
       </c>
     </row>
-    <row r="271" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A271" s="5">
         <v>271</v>
       </c>
@@ -14637,7 +14635,7 @@
         <v>{"id":271,"title":"swimlane-microservices-modules","group":"dotnet","area":"swimlane","keywords":["microservices","building","blocks","modules","cubes","plug","connect","integrate"],"description":"Microservices building blocks.","publish":1}</v>
       </c>
     </row>
-    <row r="272" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A272" s="5">
         <v>272</v>
       </c>
@@ -14664,7 +14662,7 @@
         <v>{"id":272,"title":"swimlane-brand-docker","group":"dotnet","area":"swimlane","keywords":["docker","brand","logo"],"description":"Docker logo","publish":1}</v>
       </c>
     </row>
-    <row r="273" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A273" s="5">
         <v>273</v>
       </c>
@@ -14691,7 +14689,7 @@
         <v>{"id":273,"title":"swimlane-event-driven-programming","group":"dotnet","area":"swimlane","keywords":["winform","event","trigger","click","button","control","sync","server","gear"],"description":"Event triggered in the presentation tier and passed to server.","publish":1}</v>
       </c>
     </row>
-    <row r="274" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A274" s="5">
         <v>274</v>
       </c>
@@ -14718,7 +14716,7 @@
         <v>{"id":274,"title":"swimlane-razor-cross-platform","group":"dotnet","area":"swimlane","keywords":["razor","@","html","cross","platform","windows","linux","macos","coffee","mugs","cups","tea"],"description":"Razor pages works across multiple platforms.","publish":1}</v>
       </c>
     </row>
-    <row r="275" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A275" s="5">
         <v>275</v>
       </c>
@@ -14745,7 +14743,7 @@
         <v>{"id":275,"title":"swimlane-webform","group":"dotnet","area":"swimlane","keywords":["webform","control","drag","drop","pencil","button","window","dialog"],"description":"Drag and drop designer for building Webform applications.","publish":1}</v>
       </c>
     </row>
-    <row r="276" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A276" s="5">
         <v>276</v>
       </c>
@@ -14772,7 +14770,7 @@
         <v>{"id":276,"title":"swimlane-webform-control-library","group":"dotnet","area":"swimlane","keywords":["webform","control","button","dropdown","textbox","radio","button","checkbox"],"description":"A large library of webform controls.","publish":1}</v>
       </c>
     </row>
-    <row r="277" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A277" s="5">
         <v>277</v>
       </c>
@@ -14799,7 +14797,7 @@
         <v>{"id":277,"title":"swimlane-webform-data-integration","group":"dotnet","area":"swimlane","keywords":["data","integration","webform","dropdown","input","table","database","connect"],"description":"Simple data integration with .NET web forms.","publish":1}</v>
       </c>
     </row>
-    <row r="278" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A278" s="5">
         <v>278</v>
       </c>
@@ -14826,7 +14824,7 @@
         <v>{"id":278,"title":"swimlane-community-documentation","group":"dotnet","area":"swimlane","keywords":["community","people","collaboration","documentation","open","source","hands","paper","pencil","team"],"description":"Active developer community and up to date documentation.","publish":1}</v>
       </c>
     </row>
-    <row r="279" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A279" s="5">
         <v>279</v>
       </c>
@@ -14853,7 +14851,7 @@
         <v>{"id":279,"title":"swimlane-license-certificates","group":"dotnet","area":"swimlane","keywords":["license","certificate","ribbon","copyright"],"description":"License certificates.","publish":1}</v>
       </c>
     </row>
-    <row r="280" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A280" s="5">
         <v>280</v>
       </c>
@@ -14880,7 +14878,7 @@
         <v>{"id":280,"title":"swimlane-brand-dotnet-foundation","group":"dotnet","area":"swimlane","keywords":["brand","dotnet","foundation","logo"],"description":".NET Foundation logo.","publish":1}</v>
       </c>
     </row>
-    <row r="281" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A281" s="5">
         <v>281</v>
       </c>
@@ -14907,7 +14905,7 @@
         <v>{"id":281,"title":"swimlane-brand-github-octocat","group":"dotnet","area":"swimlane","keywords":["brand","github","octocat","mascot"],"description":"GitHub Octocat.","publish":1}</v>
       </c>
     </row>
-    <row r="282" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A282" s="5">
         <v>282</v>
       </c>
@@ -14934,7 +14932,7 @@
         <v>{"id":282,"title":"swimlane-brand-microsoft","group":"dotnet","area":"swimlane","keywords":["brand","microsoft","logo"],"description":"Microsoft logo.","publish":1}</v>
       </c>
     </row>
-    <row r="283" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A283" s="5">
         <v>283</v>
       </c>
@@ -14961,7 +14959,7 @@
         <v>{"id":283,"title":"modal-man-and-dog","group":"vscom","area":"modal","keywords":["man","laptop","people","dog","work","play"],"description":"A man using a laptop, sitting on the ground with a dog.","publish":1}</v>
       </c>
     </row>
-    <row r="284" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A284" s="5">
         <v>284</v>
       </c>
@@ -14988,7 +14986,7 @@
         <v>{"id":284,"title":"modal-man-dog- rube-goldberg-machine","group":"vscom","area":"modal","keywords":["man","laptop","people","dog","work","play","productivity","rube","goldberg","machine"],"description":"A man using a laptop, sitting on the ground with a dog. A Rube Goldberg machine in the background.","publish":1}</v>
       </c>
     </row>
-    <row r="285" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A285" s="5">
         <v>285</v>
       </c>
@@ -15015,7 +15013,7 @@
         <v>{"id":285,"title":"modal-subscribe-to-news-tips","group":"vscom","area":"modal","keywords":["woman","people","laptop","subscribe","email","newsletter","newspaper","lightbulb","tips","envelope","video","tutorials"],"description":"A woman using a laptop. Newsletter related icons floating around.","publish":1}</v>
       </c>
     </row>
-    <row r="286" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A286" s="5">
         <v>286</v>
       </c>
@@ -15042,7 +15040,7 @@
         <v>{"id":286,"title":"modal-joining-live-share-session","group":"vscom","area":"modal","keywords":["code","developer","editor","collaborate","share","people","computer","monitor","laptop"],"description":"A developer joining a Live Share session.","publish":1}</v>
       </c>
     </row>
-    <row r="287" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A287" s="5">
         <v>287</v>
       </c>
@@ -15069,7 +15067,7 @@
         <v>{"id":287,"title":"modal-live-share-session-inactive","group":"vscom","area":"modal","keywords":["code","developer","editor","collaborate","share","people","computer","monitor","laptop","wait","inactive","clock"],"description":"A developer waiting to join a Live Share session but the session is inactive.","publish":1}</v>
       </c>
     </row>
-    <row r="288" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A288" s="5">
         <v>288</v>
       </c>
@@ -15096,7 +15094,7 @@
         <v>{"id":288,"title":"swimlane-dotnet-platform","group":"dotnet","area":"swimlane","keywords":["platform","tools","library","utility","framework","drill","wrench","screwdriver","ruler","pencil","book"],"description":"A workbench with varies tools.","publish":1}</v>
       </c>
     </row>
-    <row r="289" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A289" s="5">
         <v>289</v>
       </c>
@@ -15123,7 +15121,7 @@
         <v>{"id":289,"title":"swimlane-pages-realtime-apis-microservices","group":"dotnet","area":"swimlane","keywords":["page","realtime","api","microservice","scroll","puzzle","clock","cube","block","module","people","tree"],"description":"A man standing under a feature tree.","publish":1}</v>
       </c>
     </row>
-    <row r="290" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A290" s="5">
         <v>290</v>
       </c>
@@ -15150,7 +15148,7 @@
         <v>{"id":290,"title":"swimlane-aspnet-extends-dotnet","group":"dotnet","area":"swimlane","keywords":["platform","tools","utility","framework","drill","wrench","screwdriver","ruler","pencil","hammer","plier"],"description":"A blueprint with varies tools drawing and a few tools floating.","publish":1}</v>
       </c>
     </row>
-    <row r="291" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A291" s="5">
         <v>291</v>
       </c>
@@ -15177,7 +15175,7 @@
         <v>{"id":291,"title":"swimlane-backend-code","group":"dotnet","area":"swimlane","keywords":["backend","code","programming","editor","people","gear","developer"],"description":"A code editor and two developers working on backend.","publish":1}</v>
       </c>
     </row>
-    <row r="292" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A292" s="5">
         <v>292</v>
       </c>
@@ -15204,7 +15202,7 @@
         <v>{"id":292,"title":"swimlane-man-dog- rube-goldberg-machine","group":"dotnet","area":"swimlane","keywords":["man","laptop","people","dog","work","play","productivity","rube","goldberg","machine"],"description":"A man using a laptop, sitting on the ground with a dog. A Rube Goldberg machine in the background.","publish":1}</v>
       </c>
     </row>
-    <row r="293" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A293" s="5">
         <v>293</v>
       </c>
@@ -15231,7 +15229,7 @@
         <v>{"id":293,"title":"swimlane-subscribe-to-news-tips","group":"dotnet","area":"swimlane","keywords":["woman","people","laptop","subscribe","email","newsletter","newspaper","lightbulb","tips","envelope","video","tutorials"],"description":"A woman using a laptop. Newsletter related icons floating around.","publish":1}</v>
       </c>
     </row>
-    <row r="294" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A294" s="5">
         <v>294</v>
       </c>
@@ -15258,7 +15256,7 @@
         <v>{"id":294,"title":"prop-productive","group":"vscom","area":"valueprop","keywords":["productivity","machine","belt","process"],"description":"Belt and gear.","publish":1}</v>
       </c>
     </row>
-    <row r="295" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A295" s="5">
         <v>295</v>
       </c>
@@ -15285,7 +15283,7 @@
         <v>{"id":295,"title":"prop-innovate","group":"vscom","area":"valueprop","keywords":["innovative","lightbulb","idea","insight","beaker"],"description":"A lightbulb and a beaker.","publish":1}</v>
       </c>
     </row>
-    <row r="296" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A296" s="5">
         <v>296</v>
       </c>
@@ -15312,7 +15310,7 @@
         <v>{"id":296,"title":"prop-modern","group":"vscom","area":"valueprop","keywords":["modern","technology","robot","machine"],"description":"A robot pressing a button.","publish":1}</v>
       </c>
     </row>
-    <row r="297" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A297" s="5">
         <v>297</v>
       </c>
@@ -15339,7 +15337,7 @@
         <v>{"id":297,"title":"hero-race-car-blue","group":"dataacc","area":"hero","keywords":["race","car","speed","accelerate","data","science"],"description":"A running race car with data numbers speed lines.","publish":1}</v>
       </c>
     </row>
-    <row r="298" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A298" s="5">
         <v>298</v>
       </c>
@@ -15366,7 +15364,7 @@
         <v>{"id":298,"title":"hero-race-car","group":"dataacc","area":"hero","keywords":["race","car","speed","accelerate","data","science"],"description":"A running race car with data numbers speed lines.","publish":1}</v>
       </c>
     </row>
-    <row r="299" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A299" s="5">
         <v>299</v>
       </c>
@@ -15393,7 +15391,7 @@
         <v>{"id":299,"title":"prop-add-sql-to-flow","group":"dataacc","area":"valueprop","keywords":["sql","database","flow","chart","lightbulb"],"description":"Used for adding sql to flow tutorial.","publish":1}</v>
       </c>
     </row>
-    <row r="300" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A300" s="5">
         <v>300</v>
       </c>
@@ -15420,7 +15418,7 @@
         <v>{"id":300,"title":"prop-extend-and-reuse","group":"dataacc","area":"valueprop","keywords":["extend","reuse","module","cube","plug","extension"],"description":"Connected cubes that represent modular code.","publish":1}</v>
       </c>
     </row>
-    <row r="301" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A301" s="5">
         <v>301</v>
       </c>
@@ -15447,7 +15445,7 @@
         <v>{"id":301,"title":"prop-get-schema","group":"dataacc","area":"valueprop","keywords":["schema","process","flow","conveyor","belt","beaker","lab","science","chart","gear"],"description":"Used for get schema tutorial.","publish":1}</v>
       </c>
     </row>
-    <row r="302" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A302" s="5">
         <v>302</v>
       </c>
@@ -15474,7 +15472,7 @@
         <v>{"id":302,"title":"prop-home-automation","group":"dataacc","area":"valueprop","keywords":["home","automation","smart","iot","connected"],"description":"Used for home automation sample.","publish":1}</v>
       </c>
     </row>
-    <row r="303" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A303" s="5">
         <v>303</v>
       </c>
@@ -15501,7 +15499,7 @@
         <v>{"id":303,"title":"prop-live-query","group":"dataacc","area":"valueprop","keywords":["live","query","immediate","fast","lightning","bolt"],"description":"Used for live query tutorial.","publish":1}</v>
       </c>
     </row>
-    <row r="304" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A304" s="5">
         <v>304</v>
       </c>
@@ -15528,7 +15526,7 @@
         <v>{"id":304,"title":"prop-no-code-ui","group":"dataacc","area":"valueprop","keywords":["ui","drag","drop","hand"],"description":"Used for representing no code UI experience.","publish":1}</v>
       </c>
     </row>
-    <row r="305" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A305" s="5">
         <v>305</v>
       </c>
@@ -15555,7 +15553,7 @@
         <v>{"id":305,"title":"prop-sql-knowledge","group":"dataacc","area":"valueprop","keywords":["sql","database","knowledge","education","graduateion","cap"],"description":"Used for language feature tutorial.","publish":1}</v>
       </c>
     </row>
-    <row r="306" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A306" s="5">
         <v>306</v>
       </c>
@@ -15582,7 +15580,7 @@
         <v>{"id":306,"title":"hero-developer-day-2019","group":"vscom","area":"hero","keywords":["developer","day","build","seattle","feedback","bubble","lightbulb","rube","goldburg","machine","process","city","sasquatch"],"description":"Hero image for Develoepr Day 2019","publish":1}</v>
       </c>
     </row>
-    <row r="307" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A307" s="5">
         <v>307</v>
       </c>
@@ -15609,7 +15607,7 @@
         <v>{"id":307,"title":"banner-arrows-dark-blue","group":"devblog","area":"banner","keywords":["arrow","navigation","motion"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
       </c>
     </row>
-    <row r="308" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A308" s="5">
         <v>308</v>
       </c>
@@ -15636,7 +15634,7 @@
         <v>{"id":308,"title":"banner-big-code-1-purple","group":"devblog","area":"banner","keywords":["code"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
       </c>
     </row>
-    <row r="309" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A309" s="5">
         <v>309</v>
       </c>
@@ -15663,7 +15661,7 @@
         <v>{"id":309,"title":"banner-big-code-2-purple","group":"devblog","area":"banner","keywords":["code"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
       </c>
     </row>
-    <row r="310" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A310" s="5">
         <v>310</v>
       </c>
@@ -15690,7 +15688,7 @@
         <v>{"id":310,"title":"banner-big-code-dark-blue","group":"devblog","area":"banner","keywords":["code"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
       </c>
     </row>
-    <row r="311" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A311" s="5">
         <v>311</v>
       </c>
@@ -15717,7 +15715,7 @@
         <v>{"id":311,"title":"banner-big-code-turquoise","group":"devblog","area":"banner","keywords":["code"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
       </c>
     </row>
-    <row r="312" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A312" s="5">
         <v>312</v>
       </c>
@@ -15744,7 +15742,7 @@
         <v>{"id":312,"title":"banner-bugs-gray","group":"devblog","area":"banner","keywords":["bug","debug"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
       </c>
     </row>
-    <row r="313" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A313" s="5">
         <v>313</v>
       </c>
@@ -15771,7 +15769,7 @@
         <v>{"id":313,"title":"banner-bugs-purple","group":"devblog","area":"banner","keywords":["bug","debug"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
       </c>
     </row>
-    <row r="314" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A314" s="5">
         <v>314</v>
       </c>
@@ -15798,7 +15796,7 @@
         <v>{"id":314,"title":"banner-bugs-turquoise","group":"devblog","area":"banner","keywords":["bug","debug"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
       </c>
     </row>
-    <row r="315" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A315" s="5">
         <v>315</v>
       </c>
@@ -15825,7 +15823,7 @@
         <v>{"id":315,"title":"banner-cloud-vectors-blue","group":"devblog","area":"banner","keywords":["cloud"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
       </c>
     </row>
-    <row r="316" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A316" s="5">
         <v>316</v>
       </c>
@@ -15852,7 +15850,7 @@
         <v>{"id":316,"title":"banner-code-1-purple","group":"devblog","area":"banner","keywords":["code"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
       </c>
     </row>
-    <row r="317" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A317" s="5">
         <v>317</v>
       </c>
@@ -15879,7 +15877,7 @@
         <v>{"id":317,"title":"banner-code-2-purple","group":"devblog","area":"banner","keywords":["code"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
       </c>
     </row>
-    <row r="318" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A318" s="5">
         <v>318</v>
       </c>
@@ -15906,7 +15904,7 @@
         <v>{"id":318,"title":"banner-cubes-magenta","group":"devblog","area":"banner","keywords":["cube","microservice","module","component"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
       </c>
     </row>
-    <row r="319" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A319" s="5">
         <v>319</v>
       </c>
@@ -15933,7 +15931,7 @@
         <v>{"id":319,"title":"banner-devices-1-blue","group":"devblog","area":"banner","keywords":["device","mobile","phone","computer","laptop"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
       </c>
     </row>
-    <row r="320" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A320" s="5">
         <v>320</v>
       </c>
@@ -15960,7 +15958,7 @@
         <v>{"id":320,"title":"banner-devices-1-purple","group":"devblog","area":"banner","keywords":["device","mobile","phone","computer","laptop"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
       </c>
     </row>
-    <row r="321" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A321" s="5">
         <v>321</v>
       </c>
@@ -15987,7 +15985,7 @@
         <v>{"id":321,"title":"banner-mix-1-blue","group":"devblog","area":"banner","keywords":["icon"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
       </c>
     </row>
-    <row r="322" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A322" s="5">
         <v>322</v>
       </c>
@@ -16014,7 +16012,7 @@
         <v>{"id":322,"title":"banner-mix-1-gray","group":"devblog","area":"banner","keywords":["icon"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
       </c>
     </row>
-    <row r="323" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A323" s="5">
         <v>323</v>
       </c>
@@ -16041,7 +16039,7 @@
         <v>{"id":323,"title":"banner-outline-icons-blue","group":"devblog","area":"banner","keywords":["icon"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
       </c>
     </row>
-    <row r="324" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A324" s="5">
         <v>324</v>
       </c>
@@ -16068,7 +16066,7 @@
         <v>{"id":324,"title":"banner-outline-icons-purple","group":"devblog","area":"banner","keywords":["particle","line"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
       </c>
     </row>
-    <row r="325" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A325" s="5">
         <v>325</v>
       </c>
@@ -16095,7 +16093,7 @@
         <v>{"id":325,"title":"banner-particle-lines-blue","group":"devblog","area":"banner","keywords":["particle","line"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
       </c>
     </row>
-    <row r="326" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A326" s="5">
         <v>326</v>
       </c>
@@ -16122,7 +16120,7 @@
         <v>{"id":326,"title":"banner-people-purple","group":"devblog","area":"banner","keywords":["people"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
       </c>
     </row>
-    <row r="327" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A327" s="5">
         <v>327</v>
       </c>
@@ -16149,7 +16147,7 @@
         <v>{"id":327,"title":"banner-small-outline-purple","group":"devblog","area":"banner","keywords":["people"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
       </c>
     </row>
-    <row r="328" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A328" s="5">
         <v>328</v>
       </c>
@@ -16176,7 +16174,7 @@
         <v>{"id":328,"title":"banner-solid-icons-1-purple","group":"devblog","area":"banner","keywords":["icon"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
       </c>
     </row>
-    <row r="329" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A329" s="5">
         <v>329</v>
       </c>
@@ -16203,7 +16201,7 @@
         <v>{"id":329,"title":"banner-solid-icons-2-purple-dark","group":"devblog","area":"banner","keywords":["icon"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
       </c>
     </row>
-    <row r="330" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A330" s="5">
         <v>330</v>
       </c>
@@ -16230,7 +16228,7 @@
         <v>{"id":330,"title":"banner-solid-icons-2-purple","group":"devblog","area":"banner","keywords":["icon"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
       </c>
     </row>
-    <row r="331" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A331" s="5">
         <v>331</v>
       </c>
@@ -16257,7 +16255,7 @@
         <v>{"id":331,"title":"banner-triangulation-purple","group":"devblog","area":"banner","keywords":["triangle","shape","geometry"],"description":"Background images used for DevBlog banner area.","publish":1}</v>
       </c>
     </row>
-    <row r="332" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A332" s="5">
         <v>332</v>
       </c>
@@ -16284,7 +16282,7 @@
         <v>{"id":332,"title":"swimlane-blazor-shared-libraries","group":"dotnet","area":"swimlane","keywords":["blazor","browser","web","share","library","component","colde","module","book"],"description":"Blazor supports shared library and code components.","publish":1}</v>
       </c>
     </row>
-    <row r="333" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A333" s="5">
         <v>333</v>
       </c>
@@ -16311,7 +16309,7 @@
         <v>{"id":333,"title":"swimlane-browser-server","group":"dotnet","area":"swimlane","keywords":["browser","client","server","web","frontend","backend"],"description":"Blazor runs on browser and server.","publish":1}</v>
       </c>
     </row>
-    <row r="334" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A334" s="5">
         <v>334</v>
       </c>
@@ -16338,7 +16336,7 @@
         <v>{"id":334,"title":"swimlane-cross-browser","group":"dotnet","area":"swimlane","keywords":["cross","browser","chrome","firefox","edge","safari","mobile","phone","platform"],"description":"Four common browsers collage.","publish":1}</v>
       </c>
     </row>
-    <row r="335" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A335" s="5">
         <v>335</v>
       </c>
@@ -16365,7 +16363,7 @@
         <v>{"id":335,"title":"swimlane-cross-platform-desktop","group":"dotnet","area":"swimlane","keywords":["cross","platform","windows","mac","linux","computer","laptop","desktop"],"description":"Three devices collage.","publish":1}</v>
       </c>
     </row>
-    <row r="336" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A336" s="5">
         <v>336</v>
       </c>
@@ -16392,7 +16390,7 @@
         <v>{"id":336,"title":"swimlane-csharp-javascript","group":"dotnet","area":"swimlane","keywords":["c#","csharp","js","javascript","language","interop"],"description":"C# works with JavaScript.","publish":1}</v>
       </c>
     </row>
-    <row r="337" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A337" s="5">
         <v>337</v>
       </c>
@@ -16419,7 +16417,7 @@
         <v>{"id":337,"title":"swimlane-cross-platform-cloud","group":"dotnet","area":"swimlane","keywords":["cross","platform","windows","mac","linux","computer","laptop","desktop","cloud"],"description":"Three devices collage and a cloud.","publish":1}</v>
       </c>
     </row>
-    <row r="338" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A338" s="5">
         <v>338</v>
       </c>
@@ -16446,7 +16444,7 @@
         <v>{"id":338,"title":"swimlane-dotnet-for-spark-rainbow-chart","group":"dotnet","area":"swimlane","keywords":["rainbow","chart","stack"],"description":".NET for Apache Spark technology stack diagram.","publish":1}</v>
       </c>
     </row>
-    <row r="339" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A339" s="5">
         <v>339</v>
       </c>
@@ -16473,7 +16471,7 @@
         <v>{"id":339,"title":"swimlane-dotnet-speed-bar-chart","group":"dotnet","area":"swimlane","keywords":["bar","chart","performance","speed"],"description":".NET performance comapred with others.","publish":1}</v>
       </c>
     </row>
-    <row r="340" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A340" s="5">
         <v>340</v>
       </c>
@@ -16500,7 +16498,7 @@
         <v>{"id":340,"title":"swimlane-processing-data-multi-server","group":"dotnet","area":"swimlane","keywords":["data","process","cube","clustor","node","server","connected","centralized","hub"],"description":"Large amount of data being processed with a clustor of server nodes.","publish":1}</v>
       </c>
     </row>
-    <row r="341" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A341" s="5">
         <v>341</v>
       </c>
@@ -16541,158 +16539,158 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:A30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>683</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>684</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>685</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>686</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>684</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>684</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>687</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>688</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>689</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>690</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>691</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>692</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>693</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>695</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>696</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>697</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>698</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>699</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>700</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>701</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>702</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>703</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>704</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>706</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>707</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>708</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>710</v>
       </c>
@@ -16715,22 +16713,22 @@
       <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="50" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="50" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.83203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="38.1640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.796875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.796875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="38.1328125" style="2" customWidth="1"/>
     <col min="4" max="4" width="17" style="2" customWidth="1"/>
     <col min="5" max="5" width="18" style="2" customWidth="1"/>
     <col min="6" max="6" width="33.6640625" style="2" customWidth="1"/>
     <col min="7" max="7" width="20.6640625" style="2" customWidth="1"/>
-    <col min="8" max="9" width="24.1640625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="33.1640625" style="2" customWidth="1"/>
+    <col min="8" max="9" width="24.1328125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="33.1328125" style="2" customWidth="1"/>
     <col min="11" max="11" width="66.33203125" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="9.1640625" style="2"/>
+    <col min="12" max="16384" width="9.1328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="3" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>73</v>
       </c>
@@ -16765,7 +16763,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -16799,7 +16797,7 @@
         <v>{"id":1,"title":"AzureToolsForVS","category":"VSCOM","keywords":["free","hosting","bug","tools","platforms","testing","beaker","wrench","azure","logo"],"description":"Azure developer tools for Visual Studio with free hosting.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -16833,7 +16831,7 @@
         <v>{"id":2,"title":"CloudPattern","category":"Pattern","keywords":["technology","nature","cloud","sky"],"description":"Clouds on blue sky pattern.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -16867,7 +16865,7 @@
         <v>{"id":3,"title":"CollaborationChatBubbles","category":"Diagram","keywords":["work","chat","bubble","conversation","communication","collaboration","team","men","women","people"],"description":"Several chat bubbles with people inside.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -16901,7 +16899,7 @@
         <v>{"id":4,"title":"CollaborationNetwork","category":"Diagram","keywords":["man","woman","network","hub","collaboration","connection","web","idea","lightbulb","gear","cloud","chat","bubble","work"],"description":"A network of people and objects connected together.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -16935,7 +16933,7 @@
         <v>{"id":5,"title":"CommunityTranslation1","category":"VSCOM","keywords":["hand","phone","hello","word","balloon","languages"],"description":"Translate world languages with smartphone.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -16969,7 +16967,7 @@
         <v>{"id":6,"title":"CommunityTranslation2","category":"VSCOM","keywords":["group","people","tablet","languages"],"description":"People from around the world using translation app on smart device to say hello.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -17003,7 +17001,7 @@
         <v>{"id":7,"title":"CommunityTranslation3","category":"VSCOM","keywords":["group","people","tablet","languages"],"description":"People from around the world using translation app on smart device to say hello.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -17037,7 +17035,7 @@
         <v>{"id":8,"title":"CordovaToolsTwitterBanner","category":"Web","keywords":["crane","cloud","tools","tree","build","construction"],"description":"Cordova Tools Twitter account banner. Construction crane and build tools on cloud.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -17071,7 +17069,7 @@
         <v>{"id":9,"title":"DesktopComputerPattern","category":"Pattern","keywords":["desktop","computer","monitor","pc","technology"],"description":"Desktop computer pattern.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -17105,7 +17103,7 @@
         <v>{"id":10,"title":"DevEssentials1","category":"VSCOM","keywords":["download","arrow","magnifying","glass","monitor","laptop","data","graphs","gears","newsletter"],"description":"Data visualization related elements on a cloud.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -17139,7 +17137,7 @@
         <v>{"id":11,"title":"DevEssentials2","category":"VSCOM","keywords":["download","arrow","magnifying","glass","monitor","laptop","data","graphs","gears","toolbox","newsletter"],"description":"Data visualization related elements on a cloud.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -17173,7 +17171,7 @@
         <v>{"id":12,"title":"DevicesPattern","category":"Pattern","keywords":["laptop","phone","tablet","smartphone","technology"],"description":"Mixed devices pattern.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -17207,7 +17205,7 @@
         <v>{"id":13,"title":"DevOpsLifecycle","category":"Diagram","keywords":["handshake","planning","continuous","delivery","dev","test","analytics","mobius","infinity","loop"],"description":"DevOps lifecycle.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -17241,7 +17239,7 @@
         <v>{"id":14,"title":"FeedbackCommentsDiscussion","category":"Email","keywords":["chat","bubble","question","exclaimation","conversation","discussion"],"description":"Feedback comment discussion.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -17275,7 +17273,7 @@
         <v>{"id":15,"title":"FeedbackPattern","category":"Pattern","keywords":["feedback","chat","bubble","conversation","question","exclaimation","problem","comment","talk"],"description":"Chat bubble feedback pattern.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -17309,7 +17307,7 @@
         <v>{"id":16,"title":"FoodCollection","category":"Elements","keywords":["food","meal","nutrition","soup","bread","spoon","tomato","broccli","vegetable","fish","crab","seafood","meat","poultry","steak","chicken","turkey","cake","pie","dessert","measuring","cup","egg","beater","cooking","utencils","drink","cocktail","glass","toast","cracker","cheese","burger","hotdog","salad","appetizer","entree"],"description":"A collection of food icons.","style":["color","sketchy"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -17343,7 +17341,7 @@
         <v>{"id":17,"title":"IdeaFactory","category":"Web","keywords":["factory","building","gear","lightbulb","database","arrow","document","gauge","lift","truck"],"description":"Ideas being manufactured in a factory.","style":["monotone"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -17377,7 +17375,7 @@
         <v>{"id":18,"title":"IntegratedDevelopmentLoop","category":"Email","keywords":["loop","cycle","edit","pencil","script","scroll","bug","arrow","device","phone","mobile","cloud"],"description":"Lifecycle of code, debug and deployment.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -17411,7 +17409,7 @@
         <v>{"id":19,"title":"InternetOfThings","category":"Diagram","keywords":["internet","iot","globe","router","smart","phone","laptop","light","bulb","printer","desktop","media","player","car","smart","home","smart","watch","mobile","payment","device","software","development"],"description":"The Internet of Things (IoT) is the network of physical objects or things embedded with electronics, software, sensors, and network connectivity, which enables these objects to collect and exchange data.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -17445,7 +17443,7 @@
         <v>{"id":20,"title":"ManufacturingIdeas","category":"Misc","keywords":["machine","tool","lightbulb"],"description":"Ideas being manufactured by a machine.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -17479,7 +17477,7 @@
         <v>{"id":21,"title":"MicrosoftWelcomeCenter","category":"Print","keywords":["microsoft","company","building","welcome","logo","work","business"],"description":"Microsoft logo and office buildings.","style":["color","3d"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -17513,7 +17511,7 @@
         <v>{"id":22,"title":"MobileAppDevelopmentPlatform","category":"VSCOM","keywords":["building","city","cloud","billboard","people","device","laptop","phone","database","security","lock","presentation","chart","development","platform","enterprise","business"],"description":"Mobile app development platform.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -17547,7 +17545,7 @@
         <v>{"id":23,"title":"MobileAppDevelopmentWithVisualStudio","category":"VSCOM","keywords":["laptop","phone","iphone","android","windows","app","development","visual","studio"],"description":"Cross platform mobile app development with Visual Studio.","style":["color","photo","monotone"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -17581,7 +17579,7 @@
         <v>{"id":24,"title":"MultiDeviceTwitterBanner","category":"Web","keywords":["cloud","sky","field","grass","phone","smartphone","tablet","computer","desktop","pc","monitor","tv","television","microsoft","logo","technology","developer"],"description":"Cordova Tools Twitter account banner. Four device icons overlay on top of cloud and field backgournd.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -17615,7 +17613,7 @@
         <v>{"id":25,"title":"NETCoreWebsiteBanner","category":"Web","keywords":["visual","studio","html5","css3","javascript"],"description":".NET Core website banner.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -17649,7 +17647,7 @@
         <v>{"id":26,"title":"OneToolForEverything","category":"Email","keywords":["tool","laptop","mobile","phone","cloud"],"description":"One tool for all platform.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -17683,7 +17681,7 @@
         <v>{"id":27,"title":"OpenSourceComputer","category":"Web","keywords":["laptop","code","arrow","exchange"],"description":"Two laptop exchanging code.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -17717,7 +17715,7 @@
         <v>{"id":28,"title":"OpenSourceExchangeCode","category":"Diagram","keywords":["code","man","woman","laptop","desktop","exchange","share","arrow"],"description":"Developers exchange open source code.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -17751,7 +17749,7 @@
         <v>{"id":29,"title":"PlaceholderFlowers","category":"VSTS","keywords":["flower"],"description":"Placeholder images.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -17785,7 +17783,7 @@
         <v>{"id":30,"title":"PublishAndDeploy","category":"Email","keywords":["rocket","document","arrow","exchange"],"description":"Publish and deploy code.","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -17819,7 +17817,7 @@
         <v>{"id":31,"title":"PushNotifications","category":"Web","keywords":["mobile","phone","tablet","android","windows","ios","chat","bubble","notification"],"description":"Push notifications on multiple platforms.","style":["monotone"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -17853,7 +17851,7 @@
         <v>{"id":32,"title":"PythonToolsForVS","category":"VSCOM","keywords":["man","laptop","woman","gears","bug","code","phone","python","logo","magnifying","glass"],"description":"Python tools for Visual Studio.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -17887,7 +17885,7 @@
         <v>{"id":33,"title":"QuickstartFastSpeed","category":"Email","keywords":["stopwatch","run","man","time","fast","quick","speed"],"description":"Quick start","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -17921,7 +17919,7 @@
         <v>{"id":34,"title":"RocketMulticolor","category":"Elements","keywords":["rocket","launch","deployment"],"description":"Rocket","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -17955,7 +17953,7 @@
         <v>{"id":35,"title":"RocketWithCloudPattern","category":"Print","keywords":["rocket","cloud","sky"],"description":"Rocket on sky background","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -17989,7 +17987,7 @@
         <v>{"id":36,"title":"SeattlePostcard","category":"Print","keywords":["seattle","space","needle","cloud","city"],"description":"Seattle space needle postcard","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -18023,7 +18021,7 @@
         <v>{"id":37,"title":"SeattleSkyline","category":"Web","keywords":["seattle","space","needle","cloud","city","skyline","building","mount","rainier"],"description":"Seattle city skyline","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -18057,7 +18055,7 @@
         <v>{"id":38,"title":"SeattleSkylineFerrisWheel","category":"Web","keywords":["seattle","space","needle","ferris","wheel","waterfront","port"],"description":"Seattle city skyline","style":["monotone"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -18091,7 +18089,7 @@
         <v>{"id":39,"title":"SilhouetteAirportElements","category":"Elements","keywords":["airport","pilot","flight","attendant","uniform","causeway","airplane","sign","direction","loudge","coffee","terminal","seat","life"],"description":"A collection of airport related elements.","style":["silhuoette"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -18125,7 +18123,7 @@
         <v>{"id":40,"title":"SilhouetteBriefcasesAndDocuments","category":"Elements","keywords":["document","file","paper","briefcase","suitcase","handbag","work","object","business"],"description":" A collection of briefcases.","style":["silhuoette"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -18159,7 +18157,7 @@
         <v>{"id":41,"title":"SilhouetteCharacters","category":"Elements","keywords":["man","confuse","suit","woman","chair","desk","laptop","computer","office","work","business"],"description":"A collection of characters in work environment.","style":[" ","silhuoette"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -18193,7 +18191,7 @@
         <v>{"id":42,"title":"SilhouetteHandGenstures","category":"Elements","keywords":["hand","gesture","pick","grip","pinch","touch","web","press","technology"],"description":"Hand gestures.","style":["silhuoette"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -18227,7 +18225,7 @@
         <v>{"id":43,"title":"SilhouetteTabletAndPhones","category":"Elements","keywords":["technology","work","tablet","smartphone","phone","mobile","phone","pen","stylus","windows","phone","android","phone","surface","tablet"],"description":"Tablet and smartphones.","style":["silhuoette"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -18261,7 +18259,7 @@
         <v>{"id":44,"title":"SilhouetteToolCollection","category":"Pattern","keywords":["wrench","screwdriver","saw","plier","hammer","knife","c","clamp","clamp","pipe","wrench","filer","triangle","ruler","object"],"description":"A collection of hand tools.","style":["silhouette"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -18295,7 +18293,7 @@
         <v>{"id":45,"title":"SilhouetteWeatherReportElements","category":"Elements","keywords":["life","newspaper","radio","magezine","clock","news","weather","forcast","tv","sun","sunny","cloud","lightning","thunder","cloud","cloudy","rain","tripical","palm","tree","beach","table","vacation","beach","chair","hawaii","man","relax","drink"],"description":"A collection of weather related illustrations.","style":["silhuoette"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -18329,7 +18327,7 @@
         <v>{"id":46,"title":"SoftwareToolsSampleKit","category":"Email","keywords":["toolbox","hammer","checklist","wrench","cloud"],"description":"Software development toolkit","style":["color"],"artist":"Bethel Blakesley","publish":1}</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -18363,7 +18361,7 @@
         <v>{"id":47,"title":"TeamworkStairs","category":"Web","keywords":["people","man","stairs","team"],"description":"People holding hands climbing up stairs as a team.","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -18397,7 +18395,7 @@
         <v>{"id":48,"title":"Testing","category":"Email","keywords":["test","flask","lab","beaker","stopwatch","pie","chart","checklist"],"description":"Testing","style":["color"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -18431,7 +18429,7 @@
         <v>{"id":49,"title":"VSBuildALMIntegration","category":"VSCOM","keywords":["people","working","man","computer","clipboard","debug","tools","gear","bug"],"description":"ALM (Application Lifecycle Management) debug integration.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -18465,7 +18463,7 @@
         <v>{"id":50,"title":"VSBuildCloudHostedTools","category":"VSCOM","keywords":["people","laptops","desk","workers","monitors","laptops","cross","platforms","linux","windows","ios"],"description":"Developers come from different platforms and technology stacks working together.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -18499,7 +18497,7 @@
         <v>{"id":51,"title":"VSBuildContinuousIntegration","category":"VSCOM","keywords":["monitor","laptop","test","tubes","gears","checkmark"],"description":"Build continuous integration cycle with cloud.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -18533,7 +18531,7 @@
         <v>{"id":52,"title":"VSBuildContinuousIntegrationWhite","category":"VSCOM","keywords":["cross","platforms","maven","git","apache","ant","junit","gradle","xunit","mtm","test","building"],"description":"Common tools and technologies for cross-platform development.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -18567,7 +18565,7 @@
         <v>{"id":53,"title":"VSBuildCrossPlatform","category":"VSCOM","keywords":["pillars","cross","platforms","buildings","crane","java",".net","xcode","github","ios","android","windows","git"],"description":"Common tools and technologies for cross-platform development.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -18601,7 +18599,7 @@
         <v>{"id":54,"title":"VSBuildOverview","category":"VSCOM","keywords":["cross","platforms","laptop","tablet","phone","ios","android","visual","studio","cloud"],"description":"Visual Studio for building cross-platform applications.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -18635,7 +18633,7 @@
         <v>{"id":55,"title":"VSBuildTraceability","category":"VSCOM","keywords":["blueprint","document","man","beaker","tools","clipboard","timeline","printer","download","test","tubes","gears","magnifying","glass","graphs"],"description":"Build timeline and tracebility.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -18669,7 +18667,7 @@
         <v>{"id":56,"title":"VSDownload1","category":"VSCOM","keywords":["group","people","visual","studio","logo","flags","man","woman"],"description":"Visual Studio for everyone.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -18703,7 +18701,7 @@
         <v>{"id":57,"title":"VSDownload2","category":"VSCOM","keywords":["man","monitors","download","down","arrow","computer","table"],"description":"Visual Studio tools for multiplatform.","style":["color"],"artist":"Don Baker","publish":1}</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -18737,302 +18735,302 @@
         <v>{"id":58,"title":"XamarinCrossPlatformDevelopment","category":"VSCOM","keywords":["screenshot","ios","android","windows","mobile","phone","app","development","shared","code","cross-platform","xamarin"],"description":"Xamarin for developing cross-platform application.","style":["color","photo"],"artist":"Christine Daughtry","publish":1}</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A60" s="2">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A61" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A62" s="2">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A63" s="2">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A64" s="2">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A65" s="2">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A66" s="2">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A67" s="2">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A68" s="2">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A69" s="2">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A70" s="2">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A71" s="2">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A72" s="2">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A73" s="2">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A74" s="2">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A75" s="2">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A76" s="2">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A77" s="2">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A78" s="2">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A79" s="2">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A80" s="2">
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A81" s="2">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A82" s="2">
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A83" s="2">
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A84" s="2">
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A85" s="2">
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A86" s="2">
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A87" s="2">
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A88" s="2">
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A89" s="2">
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A90" s="2">
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A91" s="2">
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A92" s="2">
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A93" s="2">
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A94" s="2">
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A95" s="2">
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A96" s="2">
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A97" s="2">
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A98" s="2">
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A99" s="2">
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A100" s="2">
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A101" s="2">
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A102" s="2">
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A103" s="2">
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A104" s="2">
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A105" s="2">
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A106" s="2">
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A107" s="2">
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A108" s="2">
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A109" s="2">
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A110" s="2">
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A111" s="2">
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A112" s="2">
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A113" s="2">
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A114" s="2">
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A115" s="2">
         <v>114</v>
       </c>
     </row>
-    <row r="116" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A116" s="2">
         <v>115</v>
       </c>
     </row>
-    <row r="117" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A117" s="2">
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A118" s="2">
         <v>117</v>
       </c>
     </row>
-    <row r="119" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A119" s="2">
         <v>118</v>
       </c>
@@ -19068,9 +19066,9 @@
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="1" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>